<commit_message>
Auto refresh PaceSmart output
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -549,10 +549,10 @@
         <v>45826</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G2" t="n">
         <v>100350.37</v>
@@ -611,51 +611,51 @@
         <v>46071</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G3" t="n">
         <v>552594.63</v>
       </c>
       <c r="H3" t="n">
-        <v>365775.27</v>
+        <v>449512.12</v>
       </c>
       <c r="I3" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J3" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K3" t="n">
-        <v>414445.97</v>
+        <v>434181.49</v>
       </c>
       <c r="L3" t="n">
-        <v>88.26000000000001</v>
+        <v>103.53</v>
       </c>
       <c r="M3" t="n">
-        <v>186819.36</v>
+        <v>103082.51</v>
       </c>
       <c r="N3" t="n">
-        <v>13344.24</v>
+        <v>8590.209999999999</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>Overdelivered</t>
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>103082.51</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -677,10 +677,10 @@
         <v>45984</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G4" t="n">
         <v>294540.38</v>
@@ -739,10 +739,10 @@
         <v>45811</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G5" t="n">
         <v>509097.37</v>
@@ -801,10 +801,10 @@
         <v>45997</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G6" t="n">
         <v>382409.25</v>
@@ -863,10 +863,10 @@
         <v>46005</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G7" t="n">
         <v>525695.9399999999</v>
@@ -925,38 +925,38 @@
         <v>46102</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G8" t="n">
         <v>136840.92</v>
       </c>
       <c r="H8" t="n">
-        <v>33693.23</v>
+        <v>34460.47</v>
       </c>
       <c r="I8" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J8" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K8" t="n">
-        <v>32470.73</v>
+        <v>37109.4</v>
       </c>
       <c r="L8" t="n">
-        <v>103.76</v>
+        <v>92.86</v>
       </c>
       <c r="M8" t="n">
-        <v>103147.69</v>
+        <v>102380.45</v>
       </c>
       <c r="N8" t="n">
-        <v>2292.17</v>
+        <v>2380.94</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>On Track</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -991,10 +991,10 @@
         <v>46119</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G9" t="n">
         <v>380340.09</v>
@@ -1053,38 +1053,38 @@
         <v>46103</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G10" t="n">
         <v>448858.15</v>
       </c>
       <c r="H10" t="n">
-        <v>82310.69</v>
+        <v>90191.59</v>
       </c>
       <c r="I10" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J10" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K10" t="n">
-        <v>86621.75</v>
+        <v>102371.16</v>
       </c>
       <c r="L10" t="n">
-        <v>95.02</v>
+        <v>88.09999999999999</v>
       </c>
       <c r="M10" t="n">
-        <v>366547.46</v>
+        <v>358666.56</v>
       </c>
       <c r="N10" t="n">
-        <v>7968.42</v>
+        <v>8151.51</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>On Track</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1119,10 +1119,10 @@
         <v>46172</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G11" t="n">
         <v>432209.99</v>
@@ -1181,34 +1181,34 @@
         <v>46105</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G12" t="n">
         <v>559806.73</v>
       </c>
       <c r="H12" t="n">
-        <v>205719.64</v>
+        <v>209956.21</v>
       </c>
       <c r="I12" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J12" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K12" t="n">
-        <v>232114.99</v>
+        <v>245768.81</v>
       </c>
       <c r="L12" t="n">
-        <v>88.63</v>
+        <v>85.43000000000001</v>
       </c>
       <c r="M12" t="n">
-        <v>354087.09</v>
+        <v>349850.52</v>
       </c>
       <c r="N12" t="n">
-        <v>7376.81</v>
+        <v>7605.45</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1247,34 +1247,34 @@
         <v>46118</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G13" t="n">
         <v>169377.54</v>
       </c>
       <c r="H13" t="n">
-        <v>43755.62</v>
+        <v>48203.28</v>
       </c>
       <c r="I13" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J13" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K13" t="n">
-        <v>41821.61</v>
+        <v>46003.78</v>
       </c>
       <c r="L13" t="n">
-        <v>104.62</v>
+        <v>104.78</v>
       </c>
       <c r="M13" t="n">
-        <v>125621.92</v>
+        <v>121174.26</v>
       </c>
       <c r="N13" t="n">
-        <v>2059.38</v>
+        <v>2053.8</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1283,15 +1283,15 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>On Track</t>
+          <t>Overdelivered</t>
         </is>
       </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>121174.26</v>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1313,10 +1313,10 @@
         <v>45875</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G14" t="n">
         <v>334936.09</v>
@@ -1375,10 +1375,10 @@
         <v>46176</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G15" t="n">
         <v>394703.48</v>
@@ -1437,10 +1437,10 @@
         <v>45766</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G16" t="n">
         <v>161605.1</v>
@@ -1499,10 +1499,10 @@
         <v>45778</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G17" t="n">
         <v>95583.81</v>
@@ -1561,10 +1561,10 @@
         <v>46196</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G18" t="n">
         <v>253564.24</v>
@@ -1623,10 +1623,10 @@
         <v>46204</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G19" t="n">
         <v>111100.55</v>
@@ -1685,34 +1685,34 @@
         <v>46112</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G20" t="n">
         <v>423679.91</v>
       </c>
       <c r="H20" t="n">
-        <v>145595.79</v>
+        <v>156172.13</v>
       </c>
       <c r="I20" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J20" t="n">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K20" t="n">
-        <v>164764.41</v>
+        <v>174179.52</v>
       </c>
       <c r="L20" t="n">
-        <v>88.37</v>
+        <v>89.66</v>
       </c>
       <c r="M20" t="n">
-        <v>278084.12</v>
+        <v>267507.78</v>
       </c>
       <c r="N20" t="n">
-        <v>5056.07</v>
+        <v>5047.32</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1751,10 +1751,10 @@
         <v>46179</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G21" t="n">
         <v>224412.65</v>
@@ -1813,10 +1813,10 @@
         <v>46129</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G22" t="n">
         <v>568840.5</v>
@@ -1875,10 +1875,10 @@
         <v>45969</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G23" t="n">
         <v>105951.07</v>
@@ -1937,10 +1937,10 @@
         <v>45902</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G24" t="n">
         <v>280248.59</v>
@@ -1999,10 +1999,10 @@
         <v>45943</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G25" t="n">
         <v>285863.23</v>
@@ -2061,10 +2061,10 @@
         <v>45808</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G26" t="n">
         <v>221171.06</v>
@@ -2123,51 +2123,51 @@
         <v>46092</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G27" t="n">
         <v>577808.88</v>
       </c>
       <c r="H27" t="n">
-        <v>307670.16</v>
+        <v>361627.27</v>
       </c>
       <c r="I27" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J27" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K27" t="n">
-        <v>334154.53</v>
+        <v>348077.64</v>
       </c>
       <c r="L27" t="n">
-        <v>92.06999999999999</v>
+        <v>103.89</v>
       </c>
       <c r="M27" t="n">
-        <v>270138.72</v>
+        <v>216181.61</v>
       </c>
       <c r="N27" t="n">
-        <v>7718.25</v>
+        <v>6550.96</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>Overdelivered</t>
         </is>
       </c>
       <c r="Q27" t="n">
-        <v>0</v>
+        <v>216181.61</v>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2189,10 +2189,10 @@
         <v>45938</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G28" t="n">
         <v>196777.36</v>
@@ -2251,10 +2251,10 @@
         <v>45780</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G29" t="n">
         <v>170730.01</v>
@@ -2313,10 +2313,10 @@
         <v>45954</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G30" t="n">
         <v>355660.26</v>
@@ -2375,10 +2375,10 @@
         <v>45765</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G31" t="n">
         <v>418857.39</v>
@@ -2437,34 +2437,34 @@
         <v>46117</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G32" t="n">
         <v>574740.27</v>
       </c>
       <c r="H32" t="n">
-        <v>209100.37</v>
+        <v>243681.7</v>
       </c>
       <c r="I32" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J32" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K32" t="n">
-        <v>287370.14</v>
+        <v>296949.14</v>
       </c>
       <c r="L32" t="n">
-        <v>72.76000000000001</v>
+        <v>82.06</v>
       </c>
       <c r="M32" t="n">
-        <v>365639.9</v>
+        <v>331058.57</v>
       </c>
       <c r="N32" t="n">
-        <v>6094</v>
+        <v>5707.91</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2503,34 +2503,34 @@
         <v>46093</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G33" t="n">
         <v>129356.97</v>
       </c>
       <c r="H33" t="n">
-        <v>50696.42</v>
+        <v>54101.04</v>
       </c>
       <c r="I33" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J33" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K33" t="n">
-        <v>58798.62</v>
+        <v>62718.53</v>
       </c>
       <c r="L33" t="n">
-        <v>86.22</v>
+        <v>86.26000000000001</v>
       </c>
       <c r="M33" t="n">
-        <v>78660.55</v>
+        <v>75255.92999999999</v>
       </c>
       <c r="N33" t="n">
-        <v>2185.02</v>
+        <v>2213.41</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2569,10 +2569,10 @@
         <v>45931</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G34" t="n">
         <v>591950.49</v>
@@ -2631,10 +2631,10 @@
         <v>45972</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G35" t="n">
         <v>390381.81</v>
@@ -2693,10 +2693,10 @@
         <v>45951</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G36" t="n">
         <v>128268.79</v>
@@ -2755,10 +2755,10 @@
         <v>46095</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G37" t="n">
         <v>534024.5</v>
@@ -2817,10 +2817,10 @@
         <v>45899</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G38" t="n">
         <v>391196.57</v>
@@ -2879,10 +2879,10 @@
         <v>45969</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G39" t="n">
         <v>596378.9300000001</v>
@@ -2941,34 +2941,34 @@
         <v>46087</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G40" t="n">
         <v>120089.45</v>
       </c>
       <c r="H40" t="n">
-        <v>44964.8</v>
+        <v>46798.99</v>
       </c>
       <c r="I40" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J40" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K40" t="n">
-        <v>64663.55</v>
+        <v>68358.61</v>
       </c>
       <c r="L40" t="n">
-        <v>69.54000000000001</v>
+        <v>68.45999999999999</v>
       </c>
       <c r="M40" t="n">
-        <v>75124.64999999999</v>
+        <v>73290.46000000001</v>
       </c>
       <c r="N40" t="n">
-        <v>2504.15</v>
+        <v>2617.52</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3007,10 +3007,10 @@
         <v>46159</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G41" t="n">
         <v>326276.52</v>
@@ -3069,10 +3069,10 @@
         <v>46111</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G42" t="n">
         <v>574267.4300000001</v>
@@ -3131,10 +3131,10 @@
         <v>46015</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G43" t="n">
         <v>352257.46</v>
@@ -3193,10 +3193,10 @@
         <v>46182</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G44" t="n">
         <v>267517.39</v>
@@ -3255,51 +3255,51 @@
         <v>46082</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G45" t="n">
         <v>354611.01</v>
       </c>
       <c r="H45" t="n">
-        <v>215201.68</v>
+        <v>251835.04</v>
       </c>
       <c r="I45" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J45" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K45" t="n">
-        <v>242392.34</v>
+        <v>251369.83</v>
       </c>
       <c r="L45" t="n">
-        <v>88.78</v>
+        <v>100.19</v>
       </c>
       <c r="M45" t="n">
-        <v>139409.33</v>
+        <v>102775.97</v>
       </c>
       <c r="N45" t="n">
-        <v>5576.37</v>
+        <v>4468.52</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>Overdelivered</t>
         </is>
       </c>
       <c r="Q45" t="n">
-        <v>0</v>
+        <v>102775.97</v>
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3321,10 +3321,10 @@
         <v>46135</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>46058</v>
+        <v>46060</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="G46" t="n">
         <v>498191.26</v>
@@ -3514,7 +3514,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -3524,7 +3524,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -3534,7 +3534,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -3544,7 +3544,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>543214.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update pacing data till yesterday (ML vs Excel case)
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -558,7 +558,7 @@
         <v>100350.37</v>
       </c>
       <c r="H2" t="n">
-        <v>110279.38</v>
+        <v>100271.72</v>
       </c>
       <c r="I2" t="n">
         <v>104</v>
@@ -570,17 +570,17 @@
         <v>100350.37</v>
       </c>
       <c r="L2" t="n">
-        <v>109.89</v>
+        <v>99.92</v>
       </c>
       <c r="M2" t="n">
-        <v>-9929.01</v>
+        <v>78.65000000000001</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P2" t="inlineStr"/>
@@ -620,7 +620,7 @@
         <v>552594.63</v>
       </c>
       <c r="H3" t="n">
-        <v>532503.95</v>
+        <v>445313.96</v>
       </c>
       <c r="I3" t="n">
         <v>45</v>
@@ -632,26 +632,26 @@
         <v>444049.26</v>
       </c>
       <c r="L3" t="n">
-        <v>119.92</v>
+        <v>100.28</v>
       </c>
       <c r="M3" t="n">
-        <v>20090.68</v>
+        <v>107280.67</v>
       </c>
       <c r="N3" t="n">
-        <v>1826.43</v>
+        <v>9752.790000000001</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Overdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>20090.68000000005</v>
+        <v>0</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
@@ -686,7 +686,7 @@
         <v>294540.38</v>
       </c>
       <c r="H4" t="n">
-        <v>340164.4</v>
+        <v>294599.18</v>
       </c>
       <c r="I4" t="n">
         <v>76</v>
@@ -698,17 +698,17 @@
         <v>294540.38</v>
       </c>
       <c r="L4" t="n">
-        <v>115.49</v>
+        <v>100.02</v>
       </c>
       <c r="M4" t="n">
-        <v>-45624.02</v>
+        <v>-58.8</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P4" t="inlineStr"/>
@@ -748,7 +748,7 @@
         <v>509097.37</v>
       </c>
       <c r="H5" t="n">
-        <v>397460.02</v>
+        <v>503642.69</v>
       </c>
       <c r="I5" t="n">
         <v>28</v>
@@ -760,17 +760,17 @@
         <v>509097.37</v>
       </c>
       <c r="L5" t="n">
-        <v>78.06999999999999</v>
+        <v>98.93000000000001</v>
       </c>
       <c r="M5" t="n">
-        <v>111637.35</v>
+        <v>5454.68</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P5" t="inlineStr"/>
@@ -810,7 +810,7 @@
         <v>382409.25</v>
       </c>
       <c r="H6" t="n">
-        <v>376005.59</v>
+        <v>373866.06</v>
       </c>
       <c r="I6" t="n">
         <v>94</v>
@@ -822,10 +822,10 @@
         <v>382409.25</v>
       </c>
       <c r="L6" t="n">
-        <v>98.33</v>
+        <v>97.77</v>
       </c>
       <c r="M6" t="n">
-        <v>6403.66</v>
+        <v>8543.190000000001</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
@@ -872,7 +872,7 @@
         <v>525695.9399999999</v>
       </c>
       <c r="H7" t="n">
-        <v>450368.71</v>
+        <v>511982.16</v>
       </c>
       <c r="I7" t="n">
         <v>92</v>
@@ -884,17 +884,17 @@
         <v>525695.9399999999</v>
       </c>
       <c r="L7" t="n">
-        <v>85.67</v>
+        <v>97.39</v>
       </c>
       <c r="M7" t="n">
-        <v>75327.23</v>
+        <v>13713.78</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P7" t="inlineStr"/>
@@ -934,7 +934,7 @@
         <v>136840.92</v>
       </c>
       <c r="H8" t="n">
-        <v>54460.47</v>
+        <v>63085.98</v>
       </c>
       <c r="I8" t="n">
         <v>17</v>
@@ -946,13 +946,13 @@
         <v>39428.74</v>
       </c>
       <c r="L8" t="n">
-        <v>138.12</v>
+        <v>160</v>
       </c>
       <c r="M8" t="n">
-        <v>82380.45</v>
+        <v>73754.94</v>
       </c>
       <c r="N8" t="n">
-        <v>1961.44</v>
+        <v>1756.07</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -961,11 +961,11 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Overdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>82380.45000000001</v>
+        <v>0</v>
       </c>
       <c r="R8" t="inlineStr">
         <is>
@@ -1062,7 +1062,7 @@
         <v>448858.15</v>
       </c>
       <c r="H10" t="n">
-        <v>101191.59</v>
+        <v>110328</v>
       </c>
       <c r="I10" t="n">
         <v>14</v>
@@ -1074,22 +1074,22 @@
         <v>110245.86</v>
       </c>
       <c r="L10" t="n">
-        <v>91.79000000000001</v>
+        <v>100.07</v>
       </c>
       <c r="M10" t="n">
-        <v>347666.56</v>
+        <v>338530.15</v>
       </c>
       <c r="N10" t="n">
-        <v>8085.27</v>
+        <v>7872.79</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="Q10" t="n">
@@ -1190,7 +1190,7 @@
         <v>559806.73</v>
       </c>
       <c r="H12" t="n">
-        <v>212956.21</v>
+        <v>250343.25</v>
       </c>
       <c r="I12" t="n">
         <v>37</v>
@@ -1202,22 +1202,22 @@
         <v>252595.72</v>
       </c>
       <c r="L12" t="n">
-        <v>84.31</v>
+        <v>99.11</v>
       </c>
       <c r="M12" t="n">
-        <v>346850.52</v>
+        <v>309463.48</v>
       </c>
       <c r="N12" t="n">
-        <v>7707.79</v>
+        <v>6876.97</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="Q12" t="n">
@@ -1256,7 +1256,7 @@
         <v>169377.54</v>
       </c>
       <c r="H13" t="n">
-        <v>69760.03</v>
+        <v>51709.52</v>
       </c>
       <c r="I13" t="n">
         <v>23</v>
@@ -1268,13 +1268,13 @@
         <v>48094.86</v>
       </c>
       <c r="L13" t="n">
-        <v>145.05</v>
+        <v>107.52</v>
       </c>
       <c r="M13" t="n">
-        <v>99617.50999999999</v>
+        <v>117668.02</v>
       </c>
       <c r="N13" t="n">
-        <v>1717.54</v>
+        <v>2028.76</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1283,11 +1283,11 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Overdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="Q13" t="n">
-        <v>99617.51000000001</v>
+        <v>0</v>
       </c>
       <c r="R13" t="inlineStr">
         <is>
@@ -1322,7 +1322,7 @@
         <v>334936.09</v>
       </c>
       <c r="H14" t="n">
-        <v>421968.26</v>
+        <v>335066.17</v>
       </c>
       <c r="I14" t="n">
         <v>88</v>
@@ -1334,17 +1334,17 @@
         <v>334936.09</v>
       </c>
       <c r="L14" t="n">
-        <v>125.98</v>
+        <v>100.04</v>
       </c>
       <c r="M14" t="n">
-        <v>-87032.17</v>
+        <v>-130.08</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P14" t="inlineStr"/>
@@ -1446,7 +1446,7 @@
         <v>161605.1</v>
       </c>
       <c r="H16" t="n">
-        <v>161797.21</v>
+        <v>158329.38</v>
       </c>
       <c r="I16" t="n">
         <v>74</v>
@@ -1458,10 +1458,10 @@
         <v>161605.1</v>
       </c>
       <c r="L16" t="n">
-        <v>100.12</v>
+        <v>97.97</v>
       </c>
       <c r="M16" t="n">
-        <v>-192.11</v>
+        <v>3275.72</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
@@ -1508,7 +1508,7 @@
         <v>95583.81</v>
       </c>
       <c r="H17" t="n">
-        <v>69102.67999999999</v>
+        <v>96927.23</v>
       </c>
       <c r="I17" t="n">
         <v>74</v>
@@ -1520,17 +1520,17 @@
         <v>95583.81</v>
       </c>
       <c r="L17" t="n">
-        <v>72.3</v>
+        <v>101.41</v>
       </c>
       <c r="M17" t="n">
-        <v>26481.13</v>
+        <v>-1343.42</v>
       </c>
       <c r="N17" t="n">
         <v>0</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P17" t="inlineStr"/>
@@ -1694,7 +1694,7 @@
         <v>423679.91</v>
       </c>
       <c r="H20" t="n">
-        <v>160569.68</v>
+        <v>239614.62</v>
       </c>
       <c r="I20" t="n">
         <v>38</v>
@@ -1706,22 +1706,22 @@
         <v>178887.07</v>
       </c>
       <c r="L20" t="n">
-        <v>89.76000000000001</v>
+        <v>133.95</v>
       </c>
       <c r="M20" t="n">
-        <v>263110.23</v>
+        <v>184065.29</v>
       </c>
       <c r="N20" t="n">
-        <v>5059.81</v>
+        <v>3539.72</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>Overpacing</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="Q20" t="n">
@@ -1884,7 +1884,7 @@
         <v>105951.07</v>
       </c>
       <c r="H23" t="n">
-        <v>79078.86</v>
+        <v>106044.44</v>
       </c>
       <c r="I23" t="n">
         <v>84</v>
@@ -1896,17 +1896,17 @@
         <v>105951.07</v>
       </c>
       <c r="L23" t="n">
-        <v>74.64</v>
+        <v>100.09</v>
       </c>
       <c r="M23" t="n">
-        <v>26872.21</v>
+        <v>-93.37</v>
       </c>
       <c r="N23" t="n">
         <v>0</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P23" t="inlineStr"/>
@@ -1946,7 +1946,7 @@
         <v>280248.59</v>
       </c>
       <c r="H24" t="n">
-        <v>252857.94</v>
+        <v>274327.61</v>
       </c>
       <c r="I24" t="n">
         <v>71</v>
@@ -1958,17 +1958,17 @@
         <v>280248.59</v>
       </c>
       <c r="L24" t="n">
-        <v>90.23</v>
+        <v>97.89</v>
       </c>
       <c r="M24" t="n">
-        <v>27390.65</v>
+        <v>5920.98</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P24" t="inlineStr"/>
@@ -2008,7 +2008,7 @@
         <v>285863.23</v>
       </c>
       <c r="H25" t="n">
-        <v>223369.82</v>
+        <v>287064.14</v>
       </c>
       <c r="I25" t="n">
         <v>78</v>
@@ -2020,17 +2020,17 @@
         <v>285863.23</v>
       </c>
       <c r="L25" t="n">
-        <v>78.14</v>
+        <v>100.42</v>
       </c>
       <c r="M25" t="n">
-        <v>62493.41</v>
+        <v>-1200.91</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P25" t="inlineStr"/>
@@ -2070,7 +2070,7 @@
         <v>221171.06</v>
       </c>
       <c r="H26" t="n">
-        <v>236076.73</v>
+        <v>235916.39</v>
       </c>
       <c r="I26" t="n">
         <v>91</v>
@@ -2082,10 +2082,10 @@
         <v>221171.06</v>
       </c>
       <c r="L26" t="n">
-        <v>106.74</v>
+        <v>106.67</v>
       </c>
       <c r="M26" t="n">
-        <v>-14905.67</v>
+        <v>-14745.33</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
@@ -2132,7 +2132,7 @@
         <v>577808.88</v>
       </c>
       <c r="H27" t="n">
-        <v>438028.23</v>
+        <v>233908.29</v>
       </c>
       <c r="I27" t="n">
         <v>51</v>
@@ -2144,26 +2144,26 @@
         <v>355039.19</v>
       </c>
       <c r="L27" t="n">
-        <v>123.37</v>
+        <v>65.88</v>
       </c>
       <c r="M27" t="n">
-        <v>139780.65</v>
+        <v>343900.59</v>
       </c>
       <c r="N27" t="n">
-        <v>4368.15</v>
+        <v>10746.89</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Overdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="Q27" t="n">
-        <v>139780.65</v>
+        <v>0</v>
       </c>
       <c r="R27" t="inlineStr">
         <is>
@@ -2198,7 +2198,7 @@
         <v>196777.36</v>
       </c>
       <c r="H28" t="n">
-        <v>234386.42</v>
+        <v>198664.26</v>
       </c>
       <c r="I28" t="n">
         <v>40</v>
@@ -2210,17 +2210,17 @@
         <v>196777.36</v>
       </c>
       <c r="L28" t="n">
-        <v>119.11</v>
+        <v>100.96</v>
       </c>
       <c r="M28" t="n">
-        <v>-37609.06</v>
+        <v>-1886.9</v>
       </c>
       <c r="N28" t="n">
         <v>0</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P28" t="inlineStr"/>
@@ -2260,7 +2260,7 @@
         <v>170730.01</v>
       </c>
       <c r="H29" t="n">
-        <v>172494.89</v>
+        <v>162193.44</v>
       </c>
       <c r="I29" t="n">
         <v>96</v>
@@ -2272,17 +2272,17 @@
         <v>170730.01</v>
       </c>
       <c r="L29" t="n">
-        <v>101.03</v>
+        <v>95</v>
       </c>
       <c r="M29" t="n">
-        <v>-1764.88</v>
+        <v>8536.57</v>
       </c>
       <c r="N29" t="n">
         <v>0</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>On Track</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P29" t="inlineStr"/>
@@ -2322,7 +2322,7 @@
         <v>355660.26</v>
       </c>
       <c r="H30" t="n">
-        <v>443142.64</v>
+        <v>348450.7</v>
       </c>
       <c r="I30" t="n">
         <v>74</v>
@@ -2334,17 +2334,17 @@
         <v>355660.26</v>
       </c>
       <c r="L30" t="n">
-        <v>124.6</v>
+        <v>97.97</v>
       </c>
       <c r="M30" t="n">
-        <v>-87482.38</v>
+        <v>7209.56</v>
       </c>
       <c r="N30" t="n">
         <v>0</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P30" t="inlineStr"/>
@@ -2384,7 +2384,7 @@
         <v>418857.39</v>
       </c>
       <c r="H31" t="n">
-        <v>321029</v>
+        <v>406291.6</v>
       </c>
       <c r="I31" t="n">
         <v>100</v>
@@ -2396,17 +2396,17 @@
         <v>418857.39</v>
       </c>
       <c r="L31" t="n">
-        <v>76.64</v>
+        <v>97</v>
       </c>
       <c r="M31" t="n">
-        <v>97828.39</v>
+        <v>12565.79</v>
       </c>
       <c r="N31" t="n">
         <v>0</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P31" t="inlineStr"/>
@@ -2446,7 +2446,7 @@
         <v>574740.27</v>
       </c>
       <c r="H32" t="n">
-        <v>266945.09</v>
+        <v>366396.75</v>
       </c>
       <c r="I32" t="n">
         <v>63</v>
@@ -2458,22 +2458,22 @@
         <v>301738.64</v>
       </c>
       <c r="L32" t="n">
-        <v>88.47</v>
+        <v>121.43</v>
       </c>
       <c r="M32" t="n">
-        <v>307795.18</v>
+        <v>208343.52</v>
       </c>
       <c r="N32" t="n">
-        <v>5399.92</v>
+        <v>3655.15</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>Overpacing</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="Q32" t="n">
@@ -2512,7 +2512,7 @@
         <v>129356.97</v>
       </c>
       <c r="H33" t="n">
-        <v>54101.04</v>
+        <v>66136.17</v>
       </c>
       <c r="I33" t="n">
         <v>33</v>
@@ -2524,22 +2524,22 @@
         <v>64678.49</v>
       </c>
       <c r="L33" t="n">
-        <v>83.65000000000001</v>
+        <v>102.25</v>
       </c>
       <c r="M33" t="n">
-        <v>75255.92999999999</v>
+        <v>63220.8</v>
       </c>
       <c r="N33" t="n">
-        <v>2280.48</v>
+        <v>1915.78</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="Q33" t="n">
@@ -2578,7 +2578,7 @@
         <v>591950.49</v>
       </c>
       <c r="H34" t="n">
-        <v>559032.9</v>
+        <v>553167.48</v>
       </c>
       <c r="I34" t="n">
         <v>29</v>
@@ -2590,10 +2590,10 @@
         <v>591950.49</v>
       </c>
       <c r="L34" t="n">
-        <v>94.44</v>
+        <v>93.45</v>
       </c>
       <c r="M34" t="n">
-        <v>32917.59</v>
+        <v>38783.01</v>
       </c>
       <c r="N34" t="n">
         <v>0</v>
@@ -2640,7 +2640,7 @@
         <v>390381.81</v>
       </c>
       <c r="H35" t="n">
-        <v>350234.26</v>
+        <v>383062.2</v>
       </c>
       <c r="I35" t="n">
         <v>64</v>
@@ -2652,17 +2652,17 @@
         <v>390381.81</v>
       </c>
       <c r="L35" t="n">
-        <v>89.72</v>
+        <v>98.13</v>
       </c>
       <c r="M35" t="n">
-        <v>40147.55</v>
+        <v>7319.61</v>
       </c>
       <c r="N35" t="n">
         <v>0</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P35" t="inlineStr"/>
@@ -2702,7 +2702,7 @@
         <v>128268.79</v>
       </c>
       <c r="H36" t="n">
-        <v>112175.11</v>
+        <v>124810.24</v>
       </c>
       <c r="I36" t="n">
         <v>89</v>
@@ -2714,17 +2714,17 @@
         <v>128268.79</v>
       </c>
       <c r="L36" t="n">
-        <v>87.45</v>
+        <v>97.3</v>
       </c>
       <c r="M36" t="n">
-        <v>16093.68</v>
+        <v>3458.55</v>
       </c>
       <c r="N36" t="n">
         <v>0</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P36" t="inlineStr"/>
@@ -2826,7 +2826,7 @@
         <v>391196.57</v>
       </c>
       <c r="H38" t="n">
-        <v>377592.67</v>
+        <v>422599.07</v>
       </c>
       <c r="I38" t="n">
         <v>65</v>
@@ -2838,17 +2838,17 @@
         <v>391196.57</v>
       </c>
       <c r="L38" t="n">
-        <v>96.52</v>
+        <v>108.03</v>
       </c>
       <c r="M38" t="n">
-        <v>13603.9</v>
+        <v>-31402.5</v>
       </c>
       <c r="N38" t="n">
         <v>0</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>On Track</t>
+          <t>Overpacing</t>
         </is>
       </c>
       <c r="P38" t="inlineStr"/>
@@ -2888,7 +2888,7 @@
         <v>596378.9300000001</v>
       </c>
       <c r="H39" t="n">
-        <v>648669.52</v>
+        <v>593681.45</v>
       </c>
       <c r="I39" t="n">
         <v>83</v>
@@ -2900,17 +2900,17 @@
         <v>596378.9300000001</v>
       </c>
       <c r="L39" t="n">
-        <v>108.77</v>
+        <v>99.55</v>
       </c>
       <c r="M39" t="n">
-        <v>-52290.59</v>
+        <v>2697.48</v>
       </c>
       <c r="N39" t="n">
         <v>0</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P39" t="inlineStr"/>
@@ -2950,7 +2950,7 @@
         <v>120089.45</v>
       </c>
       <c r="H40" t="n">
-        <v>46798.99</v>
+        <v>43416.78</v>
       </c>
       <c r="I40" t="n">
         <v>38</v>
@@ -2962,13 +2962,13 @@
         <v>70206.14</v>
       </c>
       <c r="L40" t="n">
-        <v>66.66</v>
+        <v>61.84</v>
       </c>
       <c r="M40" t="n">
-        <v>73290.46000000001</v>
+        <v>76672.67</v>
       </c>
       <c r="N40" t="n">
-        <v>2714.46</v>
+        <v>2839.73</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="Q40" t="n">
@@ -3140,7 +3140,7 @@
         <v>352257.46</v>
       </c>
       <c r="H43" t="n">
-        <v>428418.67</v>
+        <v>334645.05</v>
       </c>
       <c r="I43" t="n">
         <v>118</v>
@@ -3152,17 +3152,17 @@
         <v>352257.46</v>
       </c>
       <c r="L43" t="n">
-        <v>121.62</v>
+        <v>95</v>
       </c>
       <c r="M43" t="n">
-        <v>-76161.21000000001</v>
+        <v>17612.41</v>
       </c>
       <c r="N43" t="n">
         <v>0</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P43" t="inlineStr"/>
@@ -3264,7 +3264,7 @@
         <v>354611.01</v>
       </c>
       <c r="H45" t="n">
-        <v>275754.89</v>
+        <v>196607.05</v>
       </c>
       <c r="I45" t="n">
         <v>57</v>
@@ -3276,26 +3276,26 @@
         <v>255858.58</v>
       </c>
       <c r="L45" t="n">
-        <v>107.78</v>
+        <v>76.84</v>
       </c>
       <c r="M45" t="n">
-        <v>78856.12</v>
+        <v>158003.96</v>
       </c>
       <c r="N45" t="n">
-        <v>3584.37</v>
+        <v>7182</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Overdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="Q45" t="n">
-        <v>78856.12</v>
+        <v>0</v>
       </c>
       <c r="R45" t="inlineStr">
         <is>
@@ -3403,27 +3403,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4053585339234285</v>
+        <v>0.2159633534796498</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Spend_to_Date</t>
+          <t>Spend_Velocity</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1304357401346983</v>
+        <v>0.1603340188252249</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Spend_Velocity</t>
+          <t>Flight_Days</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1097834533794496</v>
+        <v>0.1550880643428183</v>
       </c>
     </row>
     <row r="5">
@@ -3433,27 +3433,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1008820254880102</v>
+        <v>0.1407617252684994</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Flight_Days</t>
+          <t>Days_Elapsed</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.09827503893303247</v>
+        <v>0.1337881870750038</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Days_Elapsed</t>
+          <t>Spend_to_Date</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.08595930965176035</v>
+        <v>0.1271158795313068</v>
       </c>
     </row>
     <row r="8">
@@ -3463,7 +3463,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.06930589848962057</v>
+        <v>0.06694877147749694</v>
       </c>
     </row>
   </sheetData>
@@ -3504,7 +3504,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.833</v>
       </c>
     </row>
     <row r="3">
@@ -3514,7 +3514,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -3524,7 +3524,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -3544,7 +3544,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>420725.41</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refresh dashboard output with strong ML demo cases
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -549,10 +549,10 @@
         <v>46129</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G2" t="n">
         <v>156794.7</v>
@@ -561,22 +561,22 @@
         <v>608826.02</v>
       </c>
       <c r="I2" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J2" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K2" t="n">
-        <v>107393.63</v>
+        <v>108109.59</v>
       </c>
       <c r="L2" t="n">
-        <v>566.91</v>
+        <v>563.16</v>
       </c>
       <c r="M2" t="n">
         <v>-452031.32</v>
       </c>
       <c r="N2" t="n">
-        <v>-6551.18</v>
+        <v>-6647.52</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -615,10 +615,10 @@
         <v>46011</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G3" t="n">
         <v>980938.23</v>
@@ -677,10 +677,10 @@
         <v>46164</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G4" t="n">
         <v>1203003.45</v>
@@ -689,22 +689,22 @@
         <v>608474.51</v>
       </c>
       <c r="I4" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J4" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K4" t="n">
-        <v>659036.67</v>
+        <v>664267.12</v>
       </c>
       <c r="L4" t="n">
-        <v>92.33</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="M4" t="n">
         <v>594528.9399999999</v>
       </c>
       <c r="N4" t="n">
-        <v>5716.62</v>
+        <v>5772.13</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -743,10 +743,10 @@
         <v>45833</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G5" t="n">
         <v>213070.04</v>
@@ -805,10 +805,10 @@
         <v>46033</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G6" t="n">
         <v>166143.59</v>
@@ -867,10 +867,10 @@
         <v>46127</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G7" t="n">
         <v>1043499.56</v>
@@ -879,22 +879,22 @@
         <v>691277.39</v>
       </c>
       <c r="I7" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J7" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K7" t="n">
-        <v>731381.39</v>
+        <v>736039.87</v>
       </c>
       <c r="L7" t="n">
-        <v>94.52</v>
+        <v>93.92</v>
       </c>
       <c r="M7" t="n">
         <v>352222.17</v>
       </c>
       <c r="N7" t="n">
-        <v>5257.05</v>
+        <v>5336.7</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -933,10 +933,10 @@
         <v>45990</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G8" t="n">
         <v>616363.26</v>
@@ -995,10 +995,10 @@
         <v>45922</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G9" t="n">
         <v>1246850.23</v>
@@ -1057,10 +1057,10 @@
         <v>46181</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G10" t="n">
         <v>1498311.41</v>
@@ -1069,22 +1069,22 @@
         <v>1481697.54</v>
       </c>
       <c r="I10" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J10" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K10" t="n">
-        <v>919091.98</v>
+        <v>923878.92</v>
       </c>
       <c r="L10" t="n">
-        <v>161.21</v>
+        <v>160.38</v>
       </c>
       <c r="M10" t="n">
         <v>16613.87</v>
       </c>
       <c r="N10" t="n">
-        <v>137.3</v>
+        <v>138.45</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1123,10 +1123,10 @@
         <v>45844</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G11" t="n">
         <v>1430946.26</v>
@@ -1185,10 +1185,10 @@
         <v>46088</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G12" t="n">
         <v>1213115.79</v>
@@ -1197,22 +1197,22 @@
         <v>501216.88</v>
       </c>
       <c r="I12" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J12" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K12" t="n">
-        <v>943534.5</v>
+        <v>953162.41</v>
       </c>
       <c r="L12" t="n">
-        <v>53.12</v>
+        <v>52.58</v>
       </c>
       <c r="M12" t="n">
         <v>711898.91</v>
       </c>
       <c r="N12" t="n">
-        <v>25424.96</v>
+        <v>26366.63</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1251,10 +1251,10 @@
         <v>45917</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G13" t="n">
         <v>847097.25</v>
@@ -1313,10 +1313,10 @@
         <v>46012</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G14" t="n">
         <v>1196357.84</v>
@@ -1375,10 +1375,10 @@
         <v>45909</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G15" t="n">
         <v>1410829.15</v>
@@ -1437,10 +1437,10 @@
         <v>46029</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G16" t="n">
         <v>759554.55</v>
@@ -1499,10 +1499,10 @@
         <v>46038</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G17" t="n">
         <v>1299757.94</v>
@@ -1561,10 +1561,10 @@
         <v>45964</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G18" t="n">
         <v>399730.64</v>
@@ -1623,10 +1623,10 @@
         <v>45868</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G19" t="n">
         <v>349165.34</v>
@@ -1685,10 +1685,10 @@
         <v>45904</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G20" t="n">
         <v>513501.49</v>
@@ -1747,10 +1747,10 @@
         <v>45912</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G21" t="n">
         <v>486699.57</v>
@@ -1809,10 +1809,10 @@
         <v>46259</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G22" t="n">
         <v>371788.09</v>
@@ -1821,22 +1821,22 @@
         <v>236180.55</v>
       </c>
       <c r="I22" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J22" t="n">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K22" t="n">
-        <v>82780.94</v>
+        <v>84233.24000000001</v>
       </c>
       <c r="L22" t="n">
-        <v>285.31</v>
+        <v>280.39</v>
       </c>
       <c r="M22" t="n">
         <v>135607.54</v>
       </c>
       <c r="N22" t="n">
-        <v>681.4400000000001</v>
+        <v>684.89</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -1875,10 +1875,10 @@
         <v>45932</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G23" t="n">
         <v>650873.65</v>
@@ -1937,10 +1937,10 @@
         <v>46085</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G24" t="n">
         <v>251943.38</v>
@@ -1949,22 +1949,22 @@
         <v>1170281.73</v>
       </c>
       <c r="I24" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J24" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K24" t="n">
-        <v>223824.7</v>
+        <v>224949.45</v>
       </c>
       <c r="L24" t="n">
-        <v>522.86</v>
+        <v>520.24</v>
       </c>
       <c r="M24" t="n">
         <v>-918338.35</v>
       </c>
       <c r="N24" t="n">
-        <v>-36733.53</v>
+        <v>-38264.1</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2003,10 +2003,10 @@
         <v>45896</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G25" t="n">
         <v>853637.65</v>
@@ -2065,10 +2065,10 @@
         <v>46243</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>46060</v>
+        <v>46061</v>
       </c>
       <c r="G26" t="n">
         <v>1442029.05</v>
@@ -2077,22 +2077,22 @@
         <v>255270.97</v>
       </c>
       <c r="I26" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J26" t="n">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K26" t="n">
-        <v>337881.28</v>
+        <v>343914.88</v>
       </c>
       <c r="L26" t="n">
-        <v>75.55</v>
+        <v>74.23</v>
       </c>
       <c r="M26" t="n">
         <v>1186758.08</v>
       </c>
       <c r="N26" t="n">
-        <v>6485.02</v>
+        <v>6520.65</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Final ML demo output refresh
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,14 +539,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45911</v>
+        <v>45723</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>46129</v>
+        <v>45826</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>46062</v>
@@ -555,41 +555,37 @@
         <v>46061</v>
       </c>
       <c r="G2" t="n">
-        <v>156794.7</v>
+        <v>100350.37</v>
       </c>
       <c r="H2" t="n">
-        <v>608826.02</v>
+        <v>124087.18</v>
       </c>
       <c r="I2" t="n">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="J2" t="n">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>108109.59</v>
+        <v>100350.37</v>
       </c>
       <c r="L2" t="n">
-        <v>563.16</v>
+        <v>123.65</v>
       </c>
       <c r="M2" t="n">
-        <v>-452031.32</v>
+        <v>-23736.81</v>
       </c>
       <c r="N2" t="n">
-        <v>-6647.52</v>
+        <v>0</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Overdelivered</t>
-        </is>
-      </c>
+      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="n">
-        <v>-452031.32</v>
+        <v>0</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
@@ -605,14 +601,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45885</v>
+        <v>46016</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>46011</v>
+        <v>46071</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>46062</v>
@@ -621,35 +617,39 @@
         <v>46061</v>
       </c>
       <c r="G3" t="n">
-        <v>980938.23</v>
+        <v>552594.63</v>
       </c>
       <c r="H3" t="n">
-        <v>692131.28</v>
+        <v>522004.65</v>
       </c>
       <c r="I3" t="n">
-        <v>127</v>
+        <v>46</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K3" t="n">
-        <v>980938.23</v>
+        <v>453917.02</v>
       </c>
       <c r="L3" t="n">
-        <v>70.56</v>
+        <v>115</v>
       </c>
       <c r="M3" t="n">
-        <v>288806.95</v>
+        <v>30589.98</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>3059</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr"/>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
       <c r="Q3" t="n">
         <v>0</v>
       </c>
@@ -671,10 +671,10 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45935</v>
+        <v>45909</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>46164</v>
+        <v>45984</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>46062</v>
@@ -683,41 +683,37 @@
         <v>46061</v>
       </c>
       <c r="G4" t="n">
-        <v>1203003.45</v>
+        <v>294540.38</v>
       </c>
       <c r="H4" t="n">
-        <v>608474.51</v>
+        <v>364299.88</v>
       </c>
       <c r="I4" t="n">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="J4" t="n">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>664267.12</v>
+        <v>294540.38</v>
       </c>
       <c r="L4" t="n">
-        <v>91.59999999999999</v>
+        <v>123.68</v>
       </c>
       <c r="M4" t="n">
-        <v>594528.9399999999</v>
+        <v>-69759.5</v>
       </c>
       <c r="N4" t="n">
-        <v>5772.13</v>
+        <v>0</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Overdelivered</t>
-        </is>
-      </c>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr"/>
       <c r="Q4" t="n">
-        <v>594528.9399999999</v>
+        <v>0</v>
       </c>
       <c r="R4" t="inlineStr">
         <is>
@@ -737,10 +733,10 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45703</v>
+        <v>45784</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45833</v>
+        <v>45811</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>46062</v>
@@ -749,25 +745,25 @@
         <v>46061</v>
       </c>
       <c r="G5" t="n">
-        <v>213070.04</v>
+        <v>509097.37</v>
       </c>
       <c r="H5" t="n">
-        <v>957976.13</v>
+        <v>629098.9300000001</v>
       </c>
       <c r="I5" t="n">
-        <v>131</v>
+        <v>28</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>213070.04</v>
+        <v>509097.37</v>
       </c>
       <c r="L5" t="n">
-        <v>449.61</v>
+        <v>123.57</v>
       </c>
       <c r="M5" t="n">
-        <v>-744906.09</v>
+        <v>-120001.56</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -795,14 +791,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45836</v>
+        <v>45904</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>46033</v>
+        <v>45997</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>46062</v>
@@ -811,32 +807,32 @@
         <v>46061</v>
       </c>
       <c r="G6" t="n">
-        <v>166143.59</v>
+        <v>382409.25</v>
       </c>
       <c r="H6" t="n">
-        <v>847014.35</v>
+        <v>299621.42</v>
       </c>
       <c r="I6" t="n">
-        <v>198</v>
+        <v>94</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>166143.59</v>
+        <v>382409.25</v>
       </c>
       <c r="L6" t="n">
-        <v>509.81</v>
+        <v>78.34999999999999</v>
       </c>
       <c r="M6" t="n">
-        <v>-680870.76</v>
+        <v>82787.83</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P6" t="inlineStr"/>
@@ -857,14 +853,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TTD</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45904</v>
+        <v>45914</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>46127</v>
+        <v>46005</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>46062</v>
@@ -873,39 +869,35 @@
         <v>46061</v>
       </c>
       <c r="G7" t="n">
-        <v>1043499.56</v>
+        <v>525695.9399999999</v>
       </c>
       <c r="H7" t="n">
-        <v>691277.39</v>
+        <v>412557.28</v>
       </c>
       <c r="I7" t="n">
-        <v>158</v>
+        <v>92</v>
       </c>
       <c r="J7" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>736039.87</v>
+        <v>525695.9399999999</v>
       </c>
       <c r="L7" t="n">
-        <v>93.92</v>
+        <v>78.48</v>
       </c>
       <c r="M7" t="n">
-        <v>352222.17</v>
+        <v>113138.66</v>
       </c>
       <c r="N7" t="n">
-        <v>5336.7</v>
+        <v>0</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
+      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="n">
         <v>0</v>
       </c>
@@ -923,14 +915,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Amazon DSP</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45916</v>
+        <v>46044</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>45990</v>
+        <v>46102</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>46062</v>
@@ -939,35 +931,39 @@
         <v>46061</v>
       </c>
       <c r="G8" t="n">
-        <v>616363.26</v>
+        <v>136840.92</v>
       </c>
       <c r="H8" t="n">
-        <v>524492.1</v>
+        <v>40217.24</v>
       </c>
       <c r="I8" t="n">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="K8" t="n">
-        <v>616363.26</v>
+        <v>41748.08</v>
       </c>
       <c r="L8" t="n">
-        <v>85.09</v>
+        <v>96.33</v>
       </c>
       <c r="M8" t="n">
-        <v>91871.16</v>
+        <v>96623.67999999999</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>2356.68</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr"/>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
       <c r="Q8" t="n">
         <v>0</v>
       </c>
@@ -985,14 +981,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45847</v>
+        <v>46086</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>45922</v>
+        <v>46119</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>46062</v>
@@ -1001,32 +997,32 @@
         <v>46061</v>
       </c>
       <c r="G9" t="n">
-        <v>1246850.23</v>
+        <v>380340.09</v>
       </c>
       <c r="H9" t="n">
-        <v>306675.23</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="K9" t="n">
-        <v>1246850.23</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>24.6</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>940175</v>
+        <v>380340.09</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>11186.47</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="P9" t="inlineStr"/>
@@ -1051,10 +1047,10 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45869</v>
+        <v>46047</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>46181</v>
+        <v>46103</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>46062</v>
@@ -1063,32 +1059,32 @@
         <v>46061</v>
       </c>
       <c r="G10" t="n">
-        <v>1498311.41</v>
+        <v>448858.15</v>
       </c>
       <c r="H10" t="n">
-        <v>1481697.54</v>
+        <v>108040.94</v>
       </c>
       <c r="I10" t="n">
-        <v>193</v>
+        <v>15</v>
       </c>
       <c r="J10" t="n">
-        <v>120</v>
+        <v>42</v>
       </c>
       <c r="K10" t="n">
-        <v>923878.92</v>
+        <v>118120.57</v>
       </c>
       <c r="L10" t="n">
-        <v>160.38</v>
+        <v>91.47</v>
       </c>
       <c r="M10" t="n">
-        <v>16613.87</v>
+        <v>340817.21</v>
       </c>
       <c r="N10" t="n">
-        <v>138.45</v>
+        <v>8114.7</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1113,14 +1109,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TTD</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45719</v>
+        <v>46089</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>45844</v>
+        <v>46172</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>46062</v>
@@ -1129,32 +1125,32 @@
         <v>46061</v>
       </c>
       <c r="G11" t="n">
-        <v>1430946.26</v>
+        <v>432209.99</v>
       </c>
       <c r="H11" t="n">
-        <v>630019.71</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="K11" t="n">
-        <v>1430946.26</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>44.03</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>800926.55</v>
+        <v>432209.99</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>5145.36</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="P11" t="inlineStr"/>
@@ -1179,10 +1175,10 @@
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>45963</v>
+        <v>46024</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>46088</v>
+        <v>46105</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>46062</v>
@@ -1191,28 +1187,28 @@
         <v>46061</v>
       </c>
       <c r="G12" t="n">
-        <v>1213115.79</v>
+        <v>559806.73</v>
       </c>
       <c r="H12" t="n">
-        <v>501216.88</v>
+        <v>229520.65</v>
       </c>
       <c r="I12" t="n">
-        <v>99</v>
+        <v>38</v>
       </c>
       <c r="J12" t="n">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="K12" t="n">
-        <v>953162.41</v>
+        <v>259422.63</v>
       </c>
       <c r="L12" t="n">
-        <v>52.58</v>
+        <v>88.47</v>
       </c>
       <c r="M12" t="n">
-        <v>711898.91</v>
+        <v>330286.08</v>
       </c>
       <c r="N12" t="n">
-        <v>26366.63</v>
+        <v>7506.5</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1221,7 +1217,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="Q12" t="n">
@@ -1241,14 +1237,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>45720</v>
+        <v>46038</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>45917</v>
+        <v>46118</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>46062</v>
@@ -1257,35 +1253,39 @@
         <v>46061</v>
       </c>
       <c r="G13" t="n">
-        <v>847097.25</v>
+        <v>169377.54</v>
       </c>
       <c r="H13" t="n">
-        <v>998902.6</v>
+        <v>47132.98</v>
       </c>
       <c r="I13" t="n">
-        <v>198</v>
+        <v>24</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="K13" t="n">
-        <v>847097.25</v>
+        <v>50185.94</v>
       </c>
       <c r="L13" t="n">
-        <v>117.92</v>
+        <v>93.92</v>
       </c>
       <c r="M13" t="n">
-        <v>-151805.35</v>
+        <v>122244.56</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>2144.64</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Overpacing</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr"/>
+          <t>Underpacing</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
       <c r="Q13" t="n">
         <v>0</v>
       </c>
@@ -1303,14 +1303,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>Amazon DSP</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45741</v>
+        <v>45788</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>46012</v>
+        <v>45875</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>46062</v>
@@ -1319,32 +1319,32 @@
         <v>46061</v>
       </c>
       <c r="G14" t="n">
-        <v>1196357.84</v>
+        <v>334936.09</v>
       </c>
       <c r="H14" t="n">
-        <v>1538336.04</v>
+        <v>261668.67</v>
       </c>
       <c r="I14" t="n">
-        <v>272</v>
+        <v>88</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>1196357.84</v>
+        <v>334936.09</v>
       </c>
       <c r="L14" t="n">
-        <v>128.58</v>
+        <v>78.12</v>
       </c>
       <c r="M14" t="n">
-        <v>-341978.2</v>
+        <v>73267.42</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P14" t="inlineStr"/>
@@ -1365,14 +1365,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45726</v>
+        <v>46120</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>45909</v>
+        <v>46176</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>46062</v>
@@ -1381,32 +1381,32 @@
         <v>46061</v>
       </c>
       <c r="G15" t="n">
-        <v>1410829.15</v>
+        <v>394703.48</v>
       </c>
       <c r="H15" t="n">
-        <v>952843.6800000001</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>184</v>
+        <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="K15" t="n">
-        <v>1410829.15</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>67.54000000000001</v>
+        <v>0</v>
       </c>
       <c r="M15" t="n">
-        <v>457985.47</v>
+        <v>394703.48</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>6924.62</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="P15" t="inlineStr"/>
@@ -1427,14 +1427,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Amazon DSP</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45819</v>
+        <v>45693</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>46029</v>
+        <v>45766</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>46062</v>
@@ -1443,32 +1443,32 @@
         <v>46061</v>
       </c>
       <c r="G16" t="n">
-        <v>759554.55</v>
+        <v>161605.1</v>
       </c>
       <c r="H16" t="n">
-        <v>1290954.77</v>
+        <v>161062.54</v>
       </c>
       <c r="I16" t="n">
-        <v>211</v>
+        <v>74</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>759554.55</v>
+        <v>161605.1</v>
       </c>
       <c r="L16" t="n">
-        <v>169.96</v>
+        <v>99.66</v>
       </c>
       <c r="M16" t="n">
-        <v>-531400.22</v>
+        <v>542.5599999999999</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P16" t="inlineStr"/>
@@ -1489,14 +1489,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45746</v>
+        <v>45705</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>46038</v>
+        <v>45778</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>46062</v>
@@ -1505,25 +1505,25 @@
         <v>46061</v>
       </c>
       <c r="G17" t="n">
-        <v>1299757.94</v>
+        <v>95583.81</v>
       </c>
       <c r="H17" t="n">
-        <v>1246174.32</v>
+        <v>95465.89999999999</v>
       </c>
       <c r="I17" t="n">
-        <v>293</v>
+        <v>74</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>1299757.94</v>
+        <v>95583.81</v>
       </c>
       <c r="L17" t="n">
-        <v>95.88</v>
+        <v>99.88</v>
       </c>
       <c r="M17" t="n">
-        <v>53583.62</v>
+        <v>117.91</v>
       </c>
       <c r="N17" t="n">
         <v>0</v>
@@ -1551,14 +1551,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45776</v>
+        <v>46136</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>45964</v>
+        <v>46196</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>46062</v>
@@ -1567,32 +1567,32 @@
         <v>46061</v>
       </c>
       <c r="G18" t="n">
-        <v>399730.64</v>
+        <v>253564.24</v>
       </c>
       <c r="H18" t="n">
-        <v>759896.85</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>189</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="K18" t="n">
-        <v>399730.64</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>190.1</v>
+        <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>-360166.21</v>
+        <v>253564.24</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>4156.79</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="P18" t="inlineStr"/>
@@ -1613,14 +1613,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Amazon DSP</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>45807</v>
+        <v>46126</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>45868</v>
+        <v>46204</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>46062</v>
@@ -1629,32 +1629,32 @@
         <v>46061</v>
       </c>
       <c r="G19" t="n">
-        <v>349165.34</v>
+        <v>111100.55</v>
       </c>
       <c r="H19" t="n">
-        <v>387118.26</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="K19" t="n">
-        <v>349165.34</v>
+        <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>110.87</v>
+        <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>-37952.92</v>
+        <v>111100.55</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>1406.34</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="P19" t="inlineStr"/>
@@ -1675,14 +1675,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>45839</v>
+        <v>46023</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>45904</v>
+        <v>46112</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>46062</v>
@@ -1691,35 +1691,39 @@
         <v>46061</v>
       </c>
       <c r="G20" t="n">
-        <v>513501.49</v>
+        <v>423679.91</v>
       </c>
       <c r="H20" t="n">
-        <v>258916.25</v>
+        <v>165988.26</v>
       </c>
       <c r="I20" t="n">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="K20" t="n">
-        <v>513501.49</v>
+        <v>183594.63</v>
       </c>
       <c r="L20" t="n">
-        <v>50.42</v>
+        <v>90.41</v>
       </c>
       <c r="M20" t="n">
-        <v>254585.24</v>
+        <v>257691.65</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>5052.78</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr"/>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
       <c r="Q20" t="n">
         <v>0</v>
       </c>
@@ -1737,14 +1741,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45833</v>
+        <v>46102</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>45912</v>
+        <v>46179</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>46062</v>
@@ -1753,32 +1757,32 @@
         <v>46061</v>
       </c>
       <c r="G21" t="n">
-        <v>486699.57</v>
+        <v>224412.65</v>
       </c>
       <c r="H21" t="n">
-        <v>313121.11</v>
+        <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="K21" t="n">
-        <v>486699.57</v>
+        <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>64.34</v>
+        <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>173578.46</v>
+        <v>224412.65</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>2877.09</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="P21" t="inlineStr"/>
@@ -1803,10 +1807,10 @@
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>46004</v>
+        <v>46107</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>46259</v>
+        <v>46129</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>46062</v>
@@ -1815,41 +1819,37 @@
         <v>46061</v>
       </c>
       <c r="G22" t="n">
-        <v>371788.09</v>
+        <v>568840.5</v>
       </c>
       <c r="H22" t="n">
-        <v>236180.55</v>
+        <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>198</v>
+        <v>23</v>
       </c>
       <c r="K22" t="n">
-        <v>84233.24000000001</v>
+        <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>280.39</v>
+        <v>0</v>
       </c>
       <c r="M22" t="n">
-        <v>135607.54</v>
+        <v>568840.5</v>
       </c>
       <c r="N22" t="n">
-        <v>684.89</v>
+        <v>24732.2</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Overpacing</t>
-        </is>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>Overdelivered</t>
-        </is>
-      </c>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr"/>
       <c r="Q22" t="n">
-        <v>135607.54</v>
+        <v>0</v>
       </c>
       <c r="R22" t="inlineStr">
         <is>
@@ -1865,14 +1865,14 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45698</v>
+        <v>45886</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>45932</v>
+        <v>45969</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>46062</v>
@@ -1881,32 +1881,32 @@
         <v>46061</v>
       </c>
       <c r="G23" t="n">
-        <v>650873.65</v>
+        <v>105951.07</v>
       </c>
       <c r="H23" t="n">
-        <v>982755.53</v>
+        <v>105894.46</v>
       </c>
       <c r="I23" t="n">
-        <v>235</v>
+        <v>84</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>650873.65</v>
+        <v>105951.07</v>
       </c>
       <c r="L23" t="n">
-        <v>150.99</v>
+        <v>99.95</v>
       </c>
       <c r="M23" t="n">
-        <v>-331881.88</v>
+        <v>56.61</v>
       </c>
       <c r="N23" t="n">
         <v>0</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P23" t="inlineStr"/>
@@ -1931,10 +1931,10 @@
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45862</v>
+        <v>45832</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>46085</v>
+        <v>45902</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>46062</v>
@@ -1943,41 +1943,37 @@
         <v>46061</v>
       </c>
       <c r="G24" t="n">
-        <v>251943.38</v>
+        <v>280248.59</v>
       </c>
       <c r="H24" t="n">
-        <v>1170281.73</v>
+        <v>281050.14</v>
       </c>
       <c r="I24" t="n">
-        <v>200</v>
+        <v>71</v>
       </c>
       <c r="J24" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>224949.45</v>
+        <v>280248.59</v>
       </c>
       <c r="L24" t="n">
-        <v>520.24</v>
+        <v>100.29</v>
       </c>
       <c r="M24" t="n">
-        <v>-918338.35</v>
+        <v>-801.55</v>
       </c>
       <c r="N24" t="n">
-        <v>-38264.1</v>
+        <v>0</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Overpacing</t>
-        </is>
-      </c>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t>Overdelivered</t>
-        </is>
-      </c>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr"/>
       <c r="Q24" t="n">
-        <v>-918338.35</v>
+        <v>0</v>
       </c>
       <c r="R24" t="inlineStr">
         <is>
@@ -1993,14 +1989,14 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Amazon DSP</t>
+          <t>Yahoo</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>45803</v>
+        <v>45866</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>45896</v>
+        <v>45943</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>46062</v>
@@ -2009,32 +2005,32 @@
         <v>46061</v>
       </c>
       <c r="G25" t="n">
-        <v>853637.65</v>
+        <v>285863.23</v>
       </c>
       <c r="H25" t="n">
-        <v>733027.23</v>
+        <v>284623.26</v>
       </c>
       <c r="I25" t="n">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>853637.65</v>
+        <v>285863.23</v>
       </c>
       <c r="L25" t="n">
-        <v>85.87</v>
+        <v>99.56999999999999</v>
       </c>
       <c r="M25" t="n">
-        <v>120610.42</v>
+        <v>1239.97</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P25" t="inlineStr"/>
@@ -2055,59 +2051,1315 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>45718</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>45808</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G26" t="n">
+        <v>221171.06</v>
+      </c>
+      <c r="H26" t="n">
+        <v>221867.14</v>
+      </c>
+      <c r="I26" t="n">
+        <v>91</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>221171.06</v>
+      </c>
+      <c r="L26" t="n">
+        <v>100.31</v>
+      </c>
+      <c r="M26" t="n">
+        <v>-696.08</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CAMP_026</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>46010</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>46092</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G27" t="n">
+        <v>577808.88</v>
+      </c>
+      <c r="H27" t="n">
+        <v>299694.81</v>
+      </c>
+      <c r="I27" t="n">
+        <v>52</v>
+      </c>
+      <c r="J27" t="n">
+        <v>31</v>
+      </c>
+      <c r="K27" t="n">
+        <v>362000.74</v>
+      </c>
+      <c r="L27" t="n">
+        <v>82.79000000000001</v>
+      </c>
+      <c r="M27" t="n">
+        <v>278114.07</v>
+      </c>
+      <c r="N27" t="n">
+        <v>8971.42</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Underpacing</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>CAMP_027</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>45899</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>45938</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G28" t="n">
+        <v>196777.36</v>
+      </c>
+      <c r="H28" t="n">
+        <v>198381.44</v>
+      </c>
+      <c r="I28" t="n">
+        <v>40</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>196777.36</v>
+      </c>
+      <c r="L28" t="n">
+        <v>100.82</v>
+      </c>
+      <c r="M28" t="n">
+        <v>-1604.08</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>CAMP_028</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>45780</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G29" t="n">
+        <v>170730.01</v>
+      </c>
+      <c r="H29" t="n">
+        <v>170507.65</v>
+      </c>
+      <c r="I29" t="n">
+        <v>96</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>170730.01</v>
+      </c>
+      <c r="L29" t="n">
+        <v>99.87</v>
+      </c>
+      <c r="M29" t="n">
+        <v>222.36</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>CAMP_029</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G30" t="n">
+        <v>355660.26</v>
+      </c>
+      <c r="H30" t="n">
+        <v>353944.27</v>
+      </c>
+      <c r="I30" t="n">
+        <v>74</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>355660.26</v>
+      </c>
+      <c r="L30" t="n">
+        <v>99.52</v>
+      </c>
+      <c r="M30" t="n">
+        <v>1715.99</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>CAMP_030</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>45666</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>45765</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G31" t="n">
+        <v>418857.39</v>
+      </c>
+      <c r="H31" t="n">
+        <v>419072.99</v>
+      </c>
+      <c r="I31" t="n">
+        <v>100</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>418857.39</v>
+      </c>
+      <c r="L31" t="n">
+        <v>100.05</v>
+      </c>
+      <c r="M31" t="n">
+        <v>-215.6</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>CAMP_031</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>DV360</t>
         </is>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>46005</v>
-      </c>
-      <c r="D26" s="2" t="n">
-        <v>46243</v>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F26" s="2" t="n">
-        <v>46061</v>
-      </c>
-      <c r="G26" t="n">
-        <v>1442029.05</v>
-      </c>
-      <c r="H26" t="n">
-        <v>255270.97</v>
-      </c>
-      <c r="I26" t="n">
-        <v>57</v>
-      </c>
-      <c r="J26" t="n">
-        <v>182</v>
-      </c>
-      <c r="K26" t="n">
-        <v>343914.88</v>
-      </c>
-      <c r="L26" t="n">
-        <v>74.23</v>
-      </c>
-      <c r="M26" t="n">
-        <v>1186758.08</v>
-      </c>
-      <c r="N26" t="n">
-        <v>6520.65</v>
-      </c>
-      <c r="O26" t="inlineStr">
+      <c r="C32" s="2" t="n">
+        <v>45998</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>46117</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G32" t="n">
+        <v>574740.27</v>
+      </c>
+      <c r="H32" t="n">
+        <v>262512.6</v>
+      </c>
+      <c r="I32" t="n">
+        <v>64</v>
+      </c>
+      <c r="J32" t="n">
+        <v>56</v>
+      </c>
+      <c r="K32" t="n">
+        <v>306528.14</v>
+      </c>
+      <c r="L32" t="n">
+        <v>85.64</v>
+      </c>
+      <c r="M32" t="n">
+        <v>312227.67</v>
+      </c>
+      <c r="N32" t="n">
+        <v>5575.49</v>
+      </c>
+      <c r="O32" t="inlineStr">
         <is>
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P26" t="inlineStr">
+      <c r="P32" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="Q26" t="n">
-        <v>0</v>
-      </c>
-      <c r="R26" t="inlineStr">
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CAMP_032</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>46093</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G33" t="n">
+        <v>129356.97</v>
+      </c>
+      <c r="H33" t="n">
+        <v>57563.97</v>
+      </c>
+      <c r="I33" t="n">
+        <v>34</v>
+      </c>
+      <c r="J33" t="n">
+        <v>32</v>
+      </c>
+      <c r="K33" t="n">
+        <v>66638.44</v>
+      </c>
+      <c r="L33" t="n">
+        <v>86.38</v>
+      </c>
+      <c r="M33" t="n">
+        <v>71793</v>
+      </c>
+      <c r="N33" t="n">
+        <v>2243.53</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>Underpacing</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CAMP_033</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>45903</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>45931</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G34" t="n">
+        <v>591950.49</v>
+      </c>
+      <c r="H34" t="n">
+        <v>596148.96</v>
+      </c>
+      <c r="I34" t="n">
+        <v>29</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>591950.49</v>
+      </c>
+      <c r="L34" t="n">
+        <v>100.71</v>
+      </c>
+      <c r="M34" t="n">
+        <v>-4198.47</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CAMP_034</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>45972</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G35" t="n">
+        <v>390381.81</v>
+      </c>
+      <c r="H35" t="n">
+        <v>388536.56</v>
+      </c>
+      <c r="I35" t="n">
+        <v>64</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>390381.81</v>
+      </c>
+      <c r="L35" t="n">
+        <v>99.53</v>
+      </c>
+      <c r="M35" t="n">
+        <v>1845.25</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CAMP_035</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>45863</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>45951</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G36" t="n">
+        <v>128268.79</v>
+      </c>
+      <c r="H36" t="n">
+        <v>127600.3</v>
+      </c>
+      <c r="I36" t="n">
+        <v>89</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>128268.79</v>
+      </c>
+      <c r="L36" t="n">
+        <v>99.48</v>
+      </c>
+      <c r="M36" t="n">
+        <v>668.49</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>CAMP_036</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>46066</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>46095</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G37" t="n">
+        <v>534024.5</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>30</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>534024.5</v>
+      </c>
+      <c r="N37" t="n">
+        <v>17800.82</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CAMP_037</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>45835</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>45899</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G38" t="n">
+        <v>391196.57</v>
+      </c>
+      <c r="H38" t="n">
+        <v>392807.45</v>
+      </c>
+      <c r="I38" t="n">
+        <v>65</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>391196.57</v>
+      </c>
+      <c r="L38" t="n">
+        <v>100.41</v>
+      </c>
+      <c r="M38" t="n">
+        <v>-1610.88</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>CAMP_038</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>45887</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>45969</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G39" t="n">
+        <v>596378.9300000001</v>
+      </c>
+      <c r="H39" t="n">
+        <v>597062.42</v>
+      </c>
+      <c r="I39" t="n">
+        <v>83</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>596378.9300000001</v>
+      </c>
+      <c r="L39" t="n">
+        <v>100.11</v>
+      </c>
+      <c r="M39" t="n">
+        <v>-683.49</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CAMP_039</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>46023</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>46087</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G40" t="n">
+        <v>120089.45</v>
+      </c>
+      <c r="H40" t="n">
+        <v>59656.69</v>
+      </c>
+      <c r="I40" t="n">
+        <v>39</v>
+      </c>
+      <c r="J40" t="n">
+        <v>26</v>
+      </c>
+      <c r="K40" t="n">
+        <v>72053.67</v>
+      </c>
+      <c r="L40" t="n">
+        <v>82.79000000000001</v>
+      </c>
+      <c r="M40" t="n">
+        <v>60432.76</v>
+      </c>
+      <c r="N40" t="n">
+        <v>2324.34</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Underpacing</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="Q40" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CAMP_040</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>46106</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>46159</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G41" t="n">
+        <v>326276.52</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>54</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>326276.52</v>
+      </c>
+      <c r="N41" t="n">
+        <v>6042.16</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>CAMP_041</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>46065</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>46111</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G42" t="n">
+        <v>574267.4300000001</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>47</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="n">
+        <v>574267.4300000001</v>
+      </c>
+      <c r="N42" t="n">
+        <v>12218.46</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CAMP_042</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>45898</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>46015</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G43" t="n">
+        <v>352257.46</v>
+      </c>
+      <c r="H43" t="n">
+        <v>353503.96</v>
+      </c>
+      <c r="I43" t="n">
+        <v>118</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>352257.46</v>
+      </c>
+      <c r="L43" t="n">
+        <v>100.35</v>
+      </c>
+      <c r="M43" t="n">
+        <v>-1246.5</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>CAMP_043</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>46096</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>46182</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G44" t="n">
+        <v>267517.39</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>87</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" t="n">
+        <v>267517.39</v>
+      </c>
+      <c r="N44" t="n">
+        <v>3074.91</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="n">
+        <v>0</v>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>CAMP_044</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>46004</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>46082</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G45" t="n">
+        <v>354611.01</v>
+      </c>
+      <c r="H45" t="n">
+        <v>207784.17</v>
+      </c>
+      <c r="I45" t="n">
+        <v>58</v>
+      </c>
+      <c r="J45" t="n">
+        <v>21</v>
+      </c>
+      <c r="K45" t="n">
+        <v>260347.32</v>
+      </c>
+      <c r="L45" t="n">
+        <v>79.81</v>
+      </c>
+      <c r="M45" t="n">
+        <v>146826.84</v>
+      </c>
+      <c r="N45" t="n">
+        <v>6991.75</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>Underpacing</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="Q45" t="n">
+        <v>0</v>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CAMP_045</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>46091</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>46135</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F46" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="G46" t="n">
+        <v>498191.26</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>45</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>498191.26</v>
+      </c>
+      <c r="N46" t="n">
+        <v>11070.92</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2147,71 +3399,71 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pace_Ratio</t>
+          <t>Flight_Days</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3078547604714941</v>
+        <v>0.2683475731955763</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Flight_Days</t>
+          <t>Days_Elapsed</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1794553259719911</v>
+        <v>0.1860516061028757</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Days_Elapsed</t>
+          <t>DSP_enc</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1720279304375133</v>
+        <v>0.1453924550499635</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Spend_Velocity</t>
+          <t>Spend_to_Date</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1274280836808836</v>
+        <v>0.1221237536140624</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Spend_to_Date</t>
+          <t>Total_Budget</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1058853674598238</v>
+        <v>0.1120842792420423</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Total_Budget</t>
+          <t>Spend_Velocity</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.090359778336699</v>
+        <v>0.09681034624651709</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DSP_enc</t>
+          <t>Pace_Ratio</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.01698875364159517</v>
+        <v>0.06918998654896286</v>
       </c>
     </row>
   </sheetData>
@@ -2252,7 +3504,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.333</v>
       </c>
     </row>
     <row r="3">
@@ -2262,7 +3514,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -2272,7 +3524,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -2292,7 +3544,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-640233.1899999999</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add UTC refresh timestamp to dashboard output
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Excel_vs_ML" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Feature_Importance" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Exec_Summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Refresh_Info" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,9 +19,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -60,12 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -542,16 +543,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>45723</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <v>45826</v>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F2" s="2" t="n">
+      <c r="E2" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G2" t="n">
@@ -583,7 +584,6 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="n">
         <v>0</v>
       </c>
@@ -604,16 +604,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>46016</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>46071</v>
       </c>
-      <c r="E3" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F3" s="2" t="n">
+      <c r="E3" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F3" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G3" t="n">
@@ -670,16 +670,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>45909</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
         <v>45984</v>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F4" s="2" t="n">
+      <c r="E4" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F4" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G4" t="n">
@@ -711,7 +711,6 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr"/>
       <c r="Q4" t="n">
         <v>0</v>
       </c>
@@ -732,16 +731,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="3" t="n">
         <v>45784</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="3" t="n">
         <v>45811</v>
       </c>
-      <c r="E5" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F5" s="2" t="n">
+      <c r="E5" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F5" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G5" t="n">
@@ -773,7 +772,6 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr"/>
       <c r="Q5" t="n">
         <v>0</v>
       </c>
@@ -794,16 +792,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="3" t="n">
         <v>45904</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="3" t="n">
         <v>45997</v>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F6" s="2" t="n">
+      <c r="E6" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F6" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G6" t="n">
@@ -835,7 +833,6 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr"/>
       <c r="Q6" t="n">
         <v>0</v>
       </c>
@@ -856,16 +853,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="3" t="n">
         <v>45914</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="3" t="n">
         <v>46005</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F7" s="2" t="n">
+      <c r="E7" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F7" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G7" t="n">
@@ -897,7 +894,6 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="n">
         <v>0</v>
       </c>
@@ -918,16 +914,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="3" t="n">
         <v>46044</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="3" t="n">
         <v>46102</v>
       </c>
-      <c r="E8" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F8" s="2" t="n">
+      <c r="E8" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F8" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G8" t="n">
@@ -984,16 +980,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="3" t="n">
         <v>46086</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="3" t="n">
         <v>46119</v>
       </c>
-      <c r="E9" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F9" s="2" t="n">
+      <c r="E9" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F9" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G9" t="n">
@@ -1025,7 +1021,6 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="n">
         <v>0</v>
       </c>
@@ -1046,16 +1041,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="3" t="n">
         <v>46047</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="3" t="n">
         <v>46103</v>
       </c>
-      <c r="E10" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F10" s="2" t="n">
+      <c r="E10" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F10" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G10" t="n">
@@ -1112,16 +1107,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="3" t="n">
         <v>46089</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="3" t="n">
         <v>46172</v>
       </c>
-      <c r="E11" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F11" s="2" t="n">
+      <c r="E11" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F11" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G11" t="n">
@@ -1153,7 +1148,6 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr"/>
       <c r="Q11" t="n">
         <v>0</v>
       </c>
@@ -1174,16 +1168,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="3" t="n">
         <v>46024</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="3" t="n">
         <v>46105</v>
       </c>
-      <c r="E12" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F12" s="2" t="n">
+      <c r="E12" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F12" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G12" t="n">
@@ -1240,16 +1234,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="3" t="n">
         <v>46038</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="3" t="n">
         <v>46118</v>
       </c>
-      <c r="E13" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F13" s="2" t="n">
+      <c r="E13" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F13" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G13" t="n">
@@ -1306,16 +1300,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="3" t="n">
         <v>45788</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="3" t="n">
         <v>45875</v>
       </c>
-      <c r="E14" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F14" s="2" t="n">
+      <c r="E14" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F14" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G14" t="n">
@@ -1347,7 +1341,6 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr"/>
       <c r="Q14" t="n">
         <v>0</v>
       </c>
@@ -1368,16 +1361,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="3" t="n">
         <v>46120</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="3" t="n">
         <v>46176</v>
       </c>
-      <c r="E15" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F15" s="2" t="n">
+      <c r="E15" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F15" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G15" t="n">
@@ -1409,7 +1402,6 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr"/>
       <c r="Q15" t="n">
         <v>0</v>
       </c>
@@ -1430,16 +1422,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="3" t="n">
         <v>45693</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="3" t="n">
         <v>45766</v>
       </c>
-      <c r="E16" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F16" s="2" t="n">
+      <c r="E16" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F16" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G16" t="n">
@@ -1471,7 +1463,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr"/>
       <c r="Q16" t="n">
         <v>0</v>
       </c>
@@ -1492,16 +1483,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="C17" s="3" t="n">
         <v>45705</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="3" t="n">
         <v>45778</v>
       </c>
-      <c r="E17" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F17" s="2" t="n">
+      <c r="E17" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F17" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G17" t="n">
@@ -1533,7 +1524,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="n">
         <v>0</v>
       </c>
@@ -1554,16 +1544,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="3" t="n">
         <v>46136</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="3" t="n">
         <v>46196</v>
       </c>
-      <c r="E18" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F18" s="2" t="n">
+      <c r="E18" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F18" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G18" t="n">
@@ -1595,7 +1585,6 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr"/>
       <c r="Q18" t="n">
         <v>0</v>
       </c>
@@ -1616,16 +1605,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="C19" s="3" t="n">
         <v>46126</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="D19" s="3" t="n">
         <v>46204</v>
       </c>
-      <c r="E19" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F19" s="2" t="n">
+      <c r="E19" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F19" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G19" t="n">
@@ -1657,7 +1646,6 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr"/>
       <c r="Q19" t="n">
         <v>0</v>
       </c>
@@ -1678,16 +1666,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="C20" s="3" t="n">
         <v>46023</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="3" t="n">
         <v>46112</v>
       </c>
-      <c r="E20" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F20" s="2" t="n">
+      <c r="E20" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F20" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G20" t="n">
@@ -1744,16 +1732,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="C21" s="3" t="n">
         <v>46102</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="D21" s="3" t="n">
         <v>46179</v>
       </c>
-      <c r="E21" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F21" s="2" t="n">
+      <c r="E21" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F21" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G21" t="n">
@@ -1785,7 +1773,6 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P21" t="inlineStr"/>
       <c r="Q21" t="n">
         <v>0</v>
       </c>
@@ -1806,16 +1793,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="C22" s="3" t="n">
         <v>46107</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D22" s="3" t="n">
         <v>46129</v>
       </c>
-      <c r="E22" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F22" s="2" t="n">
+      <c r="E22" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F22" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G22" t="n">
@@ -1847,7 +1834,6 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr"/>
       <c r="Q22" t="n">
         <v>0</v>
       </c>
@@ -1868,16 +1854,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C23" s="2" t="n">
+      <c r="C23" s="3" t="n">
         <v>45886</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="D23" s="3" t="n">
         <v>45969</v>
       </c>
-      <c r="E23" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F23" s="2" t="n">
+      <c r="E23" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F23" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G23" t="n">
@@ -1909,7 +1895,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P23" t="inlineStr"/>
       <c r="Q23" t="n">
         <v>0</v>
       </c>
@@ -1930,16 +1915,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C24" s="2" t="n">
+      <c r="C24" s="3" t="n">
         <v>45832</v>
       </c>
-      <c r="D24" s="2" t="n">
+      <c r="D24" s="3" t="n">
         <v>45902</v>
       </c>
-      <c r="E24" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F24" s="2" t="n">
+      <c r="E24" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F24" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G24" t="n">
@@ -1971,7 +1956,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P24" t="inlineStr"/>
       <c r="Q24" t="n">
         <v>0</v>
       </c>
@@ -1992,16 +1976,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C25" s="2" t="n">
+      <c r="C25" s="3" t="n">
         <v>45866</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="D25" s="3" t="n">
         <v>45943</v>
       </c>
-      <c r="E25" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F25" s="2" t="n">
+      <c r="E25" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F25" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G25" t="n">
@@ -2033,7 +2017,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr"/>
       <c r="Q25" t="n">
         <v>0</v>
       </c>
@@ -2054,16 +2037,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C26" s="2" t="n">
+      <c r="C26" s="3" t="n">
         <v>45718</v>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="D26" s="3" t="n">
         <v>45808</v>
       </c>
-      <c r="E26" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F26" s="2" t="n">
+      <c r="E26" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F26" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G26" t="n">
@@ -2095,7 +2078,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P26" t="inlineStr"/>
       <c r="Q26" t="n">
         <v>0</v>
       </c>
@@ -2116,16 +2098,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C27" s="2" t="n">
+      <c r="C27" s="3" t="n">
         <v>46010</v>
       </c>
-      <c r="D27" s="2" t="n">
+      <c r="D27" s="3" t="n">
         <v>46092</v>
       </c>
-      <c r="E27" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F27" s="2" t="n">
+      <c r="E27" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F27" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G27" t="n">
@@ -2182,16 +2164,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C28" s="2" t="n">
+      <c r="C28" s="3" t="n">
         <v>45899</v>
       </c>
-      <c r="D28" s="2" t="n">
+      <c r="D28" s="3" t="n">
         <v>45938</v>
       </c>
-      <c r="E28" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F28" s="2" t="n">
+      <c r="E28" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F28" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G28" t="n">
@@ -2223,7 +2205,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P28" t="inlineStr"/>
       <c r="Q28" t="n">
         <v>0</v>
       </c>
@@ -2244,16 +2225,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C29" s="2" t="n">
+      <c r="C29" s="3" t="n">
         <v>45685</v>
       </c>
-      <c r="D29" s="2" t="n">
+      <c r="D29" s="3" t="n">
         <v>45780</v>
       </c>
-      <c r="E29" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F29" s="2" t="n">
+      <c r="E29" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F29" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G29" t="n">
@@ -2285,7 +2266,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P29" t="inlineStr"/>
       <c r="Q29" t="n">
         <v>0</v>
       </c>
@@ -2306,16 +2286,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C30" s="2" t="n">
+      <c r="C30" s="3" t="n">
         <v>45881</v>
       </c>
-      <c r="D30" s="2" t="n">
+      <c r="D30" s="3" t="n">
         <v>45954</v>
       </c>
-      <c r="E30" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F30" s="2" t="n">
+      <c r="E30" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F30" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G30" t="n">
@@ -2347,7 +2327,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P30" t="inlineStr"/>
       <c r="Q30" t="n">
         <v>0</v>
       </c>
@@ -2368,16 +2347,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C31" s="2" t="n">
+      <c r="C31" s="3" t="n">
         <v>45666</v>
       </c>
-      <c r="D31" s="2" t="n">
+      <c r="D31" s="3" t="n">
         <v>45765</v>
       </c>
-      <c r="E31" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F31" s="2" t="n">
+      <c r="E31" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F31" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G31" t="n">
@@ -2409,7 +2388,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P31" t="inlineStr"/>
       <c r="Q31" t="n">
         <v>0</v>
       </c>
@@ -2430,16 +2408,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C32" s="2" t="n">
+      <c r="C32" s="3" t="n">
         <v>45998</v>
       </c>
-      <c r="D32" s="2" t="n">
+      <c r="D32" s="3" t="n">
         <v>46117</v>
       </c>
-      <c r="E32" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F32" s="2" t="n">
+      <c r="E32" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F32" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G32" t="n">
@@ -2496,16 +2474,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C33" s="2" t="n">
+      <c r="C33" s="3" t="n">
         <v>46028</v>
       </c>
-      <c r="D33" s="2" t="n">
+      <c r="D33" s="3" t="n">
         <v>46093</v>
       </c>
-      <c r="E33" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F33" s="2" t="n">
+      <c r="E33" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F33" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G33" t="n">
@@ -2562,16 +2540,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C34" s="2" t="n">
+      <c r="C34" s="3" t="n">
         <v>45903</v>
       </c>
-      <c r="D34" s="2" t="n">
+      <c r="D34" s="3" t="n">
         <v>45931</v>
       </c>
-      <c r="E34" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F34" s="2" t="n">
+      <c r="E34" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F34" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G34" t="n">
@@ -2603,7 +2581,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P34" t="inlineStr"/>
       <c r="Q34" t="n">
         <v>0</v>
       </c>
@@ -2624,16 +2601,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C35" s="2" t="n">
+      <c r="C35" s="3" t="n">
         <v>45909</v>
       </c>
-      <c r="D35" s="2" t="n">
+      <c r="D35" s="3" t="n">
         <v>45972</v>
       </c>
-      <c r="E35" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F35" s="2" t="n">
+      <c r="E35" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F35" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G35" t="n">
@@ -2665,7 +2642,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P35" t="inlineStr"/>
       <c r="Q35" t="n">
         <v>0</v>
       </c>
@@ -2686,16 +2662,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C36" s="2" t="n">
+      <c r="C36" s="3" t="n">
         <v>45863</v>
       </c>
-      <c r="D36" s="2" t="n">
+      <c r="D36" s="3" t="n">
         <v>45951</v>
       </c>
-      <c r="E36" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F36" s="2" t="n">
+      <c r="E36" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F36" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G36" t="n">
@@ -2727,7 +2703,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P36" t="inlineStr"/>
       <c r="Q36" t="n">
         <v>0</v>
       </c>
@@ -2748,16 +2723,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C37" s="2" t="n">
+      <c r="C37" s="3" t="n">
         <v>46066</v>
       </c>
-      <c r="D37" s="2" t="n">
+      <c r="D37" s="3" t="n">
         <v>46095</v>
       </c>
-      <c r="E37" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F37" s="2" t="n">
+      <c r="E37" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F37" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G37" t="n">
@@ -2789,7 +2764,6 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P37" t="inlineStr"/>
       <c r="Q37" t="n">
         <v>0</v>
       </c>
@@ -2810,16 +2784,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C38" s="2" t="n">
+      <c r="C38" s="3" t="n">
         <v>45835</v>
       </c>
-      <c r="D38" s="2" t="n">
+      <c r="D38" s="3" t="n">
         <v>45899</v>
       </c>
-      <c r="E38" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F38" s="2" t="n">
+      <c r="E38" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F38" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G38" t="n">
@@ -2851,7 +2825,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P38" t="inlineStr"/>
       <c r="Q38" t="n">
         <v>0</v>
       </c>
@@ -2872,16 +2845,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C39" s="2" t="n">
+      <c r="C39" s="3" t="n">
         <v>45887</v>
       </c>
-      <c r="D39" s="2" t="n">
+      <c r="D39" s="3" t="n">
         <v>45969</v>
       </c>
-      <c r="E39" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F39" s="2" t="n">
+      <c r="E39" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F39" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G39" t="n">
@@ -2913,7 +2886,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P39" t="inlineStr"/>
       <c r="Q39" t="n">
         <v>0</v>
       </c>
@@ -2934,16 +2906,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C40" s="2" t="n">
+      <c r="C40" s="3" t="n">
         <v>46023</v>
       </c>
-      <c r="D40" s="2" t="n">
+      <c r="D40" s="3" t="n">
         <v>46087</v>
       </c>
-      <c r="E40" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F40" s="2" t="n">
+      <c r="E40" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F40" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G40" t="n">
@@ -3000,16 +2972,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C41" s="2" t="n">
+      <c r="C41" s="3" t="n">
         <v>46106</v>
       </c>
-      <c r="D41" s="2" t="n">
+      <c r="D41" s="3" t="n">
         <v>46159</v>
       </c>
-      <c r="E41" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F41" s="2" t="n">
+      <c r="E41" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F41" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G41" t="n">
@@ -3041,7 +3013,6 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P41" t="inlineStr"/>
       <c r="Q41" t="n">
         <v>0</v>
       </c>
@@ -3062,16 +3033,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C42" s="2" t="n">
+      <c r="C42" s="3" t="n">
         <v>46065</v>
       </c>
-      <c r="D42" s="2" t="n">
+      <c r="D42" s="3" t="n">
         <v>46111</v>
       </c>
-      <c r="E42" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F42" s="2" t="n">
+      <c r="E42" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F42" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G42" t="n">
@@ -3103,7 +3074,6 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P42" t="inlineStr"/>
       <c r="Q42" t="n">
         <v>0</v>
       </c>
@@ -3124,16 +3094,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C43" s="2" t="n">
+      <c r="C43" s="3" t="n">
         <v>45898</v>
       </c>
-      <c r="D43" s="2" t="n">
+      <c r="D43" s="3" t="n">
         <v>46015</v>
       </c>
-      <c r="E43" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F43" s="2" t="n">
+      <c r="E43" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F43" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G43" t="n">
@@ -3165,7 +3135,6 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P43" t="inlineStr"/>
       <c r="Q43" t="n">
         <v>0</v>
       </c>
@@ -3186,16 +3155,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C44" s="2" t="n">
+      <c r="C44" s="3" t="n">
         <v>46096</v>
       </c>
-      <c r="D44" s="2" t="n">
+      <c r="D44" s="3" t="n">
         <v>46182</v>
       </c>
-      <c r="E44" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F44" s="2" t="n">
+      <c r="E44" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F44" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G44" t="n">
@@ -3227,7 +3196,6 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P44" t="inlineStr"/>
       <c r="Q44" t="n">
         <v>0</v>
       </c>
@@ -3248,16 +3216,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C45" s="2" t="n">
+      <c r="C45" s="3" t="n">
         <v>46004</v>
       </c>
-      <c r="D45" s="2" t="n">
+      <c r="D45" s="3" t="n">
         <v>46082</v>
       </c>
-      <c r="E45" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F45" s="2" t="n">
+      <c r="E45" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F45" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G45" t="n">
@@ -3314,16 +3282,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C46" s="2" t="n">
+      <c r="C46" s="3" t="n">
         <v>46091</v>
       </c>
-      <c r="D46" s="2" t="n">
+      <c r="D46" s="3" t="n">
         <v>46135</v>
       </c>
-      <c r="E46" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F46" s="2" t="n">
+      <c r="E46" s="3" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F46" s="3" t="n">
         <v>46061</v>
       </c>
       <c r="G46" t="n">
@@ -3355,7 +3323,6 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P46" t="inlineStr"/>
       <c r="Q46" t="n">
         <v>0</v>
       </c>
@@ -3550,4 +3517,47 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Last_Refresh_UTC</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2026-02-09 07:43:58 UTC</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Stable ML vs Excel output with bulletproof budget merge
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -19,8 +19,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -60,13 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,10 +523,15 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>Campaign_Status</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>Budget_At_Risk</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>ML_Early_Warning</t>
         </is>
@@ -543,16 +548,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="2" t="n">
         <v>45723</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="2" t="n">
         <v>45826</v>
       </c>
-      <c r="E2" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F2" s="3" t="n">
+      <c r="E2" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G2" t="n">
@@ -584,10 +589,16 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="inlineStr">
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -604,16 +615,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="2" t="n">
         <v>46016</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="2" t="n">
         <v>46071</v>
       </c>
-      <c r="E3" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F3" s="3" t="n">
+      <c r="E3" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G3" t="n">
@@ -650,10 +661,15 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -670,16 +686,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="2" t="n">
         <v>45909</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="2" t="n">
         <v>45984</v>
       </c>
-      <c r="E4" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F4" s="3" t="n">
+      <c r="E4" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G4" t="n">
@@ -711,10 +727,16 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" t="inlineStr">
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -731,16 +753,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="2" t="n">
         <v>45784</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="2" t="n">
         <v>45811</v>
       </c>
-      <c r="E5" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F5" s="3" t="n">
+      <c r="E5" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G5" t="n">
@@ -772,10 +794,16 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" t="inlineStr">
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -792,16 +820,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="2" t="n">
         <v>45904</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="2" t="n">
         <v>45997</v>
       </c>
-      <c r="E6" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F6" s="3" t="n">
+      <c r="E6" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G6" t="n">
@@ -833,10 +861,16 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" t="inlineStr">
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -853,16 +887,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="2" t="n">
         <v>45914</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="2" t="n">
         <v>46005</v>
       </c>
-      <c r="E7" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F7" s="3" t="n">
+      <c r="E7" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F7" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G7" t="n">
@@ -894,10 +928,16 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="Q7" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" t="inlineStr">
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -914,16 +954,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="2" t="n">
         <v>46044</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="2" t="n">
         <v>46102</v>
       </c>
-      <c r="E8" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F8" s="3" t="n">
+      <c r="E8" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F8" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G8" t="n">
@@ -960,10 +1000,15 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -980,16 +1025,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="2" t="n">
         <v>46086</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="2" t="n">
         <v>46119</v>
       </c>
-      <c r="E9" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F9" s="3" t="n">
+      <c r="E9" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F9" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G9" t="n">
@@ -1021,10 +1066,16 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="inlineStr">
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>FUTURE</t>
+        </is>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1041,16 +1092,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="2" t="n">
         <v>46047</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="2" t="n">
         <v>46103</v>
       </c>
-      <c r="E10" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F10" s="3" t="n">
+      <c r="E10" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G10" t="n">
@@ -1087,10 +1138,15 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q10" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1107,16 +1163,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="2" t="n">
         <v>46089</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="2" t="n">
         <v>46172</v>
       </c>
-      <c r="E11" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F11" s="3" t="n">
+      <c r="E11" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F11" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G11" t="n">
@@ -1148,10 +1204,16 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" t="inlineStr">
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>FUTURE</t>
+        </is>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1168,16 +1230,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="2" t="n">
         <v>46024</v>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="2" t="n">
         <v>46105</v>
       </c>
-      <c r="E12" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F12" s="3" t="n">
+      <c r="E12" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F12" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G12" t="n">
@@ -1214,10 +1276,15 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1234,16 +1301,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="2" t="n">
         <v>46038</v>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="2" t="n">
         <v>46118</v>
       </c>
-      <c r="E13" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F13" s="3" t="n">
+      <c r="E13" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F13" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G13" t="n">
@@ -1280,10 +1347,15 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q13" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1300,16 +1372,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="2" t="n">
         <v>45788</v>
       </c>
-      <c r="D14" s="3" t="n">
+      <c r="D14" s="2" t="n">
         <v>45875</v>
       </c>
-      <c r="E14" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F14" s="3" t="n">
+      <c r="E14" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F14" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G14" t="n">
@@ -1341,10 +1413,16 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" t="inlineStr">
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1361,16 +1439,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="2" t="n">
         <v>46120</v>
       </c>
-      <c r="D15" s="3" t="n">
+      <c r="D15" s="2" t="n">
         <v>46176</v>
       </c>
-      <c r="E15" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F15" s="3" t="n">
+      <c r="E15" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F15" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G15" t="n">
@@ -1402,10 +1480,16 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" t="inlineStr">
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>FUTURE</t>
+        </is>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1422,16 +1506,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="2" t="n">
         <v>45693</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="D16" s="2" t="n">
         <v>45766</v>
       </c>
-      <c r="E16" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F16" s="3" t="n">
+      <c r="E16" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F16" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G16" t="n">
@@ -1463,10 +1547,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" t="inlineStr">
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1483,16 +1573,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="2" t="n">
         <v>45705</v>
       </c>
-      <c r="D17" s="3" t="n">
+      <c r="D17" s="2" t="n">
         <v>45778</v>
       </c>
-      <c r="E17" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F17" s="3" t="n">
+      <c r="E17" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F17" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G17" t="n">
@@ -1524,10 +1614,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q17" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" t="inlineStr">
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1544,16 +1640,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="2" t="n">
         <v>46136</v>
       </c>
-      <c r="D18" s="3" t="n">
+      <c r="D18" s="2" t="n">
         <v>46196</v>
       </c>
-      <c r="E18" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F18" s="3" t="n">
+      <c r="E18" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F18" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G18" t="n">
@@ -1585,10 +1681,16 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="Q18" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" t="inlineStr">
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>FUTURE</t>
+        </is>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1605,16 +1707,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="2" t="n">
         <v>46126</v>
       </c>
-      <c r="D19" s="3" t="n">
+      <c r="D19" s="2" t="n">
         <v>46204</v>
       </c>
-      <c r="E19" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F19" s="3" t="n">
+      <c r="E19" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F19" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G19" t="n">
@@ -1646,10 +1748,16 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="Q19" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" t="inlineStr">
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>FUTURE</t>
+        </is>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1666,16 +1774,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" s="2" t="n">
         <v>46023</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="2" t="n">
         <v>46112</v>
       </c>
-      <c r="E20" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F20" s="3" t="n">
+      <c r="E20" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F20" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G20" t="n">
@@ -1712,10 +1820,15 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q20" t="n">
-        <v>0</v>
-      </c>
-      <c r="R20" t="inlineStr">
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1732,16 +1845,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="2" t="n">
         <v>46102</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="2" t="n">
         <v>46179</v>
       </c>
-      <c r="E21" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F21" s="3" t="n">
+      <c r="E21" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F21" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G21" t="n">
@@ -1773,10 +1886,16 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="Q21" t="n">
-        <v>0</v>
-      </c>
-      <c r="R21" t="inlineStr">
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>FUTURE</t>
+        </is>
+      </c>
+      <c r="R21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1793,16 +1912,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="2" t="n">
         <v>46107</v>
       </c>
-      <c r="D22" s="3" t="n">
+      <c r="D22" s="2" t="n">
         <v>46129</v>
       </c>
-      <c r="E22" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F22" s="3" t="n">
+      <c r="E22" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F22" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G22" t="n">
@@ -1834,10 +1953,16 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="Q22" t="n">
-        <v>0</v>
-      </c>
-      <c r="R22" t="inlineStr">
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>FUTURE</t>
+        </is>
+      </c>
+      <c r="R22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1854,16 +1979,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" s="2" t="n">
         <v>45886</v>
       </c>
-      <c r="D23" s="3" t="n">
+      <c r="D23" s="2" t="n">
         <v>45969</v>
       </c>
-      <c r="E23" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F23" s="3" t="n">
+      <c r="E23" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F23" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G23" t="n">
@@ -1895,10 +2020,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q23" t="n">
-        <v>0</v>
-      </c>
-      <c r="R23" t="inlineStr">
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1915,16 +2046,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="2" t="n">
         <v>45832</v>
       </c>
-      <c r="D24" s="3" t="n">
+      <c r="D24" s="2" t="n">
         <v>45902</v>
       </c>
-      <c r="E24" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F24" s="3" t="n">
+      <c r="E24" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F24" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G24" t="n">
@@ -1956,10 +2087,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" t="inlineStr">
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1976,16 +2113,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C25" s="3" t="n">
+      <c r="C25" s="2" t="n">
         <v>45866</v>
       </c>
-      <c r="D25" s="3" t="n">
+      <c r="D25" s="2" t="n">
         <v>45943</v>
       </c>
-      <c r="E25" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F25" s="3" t="n">
+      <c r="E25" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F25" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G25" t="n">
@@ -2017,10 +2154,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q25" t="n">
-        <v>0</v>
-      </c>
-      <c r="R25" t="inlineStr">
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2037,16 +2180,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C26" s="3" t="n">
+      <c r="C26" s="2" t="n">
         <v>45718</v>
       </c>
-      <c r="D26" s="3" t="n">
+      <c r="D26" s="2" t="n">
         <v>45808</v>
       </c>
-      <c r="E26" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F26" s="3" t="n">
+      <c r="E26" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F26" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G26" t="n">
@@ -2078,10 +2221,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q26" t="n">
-        <v>0</v>
-      </c>
-      <c r="R26" t="inlineStr">
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2098,16 +2247,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" s="2" t="n">
         <v>46010</v>
       </c>
-      <c r="D27" s="3" t="n">
+      <c r="D27" s="2" t="n">
         <v>46092</v>
       </c>
-      <c r="E27" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F27" s="3" t="n">
+      <c r="E27" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F27" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G27" t="n">
@@ -2144,10 +2293,15 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q27" t="n">
-        <v>0</v>
-      </c>
-      <c r="R27" t="inlineStr">
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2164,16 +2318,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="C28" s="2" t="n">
         <v>45899</v>
       </c>
-      <c r="D28" s="3" t="n">
+      <c r="D28" s="2" t="n">
         <v>45938</v>
       </c>
-      <c r="E28" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F28" s="3" t="n">
+      <c r="E28" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F28" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G28" t="n">
@@ -2205,10 +2359,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R28" t="inlineStr">
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2225,16 +2385,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="2" t="n">
         <v>45685</v>
       </c>
-      <c r="D29" s="3" t="n">
+      <c r="D29" s="2" t="n">
         <v>45780</v>
       </c>
-      <c r="E29" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F29" s="3" t="n">
+      <c r="E29" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F29" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G29" t="n">
@@ -2266,10 +2426,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q29" t="n">
-        <v>0</v>
-      </c>
-      <c r="R29" t="inlineStr">
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R29" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2286,16 +2452,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="2" t="n">
         <v>45881</v>
       </c>
-      <c r="D30" s="3" t="n">
+      <c r="D30" s="2" t="n">
         <v>45954</v>
       </c>
-      <c r="E30" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F30" s="3" t="n">
+      <c r="E30" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F30" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G30" t="n">
@@ -2327,10 +2493,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q30" t="n">
-        <v>0</v>
-      </c>
-      <c r="R30" t="inlineStr">
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2347,16 +2519,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C31" s="2" t="n">
         <v>45666</v>
       </c>
-      <c r="D31" s="3" t="n">
+      <c r="D31" s="2" t="n">
         <v>45765</v>
       </c>
-      <c r="E31" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F31" s="3" t="n">
+      <c r="E31" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F31" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G31" t="n">
@@ -2388,10 +2560,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q31" t="n">
-        <v>0</v>
-      </c>
-      <c r="R31" t="inlineStr">
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2408,16 +2586,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C32" s="3" t="n">
+      <c r="C32" s="2" t="n">
         <v>45998</v>
       </c>
-      <c r="D32" s="3" t="n">
+      <c r="D32" s="2" t="n">
         <v>46117</v>
       </c>
-      <c r="E32" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F32" s="3" t="n">
+      <c r="E32" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F32" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G32" t="n">
@@ -2454,10 +2632,15 @@
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="Q32" t="n">
-        <v>0</v>
-      </c>
-      <c r="R32" t="inlineStr">
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2474,16 +2657,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C33" s="2" t="n">
         <v>46028</v>
       </c>
-      <c r="D33" s="3" t="n">
+      <c r="D33" s="2" t="n">
         <v>46093</v>
       </c>
-      <c r="E33" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F33" s="3" t="n">
+      <c r="E33" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F33" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G33" t="n">
@@ -2520,10 +2703,15 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q33" t="n">
-        <v>0</v>
-      </c>
-      <c r="R33" t="inlineStr">
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2540,16 +2728,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C34" s="2" t="n">
         <v>45903</v>
       </c>
-      <c r="D34" s="3" t="n">
+      <c r="D34" s="2" t="n">
         <v>45931</v>
       </c>
-      <c r="E34" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F34" s="3" t="n">
+      <c r="E34" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F34" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G34" t="n">
@@ -2581,10 +2769,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q34" t="n">
-        <v>0</v>
-      </c>
-      <c r="R34" t="inlineStr">
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R34" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2601,16 +2795,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C35" s="3" t="n">
+      <c r="C35" s="2" t="n">
         <v>45909</v>
       </c>
-      <c r="D35" s="3" t="n">
+      <c r="D35" s="2" t="n">
         <v>45972</v>
       </c>
-      <c r="E35" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F35" s="3" t="n">
+      <c r="E35" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F35" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G35" t="n">
@@ -2642,10 +2836,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q35" t="n">
-        <v>0</v>
-      </c>
-      <c r="R35" t="inlineStr">
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R35" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2662,16 +2862,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C36" s="2" t="n">
         <v>45863</v>
       </c>
-      <c r="D36" s="3" t="n">
+      <c r="D36" s="2" t="n">
         <v>45951</v>
       </c>
-      <c r="E36" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F36" s="3" t="n">
+      <c r="E36" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F36" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G36" t="n">
@@ -2703,10 +2903,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q36" t="n">
-        <v>0</v>
-      </c>
-      <c r="R36" t="inlineStr">
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R36" t="n">
+        <v>0</v>
+      </c>
+      <c r="S36" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2723,16 +2929,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" s="2" t="n">
         <v>46066</v>
       </c>
-      <c r="D37" s="3" t="n">
+      <c r="D37" s="2" t="n">
         <v>46095</v>
       </c>
-      <c r="E37" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F37" s="3" t="n">
+      <c r="E37" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F37" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G37" t="n">
@@ -2764,10 +2970,16 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="Q37" t="n">
-        <v>0</v>
-      </c>
-      <c r="R37" t="inlineStr">
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>FUTURE</t>
+        </is>
+      </c>
+      <c r="R37" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2784,16 +2996,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C38" s="3" t="n">
+      <c r="C38" s="2" t="n">
         <v>45835</v>
       </c>
-      <c r="D38" s="3" t="n">
+      <c r="D38" s="2" t="n">
         <v>45899</v>
       </c>
-      <c r="E38" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F38" s="3" t="n">
+      <c r="E38" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F38" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G38" t="n">
@@ -2825,10 +3037,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q38" t="n">
-        <v>0</v>
-      </c>
-      <c r="R38" t="inlineStr">
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R38" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2845,16 +3063,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" s="2" t="n">
         <v>45887</v>
       </c>
-      <c r="D39" s="3" t="n">
+      <c r="D39" s="2" t="n">
         <v>45969</v>
       </c>
-      <c r="E39" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F39" s="3" t="n">
+      <c r="E39" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F39" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G39" t="n">
@@ -2886,10 +3104,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q39" t="n">
-        <v>0</v>
-      </c>
-      <c r="R39" t="inlineStr">
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R39" t="n">
+        <v>0</v>
+      </c>
+      <c r="S39" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2906,16 +3130,16 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="C40" s="3" t="n">
+      <c r="C40" s="2" t="n">
         <v>46023</v>
       </c>
-      <c r="D40" s="3" t="n">
+      <c r="D40" s="2" t="n">
         <v>46087</v>
       </c>
-      <c r="E40" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F40" s="3" t="n">
+      <c r="E40" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F40" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G40" t="n">
@@ -2952,10 +3176,15 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q40" t="n">
-        <v>0</v>
-      </c>
-      <c r="R40" t="inlineStr">
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="R40" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2972,16 +3201,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C41" s="3" t="n">
+      <c r="C41" s="2" t="n">
         <v>46106</v>
       </c>
-      <c r="D41" s="3" t="n">
+      <c r="D41" s="2" t="n">
         <v>46159</v>
       </c>
-      <c r="E41" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F41" s="3" t="n">
+      <c r="E41" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F41" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G41" t="n">
@@ -3013,10 +3242,16 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="Q41" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" t="inlineStr">
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>FUTURE</t>
+        </is>
+      </c>
+      <c r="R41" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -3033,16 +3268,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C42" s="3" t="n">
+      <c r="C42" s="2" t="n">
         <v>46065</v>
       </c>
-      <c r="D42" s="3" t="n">
+      <c r="D42" s="2" t="n">
         <v>46111</v>
       </c>
-      <c r="E42" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F42" s="3" t="n">
+      <c r="E42" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F42" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G42" t="n">
@@ -3074,10 +3309,16 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="Q42" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" t="inlineStr">
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>FUTURE</t>
+        </is>
+      </c>
+      <c r="R42" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -3094,16 +3335,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C43" s="3" t="n">
+      <c r="C43" s="2" t="n">
         <v>45898</v>
       </c>
-      <c r="D43" s="3" t="n">
+      <c r="D43" s="2" t="n">
         <v>46015</v>
       </c>
-      <c r="E43" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F43" s="3" t="n">
+      <c r="E43" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F43" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G43" t="n">
@@ -3135,10 +3376,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q43" t="n">
-        <v>0</v>
-      </c>
-      <c r="R43" t="inlineStr">
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="R43" t="n">
+        <v>0</v>
+      </c>
+      <c r="S43" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -3155,16 +3402,16 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="C44" s="3" t="n">
+      <c r="C44" s="2" t="n">
         <v>46096</v>
       </c>
-      <c r="D44" s="3" t="n">
+      <c r="D44" s="2" t="n">
         <v>46182</v>
       </c>
-      <c r="E44" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F44" s="3" t="n">
+      <c r="E44" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F44" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G44" t="n">
@@ -3196,10 +3443,16 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="Q44" t="n">
-        <v>0</v>
-      </c>
-      <c r="R44" t="inlineStr">
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>FUTURE</t>
+        </is>
+      </c>
+      <c r="R44" t="n">
+        <v>0</v>
+      </c>
+      <c r="S44" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -3216,16 +3469,16 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="C45" s="3" t="n">
+      <c r="C45" s="2" t="n">
         <v>46004</v>
       </c>
-      <c r="D45" s="3" t="n">
+      <c r="D45" s="2" t="n">
         <v>46082</v>
       </c>
-      <c r="E45" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F45" s="3" t="n">
+      <c r="E45" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F45" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G45" t="n">
@@ -3262,10 +3515,15 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="Q45" t="n">
-        <v>0</v>
-      </c>
-      <c r="R45" t="inlineStr">
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="R45" t="n">
+        <v>0</v>
+      </c>
+      <c r="S45" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -3282,16 +3540,16 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="C46" s="3" t="n">
+      <c r="C46" s="2" t="n">
         <v>46091</v>
       </c>
-      <c r="D46" s="3" t="n">
+      <c r="D46" s="2" t="n">
         <v>46135</v>
       </c>
-      <c r="E46" s="3" t="n">
-        <v>46062</v>
-      </c>
-      <c r="F46" s="3" t="n">
+      <c r="E46" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="F46" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="G46" t="n">
@@ -3323,10 +3581,16 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="Q46" t="n">
-        <v>0</v>
-      </c>
-      <c r="R46" t="inlineStr">
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>FUTURE</t>
+        </is>
+      </c>
+      <c r="R46" t="n">
+        <v>0</v>
+      </c>
+      <c r="S46" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -3553,7 +3817,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2026-02-09 07:43:58 UTC</t>
+          <t>2026-02-09 08:15:22 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update PaceSmart ML vs Excel output (latest spend + UTC fix)
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -631,7 +631,7 @@
         <v>552594.63</v>
       </c>
       <c r="H3" t="n">
-        <v>522004.65</v>
+        <v>532635.88</v>
       </c>
       <c r="I3" t="n">
         <v>46</v>
@@ -643,13 +643,13 @@
         <v>453917.02</v>
       </c>
       <c r="L3" t="n">
-        <v>115</v>
+        <v>117.34</v>
       </c>
       <c r="M3" t="n">
-        <v>30589.98</v>
+        <v>19958.75</v>
       </c>
       <c r="N3" t="n">
-        <v>3059</v>
+        <v>1995.87</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -970,7 +970,7 @@
         <v>136840.92</v>
       </c>
       <c r="H8" t="n">
-        <v>40217.24</v>
+        <v>42814.76</v>
       </c>
       <c r="I8" t="n">
         <v>18</v>
@@ -982,13 +982,13 @@
         <v>41748.08</v>
       </c>
       <c r="L8" t="n">
-        <v>96.33</v>
+        <v>102.56</v>
       </c>
       <c r="M8" t="n">
-        <v>96623.67999999999</v>
+        <v>94026.16</v>
       </c>
       <c r="N8" t="n">
-        <v>2356.68</v>
+        <v>2293.32</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1108,7 +1108,7 @@
         <v>448858.15</v>
       </c>
       <c r="H10" t="n">
-        <v>108040.94</v>
+        <v>115714.46</v>
       </c>
       <c r="I10" t="n">
         <v>15</v>
@@ -1120,17 +1120,17 @@
         <v>118120.57</v>
       </c>
       <c r="L10" t="n">
-        <v>91.47</v>
+        <v>97.95999999999999</v>
       </c>
       <c r="M10" t="n">
-        <v>340817.21</v>
+        <v>333143.69</v>
       </c>
       <c r="N10" t="n">
-        <v>8114.7</v>
+        <v>7931.99</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1246,7 +1246,7 @@
         <v>559806.73</v>
       </c>
       <c r="H12" t="n">
-        <v>229520.65</v>
+        <v>235081.3</v>
       </c>
       <c r="I12" t="n">
         <v>38</v>
@@ -1258,13 +1258,13 @@
         <v>259422.63</v>
       </c>
       <c r="L12" t="n">
-        <v>88.47</v>
+        <v>90.62</v>
       </c>
       <c r="M12" t="n">
-        <v>330286.08</v>
+        <v>324725.43</v>
       </c>
       <c r="N12" t="n">
-        <v>7506.5</v>
+        <v>7380.12</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1317,7 +1317,7 @@
         <v>169377.54</v>
       </c>
       <c r="H13" t="n">
-        <v>47132.98</v>
+        <v>48607.61</v>
       </c>
       <c r="I13" t="n">
         <v>24</v>
@@ -1329,17 +1329,17 @@
         <v>50185.94</v>
       </c>
       <c r="L13" t="n">
-        <v>93.92</v>
+        <v>96.86</v>
       </c>
       <c r="M13" t="n">
-        <v>122244.56</v>
+        <v>120769.93</v>
       </c>
       <c r="N13" t="n">
-        <v>2144.64</v>
+        <v>2118.77</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1790,7 +1790,7 @@
         <v>423679.91</v>
       </c>
       <c r="H20" t="n">
-        <v>165988.26</v>
+        <v>169960.87</v>
       </c>
       <c r="I20" t="n">
         <v>39</v>
@@ -1802,13 +1802,13 @@
         <v>183594.63</v>
       </c>
       <c r="L20" t="n">
-        <v>90.41</v>
+        <v>92.56999999999999</v>
       </c>
       <c r="M20" t="n">
-        <v>257691.65</v>
+        <v>253719.04</v>
       </c>
       <c r="N20" t="n">
-        <v>5052.78</v>
+        <v>4974.88</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         <v>577808.88</v>
       </c>
       <c r="H27" t="n">
-        <v>299694.81</v>
+        <v>309711.19</v>
       </c>
       <c r="I27" t="n">
         <v>52</v>
@@ -2275,13 +2275,13 @@
         <v>362000.74</v>
       </c>
       <c r="L27" t="n">
-        <v>82.79000000000001</v>
+        <v>85.56</v>
       </c>
       <c r="M27" t="n">
-        <v>278114.07</v>
+        <v>268097.69</v>
       </c>
       <c r="N27" t="n">
-        <v>8971.42</v>
+        <v>8648.309999999999</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2602,7 +2602,7 @@
         <v>574740.27</v>
       </c>
       <c r="H32" t="n">
-        <v>262512.6</v>
+        <v>268232.52</v>
       </c>
       <c r="I32" t="n">
         <v>64</v>
@@ -2614,13 +2614,13 @@
         <v>306528.14</v>
       </c>
       <c r="L32" t="n">
-        <v>85.64</v>
+        <v>87.51000000000001</v>
       </c>
       <c r="M32" t="n">
-        <v>312227.67</v>
+        <v>306507.75</v>
       </c>
       <c r="N32" t="n">
-        <v>5575.49</v>
+        <v>5473.35</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2673,7 +2673,7 @@
         <v>129356.97</v>
       </c>
       <c r="H33" t="n">
-        <v>57563.97</v>
+        <v>58770.34</v>
       </c>
       <c r="I33" t="n">
         <v>34</v>
@@ -2685,13 +2685,13 @@
         <v>66638.44</v>
       </c>
       <c r="L33" t="n">
-        <v>86.38</v>
+        <v>88.19</v>
       </c>
       <c r="M33" t="n">
-        <v>71793</v>
+        <v>70586.63</v>
       </c>
       <c r="N33" t="n">
-        <v>2243.53</v>
+        <v>2205.83</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -3146,7 +3146,7 @@
         <v>120089.45</v>
       </c>
       <c r="H40" t="n">
-        <v>59656.69</v>
+        <v>61500.82</v>
       </c>
       <c r="I40" t="n">
         <v>39</v>
@@ -3158,13 +3158,13 @@
         <v>72053.67</v>
       </c>
       <c r="L40" t="n">
-        <v>82.79000000000001</v>
+        <v>85.34999999999999</v>
       </c>
       <c r="M40" t="n">
-        <v>60432.76</v>
+        <v>58588.63</v>
       </c>
       <c r="N40" t="n">
-        <v>2324.34</v>
+        <v>2253.41</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3485,7 +3485,7 @@
         <v>354611.01</v>
       </c>
       <c r="H45" t="n">
-        <v>207784.17</v>
+        <v>214156.48</v>
       </c>
       <c r="I45" t="n">
         <v>58</v>
@@ -3497,13 +3497,13 @@
         <v>260347.32</v>
       </c>
       <c r="L45" t="n">
-        <v>79.81</v>
+        <v>82.26000000000001</v>
       </c>
       <c r="M45" t="n">
-        <v>146826.84</v>
+        <v>140454.53</v>
       </c>
       <c r="N45" t="n">
-        <v>6991.75</v>
+        <v>6688.31</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3745,7 +3745,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -3817,7 +3817,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2026-02-09 08:28:02 UTC</t>
+          <t>2026-02-09 08:53:35 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
New raw data variation
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -8,9 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Excel_vs_ML" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Feature_Importance" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Exec_Summary" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Refresh_Info" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Exec_Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -478,62 +476,62 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Days_Elapsed</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Days_Left</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Expected_Spend_Till_Date</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pacing_%_vs_Ideal</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Remaining_Budget</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Ideal_Daily_Spend</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Pacing_Status</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ML_Prediction</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>Spend_to_Date</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Days_Elapsed</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Days_Left</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Expected_Spend_Till_Date</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Pacing_%_vs_Ideal</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Remaining_Budget</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Ideal_Daily_Spend</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Pacing_Status</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>ML_Prediction</t>
-        </is>
-      </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Campaign_Status</t>
+          <t>Budget_At_Risk</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Budget_At_Risk</t>
+          <t>ML_Early_Warning</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>ML_Early_Warning</t>
+          <t>LAST_REFRESH_DATE</t>
         </is>
       </c>
     </row>
@@ -564,43 +562,43 @@
         <v>100350.37</v>
       </c>
       <c r="H2" t="n">
-        <v>124087.18</v>
+        <v>104</v>
       </c>
       <c r="I2" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100350.37</v>
       </c>
       <c r="K2" t="n">
-        <v>100350.37</v>
+        <v>142.05</v>
       </c>
       <c r="L2" t="n">
-        <v>123.65</v>
+        <v>-42198.76</v>
       </c>
       <c r="M2" t="n">
-        <v>-23736.81</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="N2" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>142549.13</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -631,47 +629,47 @@
         <v>552594.63</v>
       </c>
       <c r="H3" t="n">
-        <v>532635.88</v>
+        <v>46</v>
       </c>
       <c r="I3" t="n">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="J3" t="n">
-        <v>10</v>
+        <v>453917.02</v>
       </c>
       <c r="K3" t="n">
-        <v>453917.02</v>
+        <v>108.02</v>
       </c>
       <c r="L3" t="n">
-        <v>117.34</v>
+        <v>62259.68</v>
       </c>
       <c r="M3" t="n">
-        <v>19958.75</v>
-      </c>
-      <c r="N3" t="n">
-        <v>1995.87</v>
+        <v>6225.97</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Overpacing</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
+          <t>Overdelivered</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
+        <v>490334.95</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>62259.67999999999</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -702,43 +700,43 @@
         <v>294540.38</v>
       </c>
       <c r="H4" t="n">
-        <v>364299.88</v>
+        <v>76</v>
       </c>
       <c r="I4" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>294540.38</v>
       </c>
       <c r="K4" t="n">
-        <v>294540.38</v>
+        <v>134.48</v>
       </c>
       <c r="L4" t="n">
-        <v>123.68</v>
+        <v>-101556.74</v>
       </c>
       <c r="M4" t="n">
-        <v>-69759.5</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="N4" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R4" t="n">
-        <v>0</v>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>396097.12</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -769,43 +767,43 @@
         <v>509097.37</v>
       </c>
       <c r="H5" t="n">
-        <v>629098.9300000001</v>
+        <v>28</v>
       </c>
       <c r="I5" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>509097.37</v>
       </c>
       <c r="K5" t="n">
-        <v>509097.37</v>
+        <v>132.73</v>
       </c>
       <c r="L5" t="n">
-        <v>123.57</v>
+        <v>-166631.37</v>
       </c>
       <c r="M5" t="n">
-        <v>-120001.56</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="N5" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>675728.74</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -836,43 +834,43 @@
         <v>382409.25</v>
       </c>
       <c r="H6" t="n">
-        <v>299621.42</v>
+        <v>94</v>
       </c>
       <c r="I6" t="n">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>382409.25</v>
       </c>
       <c r="K6" t="n">
-        <v>382409.25</v>
+        <v>88.55</v>
       </c>
       <c r="L6" t="n">
-        <v>78.34999999999999</v>
+        <v>43791.1</v>
       </c>
       <c r="M6" t="n">
-        <v>82787.83</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="N6" t="inlineStr">
         <is>
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R6" t="n">
-        <v>0</v>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>338618.15</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -903,43 +901,43 @@
         <v>525695.9399999999</v>
       </c>
       <c r="H7" t="n">
-        <v>412557.28</v>
+        <v>92</v>
       </c>
       <c r="I7" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>525695.9399999999</v>
       </c>
       <c r="K7" t="n">
-        <v>525695.9399999999</v>
+        <v>93.41</v>
       </c>
       <c r="L7" t="n">
-        <v>78.48</v>
+        <v>34623.37</v>
       </c>
       <c r="M7" t="n">
-        <v>113138.66</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="N7" t="inlineStr">
         <is>
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R7" t="n">
-        <v>0</v>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>491072.57</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -970,47 +968,47 @@
         <v>136840.92</v>
       </c>
       <c r="H8" t="n">
-        <v>42814.76</v>
+        <v>18</v>
       </c>
       <c r="I8" t="n">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="J8" t="n">
-        <v>41</v>
+        <v>41748.08</v>
       </c>
       <c r="K8" t="n">
-        <v>41748.08</v>
+        <v>91.34999999999999</v>
       </c>
       <c r="L8" t="n">
-        <v>102.56</v>
+        <v>98705.24000000001</v>
       </c>
       <c r="M8" t="n">
-        <v>94026.16</v>
-      </c>
-      <c r="N8" t="n">
-        <v>2293.32</v>
+        <v>2407.44</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Underpacing</t>
+        </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
-      <c r="R8" t="n">
-        <v>0</v>
+          <t>Overdelivered</t>
+        </is>
+      </c>
+      <c r="P8" t="n">
+        <v>38135.68</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>98705.24000000002</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1044,40 +1042,40 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="J9" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>380340.09</v>
       </c>
       <c r="M9" t="n">
-        <v>380340.09</v>
-      </c>
-      <c r="N9" t="n">
         <v>11186.47</v>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>FUTURE</t>
-        </is>
-      </c>
-      <c r="R9" t="n">
-        <v>0</v>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1108,47 +1106,47 @@
         <v>448858.15</v>
       </c>
       <c r="H10" t="n">
-        <v>115714.46</v>
+        <v>15</v>
       </c>
       <c r="I10" t="n">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="J10" t="n">
-        <v>42</v>
+        <v>118120.57</v>
       </c>
       <c r="K10" t="n">
-        <v>118120.57</v>
+        <v>90.72</v>
       </c>
       <c r="L10" t="n">
-        <v>97.95999999999999</v>
+        <v>341695.11</v>
       </c>
       <c r="M10" t="n">
-        <v>333143.69</v>
-      </c>
-      <c r="N10" t="n">
-        <v>7931.99</v>
+        <v>8135.6</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Underpacing</t>
+        </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
-      <c r="R10" t="n">
-        <v>0</v>
+          <t>Overdelivered</t>
+        </is>
+      </c>
+      <c r="P10" t="n">
+        <v>107163.04</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>341695.11</v>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1182,40 +1180,40 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="J11" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>432209.99</v>
       </c>
       <c r="M11" t="n">
-        <v>432209.99</v>
-      </c>
-      <c r="N11" t="n">
         <v>5145.36</v>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>FUTURE</t>
-        </is>
-      </c>
-      <c r="R11" t="n">
-        <v>0</v>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1246,47 +1244,47 @@
         <v>559806.73</v>
       </c>
       <c r="H12" t="n">
-        <v>235081.3</v>
+        <v>38</v>
       </c>
       <c r="I12" t="n">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="J12" t="n">
-        <v>44</v>
+        <v>259422.63</v>
       </c>
       <c r="K12" t="n">
-        <v>259422.63</v>
+        <v>102.12</v>
       </c>
       <c r="L12" t="n">
-        <v>90.62</v>
+        <v>294892.86</v>
       </c>
       <c r="M12" t="n">
-        <v>324725.43</v>
-      </c>
-      <c r="N12" t="n">
-        <v>7380.12</v>
+        <v>6702.11</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
-      <c r="R12" t="n">
-        <v>0</v>
+          <t>Overdelivered</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>264913.87</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>294892.86</v>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1317,47 +1315,47 @@
         <v>169377.54</v>
       </c>
       <c r="H13" t="n">
-        <v>48607.61</v>
+        <v>24</v>
       </c>
       <c r="I13" t="n">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="J13" t="n">
-        <v>57</v>
+        <v>50185.94</v>
       </c>
       <c r="K13" t="n">
-        <v>50185.94</v>
+        <v>90.75</v>
       </c>
       <c r="L13" t="n">
-        <v>96.86</v>
+        <v>123835.24</v>
       </c>
       <c r="M13" t="n">
-        <v>120769.93</v>
-      </c>
-      <c r="N13" t="n">
-        <v>2118.77</v>
+        <v>2172.55</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Underpacing</t>
+        </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
-      <c r="R13" t="n">
-        <v>0</v>
+          <t>Overdelivered</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>45542.3</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>123835.24</v>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1388,43 +1386,43 @@
         <v>334936.09</v>
       </c>
       <c r="H14" t="n">
-        <v>261668.67</v>
+        <v>88</v>
       </c>
       <c r="I14" t="n">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>334936.09</v>
       </c>
       <c r="K14" t="n">
-        <v>334936.09</v>
+        <v>93.06</v>
       </c>
       <c r="L14" t="n">
-        <v>78.12</v>
+        <v>23236.85</v>
       </c>
       <c r="M14" t="n">
-        <v>73267.42</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="N14" t="inlineStr">
         <is>
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R14" t="n">
-        <v>0</v>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="n">
+        <v>311699.24</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1458,40 +1456,40 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="J15" t="n">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>394703.48</v>
       </c>
       <c r="M15" t="n">
-        <v>394703.48</v>
-      </c>
-      <c r="N15" t="n">
         <v>6924.62</v>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>FUTURE</t>
-        </is>
-      </c>
-      <c r="R15" t="n">
-        <v>0</v>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1522,43 +1520,43 @@
         <v>161605.1</v>
       </c>
       <c r="H16" t="n">
-        <v>161062.54</v>
+        <v>74</v>
       </c>
       <c r="I16" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>161605.1</v>
       </c>
       <c r="K16" t="n">
-        <v>161605.1</v>
+        <v>116.22</v>
       </c>
       <c r="L16" t="n">
-        <v>99.66</v>
+        <v>-26205.26</v>
       </c>
       <c r="M16" t="n">
-        <v>542.5599999999999</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R16" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="n">
+        <v>187810.36</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1589,43 +1587,43 @@
         <v>95583.81</v>
       </c>
       <c r="H17" t="n">
-        <v>95465.89999999999</v>
+        <v>74</v>
       </c>
       <c r="I17" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>95583.81</v>
       </c>
       <c r="K17" t="n">
-        <v>95583.81</v>
+        <v>119.6</v>
       </c>
       <c r="L17" t="n">
-        <v>99.88</v>
+        <v>-18729.87</v>
       </c>
       <c r="M17" t="n">
-        <v>117.91</v>
-      </c>
-      <c r="N17" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R17" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="n">
+        <v>114313.68</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1659,40 +1657,40 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="J18" t="n">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>253564.24</v>
       </c>
       <c r="M18" t="n">
-        <v>253564.24</v>
-      </c>
-      <c r="N18" t="n">
         <v>4156.79</v>
       </c>
-      <c r="O18" t="inlineStr">
+      <c r="N18" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>FUTURE</t>
-        </is>
-      </c>
-      <c r="R18" t="n">
-        <v>0</v>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1726,40 +1724,40 @@
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="J19" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>111100.55</v>
       </c>
       <c r="M19" t="n">
-        <v>111100.55</v>
-      </c>
-      <c r="N19" t="n">
         <v>1406.34</v>
       </c>
-      <c r="O19" t="inlineStr">
+      <c r="N19" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>FUTURE</t>
-        </is>
-      </c>
-      <c r="R19" t="n">
-        <v>0</v>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1790,47 +1788,47 @@
         <v>423679.91</v>
       </c>
       <c r="H20" t="n">
-        <v>169960.87</v>
+        <v>39</v>
       </c>
       <c r="I20" t="n">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J20" t="n">
-        <v>51</v>
+        <v>183594.63</v>
       </c>
       <c r="K20" t="n">
-        <v>183594.63</v>
+        <v>115.53</v>
       </c>
       <c r="L20" t="n">
-        <v>92.56999999999999</v>
+        <v>211580.94</v>
       </c>
       <c r="M20" t="n">
-        <v>253719.04</v>
-      </c>
-      <c r="N20" t="n">
-        <v>4974.88</v>
+        <v>4148.65</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
-      <c r="R20" t="n">
-        <v>0</v>
+          <t>Overdelivered</t>
+        </is>
+      </c>
+      <c r="P20" t="n">
+        <v>212098.97</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>211580.94</v>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1864,40 +1862,40 @@
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="J21" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>224412.65</v>
       </c>
       <c r="M21" t="n">
-        <v>224412.65</v>
-      </c>
-      <c r="N21" t="n">
         <v>2877.09</v>
       </c>
-      <c r="O21" t="inlineStr">
+      <c r="N21" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>FUTURE</t>
-        </is>
-      </c>
-      <c r="R21" t="n">
-        <v>0</v>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1931,40 +1929,40 @@
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J22" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K22" t="n">
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>568840.5</v>
       </c>
       <c r="M22" t="n">
-        <v>568840.5</v>
-      </c>
-      <c r="N22" t="n">
         <v>24732.2</v>
       </c>
-      <c r="O22" t="inlineStr">
+      <c r="N22" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>FUTURE</t>
-        </is>
-      </c>
-      <c r="R22" t="n">
-        <v>0</v>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1995,43 +1993,43 @@
         <v>105951.07</v>
       </c>
       <c r="H23" t="n">
-        <v>105894.46</v>
+        <v>84</v>
       </c>
       <c r="I23" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>105951.07</v>
       </c>
       <c r="K23" t="n">
-        <v>105951.07</v>
+        <v>109.62</v>
       </c>
       <c r="L23" t="n">
-        <v>99.95</v>
+        <v>-10192.81</v>
       </c>
       <c r="M23" t="n">
-        <v>56.61</v>
-      </c>
-      <c r="N23" t="n">
-        <v>0</v>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R23" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="n">
+        <v>116143.88</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2062,43 +2060,43 @@
         <v>280248.59</v>
       </c>
       <c r="H24" t="n">
-        <v>281050.14</v>
+        <v>71</v>
       </c>
       <c r="I24" t="n">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>0</v>
+        <v>280248.59</v>
       </c>
       <c r="K24" t="n">
-        <v>280248.59</v>
+        <v>120.35</v>
       </c>
       <c r="L24" t="n">
-        <v>100.29</v>
+        <v>-57026.17</v>
       </c>
       <c r="M24" t="n">
-        <v>-801.55</v>
-      </c>
-      <c r="N24" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R24" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="n">
+        <v>337274.76</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2129,43 +2127,43 @@
         <v>285863.23</v>
       </c>
       <c r="H25" t="n">
-        <v>284623.26</v>
+        <v>78</v>
       </c>
       <c r="I25" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>285863.23</v>
       </c>
       <c r="K25" t="n">
-        <v>285863.23</v>
+        <v>117.98</v>
       </c>
       <c r="L25" t="n">
-        <v>99.56999999999999</v>
+        <v>-51386.35</v>
       </c>
       <c r="M25" t="n">
-        <v>1239.97</v>
-      </c>
-      <c r="N25" t="n">
-        <v>0</v>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R25" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="n">
+        <v>337249.58</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2196,43 +2194,43 @@
         <v>221171.06</v>
       </c>
       <c r="H26" t="n">
-        <v>221867.14</v>
+        <v>91</v>
       </c>
       <c r="I26" t="n">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>221171.06</v>
       </c>
       <c r="K26" t="n">
-        <v>221171.06</v>
+        <v>114.35</v>
       </c>
       <c r="L26" t="n">
-        <v>100.31</v>
+        <v>-31746.73</v>
       </c>
       <c r="M26" t="n">
-        <v>-696.08</v>
-      </c>
-      <c r="N26" t="n">
-        <v>0</v>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R26" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="n">
+        <v>252917.79</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2263,47 +2261,47 @@
         <v>577808.88</v>
       </c>
       <c r="H27" t="n">
-        <v>309711.19</v>
+        <v>52</v>
       </c>
       <c r="I27" t="n">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="J27" t="n">
-        <v>31</v>
+        <v>362000.74</v>
       </c>
       <c r="K27" t="n">
-        <v>362000.74</v>
+        <v>102.97</v>
       </c>
       <c r="L27" t="n">
-        <v>85.56</v>
+        <v>205056.15</v>
       </c>
       <c r="M27" t="n">
-        <v>268097.69</v>
-      </c>
-      <c r="N27" t="n">
-        <v>8648.309999999999</v>
+        <v>6614.71</v>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
-      <c r="R27" t="n">
-        <v>0</v>
+          <t>Overdelivered</t>
+        </is>
+      </c>
+      <c r="P27" t="n">
+        <v>372752.73</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>205056.15</v>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2334,43 +2332,43 @@
         <v>196777.36</v>
       </c>
       <c r="H28" t="n">
-        <v>198381.44</v>
+        <v>40</v>
       </c>
       <c r="I28" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>0</v>
+        <v>196777.36</v>
       </c>
       <c r="K28" t="n">
-        <v>196777.36</v>
+        <v>115.49</v>
       </c>
       <c r="L28" t="n">
-        <v>100.82</v>
+        <v>-30482.21</v>
       </c>
       <c r="M28" t="n">
-        <v>-1604.08</v>
-      </c>
-      <c r="N28" t="n">
-        <v>0</v>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R28" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="n">
+        <v>227259.57</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2401,43 +2399,43 @@
         <v>170730.01</v>
       </c>
       <c r="H29" t="n">
-        <v>170507.65</v>
+        <v>96</v>
       </c>
       <c r="I29" t="n">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>170730.01</v>
       </c>
       <c r="K29" t="n">
-        <v>170730.01</v>
+        <v>110.33</v>
       </c>
       <c r="L29" t="n">
-        <v>99.87</v>
+        <v>-17629.03</v>
       </c>
       <c r="M29" t="n">
-        <v>222.36</v>
-      </c>
-      <c r="N29" t="n">
-        <v>0</v>
-      </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R29" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="n">
+        <v>188359.04</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2468,43 +2466,43 @@
         <v>355660.26</v>
       </c>
       <c r="H30" t="n">
-        <v>353944.27</v>
+        <v>74</v>
       </c>
       <c r="I30" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>355660.26</v>
       </c>
       <c r="K30" t="n">
-        <v>355660.26</v>
+        <v>113.39</v>
       </c>
       <c r="L30" t="n">
-        <v>99.52</v>
+        <v>-47613.01</v>
       </c>
       <c r="M30" t="n">
-        <v>1715.99</v>
-      </c>
-      <c r="N30" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P30" t="inlineStr"/>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R30" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="n">
+        <v>403273.27</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2535,43 +2533,43 @@
         <v>418857.39</v>
       </c>
       <c r="H31" t="n">
-        <v>419072.99</v>
+        <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>418857.39</v>
       </c>
       <c r="K31" t="n">
-        <v>418857.39</v>
+        <v>109.48</v>
       </c>
       <c r="L31" t="n">
-        <v>100.05</v>
+        <v>-39706.02</v>
       </c>
       <c r="M31" t="n">
-        <v>-215.6</v>
-      </c>
-      <c r="N31" t="n">
-        <v>0</v>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P31" t="inlineStr"/>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R31" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="n">
+        <v>458563.41</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2602,47 +2600,47 @@
         <v>574740.27</v>
       </c>
       <c r="H32" t="n">
-        <v>268232.52</v>
+        <v>64</v>
       </c>
       <c r="I32" t="n">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="J32" t="n">
-        <v>56</v>
+        <v>306528.14</v>
       </c>
       <c r="K32" t="n">
-        <v>306528.14</v>
+        <v>104.14</v>
       </c>
       <c r="L32" t="n">
-        <v>87.51000000000001</v>
+        <v>255534.57</v>
       </c>
       <c r="M32" t="n">
-        <v>306507.75</v>
-      </c>
-      <c r="N32" t="n">
-        <v>5473.35</v>
+        <v>4563.12</v>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P32" t="inlineStr">
-        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
-      <c r="R32" t="n">
-        <v>0</v>
+      <c r="P32" t="n">
+        <v>319205.7</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
       </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2673,47 +2671,47 @@
         <v>129356.97</v>
       </c>
       <c r="H33" t="n">
-        <v>58770.34</v>
+        <v>34</v>
       </c>
       <c r="I33" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J33" t="n">
-        <v>32</v>
+        <v>66638.44</v>
       </c>
       <c r="K33" t="n">
-        <v>66638.44</v>
+        <v>120.64</v>
       </c>
       <c r="L33" t="n">
-        <v>88.19</v>
+        <v>48962.46</v>
       </c>
       <c r="M33" t="n">
-        <v>70586.63</v>
-      </c>
-      <c r="N33" t="n">
-        <v>2205.83</v>
+        <v>1530.08</v>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
-      <c r="R33" t="n">
-        <v>0</v>
+          <t>Overdelivered</t>
+        </is>
+      </c>
+      <c r="P33" t="n">
+        <v>80394.50999999999</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>48962.46000000001</v>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2744,43 +2742,43 @@
         <v>591950.49</v>
       </c>
       <c r="H34" t="n">
-        <v>596148.96</v>
+        <v>29</v>
       </c>
       <c r="I34" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>591950.49</v>
       </c>
       <c r="K34" t="n">
-        <v>591950.49</v>
+        <v>109.14</v>
       </c>
       <c r="L34" t="n">
-        <v>100.71</v>
+        <v>-54127.66</v>
       </c>
       <c r="M34" t="n">
-        <v>-4198.47</v>
-      </c>
-      <c r="N34" t="n">
-        <v>0</v>
-      </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P34" t="inlineStr"/>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R34" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="n">
+        <v>646078.15</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2811,43 +2809,43 @@
         <v>390381.81</v>
       </c>
       <c r="H35" t="n">
-        <v>388536.56</v>
+        <v>64</v>
       </c>
       <c r="I35" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>390381.81</v>
       </c>
       <c r="K35" t="n">
-        <v>390381.81</v>
+        <v>115.43</v>
       </c>
       <c r="L35" t="n">
-        <v>99.53</v>
+        <v>-60239.51</v>
       </c>
       <c r="M35" t="n">
-        <v>1845.25</v>
-      </c>
-      <c r="N35" t="n">
-        <v>0</v>
-      </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P35" t="inlineStr"/>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R35" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="n">
+        <v>450621.32</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2878,43 +2876,43 @@
         <v>128268.79</v>
       </c>
       <c r="H36" t="n">
-        <v>127600.3</v>
+        <v>89</v>
       </c>
       <c r="I36" t="n">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>128268.79</v>
       </c>
       <c r="K36" t="n">
-        <v>128268.79</v>
+        <v>111.86</v>
       </c>
       <c r="L36" t="n">
-        <v>99.48</v>
+        <v>-15208.71</v>
       </c>
       <c r="M36" t="n">
-        <v>668.49</v>
-      </c>
-      <c r="N36" t="n">
-        <v>0</v>
-      </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R36" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="n">
+        <v>143477.5</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2948,40 +2946,40 @@
         <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J37" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K37" t="n">
         <v>0</v>
       </c>
       <c r="L37" t="n">
-        <v>0</v>
+        <v>534024.5</v>
       </c>
       <c r="M37" t="n">
-        <v>534024.5</v>
-      </c>
-      <c r="N37" t="n">
         <v>17800.82</v>
       </c>
-      <c r="O37" t="inlineStr">
+      <c r="N37" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="P37" t="inlineStr"/>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>FUTURE</t>
-        </is>
-      </c>
-      <c r="R37" t="n">
-        <v>0</v>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -3012,43 +3010,43 @@
         <v>391196.57</v>
       </c>
       <c r="H38" t="n">
-        <v>392807.45</v>
+        <v>65</v>
       </c>
       <c r="I38" t="n">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>0</v>
+        <v>391196.57</v>
       </c>
       <c r="K38" t="n">
-        <v>391196.57</v>
+        <v>103.79</v>
       </c>
       <c r="L38" t="n">
-        <v>100.41</v>
+        <v>-14841.8</v>
       </c>
       <c r="M38" t="n">
-        <v>-1610.88</v>
-      </c>
-      <c r="N38" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="N38" t="inlineStr">
         <is>
           <t>On Track</t>
         </is>
       </c>
-      <c r="P38" t="inlineStr"/>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R38" t="n">
-        <v>0</v>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="n">
+        <v>406038.37</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -3079,43 +3077,43 @@
         <v>596378.9300000001</v>
       </c>
       <c r="H39" t="n">
-        <v>597062.42</v>
+        <v>83</v>
       </c>
       <c r="I39" t="n">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>0</v>
+        <v>596378.9300000001</v>
       </c>
       <c r="K39" t="n">
-        <v>596378.9300000001</v>
+        <v>122</v>
       </c>
       <c r="L39" t="n">
-        <v>100.11</v>
+        <v>-131191.73</v>
       </c>
       <c r="M39" t="n">
-        <v>-683.49</v>
-      </c>
-      <c r="N39" t="n">
-        <v>0</v>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R39" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="n">
+        <v>727570.66</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -3146,47 +3144,47 @@
         <v>120089.45</v>
       </c>
       <c r="H40" t="n">
-        <v>61500.82</v>
+        <v>39</v>
       </c>
       <c r="I40" t="n">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="J40" t="n">
-        <v>26</v>
+        <v>72053.67</v>
       </c>
       <c r="K40" t="n">
-        <v>72053.67</v>
+        <v>96.38</v>
       </c>
       <c r="L40" t="n">
-        <v>85.34999999999999</v>
+        <v>50643.69</v>
       </c>
       <c r="M40" t="n">
-        <v>58588.63</v>
-      </c>
-      <c r="N40" t="n">
-        <v>2253.41</v>
+        <v>1947.83</v>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P40" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
-      <c r="R40" t="n">
-        <v>0</v>
+          <t>Overdelivered</t>
+        </is>
+      </c>
+      <c r="P40" t="n">
+        <v>69445.75999999999</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>50643.69</v>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -3220,40 +3218,40 @@
         <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="J41" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K41" t="n">
         <v>0</v>
       </c>
       <c r="L41" t="n">
-        <v>0</v>
+        <v>326276.52</v>
       </c>
       <c r="M41" t="n">
-        <v>326276.52</v>
-      </c>
-      <c r="N41" t="n">
         <v>6042.16</v>
       </c>
-      <c r="O41" t="inlineStr">
+      <c r="N41" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="P41" t="inlineStr"/>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>FUTURE</t>
-        </is>
-      </c>
-      <c r="R41" t="n">
-        <v>0</v>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -3287,40 +3285,40 @@
         <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="J42" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="K42" t="n">
         <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>574267.4300000001</v>
       </c>
       <c r="M42" t="n">
-        <v>574267.4300000001</v>
-      </c>
-      <c r="N42" t="n">
         <v>12218.46</v>
       </c>
-      <c r="O42" t="inlineStr">
+      <c r="N42" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="P42" t="inlineStr"/>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>FUTURE</t>
-        </is>
-      </c>
-      <c r="R42" t="n">
-        <v>0</v>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -3351,43 +3349,43 @@
         <v>352257.46</v>
       </c>
       <c r="H43" t="n">
-        <v>353503.96</v>
+        <v>118</v>
       </c>
       <c r="I43" t="n">
-        <v>118</v>
+        <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>0</v>
+        <v>352257.46</v>
       </c>
       <c r="K43" t="n">
-        <v>352257.46</v>
+        <v>113.66</v>
       </c>
       <c r="L43" t="n">
-        <v>100.35</v>
+        <v>-48121.89</v>
       </c>
       <c r="M43" t="n">
-        <v>-1246.5</v>
-      </c>
-      <c r="N43" t="n">
-        <v>0</v>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="P43" t="inlineStr"/>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
-      <c r="R43" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="n">
+        <v>400379.35</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S43" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -3421,40 +3419,40 @@
         <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="J44" t="n">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="K44" t="n">
         <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>0</v>
+        <v>267517.39</v>
       </c>
       <c r="M44" t="n">
-        <v>267517.39</v>
-      </c>
-      <c r="N44" t="n">
         <v>3074.91</v>
       </c>
-      <c r="O44" t="inlineStr">
+      <c r="N44" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="P44" t="inlineStr"/>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>FUTURE</t>
-        </is>
-      </c>
-      <c r="R44" t="n">
-        <v>0</v>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>0</v>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -3485,47 +3483,47 @@
         <v>354611.01</v>
       </c>
       <c r="H45" t="n">
-        <v>214156.48</v>
+        <v>58</v>
       </c>
       <c r="I45" t="n">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="J45" t="n">
-        <v>21</v>
+        <v>260347.32</v>
       </c>
       <c r="K45" t="n">
-        <v>260347.32</v>
+        <v>114.2</v>
       </c>
       <c r="L45" t="n">
-        <v>82.26000000000001</v>
+        <v>57296.48</v>
       </c>
       <c r="M45" t="n">
-        <v>140454.53</v>
-      </c>
-      <c r="N45" t="n">
-        <v>6688.31</v>
+        <v>2728.4</v>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>Overpacing</t>
+        </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P45" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
-      </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
-      <c r="R45" t="n">
-        <v>0</v>
+          <t>Overdelivered</t>
+        </is>
+      </c>
+      <c r="P45" t="n">
+        <v>297314.53</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>57296.47999999998</v>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -3559,40 +3557,40 @@
         <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J46" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="K46" t="n">
         <v>0</v>
       </c>
       <c r="L46" t="n">
-        <v>0</v>
+        <v>498191.26</v>
       </c>
       <c r="M46" t="n">
-        <v>498191.26</v>
-      </c>
-      <c r="N46" t="n">
         <v>11070.92</v>
       </c>
-      <c r="O46" t="inlineStr">
+      <c r="N46" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="P46" t="inlineStr"/>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>FUTURE</t>
-        </is>
-      </c>
-      <c r="R46" t="n">
-        <v>0</v>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -3607,7 +3605,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3618,206 +3616,74 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Feature</t>
+          <t>Metric</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Importance</t>
+          <t>Value</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Flight_Days</t>
+          <t>ML Validation Accuracy</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2683475731955763</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Days_Elapsed</t>
+          <t>Total Campaigns</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1860516061028757</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DSP_enc</t>
+          <t>ML Risk Alerts</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1453924550499635</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Spend_to_Date</t>
+          <t>Early Warnings</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1221237536140624</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Total_Budget</t>
+          <t>Total Budget At Risk</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1120842792420423</v>
+        <v>1494927.85</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Spend_Velocity</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.09681034624651709</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Pace_Ratio</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.06918998654896286</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Metric</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ML Validation Accuracy</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.333</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Excel Alerts</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ML Risk Alerts</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Early Warnings</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Total Budget At Risk</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Metric</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Last_Refresh_UTC</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2026-02-09 08:53:35 UTC</t>
+          <t>Last Refresh Date</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Stabilize pipeline – Total_Budget safety
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Excel_vs_ML" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Exec_Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Feature_Importance" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Exec_Summary" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -430,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:T46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,67 +472,72 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Total_Budget_x</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Spend_to_Date</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Days_Elapsed</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Days_Left</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Expected_Spend_Till_Date</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Pacing_%_vs_Ideal</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Remaining_Budget</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Ideal_Daily_Spend</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Pacing_Status</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Total_Budget_y</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>ML_Prediction</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>Total_Budget</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Days_Elapsed</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Days_Left</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Expected_Spend_Till_Date</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Pacing_%_vs_Ideal</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Remaining_Budget</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Ideal_Daily_Spend</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Pacing_Status</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>ML_Prediction</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Spend_to_Date</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Budget_At_Risk</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>ML_Early_Warning</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>LAST_REFRESH_DATE</t>
         </is>
       </c>
     </row>
@@ -562,43 +568,44 @@
         <v>100350.37</v>
       </c>
       <c r="H2" t="n">
+        <v>142549.13</v>
+      </c>
+      <c r="I2" t="n">
         <v>104</v>
       </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
       <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
         <v>100350.37</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>142.05</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>-42198.76</v>
       </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="inlineStr">
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
-        <v>142549.13</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>100350.37</v>
+      </c>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="n">
+        <v>100350.37</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -629,47 +636,48 @@
         <v>552594.63</v>
       </c>
       <c r="H3" t="n">
+        <v>490334.95</v>
+      </c>
+      <c r="I3" t="n">
         <v>46</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>10</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>453917.02</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>108.02</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>62259.68</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>6225.97</v>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="n">
+        <v>552594.63</v>
+      </c>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Overdelivered</t>
         </is>
       </c>
-      <c r="P3" t="n">
-        <v>490334.95</v>
-      </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
+        <v>552594.63</v>
+      </c>
+      <c r="S3" t="n">
         <v>62259.67999999999</v>
       </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -700,43 +708,44 @@
         <v>294540.38</v>
       </c>
       <c r="H4" t="n">
+        <v>396097.12</v>
+      </c>
+      <c r="I4" t="n">
         <v>76</v>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
       <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
         <v>294540.38</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>134.48</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>-101556.74</v>
       </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="inlineStr">
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr"/>
       <c r="P4" t="n">
-        <v>396097.12</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>294540.38</v>
+      </c>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="n">
+        <v>294540.38</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -767,43 +776,44 @@
         <v>509097.37</v>
       </c>
       <c r="H5" t="n">
+        <v>675728.74</v>
+      </c>
+      <c r="I5" t="n">
         <v>28</v>
       </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
       <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
         <v>509097.37</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>132.73</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>-166631.37</v>
       </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="inlineStr">
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr"/>
       <c r="P5" t="n">
-        <v>675728.74</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>509097.37</v>
+      </c>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="n">
+        <v>509097.37</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -834,43 +844,44 @@
         <v>382409.25</v>
       </c>
       <c r="H6" t="n">
+        <v>338618.15</v>
+      </c>
+      <c r="I6" t="n">
         <v>94</v>
       </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
       <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
         <v>382409.25</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>88.55</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>43791.1</v>
       </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="inlineStr">
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="inlineStr">
         <is>
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr"/>
       <c r="P6" t="n">
-        <v>338618.15</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>382409.25</v>
+      </c>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="n">
+        <v>382409.25</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -901,43 +912,44 @@
         <v>525695.9399999999</v>
       </c>
       <c r="H7" t="n">
+        <v>491072.57</v>
+      </c>
+      <c r="I7" t="n">
         <v>92</v>
       </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
       <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
         <v>525695.9399999999</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>93.41</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>34623.37</v>
       </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="inlineStr">
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="inlineStr">
         <is>
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr"/>
       <c r="P7" t="n">
-        <v>491072.57</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>525695.9399999999</v>
+      </c>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="n">
+        <v>525695.9399999999</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -968,47 +980,48 @@
         <v>136840.92</v>
       </c>
       <c r="H8" t="n">
+        <v>38135.68</v>
+      </c>
+      <c r="I8" t="n">
         <v>18</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>41</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>41748.08</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>91.34999999999999</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>98705.24000000001</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>2407.44</v>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="P8" t="n">
+        <v>136840.92</v>
+      </c>
+      <c r="Q8" t="inlineStr">
         <is>
           <t>Overdelivered</t>
         </is>
       </c>
-      <c r="P8" t="n">
-        <v>38135.68</v>
-      </c>
-      <c r="Q8" t="n">
+      <c r="R8" t="n">
+        <v>136840.92</v>
+      </c>
+      <c r="S8" t="n">
         <v>98705.24000000002</v>
       </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1042,40 +1055,41 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
         <v>34</v>
       </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
       <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
         <v>380340.09</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>11186.47</v>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr"/>
       <c r="P9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>380340.09</v>
+      </c>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="n">
+        <v>380340.09</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1106,47 +1120,48 @@
         <v>448858.15</v>
       </c>
       <c r="H10" t="n">
+        <v>107163.04</v>
+      </c>
+      <c r="I10" t="n">
         <v>15</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>42</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>118120.57</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>90.72</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>341695.11</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>8135.6</v>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="P10" t="n">
+        <v>448858.15</v>
+      </c>
+      <c r="Q10" t="inlineStr">
         <is>
           <t>Overdelivered</t>
         </is>
       </c>
-      <c r="P10" t="n">
-        <v>107163.04</v>
-      </c>
-      <c r="Q10" t="n">
+      <c r="R10" t="n">
+        <v>448858.15</v>
+      </c>
+      <c r="S10" t="n">
         <v>341695.11</v>
       </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1180,40 +1195,41 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
         <v>84</v>
       </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
         <v>432209.99</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>5145.36</v>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr"/>
       <c r="P11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>432209.99</v>
+      </c>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="n">
+        <v>432209.99</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1244,47 +1260,48 @@
         <v>559806.73</v>
       </c>
       <c r="H12" t="n">
+        <v>264913.87</v>
+      </c>
+      <c r="I12" t="n">
         <v>38</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>44</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>259422.63</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>102.12</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>294892.86</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>6702.11</v>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>On Track</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="P12" t="n">
+        <v>559806.73</v>
+      </c>
+      <c r="Q12" t="inlineStr">
         <is>
           <t>Overdelivered</t>
         </is>
       </c>
-      <c r="P12" t="n">
-        <v>264913.87</v>
-      </c>
-      <c r="Q12" t="n">
+      <c r="R12" t="n">
+        <v>559806.73</v>
+      </c>
+      <c r="S12" t="n">
         <v>294892.86</v>
       </c>
-      <c r="R12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>YES</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1315,47 +1332,48 @@
         <v>169377.54</v>
       </c>
       <c r="H13" t="n">
+        <v>45542.3</v>
+      </c>
+      <c r="I13" t="n">
         <v>24</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>57</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>50185.94</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>90.75</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>123835.24</v>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>2172.55</v>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="P13" t="n">
+        <v>169377.54</v>
+      </c>
+      <c r="Q13" t="inlineStr">
         <is>
           <t>Overdelivered</t>
         </is>
       </c>
-      <c r="P13" t="n">
-        <v>45542.3</v>
-      </c>
-      <c r="Q13" t="n">
+      <c r="R13" t="n">
+        <v>169377.54</v>
+      </c>
+      <c r="S13" t="n">
         <v>123835.24</v>
       </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1386,43 +1404,44 @@
         <v>334936.09</v>
       </c>
       <c r="H14" t="n">
+        <v>311699.24</v>
+      </c>
+      <c r="I14" t="n">
         <v>88</v>
       </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
       <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
         <v>334936.09</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>93.06</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
         <v>23236.85</v>
       </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="inlineStr">
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="inlineStr">
         <is>
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr"/>
       <c r="P14" t="n">
-        <v>311699.24</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>334936.09</v>
+      </c>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="n">
+        <v>334936.09</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1456,40 +1475,41 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
         <v>57</v>
       </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
       <c r="K15" t="n">
         <v>0</v>
       </c>
       <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
         <v>394703.48</v>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>6924.62</v>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr"/>
       <c r="P15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>394703.48</v>
+      </c>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="n">
+        <v>394703.48</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1520,43 +1540,44 @@
         <v>161605.1</v>
       </c>
       <c r="H16" t="n">
+        <v>187810.36</v>
+      </c>
+      <c r="I16" t="n">
         <v>74</v>
       </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
       <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
         <v>161605.1</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>116.22</v>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="n">
         <v>-26205.26</v>
       </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" t="inlineStr">
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr"/>
       <c r="P16" t="n">
-        <v>187810.36</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>161605.1</v>
+      </c>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="n">
+        <v>161605.1</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1587,43 +1608,44 @@
         <v>95583.81</v>
       </c>
       <c r="H17" t="n">
+        <v>114313.68</v>
+      </c>
+      <c r="I17" t="n">
         <v>74</v>
       </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
       <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
         <v>95583.81</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>119.6</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
         <v>-18729.87</v>
       </c>
-      <c r="M17" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" t="inlineStr">
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O17" t="inlineStr"/>
       <c r="P17" t="n">
-        <v>114313.68</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>95583.81</v>
+      </c>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="n">
+        <v>95583.81</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1657,40 +1679,41 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
         <v>61</v>
       </c>
-      <c r="J18" t="n">
-        <v>0</v>
-      </c>
       <c r="K18" t="n">
         <v>0</v>
       </c>
       <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
         <v>253564.24</v>
       </c>
-      <c r="M18" t="n">
+      <c r="N18" t="n">
         <v>4156.79</v>
       </c>
-      <c r="N18" t="inlineStr">
+      <c r="O18" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr"/>
       <c r="P18" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>253564.24</v>
+      </c>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="n">
+        <v>253564.24</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1724,40 +1747,41 @@
         <v>0</v>
       </c>
       <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
         <v>79</v>
       </c>
-      <c r="J19" t="n">
-        <v>0</v>
-      </c>
       <c r="K19" t="n">
         <v>0</v>
       </c>
       <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
         <v>111100.55</v>
       </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>1406.34</v>
       </c>
-      <c r="N19" t="inlineStr">
+      <c r="O19" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="O19" t="inlineStr"/>
       <c r="P19" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>111100.55</v>
+      </c>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="n">
+        <v>111100.55</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1788,47 +1812,48 @@
         <v>423679.91</v>
       </c>
       <c r="H20" t="n">
+        <v>212098.97</v>
+      </c>
+      <c r="I20" t="n">
         <v>39</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>51</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>183594.63</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>115.53</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>211580.94</v>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>4148.65</v>
       </c>
-      <c r="N20" t="inlineStr">
+      <c r="O20" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O20" t="inlineStr">
+      <c r="P20" t="n">
+        <v>423679.91</v>
+      </c>
+      <c r="Q20" t="inlineStr">
         <is>
           <t>Overdelivered</t>
         </is>
       </c>
-      <c r="P20" t="n">
-        <v>212098.97</v>
-      </c>
-      <c r="Q20" t="n">
+      <c r="R20" t="n">
+        <v>423679.91</v>
+      </c>
+      <c r="S20" t="n">
         <v>211580.94</v>
       </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1862,40 +1887,41 @@
         <v>0</v>
       </c>
       <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
         <v>78</v>
       </c>
-      <c r="J21" t="n">
-        <v>0</v>
-      </c>
       <c r="K21" t="n">
         <v>0</v>
       </c>
       <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
         <v>224412.65</v>
       </c>
-      <c r="M21" t="n">
+      <c r="N21" t="n">
         <v>2877.09</v>
       </c>
-      <c r="N21" t="inlineStr">
+      <c r="O21" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="O21" t="inlineStr"/>
       <c r="P21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>0</v>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>224412.65</v>
+      </c>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="n">
+        <v>224412.65</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1929,40 +1955,41 @@
         <v>0</v>
       </c>
       <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
         <v>23</v>
       </c>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
       <c r="K22" t="n">
         <v>0</v>
       </c>
       <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
         <v>568840.5</v>
       </c>
-      <c r="M22" t="n">
+      <c r="N22" t="n">
         <v>24732.2</v>
       </c>
-      <c r="N22" t="inlineStr">
+      <c r="O22" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="O22" t="inlineStr"/>
       <c r="P22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>0</v>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>568840.5</v>
+      </c>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="n">
+        <v>568840.5</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1993,43 +2020,44 @@
         <v>105951.07</v>
       </c>
       <c r="H23" t="n">
+        <v>116143.88</v>
+      </c>
+      <c r="I23" t="n">
         <v>84</v>
       </c>
-      <c r="I23" t="n">
-        <v>0</v>
-      </c>
       <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
         <v>105951.07</v>
       </c>
-      <c r="K23" t="n">
+      <c r="L23" t="n">
         <v>109.62</v>
       </c>
-      <c r="L23" t="n">
+      <c r="M23" t="n">
         <v>-10192.81</v>
       </c>
-      <c r="M23" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" t="inlineStr">
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O23" t="inlineStr"/>
       <c r="P23" t="n">
-        <v>116143.88</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>0</v>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>105951.07</v>
+      </c>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="n">
+        <v>105951.07</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2060,43 +2088,44 @@
         <v>280248.59</v>
       </c>
       <c r="H24" t="n">
+        <v>337274.76</v>
+      </c>
+      <c r="I24" t="n">
         <v>71</v>
       </c>
-      <c r="I24" t="n">
-        <v>0</v>
-      </c>
       <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
         <v>280248.59</v>
       </c>
-      <c r="K24" t="n">
+      <c r="L24" t="n">
         <v>120.35</v>
       </c>
-      <c r="L24" t="n">
+      <c r="M24" t="n">
         <v>-57026.17</v>
       </c>
-      <c r="M24" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" t="inlineStr">
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O24" t="inlineStr"/>
       <c r="P24" t="n">
-        <v>337274.76</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>280248.59</v>
+      </c>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="n">
+        <v>280248.59</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2127,43 +2156,44 @@
         <v>285863.23</v>
       </c>
       <c r="H25" t="n">
+        <v>337249.58</v>
+      </c>
+      <c r="I25" t="n">
         <v>78</v>
       </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
       <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
         <v>285863.23</v>
       </c>
-      <c r="K25" t="n">
+      <c r="L25" t="n">
         <v>117.98</v>
       </c>
-      <c r="L25" t="n">
+      <c r="M25" t="n">
         <v>-51386.35</v>
       </c>
-      <c r="M25" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" t="inlineStr">
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O25" t="inlineStr"/>
       <c r="P25" t="n">
-        <v>337249.58</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>0</v>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>285863.23</v>
+      </c>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="n">
+        <v>285863.23</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2194,43 +2224,44 @@
         <v>221171.06</v>
       </c>
       <c r="H26" t="n">
+        <v>252917.79</v>
+      </c>
+      <c r="I26" t="n">
         <v>91</v>
       </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
       <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
         <v>221171.06</v>
       </c>
-      <c r="K26" t="n">
+      <c r="L26" t="n">
         <v>114.35</v>
       </c>
-      <c r="L26" t="n">
+      <c r="M26" t="n">
         <v>-31746.73</v>
       </c>
-      <c r="M26" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" t="inlineStr">
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O26" t="inlineStr"/>
       <c r="P26" t="n">
-        <v>252917.79</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>0</v>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>221171.06</v>
+      </c>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="n">
+        <v>221171.06</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2261,47 +2292,48 @@
         <v>577808.88</v>
       </c>
       <c r="H27" t="n">
+        <v>372752.73</v>
+      </c>
+      <c r="I27" t="n">
         <v>52</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>31</v>
       </c>
-      <c r="J27" t="n">
+      <c r="K27" t="n">
         <v>362000.74</v>
       </c>
-      <c r="K27" t="n">
+      <c r="L27" t="n">
         <v>102.97</v>
       </c>
-      <c r="L27" t="n">
+      <c r="M27" t="n">
         <v>205056.15</v>
       </c>
-      <c r="M27" t="n">
+      <c r="N27" t="n">
         <v>6614.71</v>
       </c>
-      <c r="N27" t="inlineStr">
+      <c r="O27" t="inlineStr">
         <is>
           <t>On Track</t>
         </is>
       </c>
-      <c r="O27" t="inlineStr">
+      <c r="P27" t="n">
+        <v>577808.88</v>
+      </c>
+      <c r="Q27" t="inlineStr">
         <is>
           <t>Overdelivered</t>
         </is>
       </c>
-      <c r="P27" t="n">
-        <v>372752.73</v>
-      </c>
-      <c r="Q27" t="n">
+      <c r="R27" t="n">
+        <v>577808.88</v>
+      </c>
+      <c r="S27" t="n">
         <v>205056.15</v>
       </c>
-      <c r="R27" t="inlineStr">
+      <c r="T27" t="inlineStr">
         <is>
           <t>YES</t>
-        </is>
-      </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2332,43 +2364,44 @@
         <v>196777.36</v>
       </c>
       <c r="H28" t="n">
+        <v>227259.57</v>
+      </c>
+      <c r="I28" t="n">
         <v>40</v>
       </c>
-      <c r="I28" t="n">
-        <v>0</v>
-      </c>
       <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
         <v>196777.36</v>
       </c>
-      <c r="K28" t="n">
+      <c r="L28" t="n">
         <v>115.49</v>
       </c>
-      <c r="L28" t="n">
+      <c r="M28" t="n">
         <v>-30482.21</v>
       </c>
-      <c r="M28" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" t="inlineStr">
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O28" t="inlineStr"/>
       <c r="P28" t="n">
-        <v>227259.57</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>196777.36</v>
+      </c>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="n">
+        <v>196777.36</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2399,43 +2432,44 @@
         <v>170730.01</v>
       </c>
       <c r="H29" t="n">
+        <v>188359.04</v>
+      </c>
+      <c r="I29" t="n">
         <v>96</v>
       </c>
-      <c r="I29" t="n">
-        <v>0</v>
-      </c>
       <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
         <v>170730.01</v>
       </c>
-      <c r="K29" t="n">
+      <c r="L29" t="n">
         <v>110.33</v>
       </c>
-      <c r="L29" t="n">
+      <c r="M29" t="n">
         <v>-17629.03</v>
       </c>
-      <c r="M29" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" t="inlineStr">
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O29" t="inlineStr"/>
       <c r="P29" t="n">
-        <v>188359.04</v>
-      </c>
-      <c r="Q29" t="n">
-        <v>0</v>
-      </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>170730.01</v>
+      </c>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="n">
+        <v>170730.01</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2466,43 +2500,44 @@
         <v>355660.26</v>
       </c>
       <c r="H30" t="n">
+        <v>403273.27</v>
+      </c>
+      <c r="I30" t="n">
         <v>74</v>
       </c>
-      <c r="I30" t="n">
-        <v>0</v>
-      </c>
       <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
         <v>355660.26</v>
       </c>
-      <c r="K30" t="n">
+      <c r="L30" t="n">
         <v>113.39</v>
       </c>
-      <c r="L30" t="n">
+      <c r="M30" t="n">
         <v>-47613.01</v>
       </c>
-      <c r="M30" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" t="inlineStr">
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O30" t="inlineStr"/>
       <c r="P30" t="n">
-        <v>403273.27</v>
-      </c>
-      <c r="Q30" t="n">
-        <v>0</v>
-      </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>355660.26</v>
+      </c>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="n">
+        <v>355660.26</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2533,43 +2568,44 @@
         <v>418857.39</v>
       </c>
       <c r="H31" t="n">
+        <v>458563.41</v>
+      </c>
+      <c r="I31" t="n">
         <v>100</v>
       </c>
-      <c r="I31" t="n">
-        <v>0</v>
-      </c>
       <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
         <v>418857.39</v>
       </c>
-      <c r="K31" t="n">
+      <c r="L31" t="n">
         <v>109.48</v>
       </c>
-      <c r="L31" t="n">
+      <c r="M31" t="n">
         <v>-39706.02</v>
       </c>
-      <c r="M31" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" t="inlineStr">
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O31" t="inlineStr"/>
       <c r="P31" t="n">
-        <v>458563.41</v>
-      </c>
-      <c r="Q31" t="n">
-        <v>0</v>
-      </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>418857.39</v>
+      </c>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="n">
+        <v>418857.39</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2600,47 +2636,48 @@
         <v>574740.27</v>
       </c>
       <c r="H32" t="n">
+        <v>319205.7</v>
+      </c>
+      <c r="I32" t="n">
         <v>64</v>
       </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
         <v>56</v>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>306528.14</v>
       </c>
-      <c r="K32" t="n">
+      <c r="L32" t="n">
         <v>104.14</v>
       </c>
-      <c r="L32" t="n">
+      <c r="M32" t="n">
         <v>255534.57</v>
       </c>
-      <c r="M32" t="n">
+      <c r="N32" t="n">
         <v>4563.12</v>
       </c>
-      <c r="N32" t="inlineStr">
+      <c r="O32" t="inlineStr">
         <is>
           <t>On Track</t>
         </is>
       </c>
-      <c r="O32" t="inlineStr">
+      <c r="P32" t="n">
+        <v>574740.27</v>
+      </c>
+      <c r="Q32" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="P32" t="n">
-        <v>319205.7</v>
-      </c>
-      <c r="Q32" t="n">
-        <v>0</v>
-      </c>
-      <c r="R32" t="inlineStr">
+      <c r="R32" t="n">
+        <v>574740.27</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="inlineStr">
         <is>
           <t>YES</t>
-        </is>
-      </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2671,47 +2708,48 @@
         <v>129356.97</v>
       </c>
       <c r="H33" t="n">
+        <v>80394.50999999999</v>
+      </c>
+      <c r="I33" t="n">
         <v>34</v>
       </c>
-      <c r="I33" t="n">
+      <c r="J33" t="n">
         <v>32</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>66638.44</v>
       </c>
-      <c r="K33" t="n">
+      <c r="L33" t="n">
         <v>120.64</v>
       </c>
-      <c r="L33" t="n">
+      <c r="M33" t="n">
         <v>48962.46</v>
       </c>
-      <c r="M33" t="n">
+      <c r="N33" t="n">
         <v>1530.08</v>
       </c>
-      <c r="N33" t="inlineStr">
+      <c r="O33" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O33" t="inlineStr">
+      <c r="P33" t="n">
+        <v>129356.97</v>
+      </c>
+      <c r="Q33" t="inlineStr">
         <is>
           <t>Overdelivered</t>
         </is>
       </c>
-      <c r="P33" t="n">
-        <v>80394.50999999999</v>
-      </c>
-      <c r="Q33" t="n">
+      <c r="R33" t="n">
+        <v>129356.97</v>
+      </c>
+      <c r="S33" t="n">
         <v>48962.46000000001</v>
       </c>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2742,43 +2780,44 @@
         <v>591950.49</v>
       </c>
       <c r="H34" t="n">
+        <v>646078.15</v>
+      </c>
+      <c r="I34" t="n">
         <v>29</v>
       </c>
-      <c r="I34" t="n">
-        <v>0</v>
-      </c>
       <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
         <v>591950.49</v>
       </c>
-      <c r="K34" t="n">
+      <c r="L34" t="n">
         <v>109.14</v>
       </c>
-      <c r="L34" t="n">
+      <c r="M34" t="n">
         <v>-54127.66</v>
       </c>
-      <c r="M34" t="n">
-        <v>0</v>
-      </c>
-      <c r="N34" t="inlineStr">
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O34" t="inlineStr"/>
       <c r="P34" t="n">
-        <v>646078.15</v>
-      </c>
-      <c r="Q34" t="n">
-        <v>0</v>
-      </c>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>591950.49</v>
+      </c>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="n">
+        <v>591950.49</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2809,43 +2848,44 @@
         <v>390381.81</v>
       </c>
       <c r="H35" t="n">
+        <v>450621.32</v>
+      </c>
+      <c r="I35" t="n">
         <v>64</v>
       </c>
-      <c r="I35" t="n">
-        <v>0</v>
-      </c>
       <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
         <v>390381.81</v>
       </c>
-      <c r="K35" t="n">
+      <c r="L35" t="n">
         <v>115.43</v>
       </c>
-      <c r="L35" t="n">
+      <c r="M35" t="n">
         <v>-60239.51</v>
       </c>
-      <c r="M35" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" t="inlineStr">
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O35" t="inlineStr"/>
       <c r="P35" t="n">
-        <v>450621.32</v>
-      </c>
-      <c r="Q35" t="n">
-        <v>0</v>
-      </c>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>390381.81</v>
+      </c>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="n">
+        <v>390381.81</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2876,43 +2916,44 @@
         <v>128268.79</v>
       </c>
       <c r="H36" t="n">
+        <v>143477.5</v>
+      </c>
+      <c r="I36" t="n">
         <v>89</v>
       </c>
-      <c r="I36" t="n">
-        <v>0</v>
-      </c>
       <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
         <v>128268.79</v>
       </c>
-      <c r="K36" t="n">
+      <c r="L36" t="n">
         <v>111.86</v>
       </c>
-      <c r="L36" t="n">
+      <c r="M36" t="n">
         <v>-15208.71</v>
       </c>
-      <c r="M36" t="n">
-        <v>0</v>
-      </c>
-      <c r="N36" t="inlineStr">
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O36" t="inlineStr"/>
       <c r="P36" t="n">
-        <v>143477.5</v>
-      </c>
-      <c r="Q36" t="n">
-        <v>0</v>
-      </c>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S36" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>128268.79</v>
+      </c>
+      <c r="Q36" t="inlineStr"/>
+      <c r="R36" t="n">
+        <v>128268.79</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2946,40 +2987,41 @@
         <v>0</v>
       </c>
       <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
         <v>30</v>
       </c>
-      <c r="J37" t="n">
-        <v>0</v>
-      </c>
       <c r="K37" t="n">
         <v>0</v>
       </c>
       <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
         <v>534024.5</v>
       </c>
-      <c r="M37" t="n">
+      <c r="N37" t="n">
         <v>17800.82</v>
       </c>
-      <c r="N37" t="inlineStr">
+      <c r="O37" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="O37" t="inlineStr"/>
       <c r="P37" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q37" t="n">
-        <v>0</v>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>534024.5</v>
+      </c>
+      <c r="Q37" t="inlineStr"/>
+      <c r="R37" t="n">
+        <v>534024.5</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0</v>
+      </c>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3010,43 +3052,44 @@
         <v>391196.57</v>
       </c>
       <c r="H38" t="n">
+        <v>406038.37</v>
+      </c>
+      <c r="I38" t="n">
         <v>65</v>
       </c>
-      <c r="I38" t="n">
-        <v>0</v>
-      </c>
       <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
         <v>391196.57</v>
       </c>
-      <c r="K38" t="n">
+      <c r="L38" t="n">
         <v>103.79</v>
       </c>
-      <c r="L38" t="n">
+      <c r="M38" t="n">
         <v>-14841.8</v>
       </c>
-      <c r="M38" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" t="inlineStr">
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="inlineStr">
         <is>
           <t>On Track</t>
         </is>
       </c>
-      <c r="O38" t="inlineStr"/>
       <c r="P38" t="n">
-        <v>406038.37</v>
-      </c>
-      <c r="Q38" t="n">
-        <v>0</v>
-      </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>391196.57</v>
+      </c>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="n">
+        <v>391196.57</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3077,43 +3120,44 @@
         <v>596378.9300000001</v>
       </c>
       <c r="H39" t="n">
+        <v>727570.66</v>
+      </c>
+      <c r="I39" t="n">
         <v>83</v>
       </c>
-      <c r="I39" t="n">
-        <v>0</v>
-      </c>
       <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
         <v>596378.9300000001</v>
       </c>
-      <c r="K39" t="n">
+      <c r="L39" t="n">
         <v>122</v>
       </c>
-      <c r="L39" t="n">
+      <c r="M39" t="n">
         <v>-131191.73</v>
       </c>
-      <c r="M39" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" t="inlineStr">
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O39" t="inlineStr"/>
       <c r="P39" t="n">
-        <v>727570.66</v>
-      </c>
-      <c r="Q39" t="n">
-        <v>0</v>
-      </c>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>596378.9300000001</v>
+      </c>
+      <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="n">
+        <v>596378.9300000001</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3144,47 +3188,48 @@
         <v>120089.45</v>
       </c>
       <c r="H40" t="n">
+        <v>69445.75999999999</v>
+      </c>
+      <c r="I40" t="n">
         <v>39</v>
       </c>
-      <c r="I40" t="n">
+      <c r="J40" t="n">
         <v>26</v>
       </c>
-      <c r="J40" t="n">
+      <c r="K40" t="n">
         <v>72053.67</v>
       </c>
-      <c r="K40" t="n">
+      <c r="L40" t="n">
         <v>96.38</v>
       </c>
-      <c r="L40" t="n">
+      <c r="M40" t="n">
         <v>50643.69</v>
       </c>
-      <c r="M40" t="n">
+      <c r="N40" t="n">
         <v>1947.83</v>
       </c>
-      <c r="N40" t="inlineStr">
+      <c r="O40" t="inlineStr">
         <is>
           <t>On Track</t>
         </is>
       </c>
-      <c r="O40" t="inlineStr">
+      <c r="P40" t="n">
+        <v>120089.45</v>
+      </c>
+      <c r="Q40" t="inlineStr">
         <is>
           <t>Overdelivered</t>
         </is>
       </c>
-      <c r="P40" t="n">
-        <v>69445.75999999999</v>
-      </c>
-      <c r="Q40" t="n">
+      <c r="R40" t="n">
+        <v>120089.45</v>
+      </c>
+      <c r="S40" t="n">
         <v>50643.69</v>
       </c>
-      <c r="R40" t="inlineStr">
+      <c r="T40" t="inlineStr">
         <is>
           <t>YES</t>
-        </is>
-      </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -3218,40 +3263,41 @@
         <v>0</v>
       </c>
       <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
         <v>54</v>
       </c>
-      <c r="J41" t="n">
-        <v>0</v>
-      </c>
       <c r="K41" t="n">
         <v>0</v>
       </c>
       <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
         <v>326276.52</v>
       </c>
-      <c r="M41" t="n">
+      <c r="N41" t="n">
         <v>6042.16</v>
       </c>
-      <c r="N41" t="inlineStr">
+      <c r="O41" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="O41" t="inlineStr"/>
       <c r="P41" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q41" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>326276.52</v>
+      </c>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="n">
+        <v>326276.52</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0</v>
+      </c>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3285,40 +3331,41 @@
         <v>0</v>
       </c>
       <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
         <v>47</v>
       </c>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
       <c r="K42" t="n">
         <v>0</v>
       </c>
       <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="n">
         <v>574267.4300000001</v>
       </c>
-      <c r="M42" t="n">
+      <c r="N42" t="n">
         <v>12218.46</v>
       </c>
-      <c r="N42" t="inlineStr">
+      <c r="O42" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="O42" t="inlineStr"/>
       <c r="P42" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q42" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>574267.4300000001</v>
+      </c>
+      <c r="Q42" t="inlineStr"/>
+      <c r="R42" t="n">
+        <v>574267.4300000001</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0</v>
+      </c>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3349,43 +3396,44 @@
         <v>352257.46</v>
       </c>
       <c r="H43" t="n">
+        <v>400379.35</v>
+      </c>
+      <c r="I43" t="n">
         <v>118</v>
       </c>
-      <c r="I43" t="n">
-        <v>0</v>
-      </c>
       <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
         <v>352257.46</v>
       </c>
-      <c r="K43" t="n">
+      <c r="L43" t="n">
         <v>113.66</v>
       </c>
-      <c r="L43" t="n">
+      <c r="M43" t="n">
         <v>-48121.89</v>
       </c>
-      <c r="M43" t="n">
-        <v>0</v>
-      </c>
-      <c r="N43" t="inlineStr">
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O43" t="inlineStr"/>
       <c r="P43" t="n">
-        <v>400379.35</v>
-      </c>
-      <c r="Q43" t="n">
-        <v>0</v>
-      </c>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>352257.46</v>
+      </c>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="n">
+        <v>352257.46</v>
+      </c>
+      <c r="S43" t="n">
+        <v>0</v>
+      </c>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3419,40 +3467,41 @@
         <v>0</v>
       </c>
       <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
         <v>87</v>
       </c>
-      <c r="J44" t="n">
-        <v>0</v>
-      </c>
       <c r="K44" t="n">
         <v>0</v>
       </c>
       <c r="L44" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" t="n">
         <v>267517.39</v>
       </c>
-      <c r="M44" t="n">
+      <c r="N44" t="n">
         <v>3074.91</v>
       </c>
-      <c r="N44" t="inlineStr">
+      <c r="O44" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="O44" t="inlineStr"/>
       <c r="P44" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q44" t="n">
-        <v>0</v>
-      </c>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S44" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>267517.39</v>
+      </c>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="n">
+        <v>267517.39</v>
+      </c>
+      <c r="S44" t="n">
+        <v>0</v>
+      </c>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3483,47 +3532,48 @@
         <v>354611.01</v>
       </c>
       <c r="H45" t="n">
+        <v>297314.53</v>
+      </c>
+      <c r="I45" t="n">
         <v>58</v>
       </c>
-      <c r="I45" t="n">
+      <c r="J45" t="n">
         <v>21</v>
       </c>
-      <c r="J45" t="n">
+      <c r="K45" t="n">
         <v>260347.32</v>
       </c>
-      <c r="K45" t="n">
+      <c r="L45" t="n">
         <v>114.2</v>
       </c>
-      <c r="L45" t="n">
+      <c r="M45" t="n">
         <v>57296.48</v>
       </c>
-      <c r="M45" t="n">
+      <c r="N45" t="n">
         <v>2728.4</v>
       </c>
-      <c r="N45" t="inlineStr">
+      <c r="O45" t="inlineStr">
         <is>
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="O45" t="inlineStr">
+      <c r="P45" t="n">
+        <v>354611.01</v>
+      </c>
+      <c r="Q45" t="inlineStr">
         <is>
           <t>Overdelivered</t>
         </is>
       </c>
-      <c r="P45" t="n">
-        <v>297314.53</v>
-      </c>
-      <c r="Q45" t="n">
+      <c r="R45" t="n">
+        <v>354611.01</v>
+      </c>
+      <c r="S45" t="n">
         <v>57296.47999999998</v>
       </c>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S45" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3557,40 +3607,41 @@
         <v>0</v>
       </c>
       <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
         <v>45</v>
       </c>
-      <c r="J46" t="n">
-        <v>0</v>
-      </c>
       <c r="K46" t="n">
         <v>0</v>
       </c>
       <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
         <v>498191.26</v>
       </c>
-      <c r="M46" t="n">
+      <c r="N46" t="n">
         <v>11070.92</v>
       </c>
-      <c r="N46" t="inlineStr">
+      <c r="O46" t="inlineStr">
         <is>
           <t>No Data</t>
         </is>
       </c>
-      <c r="O46" t="inlineStr"/>
       <c r="P46" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q46" t="n">
-        <v>0</v>
-      </c>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+        <v>498191.26</v>
+      </c>
+      <c r="Q46" t="inlineStr"/>
+      <c r="R46" t="n">
+        <v>498191.26</v>
+      </c>
+      <c r="S46" t="n">
+        <v>0</v>
+      </c>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3605,7 +3656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3616,18 +3667,119 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Metric</t>
+          <t>Feature</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>Importance</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Flight_Days</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.20614220934099</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Pace_Ratio</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.20390132996488</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Days_Elapsed</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1877645364903143</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Total_Budget</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.1321115504085586</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Spend_to_Date</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1072231073419659</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Spend_Velocity</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.08284332691757575</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>DSP_enc</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.08001393953571562</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>ML Validation Accuracy</t>
         </is>
       </c>
@@ -3638,52 +3790,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Total Campaigns</t>
+          <t>Total Budget At Risk</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>45</v>
+        <v>1494927.85</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ML Risk Alerts</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Early Warnings</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Total Budget At Risk</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1494927.85</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Last Refresh Date</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
+          <t>LAST_REFRESH_UTC</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2026-02-09 12:17 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily refresh: updated pacing output till yesterday
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -559,16 +559,16 @@
         <v>45826</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G2" t="n">
         <v>100350.37</v>
       </c>
       <c r="H2" t="n">
-        <v>149115.72</v>
+        <v>152252.76</v>
       </c>
       <c r="I2" t="n">
         <v>104</v>
@@ -580,10 +580,10 @@
         <v>100350.37</v>
       </c>
       <c r="L2" t="n">
-        <v>148.6</v>
+        <v>151.72</v>
       </c>
       <c r="M2" t="n">
-        <v>-48765.35</v>
+        <v>-51902.39</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
@@ -627,34 +627,34 @@
         <v>46071</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G3" t="n">
         <v>552594.63</v>
       </c>
       <c r="H3" t="n">
-        <v>514393.08</v>
+        <v>529757.87</v>
       </c>
       <c r="I3" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K3" t="n">
-        <v>453917.02</v>
+        <v>463784.78</v>
       </c>
       <c r="L3" t="n">
-        <v>113.32</v>
+        <v>114.22</v>
       </c>
       <c r="M3" t="n">
-        <v>38201.55</v>
+        <v>22836.76</v>
       </c>
       <c r="N3" t="n">
-        <v>3820.15</v>
+        <v>2537.42</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>552594.63</v>
       </c>
       <c r="S3" t="n">
-        <v>38201.54999999999</v>
+        <v>22836.76000000001</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
@@ -699,16 +699,16 @@
         <v>45984</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G4" t="n">
         <v>294540.38</v>
       </c>
       <c r="H4" t="n">
-        <v>408711.91</v>
+        <v>428119.9</v>
       </c>
       <c r="I4" t="n">
         <v>76</v>
@@ -720,10 +720,10 @@
         <v>294540.38</v>
       </c>
       <c r="L4" t="n">
-        <v>138.76</v>
+        <v>145.35</v>
       </c>
       <c r="M4" t="n">
-        <v>-114171.53</v>
+        <v>-133579.52</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -767,16 +767,16 @@
         <v>45811</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G5" t="n">
         <v>509097.37</v>
       </c>
       <c r="H5" t="n">
-        <v>760006.08</v>
+        <v>781733.62</v>
       </c>
       <c r="I5" t="n">
         <v>28</v>
@@ -788,10 +788,10 @@
         <v>509097.37</v>
       </c>
       <c r="L5" t="n">
-        <v>149.29</v>
+        <v>153.55</v>
       </c>
       <c r="M5" t="n">
-        <v>-250908.71</v>
+        <v>-272636.25</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -835,16 +835,16 @@
         <v>45997</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G6" t="n">
         <v>382409.25</v>
       </c>
       <c r="H6" t="n">
-        <v>362804.55</v>
+        <v>371764.94</v>
       </c>
       <c r="I6" t="n">
         <v>94</v>
@@ -856,17 +856,17 @@
         <v>382409.25</v>
       </c>
       <c r="L6" t="n">
-        <v>94.87</v>
+        <v>97.22</v>
       </c>
       <c r="M6" t="n">
-        <v>19604.7</v>
+        <v>10644.31</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P6" t="n">
@@ -903,16 +903,16 @@
         <v>46005</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G7" t="n">
         <v>525695.9399999999</v>
       </c>
       <c r="H7" t="n">
-        <v>528535.6899999999</v>
+        <v>537559.8199999999</v>
       </c>
       <c r="I7" t="n">
         <v>92</v>
@@ -924,10 +924,10 @@
         <v>525695.9399999999</v>
       </c>
       <c r="L7" t="n">
-        <v>100.54</v>
+        <v>102.26</v>
       </c>
       <c r="M7" t="n">
-        <v>-2839.75</v>
+        <v>-11863.88</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
@@ -971,38 +971,38 @@
         <v>46102</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G8" t="n">
         <v>136840.92</v>
       </c>
       <c r="H8" t="n">
-        <v>38505.81</v>
+        <v>41889.88</v>
       </c>
       <c r="I8" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J8" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K8" t="n">
-        <v>41748.08</v>
+        <v>44067.41</v>
       </c>
       <c r="L8" t="n">
-        <v>92.23</v>
+        <v>95.06</v>
       </c>
       <c r="M8" t="n">
-        <v>98335.11</v>
+        <v>94951.03999999999</v>
       </c>
       <c r="N8" t="n">
-        <v>2398.42</v>
+        <v>2373.78</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P8" t="n">
@@ -1017,11 +1017,11 @@
         <v>136840.92</v>
       </c>
       <c r="S8" t="n">
-        <v>98335.11000000002</v>
+        <v>94951.04000000001</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1043,10 +1043,10 @@
         <v>46119</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G9" t="n">
         <v>380340.09</v>
@@ -1111,34 +1111,34 @@
         <v>46103</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G10" t="n">
         <v>448858.15</v>
       </c>
       <c r="H10" t="n">
-        <v>115615.11</v>
+        <v>120193.43</v>
       </c>
       <c r="I10" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J10" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K10" t="n">
-        <v>118120.57</v>
+        <v>125995.27</v>
       </c>
       <c r="L10" t="n">
-        <v>97.88</v>
+        <v>95.40000000000001</v>
       </c>
       <c r="M10" t="n">
-        <v>333243.04</v>
+        <v>328664.72</v>
       </c>
       <c r="N10" t="n">
-        <v>7934.36</v>
+        <v>8016.21</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1157,7 +1157,7 @@
         <v>448858.15</v>
       </c>
       <c r="S10" t="n">
-        <v>333243.04</v>
+        <v>328664.72</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
@@ -1183,10 +1183,10 @@
         <v>46172</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G11" t="n">
         <v>432209.99</v>
@@ -1251,34 +1251,34 @@
         <v>46105</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G12" t="n">
         <v>559806.73</v>
       </c>
       <c r="H12" t="n">
-        <v>285615.72</v>
+        <v>298551.78</v>
       </c>
       <c r="I12" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J12" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K12" t="n">
-        <v>259422.63</v>
+        <v>266249.54</v>
       </c>
       <c r="L12" t="n">
-        <v>110.1</v>
+        <v>112.13</v>
       </c>
       <c r="M12" t="n">
-        <v>274191.01</v>
+        <v>261254.95</v>
       </c>
       <c r="N12" t="n">
-        <v>6231.61</v>
+        <v>6075.7</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1297,7 +1297,7 @@
         <v>559806.73</v>
       </c>
       <c r="S12" t="n">
-        <v>274191.01</v>
+        <v>261254.95</v>
       </c>
       <c r="T12" t="inlineStr">
         <is>
@@ -1323,34 +1323,34 @@
         <v>46118</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G13" t="n">
         <v>169377.54</v>
       </c>
       <c r="H13" t="n">
-        <v>47892.43</v>
+        <v>51987.04</v>
       </c>
       <c r="I13" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J13" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K13" t="n">
-        <v>50185.94</v>
+        <v>52277.02</v>
       </c>
       <c r="L13" t="n">
-        <v>95.43000000000001</v>
+        <v>99.45</v>
       </c>
       <c r="M13" t="n">
-        <v>121485.11</v>
+        <v>117390.5</v>
       </c>
       <c r="N13" t="n">
-        <v>2131.32</v>
+        <v>2096.26</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1369,7 +1369,7 @@
         <v>169377.54</v>
       </c>
       <c r="S13" t="n">
-        <v>121485.11</v>
+        <v>117390.5</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
@@ -1395,16 +1395,16 @@
         <v>45875</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G14" t="n">
         <v>334936.09</v>
       </c>
       <c r="H14" t="n">
-        <v>322426.62</v>
+        <v>325258.34</v>
       </c>
       <c r="I14" t="n">
         <v>88</v>
@@ -1416,10 +1416,10 @@
         <v>334936.09</v>
       </c>
       <c r="L14" t="n">
-        <v>96.27</v>
+        <v>97.11</v>
       </c>
       <c r="M14" t="n">
-        <v>12509.47</v>
+        <v>9677.75</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
@@ -1463,10 +1463,10 @@
         <v>46176</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G15" t="n">
         <v>394703.48</v>
@@ -1531,16 +1531,16 @@
         <v>45766</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G16" t="n">
         <v>161605.1</v>
       </c>
       <c r="H16" t="n">
-        <v>195465.22</v>
+        <v>194329.94</v>
       </c>
       <c r="I16" t="n">
         <v>74</v>
@@ -1552,10 +1552,10 @@
         <v>161605.1</v>
       </c>
       <c r="L16" t="n">
-        <v>120.95</v>
+        <v>120.25</v>
       </c>
       <c r="M16" t="n">
-        <v>-33860.12</v>
+        <v>-32724.84</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
@@ -1599,16 +1599,16 @@
         <v>45778</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G17" t="n">
         <v>95583.81</v>
       </c>
       <c r="H17" t="n">
-        <v>123864.18</v>
+        <v>126689.71</v>
       </c>
       <c r="I17" t="n">
         <v>74</v>
@@ -1620,10 +1620,10 @@
         <v>95583.81</v>
       </c>
       <c r="L17" t="n">
-        <v>129.59</v>
+        <v>132.54</v>
       </c>
       <c r="M17" t="n">
-        <v>-28280.37</v>
+        <v>-31105.9</v>
       </c>
       <c r="N17" t="n">
         <v>0</v>
@@ -1667,10 +1667,10 @@
         <v>46196</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G18" t="n">
         <v>253564.24</v>
@@ -1735,10 +1735,10 @@
         <v>46204</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G19" t="n">
         <v>111100.55</v>
@@ -1803,34 +1803,34 @@
         <v>46112</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G20" t="n">
         <v>423679.91</v>
       </c>
       <c r="H20" t="n">
-        <v>221276.88</v>
+        <v>236140.97</v>
       </c>
       <c r="I20" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J20" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K20" t="n">
-        <v>183594.63</v>
+        <v>188302.18</v>
       </c>
       <c r="L20" t="n">
-        <v>120.52</v>
+        <v>125.41</v>
       </c>
       <c r="M20" t="n">
-        <v>202403.03</v>
+        <v>187538.94</v>
       </c>
       <c r="N20" t="n">
-        <v>3968.69</v>
+        <v>3750.78</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1849,7 +1849,7 @@
         <v>423679.91</v>
       </c>
       <c r="S20" t="n">
-        <v>202403.03</v>
+        <v>187538.94</v>
       </c>
       <c r="T20" t="inlineStr">
         <is>
@@ -1875,10 +1875,10 @@
         <v>46179</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G21" t="n">
         <v>224412.65</v>
@@ -1943,10 +1943,10 @@
         <v>46129</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G22" t="n">
         <v>568840.5</v>
@@ -2011,16 +2011,16 @@
         <v>45969</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G23" t="n">
         <v>105951.07</v>
       </c>
       <c r="H23" t="n">
-        <v>124882.54</v>
+        <v>125815.64</v>
       </c>
       <c r="I23" t="n">
         <v>84</v>
@@ -2032,10 +2032,10 @@
         <v>105951.07</v>
       </c>
       <c r="L23" t="n">
-        <v>117.87</v>
+        <v>118.75</v>
       </c>
       <c r="M23" t="n">
-        <v>-18931.47</v>
+        <v>-19864.57</v>
       </c>
       <c r="N23" t="n">
         <v>0</v>
@@ -2079,16 +2079,16 @@
         <v>45902</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G24" t="n">
         <v>280248.59</v>
       </c>
       <c r="H24" t="n">
-        <v>369255</v>
+        <v>376472.46</v>
       </c>
       <c r="I24" t="n">
         <v>71</v>
@@ -2100,10 +2100,10 @@
         <v>280248.59</v>
       </c>
       <c r="L24" t="n">
-        <v>131.76</v>
+        <v>134.34</v>
       </c>
       <c r="M24" t="n">
-        <v>-89006.41</v>
+        <v>-96223.87</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
@@ -2147,16 +2147,16 @@
         <v>45943</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G25" t="n">
         <v>285863.23</v>
       </c>
       <c r="H25" t="n">
-        <v>352204.5</v>
+        <v>363575.94</v>
       </c>
       <c r="I25" t="n">
         <v>78</v>
@@ -2168,10 +2168,10 @@
         <v>285863.23</v>
       </c>
       <c r="L25" t="n">
-        <v>123.21</v>
+        <v>127.19</v>
       </c>
       <c r="M25" t="n">
-        <v>-66341.27</v>
+        <v>-77712.71000000001</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
@@ -2215,16 +2215,16 @@
         <v>45808</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G26" t="n">
         <v>221171.06</v>
       </c>
       <c r="H26" t="n">
-        <v>264835.89</v>
+        <v>273766.69</v>
       </c>
       <c r="I26" t="n">
         <v>91</v>
@@ -2236,10 +2236,10 @@
         <v>221171.06</v>
       </c>
       <c r="L26" t="n">
-        <v>119.74</v>
+        <v>123.78</v>
       </c>
       <c r="M26" t="n">
-        <v>-43664.83</v>
+        <v>-52595.63</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
@@ -2283,34 +2283,34 @@
         <v>46092</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G27" t="n">
         <v>577808.88</v>
       </c>
       <c r="H27" t="n">
-        <v>403946.75</v>
+        <v>411671.4</v>
       </c>
       <c r="I27" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J27" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K27" t="n">
-        <v>362000.74</v>
+        <v>368962.3</v>
       </c>
       <c r="L27" t="n">
-        <v>111.59</v>
+        <v>111.58</v>
       </c>
       <c r="M27" t="n">
-        <v>173862.13</v>
+        <v>166137.48</v>
       </c>
       <c r="N27" t="n">
-        <v>5608.46</v>
+        <v>5537.92</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2329,7 +2329,7 @@
         <v>577808.88</v>
       </c>
       <c r="S27" t="n">
-        <v>173862.13</v>
+        <v>166137.48</v>
       </c>
       <c r="T27" t="inlineStr">
         <is>
@@ -2355,16 +2355,16 @@
         <v>45938</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G28" t="n">
         <v>196777.36</v>
       </c>
       <c r="H28" t="n">
-        <v>246887.79</v>
+        <v>254593.51</v>
       </c>
       <c r="I28" t="n">
         <v>40</v>
@@ -2376,10 +2376,10 @@
         <v>196777.36</v>
       </c>
       <c r="L28" t="n">
-        <v>125.47</v>
+        <v>129.38</v>
       </c>
       <c r="M28" t="n">
-        <v>-50110.43</v>
+        <v>-57816.15</v>
       </c>
       <c r="N28" t="n">
         <v>0</v>
@@ -2423,16 +2423,16 @@
         <v>45780</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G29" t="n">
         <v>170730.01</v>
       </c>
       <c r="H29" t="n">
-        <v>198094.87</v>
+        <v>240367.01</v>
       </c>
       <c r="I29" t="n">
         <v>96</v>
@@ -2444,10 +2444,10 @@
         <v>170730.01</v>
       </c>
       <c r="L29" t="n">
-        <v>116.03</v>
+        <v>140.79</v>
       </c>
       <c r="M29" t="n">
-        <v>-27364.86</v>
+        <v>-69637</v>
       </c>
       <c r="N29" t="n">
         <v>0</v>
@@ -2491,16 +2491,16 @@
         <v>45954</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G30" t="n">
         <v>355660.26</v>
       </c>
       <c r="H30" t="n">
-        <v>426710.91</v>
+        <v>446945.37</v>
       </c>
       <c r="I30" t="n">
         <v>74</v>
@@ -2512,10 +2512,10 @@
         <v>355660.26</v>
       </c>
       <c r="L30" t="n">
-        <v>119.98</v>
+        <v>125.67</v>
       </c>
       <c r="M30" t="n">
-        <v>-71050.64999999999</v>
+        <v>-91285.11</v>
       </c>
       <c r="N30" t="n">
         <v>0</v>
@@ -2559,16 +2559,16 @@
         <v>45765</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G31" t="n">
         <v>418857.39</v>
       </c>
       <c r="H31" t="n">
-        <v>495019.74</v>
+        <v>523828.99</v>
       </c>
       <c r="I31" t="n">
         <v>100</v>
@@ -2580,10 +2580,10 @@
         <v>418857.39</v>
       </c>
       <c r="L31" t="n">
-        <v>118.18</v>
+        <v>125.06</v>
       </c>
       <c r="M31" t="n">
-        <v>-76162.35000000001</v>
+        <v>-104971.6</v>
       </c>
       <c r="N31" t="n">
         <v>0</v>
@@ -2627,34 +2627,34 @@
         <v>46117</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G32" t="n">
         <v>574740.27</v>
       </c>
       <c r="H32" t="n">
-        <v>337579.23</v>
+        <v>380353.47</v>
       </c>
       <c r="I32" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J32" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K32" t="n">
-        <v>306528.14</v>
+        <v>311317.65</v>
       </c>
       <c r="L32" t="n">
-        <v>110.13</v>
+        <v>122.18</v>
       </c>
       <c r="M32" t="n">
-        <v>237161.04</v>
+        <v>194386.8</v>
       </c>
       <c r="N32" t="n">
-        <v>4235.02</v>
+        <v>3534.31</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2666,7 +2666,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="R32" t="n">
@@ -2699,34 +2699,34 @@
         <v>46093</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G33" t="n">
         <v>129356.97</v>
       </c>
       <c r="H33" t="n">
-        <v>85708.21000000001</v>
+        <v>87111.62</v>
       </c>
       <c r="I33" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J33" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K33" t="n">
-        <v>66638.44</v>
+        <v>68598.39</v>
       </c>
       <c r="L33" t="n">
-        <v>128.62</v>
+        <v>126.99</v>
       </c>
       <c r="M33" t="n">
-        <v>43648.76</v>
+        <v>42245.35</v>
       </c>
       <c r="N33" t="n">
-        <v>1364.02</v>
+        <v>1362.75</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2745,7 +2745,7 @@
         <v>129356.97</v>
       </c>
       <c r="S33" t="n">
-        <v>43648.75999999999</v>
+        <v>42245.35000000001</v>
       </c>
       <c r="T33" t="inlineStr">
         <is>
@@ -2771,16 +2771,16 @@
         <v>45931</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G34" t="n">
         <v>591950.49</v>
       </c>
       <c r="H34" t="n">
-        <v>700592.98</v>
+        <v>768780.63</v>
       </c>
       <c r="I34" t="n">
         <v>29</v>
@@ -2792,10 +2792,10 @@
         <v>591950.49</v>
       </c>
       <c r="L34" t="n">
-        <v>118.35</v>
+        <v>129.87</v>
       </c>
       <c r="M34" t="n">
-        <v>-108642.49</v>
+        <v>-176830.14</v>
       </c>
       <c r="N34" t="n">
         <v>0</v>
@@ -2839,16 +2839,16 @@
         <v>45972</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G35" t="n">
         <v>390381.81</v>
       </c>
       <c r="H35" t="n">
-        <v>480350.28</v>
+        <v>482029.86</v>
       </c>
       <c r="I35" t="n">
         <v>64</v>
@@ -2860,10 +2860,10 @@
         <v>390381.81</v>
       </c>
       <c r="L35" t="n">
-        <v>123.05</v>
+        <v>123.48</v>
       </c>
       <c r="M35" t="n">
-        <v>-89968.47</v>
+        <v>-91648.05</v>
       </c>
       <c r="N35" t="n">
         <v>0</v>
@@ -2907,16 +2907,16 @@
         <v>45951</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G36" t="n">
         <v>128268.79</v>
       </c>
       <c r="H36" t="n">
-        <v>150204.07</v>
+        <v>158422.37</v>
       </c>
       <c r="I36" t="n">
         <v>89</v>
@@ -2928,10 +2928,10 @@
         <v>128268.79</v>
       </c>
       <c r="L36" t="n">
-        <v>117.1</v>
+        <v>123.51</v>
       </c>
       <c r="M36" t="n">
-        <v>-21935.28</v>
+        <v>-30153.58</v>
       </c>
       <c r="N36" t="n">
         <v>0</v>
@@ -2975,10 +2975,10 @@
         <v>46095</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G37" t="n">
         <v>534024.5</v>
@@ -3043,16 +3043,16 @@
         <v>45899</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G38" t="n">
         <v>391196.57</v>
       </c>
       <c r="H38" t="n">
-        <v>436987.23</v>
+        <v>430267.72</v>
       </c>
       <c r="I38" t="n">
         <v>65</v>
@@ -3064,10 +3064,10 @@
         <v>391196.57</v>
       </c>
       <c r="L38" t="n">
-        <v>111.71</v>
+        <v>109.99</v>
       </c>
       <c r="M38" t="n">
-        <v>-45790.66</v>
+        <v>-39071.15</v>
       </c>
       <c r="N38" t="n">
         <v>0</v>
@@ -3111,16 +3111,16 @@
         <v>45969</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G39" t="n">
         <v>596378.9300000001</v>
       </c>
       <c r="H39" t="n">
-        <v>775972.6899999999</v>
+        <v>786642.95</v>
       </c>
       <c r="I39" t="n">
         <v>83</v>
@@ -3132,10 +3132,10 @@
         <v>596378.9300000001</v>
       </c>
       <c r="L39" t="n">
-        <v>130.11</v>
+        <v>131.9</v>
       </c>
       <c r="M39" t="n">
-        <v>-179593.76</v>
+        <v>-190264.02</v>
       </c>
       <c r="N39" t="n">
         <v>0</v>
@@ -3179,34 +3179,34 @@
         <v>46087</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G40" t="n">
         <v>120089.45</v>
       </c>
       <c r="H40" t="n">
-        <v>71058.67</v>
+        <v>73168.13</v>
       </c>
       <c r="I40" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J40" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K40" t="n">
-        <v>72053.67</v>
+        <v>73901.2</v>
       </c>
       <c r="L40" t="n">
-        <v>98.62</v>
+        <v>99.01000000000001</v>
       </c>
       <c r="M40" t="n">
-        <v>49030.78</v>
+        <v>46921.32</v>
       </c>
       <c r="N40" t="n">
-        <v>1885.8</v>
+        <v>1876.85</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3225,7 +3225,7 @@
         <v>120089.45</v>
       </c>
       <c r="S40" t="n">
-        <v>49030.78</v>
+        <v>46921.31999999999</v>
       </c>
       <c r="T40" t="inlineStr">
         <is>
@@ -3251,10 +3251,10 @@
         <v>46159</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G41" t="n">
         <v>326276.52</v>
@@ -3319,10 +3319,10 @@
         <v>46111</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G42" t="n">
         <v>574267.4300000001</v>
@@ -3387,16 +3387,16 @@
         <v>46015</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G43" t="n">
         <v>352257.46</v>
       </c>
       <c r="H43" t="n">
-        <v>450187.93</v>
+        <v>474053.01</v>
       </c>
       <c r="I43" t="n">
         <v>118</v>
@@ -3408,10 +3408,10 @@
         <v>352257.46</v>
       </c>
       <c r="L43" t="n">
-        <v>127.8</v>
+        <v>134.58</v>
       </c>
       <c r="M43" t="n">
-        <v>-97930.47</v>
+        <v>-121795.55</v>
       </c>
       <c r="N43" t="n">
         <v>0</v>
@@ -3455,10 +3455,10 @@
         <v>46182</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G44" t="n">
         <v>267517.39</v>
@@ -3523,34 +3523,34 @@
         <v>46082</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G45" t="n">
         <v>354611.01</v>
       </c>
       <c r="H45" t="n">
-        <v>305824.04</v>
+        <v>323509.34</v>
       </c>
       <c r="I45" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J45" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K45" t="n">
-        <v>260347.32</v>
+        <v>264836.07</v>
       </c>
       <c r="L45" t="n">
-        <v>117.47</v>
+        <v>122.15</v>
       </c>
       <c r="M45" t="n">
-        <v>48786.97</v>
+        <v>31101.67</v>
       </c>
       <c r="N45" t="n">
-        <v>2323.19</v>
+        <v>1555.08</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3569,7 +3569,7 @@
         <v>354611.01</v>
       </c>
       <c r="S45" t="n">
-        <v>48786.97000000003</v>
+        <v>31101.66999999998</v>
       </c>
       <c r="T45" t="inlineStr">
         <is>
@@ -3595,10 +3595,10 @@
         <v>46135</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="G46" t="n">
         <v>498191.26</v>
@@ -3683,7 +3683,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2612529686759745</v>
+        <v>0.2906904624197857</v>
       </c>
     </row>
     <row r="3">
@@ -3693,57 +3693,57 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2201912516487678</v>
+        <v>0.2429200761048236</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Spend_to_Date</t>
+          <t>Total_Budget</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1277462596841187</v>
+        <v>0.1177042667321937</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Total_Budget</t>
+          <t>Pace_Ratio</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1207321921315315</v>
+        <v>0.09836046815101597</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Spend_Velocity</t>
+          <t>DSP_enc</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.09635746771991167</v>
+        <v>0.09156165329799966</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Pace_Ratio</t>
+          <t>Spend_to_Date</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.08994689671939443</v>
+        <v>0.09033545401966457</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DSP_enc</t>
+          <t>Spend_Velocity</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.08377296342030142</v>
+        <v>0.06842761927451674</v>
       </c>
     </row>
   </sheetData>
@@ -3794,7 +3794,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1383187.49</v>
+        <v>1299042.73</v>
       </c>
     </row>
     <row r="4">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2026-02-09 12:45 UTC</t>
+          <t>2026-02-10 07:41 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto refresh pacing dashboard
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -3012,7 +3012,11 @@
       <c r="P37" t="n">
         <v>534024.5</v>
       </c>
-      <c r="Q37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>Underdelivered</t>
+        </is>
+      </c>
       <c r="R37" t="n">
         <v>534024.5</v>
       </c>
@@ -3021,7 +3025,7 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3687,7 +3691,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3394570569242933</v>
+        <v>0.3367483364832408</v>
       </c>
     </row>
     <row r="3">
@@ -3697,7 +3701,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.33236008318548</v>
+        <v>0.3346764346764347</v>
       </c>
     </row>
     <row r="4">
@@ -3707,7 +3711,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1096964836065365</v>
+        <v>0.1289845549639365</v>
       </c>
     </row>
     <row r="5">
@@ -3717,27 +3721,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0878396195221592</v>
+        <v>0.1122651580678091</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Days_Elapsed</t>
+          <t>Flight_Days</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.06046995195672446</v>
+        <v>0.03702444939558342</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Flight_Days</t>
+          <t>Days_Elapsed</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.05149027652731356</v>
+        <v>0.0321754381548196</v>
       </c>
     </row>
     <row r="8">
@@ -3747,7 +3751,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.01868652827749287</v>
+        <v>0.01812562825817613</v>
       </c>
     </row>
   </sheetData>
@@ -3809,7 +3813,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2026-02-15 05:12 UTC</t>
+          <t>2026-02-15 05:14 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto refresh - 15-02-2026 11:05:02.07
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -559,16 +559,16 @@
         <v>45826</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G2" t="n">
         <v>100350.37</v>
       </c>
       <c r="H2" t="n">
-        <v>158690.48</v>
+        <v>157738.34</v>
       </c>
       <c r="I2" t="n">
         <v>104</v>
@@ -580,10 +580,10 @@
         <v>100350.37</v>
       </c>
       <c r="L2" t="n">
-        <v>158.14</v>
+        <v>157.19</v>
       </c>
       <c r="M2" t="n">
-        <v>-58340.11</v>
+        <v>-57387.97</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
@@ -627,34 +627,34 @@
         <v>46071</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G3" t="n">
         <v>552594.63</v>
       </c>
       <c r="H3" t="n">
-        <v>90145.39999999999</v>
+        <v>87823.07000000001</v>
       </c>
       <c r="I3" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K3" t="n">
-        <v>493388.06</v>
+        <v>513123.59</v>
       </c>
       <c r="L3" t="n">
-        <v>18.27</v>
+        <v>17.12</v>
       </c>
       <c r="M3" t="n">
-        <v>462449.23</v>
+        <v>464771.56</v>
       </c>
       <c r="N3" t="n">
-        <v>77074.87</v>
+        <v>116192.89</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -699,16 +699,16 @@
         <v>45984</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G4" t="n">
         <v>294540.38</v>
       </c>
       <c r="H4" t="n">
-        <v>83660.44</v>
+        <v>133057.46</v>
       </c>
       <c r="I4" t="n">
         <v>76</v>
@@ -720,10 +720,10 @@
         <v>294540.38</v>
       </c>
       <c r="L4" t="n">
-        <v>28.4</v>
+        <v>45.17</v>
       </c>
       <c r="M4" t="n">
-        <v>210879.94</v>
+        <v>161482.92</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -767,16 +767,16 @@
         <v>45811</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G5" t="n">
         <v>509097.37</v>
       </c>
       <c r="H5" t="n">
-        <v>39895.84</v>
+        <v>28952.07</v>
       </c>
       <c r="I5" t="n">
         <v>28</v>
@@ -788,10 +788,10 @@
         <v>509097.37</v>
       </c>
       <c r="L5" t="n">
-        <v>7.84</v>
+        <v>5.69</v>
       </c>
       <c r="M5" t="n">
-        <v>469201.53</v>
+        <v>480145.3</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -835,16 +835,16 @@
         <v>45997</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G6" t="n">
         <v>382409.25</v>
       </c>
       <c r="H6" t="n">
-        <v>96617.66</v>
+        <v>88566.33</v>
       </c>
       <c r="I6" t="n">
         <v>94</v>
@@ -856,10 +856,10 @@
         <v>382409.25</v>
       </c>
       <c r="L6" t="n">
-        <v>25.27</v>
+        <v>23.16</v>
       </c>
       <c r="M6" t="n">
-        <v>285791.59</v>
+        <v>293842.92</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
@@ -903,16 +903,16 @@
         <v>46005</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G7" t="n">
         <v>525695.9399999999</v>
       </c>
       <c r="H7" t="n">
-        <v>81592.46000000001</v>
+        <v>187552.69</v>
       </c>
       <c r="I7" t="n">
         <v>92</v>
@@ -924,10 +924,10 @@
         <v>525695.9399999999</v>
       </c>
       <c r="L7" t="n">
-        <v>15.52</v>
+        <v>35.68</v>
       </c>
       <c r="M7" t="n">
-        <v>444103.48</v>
+        <v>338143.25</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
@@ -971,34 +971,34 @@
         <v>46102</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G8" t="n">
         <v>136840.92</v>
       </c>
       <c r="H8" t="n">
-        <v>21172.1</v>
+        <v>41169.63</v>
       </c>
       <c r="I8" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J8" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K8" t="n">
-        <v>51025.43</v>
+        <v>55664.1</v>
       </c>
       <c r="L8" t="n">
-        <v>41.49</v>
+        <v>73.95999999999999</v>
       </c>
       <c r="M8" t="n">
-        <v>115668.82</v>
+        <v>95671.28999999999</v>
       </c>
       <c r="N8" t="n">
-        <v>3126.18</v>
+        <v>2733.47</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1043,10 +1043,10 @@
         <v>46119</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G9" t="n">
         <v>380340.09</v>
@@ -1111,34 +1111,34 @@
         <v>46103</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G10" t="n">
         <v>448858.15</v>
       </c>
       <c r="H10" t="n">
-        <v>25754</v>
+        <v>35389.47</v>
       </c>
       <c r="I10" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J10" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K10" t="n">
-        <v>149619.38</v>
+        <v>165368.79</v>
       </c>
       <c r="L10" t="n">
-        <v>17.21</v>
+        <v>21.4</v>
       </c>
       <c r="M10" t="n">
-        <v>423104.15</v>
+        <v>413468.68</v>
       </c>
       <c r="N10" t="n">
-        <v>11134.32</v>
+        <v>11485.24</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1183,10 +1183,10 @@
         <v>46172</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G11" t="n">
         <v>432209.99</v>
@@ -1251,34 +1251,34 @@
         <v>46105</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G12" t="n">
         <v>559806.73</v>
       </c>
       <c r="H12" t="n">
-        <v>56940.19</v>
+        <v>64081.81</v>
       </c>
       <c r="I12" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J12" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K12" t="n">
-        <v>286730.28</v>
+        <v>300384.1</v>
       </c>
       <c r="L12" t="n">
-        <v>19.86</v>
+        <v>21.33</v>
       </c>
       <c r="M12" t="n">
-        <v>502866.54</v>
+        <v>495724.92</v>
       </c>
       <c r="N12" t="n">
-        <v>12571.66</v>
+        <v>13045.39</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1323,34 +1323,34 @@
         <v>46118</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G13" t="n">
         <v>169377.54</v>
       </c>
       <c r="H13" t="n">
-        <v>45603.41</v>
+        <v>38713.84</v>
       </c>
       <c r="I13" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J13" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K13" t="n">
-        <v>58550.26</v>
+        <v>62732.42</v>
       </c>
       <c r="L13" t="n">
-        <v>77.89</v>
+        <v>61.71</v>
       </c>
       <c r="M13" t="n">
-        <v>123774.13</v>
+        <v>130663.7</v>
       </c>
       <c r="N13" t="n">
-        <v>2335.36</v>
+        <v>2562.03</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1395,16 +1395,16 @@
         <v>45875</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G14" t="n">
         <v>334936.09</v>
       </c>
       <c r="H14" t="n">
-        <v>174684.66</v>
+        <v>164342.59</v>
       </c>
       <c r="I14" t="n">
         <v>88</v>
@@ -1416,10 +1416,10 @@
         <v>334936.09</v>
       </c>
       <c r="L14" t="n">
-        <v>52.15</v>
+        <v>49.07</v>
       </c>
       <c r="M14" t="n">
-        <v>160251.43</v>
+        <v>170593.5</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
@@ -1463,10 +1463,10 @@
         <v>46176</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G15" t="n">
         <v>394703.48</v>
@@ -1531,16 +1531,16 @@
         <v>45766</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G16" t="n">
         <v>161605.1</v>
       </c>
       <c r="H16" t="n">
-        <v>109535.58</v>
+        <v>131961.07</v>
       </c>
       <c r="I16" t="n">
         <v>74</v>
@@ -1552,10 +1552,10 @@
         <v>161605.1</v>
       </c>
       <c r="L16" t="n">
-        <v>67.78</v>
+        <v>81.66</v>
       </c>
       <c r="M16" t="n">
-        <v>52069.52</v>
+        <v>29644.03</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
@@ -1599,16 +1599,16 @@
         <v>45778</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G17" t="n">
         <v>95583.81</v>
       </c>
       <c r="H17" t="n">
-        <v>120662.9</v>
+        <v>127061.04</v>
       </c>
       <c r="I17" t="n">
         <v>74</v>
@@ -1620,10 +1620,10 @@
         <v>95583.81</v>
       </c>
       <c r="L17" t="n">
-        <v>126.24</v>
+        <v>132.93</v>
       </c>
       <c r="M17" t="n">
-        <v>-25079.09</v>
+        <v>-31477.23</v>
       </c>
       <c r="N17" t="n">
         <v>0</v>
@@ -1667,10 +1667,10 @@
         <v>46196</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G18" t="n">
         <v>253564.24</v>
@@ -1735,10 +1735,10 @@
         <v>46204</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G19" t="n">
         <v>111100.55</v>
@@ -1803,34 +1803,34 @@
         <v>46112</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G20" t="n">
         <v>423679.91</v>
       </c>
       <c r="H20" t="n">
-        <v>51649.79</v>
+        <v>96281.41</v>
       </c>
       <c r="I20" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J20" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K20" t="n">
-        <v>202424.85</v>
+        <v>211839.95</v>
       </c>
       <c r="L20" t="n">
-        <v>25.52</v>
+        <v>45.45</v>
       </c>
       <c r="M20" t="n">
-        <v>372030.12</v>
+        <v>327398.5</v>
       </c>
       <c r="N20" t="n">
-        <v>7915.53</v>
+        <v>7275.52</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1875,10 +1875,10 @@
         <v>46179</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G21" t="n">
         <v>224412.65</v>
@@ -1943,10 +1943,10 @@
         <v>46129</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G22" t="n">
         <v>568840.5</v>
@@ -2011,16 +2011,16 @@
         <v>45969</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G23" t="n">
         <v>105951.07</v>
       </c>
       <c r="H23" t="n">
-        <v>122800.77</v>
+        <v>80082.50999999999</v>
       </c>
       <c r="I23" t="n">
         <v>84</v>
@@ -2032,17 +2032,17 @@
         <v>105951.07</v>
       </c>
       <c r="L23" t="n">
-        <v>115.9</v>
+        <v>75.58</v>
       </c>
       <c r="M23" t="n">
-        <v>-16849.7</v>
+        <v>25868.56</v>
       </c>
       <c r="N23" t="n">
         <v>0</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P23" t="n">
@@ -2079,16 +2079,16 @@
         <v>45902</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G24" t="n">
         <v>280248.59</v>
       </c>
       <c r="H24" t="n">
-        <v>139817.97</v>
+        <v>122270.66</v>
       </c>
       <c r="I24" t="n">
         <v>71</v>
@@ -2100,10 +2100,10 @@
         <v>280248.59</v>
       </c>
       <c r="L24" t="n">
-        <v>49.89</v>
+        <v>43.63</v>
       </c>
       <c r="M24" t="n">
-        <v>140430.62</v>
+        <v>157977.93</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
@@ -2147,16 +2147,16 @@
         <v>45943</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G25" t="n">
         <v>285863.23</v>
       </c>
       <c r="H25" t="n">
-        <v>77096.25999999999</v>
+        <v>136777.09</v>
       </c>
       <c r="I25" t="n">
         <v>78</v>
@@ -2168,10 +2168,10 @@
         <v>285863.23</v>
       </c>
       <c r="L25" t="n">
-        <v>26.97</v>
+        <v>47.85</v>
       </c>
       <c r="M25" t="n">
-        <v>208766.97</v>
+        <v>149086.14</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
@@ -2215,16 +2215,16 @@
         <v>45808</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G26" t="n">
         <v>221171.06</v>
       </c>
       <c r="H26" t="n">
-        <v>136496.72</v>
+        <v>159211.39</v>
       </c>
       <c r="I26" t="n">
         <v>91</v>
@@ -2236,10 +2236,10 @@
         <v>221171.06</v>
       </c>
       <c r="L26" t="n">
-        <v>61.72</v>
+        <v>71.98999999999999</v>
       </c>
       <c r="M26" t="n">
-        <v>84674.34</v>
+        <v>61959.67</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
@@ -2283,34 +2283,34 @@
         <v>46092</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G27" t="n">
         <v>577808.88</v>
       </c>
       <c r="H27" t="n">
-        <v>108681.58</v>
+        <v>107249.68</v>
       </c>
       <c r="I27" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J27" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K27" t="n">
-        <v>389846.96</v>
+        <v>403770.06</v>
       </c>
       <c r="L27" t="n">
-        <v>27.88</v>
+        <v>26.56</v>
       </c>
       <c r="M27" t="n">
-        <v>469127.3</v>
+        <v>470559.2</v>
       </c>
       <c r="N27" t="n">
-        <v>17375.09</v>
+        <v>18822.37</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2355,16 +2355,16 @@
         <v>45938</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G28" t="n">
         <v>196777.36</v>
       </c>
       <c r="H28" t="n">
-        <v>43250.63</v>
+        <v>40638.37</v>
       </c>
       <c r="I28" t="n">
         <v>40</v>
@@ -2376,10 +2376,10 @@
         <v>196777.36</v>
       </c>
       <c r="L28" t="n">
-        <v>21.98</v>
+        <v>20.65</v>
       </c>
       <c r="M28" t="n">
-        <v>153526.73</v>
+        <v>156138.99</v>
       </c>
       <c r="N28" t="n">
         <v>0</v>
@@ -2423,16 +2423,16 @@
         <v>45780</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G29" t="n">
         <v>170730.01</v>
       </c>
       <c r="H29" t="n">
-        <v>173453.58</v>
+        <v>159714.06</v>
       </c>
       <c r="I29" t="n">
         <v>96</v>
@@ -2444,17 +2444,17 @@
         <v>170730.01</v>
       </c>
       <c r="L29" t="n">
-        <v>101.6</v>
+        <v>93.55</v>
       </c>
       <c r="M29" t="n">
-        <v>-2723.57</v>
+        <v>11015.95</v>
       </c>
       <c r="N29" t="n">
         <v>0</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>On Track</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P29" t="n">
@@ -2491,16 +2491,16 @@
         <v>45954</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G30" t="n">
         <v>355660.26</v>
       </c>
       <c r="H30" t="n">
-        <v>93322.57000000001</v>
+        <v>82464.85000000001</v>
       </c>
       <c r="I30" t="n">
         <v>74</v>
@@ -2512,10 +2512,10 @@
         <v>355660.26</v>
       </c>
       <c r="L30" t="n">
-        <v>26.24</v>
+        <v>23.19</v>
       </c>
       <c r="M30" t="n">
-        <v>262337.69</v>
+        <v>273195.41</v>
       </c>
       <c r="N30" t="n">
         <v>0</v>
@@ -2559,16 +2559,16 @@
         <v>45765</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G31" t="n">
         <v>418857.39</v>
       </c>
       <c r="H31" t="n">
-        <v>148534.49</v>
+        <v>133740.94</v>
       </c>
       <c r="I31" t="n">
         <v>100</v>
@@ -2580,10 +2580,10 @@
         <v>418857.39</v>
       </c>
       <c r="L31" t="n">
-        <v>35.46</v>
+        <v>31.93</v>
       </c>
       <c r="M31" t="n">
-        <v>270322.9</v>
+        <v>285116.45</v>
       </c>
       <c r="N31" t="n">
         <v>0</v>
@@ -2627,34 +2627,34 @@
         <v>46117</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G32" t="n">
         <v>574740.27</v>
       </c>
       <c r="H32" t="n">
-        <v>64782.24</v>
+        <v>109593.36</v>
       </c>
       <c r="I32" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J32" t="n">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K32" t="n">
-        <v>325686.15</v>
+        <v>335265.16</v>
       </c>
       <c r="L32" t="n">
-        <v>19.89</v>
+        <v>32.69</v>
       </c>
       <c r="M32" t="n">
-        <v>509958.03</v>
+        <v>465146.91</v>
       </c>
       <c r="N32" t="n">
-        <v>9806.889999999999</v>
+        <v>9302.940000000001</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2699,34 +2699,34 @@
         <v>46093</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G33" t="n">
         <v>129356.97</v>
       </c>
       <c r="H33" t="n">
-        <v>47098.36</v>
+        <v>44817.85</v>
       </c>
       <c r="I33" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J33" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K33" t="n">
-        <v>74478.25999999999</v>
+        <v>78398.16</v>
       </c>
       <c r="L33" t="n">
-        <v>63.24</v>
+        <v>57.17</v>
       </c>
       <c r="M33" t="n">
-        <v>82258.61</v>
+        <v>84539.12</v>
       </c>
       <c r="N33" t="n">
-        <v>2937.81</v>
+        <v>3251.5</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2771,16 +2771,16 @@
         <v>45931</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G34" t="n">
         <v>591950.49</v>
       </c>
       <c r="H34" t="n">
-        <v>28438.88</v>
+        <v>68647.25999999999</v>
       </c>
       <c r="I34" t="n">
         <v>29</v>
@@ -2792,10 +2792,10 @@
         <v>591950.49</v>
       </c>
       <c r="L34" t="n">
-        <v>4.8</v>
+        <v>11.6</v>
       </c>
       <c r="M34" t="n">
-        <v>563511.61</v>
+        <v>523303.23</v>
       </c>
       <c r="N34" t="n">
         <v>0</v>
@@ -2839,16 +2839,16 @@
         <v>45972</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G35" t="n">
         <v>390381.81</v>
       </c>
       <c r="H35" t="n">
-        <v>127397.15</v>
+        <v>71073.24000000001</v>
       </c>
       <c r="I35" t="n">
         <v>64</v>
@@ -2860,10 +2860,10 @@
         <v>390381.81</v>
       </c>
       <c r="L35" t="n">
-        <v>32.63</v>
+        <v>18.21</v>
       </c>
       <c r="M35" t="n">
-        <v>262984.66</v>
+        <v>319308.57</v>
       </c>
       <c r="N35" t="n">
         <v>0</v>
@@ -2907,16 +2907,16 @@
         <v>45951</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G36" t="n">
         <v>128268.79</v>
       </c>
       <c r="H36" t="n">
-        <v>138076.93</v>
+        <v>85483.77</v>
       </c>
       <c r="I36" t="n">
         <v>89</v>
@@ -2928,17 +2928,17 @@
         <v>128268.79</v>
       </c>
       <c r="L36" t="n">
-        <v>107.65</v>
+        <v>66.64</v>
       </c>
       <c r="M36" t="n">
-        <v>-9808.139999999999</v>
+        <v>42785.02</v>
       </c>
       <c r="N36" t="n">
         <v>0</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P36" t="n">
@@ -2975,38 +2975,38 @@
         <v>46095</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G37" t="n">
         <v>534024.5</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>1884.06</v>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J37" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>35601.63</v>
       </c>
       <c r="L37" t="n">
-        <v>0</v>
+        <v>5.29</v>
       </c>
       <c r="M37" t="n">
-        <v>534024.5</v>
+        <v>532140.4399999999</v>
       </c>
       <c r="N37" t="n">
-        <v>17800.82</v>
+        <v>19005.02</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P37" t="n">
@@ -3025,7 +3025,7 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3047,16 +3047,16 @@
         <v>45899</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G38" t="n">
         <v>391196.57</v>
       </c>
       <c r="H38" t="n">
-        <v>119720.31</v>
+        <v>134655.18</v>
       </c>
       <c r="I38" t="n">
         <v>65</v>
@@ -3068,10 +3068,10 @@
         <v>391196.57</v>
       </c>
       <c r="L38" t="n">
-        <v>30.6</v>
+        <v>34.42</v>
       </c>
       <c r="M38" t="n">
-        <v>271476.26</v>
+        <v>256541.39</v>
       </c>
       <c r="N38" t="n">
         <v>0</v>
@@ -3115,16 +3115,16 @@
         <v>45969</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G39" t="n">
         <v>596378.9300000001</v>
       </c>
       <c r="H39" t="n">
-        <v>94528.91</v>
+        <v>75061.8</v>
       </c>
       <c r="I39" t="n">
         <v>83</v>
@@ -3136,10 +3136,10 @@
         <v>596378.9300000001</v>
       </c>
       <c r="L39" t="n">
-        <v>15.85</v>
+        <v>12.59</v>
       </c>
       <c r="M39" t="n">
-        <v>501850.02</v>
+        <v>521317.13</v>
       </c>
       <c r="N39" t="n">
         <v>0</v>
@@ -3183,34 +3183,34 @@
         <v>46087</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G40" t="n">
         <v>120089.45</v>
       </c>
       <c r="H40" t="n">
-        <v>61515.08</v>
+        <v>40142.96</v>
       </c>
       <c r="I40" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J40" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K40" t="n">
-        <v>79443.78999999999</v>
+        <v>83138.85000000001</v>
       </c>
       <c r="L40" t="n">
-        <v>77.43000000000001</v>
+        <v>48.28</v>
       </c>
       <c r="M40" t="n">
-        <v>58574.37</v>
+        <v>79946.49000000001</v>
       </c>
       <c r="N40" t="n">
-        <v>2662.47</v>
+        <v>3997.32</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3255,10 +3255,10 @@
         <v>46159</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G41" t="n">
         <v>326276.52</v>
@@ -3323,34 +3323,34 @@
         <v>46111</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G42" t="n">
         <v>574267.4300000001</v>
       </c>
       <c r="H42" t="n">
-        <v>1311.55</v>
+        <v>2699.06</v>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J42" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K42" t="n">
-        <v>12218.46</v>
+        <v>36655.37</v>
       </c>
       <c r="L42" t="n">
-        <v>10.73</v>
+        <v>7.36</v>
       </c>
       <c r="M42" t="n">
-        <v>572955.88</v>
+        <v>571568.37</v>
       </c>
       <c r="N42" t="n">
-        <v>12455.56</v>
+        <v>12990.19</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3395,16 +3395,16 @@
         <v>46015</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G43" t="n">
         <v>352257.46</v>
       </c>
       <c r="H43" t="n">
-        <v>115119.38</v>
+        <v>251672.33</v>
       </c>
       <c r="I43" t="n">
         <v>118</v>
@@ -3416,10 +3416,10 @@
         <v>352257.46</v>
       </c>
       <c r="L43" t="n">
-        <v>32.68</v>
+        <v>71.45</v>
       </c>
       <c r="M43" t="n">
-        <v>237138.08</v>
+        <v>100585.13</v>
       </c>
       <c r="N43" t="n">
         <v>0</v>
@@ -3463,10 +3463,10 @@
         <v>46182</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G44" t="n">
         <v>267517.39</v>
@@ -3531,34 +3531,34 @@
         <v>46082</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G45" t="n">
         <v>354611.01</v>
       </c>
       <c r="H45" t="n">
-        <v>106837.53</v>
+        <v>91143.19</v>
       </c>
       <c r="I45" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J45" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K45" t="n">
-        <v>278302.31</v>
+        <v>287279.81</v>
       </c>
       <c r="L45" t="n">
-        <v>38.39</v>
+        <v>31.73</v>
       </c>
       <c r="M45" t="n">
-        <v>247773.48</v>
+        <v>263467.82</v>
       </c>
       <c r="N45" t="n">
-        <v>14574.91</v>
+        <v>17564.52</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3603,10 +3603,10 @@
         <v>46135</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>46066</v>
+        <v>46068</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>46065</v>
+        <v>46067</v>
       </c>
       <c r="G46" t="n">
         <v>498191.26</v>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2026-02-15 05:14 UTC</t>
+          <t>2026-02-15 05:35 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto refresh - 15-02-2026 11:55:27.76
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,7 +472,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Total_Budget_x</t>
+          <t>Total_Budget</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -517,27 +517,42 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Total_Budget_y</t>
+          <t>Total_Budget_meta</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>Flight_Start_Date_meta</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Flight_End_Date_meta</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>ML_Prediction</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Total_Budget</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Campaign_Status</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Budget_At_Risk</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>ML_Early_Warning</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Excel_vs_ML_Disagree</t>
         </is>
       </c>
     </row>
@@ -596,16 +611,29 @@
       <c r="P2" t="n">
         <v>100350.37</v>
       </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="n">
-        <v>100350.37</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q2" s="2" t="n">
+        <v>45723</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>45826</v>
+      </c>
+      <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -664,20 +692,33 @@
       <c r="P3" t="n">
         <v>552594.63</v>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="Q3" s="2" t="n">
+        <v>46016</v>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>46071</v>
+      </c>
+      <c r="S3" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R3" t="n">
-        <v>552594.63</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
       <c r="T3" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -736,16 +777,29 @@
       <c r="P4" t="n">
         <v>294540.38</v>
       </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="n">
-        <v>294540.38</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q4" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>45984</v>
+      </c>
+      <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -804,16 +858,29 @@
       <c r="P5" t="n">
         <v>509097.37</v>
       </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="n">
-        <v>509097.37</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q5" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="R5" s="2" t="n">
+        <v>45811</v>
+      </c>
+      <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -872,16 +939,29 @@
       <c r="P6" t="n">
         <v>382409.25</v>
       </c>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="n">
-        <v>382409.25</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q6" s="2" t="n">
+        <v>45904</v>
+      </c>
+      <c r="R6" s="2" t="n">
+        <v>45997</v>
+      </c>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -940,16 +1020,29 @@
       <c r="P7" t="n">
         <v>525695.9399999999</v>
       </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="n">
-        <v>525695.9399999999</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q7" s="2" t="n">
+        <v>45914</v>
+      </c>
+      <c r="R7" s="2" t="n">
+        <v>46005</v>
+      </c>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1008,20 +1101,33 @@
       <c r="P8" t="n">
         <v>136840.92</v>
       </c>
-      <c r="Q8" t="inlineStr">
+      <c r="Q8" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="R8" s="2" t="n">
+        <v>46102</v>
+      </c>
+      <c r="S8" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R8" t="n">
-        <v>136840.92</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0</v>
-      </c>
       <c r="T8" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1080,16 +1186,29 @@
       <c r="P9" t="n">
         <v>380340.09</v>
       </c>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="n">
-        <v>380340.09</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q9" s="2" t="n">
+        <v>46086</v>
+      </c>
+      <c r="R9" s="2" t="n">
+        <v>46119</v>
+      </c>
+      <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1148,20 +1267,33 @@
       <c r="P10" t="n">
         <v>448858.15</v>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="Q10" s="2" t="n">
+        <v>46047</v>
+      </c>
+      <c r="R10" s="2" t="n">
+        <v>46103</v>
+      </c>
+      <c r="S10" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R10" t="n">
-        <v>448858.15</v>
-      </c>
-      <c r="S10" t="n">
-        <v>0</v>
-      </c>
       <c r="T10" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1220,16 +1352,29 @@
       <c r="P11" t="n">
         <v>432209.99</v>
       </c>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="n">
-        <v>432209.99</v>
-      </c>
-      <c r="S11" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q11" s="2" t="n">
+        <v>46089</v>
+      </c>
+      <c r="R11" s="2" t="n">
+        <v>46172</v>
+      </c>
+      <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1288,20 +1433,33 @@
       <c r="P12" t="n">
         <v>559806.73</v>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="Q12" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="R12" s="2" t="n">
+        <v>46105</v>
+      </c>
+      <c r="S12" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R12" t="n">
-        <v>559806.73</v>
-      </c>
-      <c r="S12" t="n">
-        <v>0</v>
-      </c>
       <c r="T12" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1360,20 +1518,33 @@
       <c r="P13" t="n">
         <v>169377.54</v>
       </c>
-      <c r="Q13" t="inlineStr">
+      <c r="Q13" s="2" t="n">
+        <v>46038</v>
+      </c>
+      <c r="R13" s="2" t="n">
+        <v>46118</v>
+      </c>
+      <c r="S13" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R13" t="n">
-        <v>169377.54</v>
-      </c>
-      <c r="S13" t="n">
-        <v>0</v>
-      </c>
       <c r="T13" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U13" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1432,16 +1603,29 @@
       <c r="P14" t="n">
         <v>334936.09</v>
       </c>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="n">
-        <v>334936.09</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q14" s="2" t="n">
+        <v>45788</v>
+      </c>
+      <c r="R14" s="2" t="n">
+        <v>45875</v>
+      </c>
+      <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1500,16 +1684,29 @@
       <c r="P15" t="n">
         <v>394703.48</v>
       </c>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="n">
-        <v>394703.48</v>
-      </c>
-      <c r="S15" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q15" s="2" t="n">
+        <v>46120</v>
+      </c>
+      <c r="R15" s="2" t="n">
+        <v>46176</v>
+      </c>
+      <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1568,16 +1765,29 @@
       <c r="P16" t="n">
         <v>161605.1</v>
       </c>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="n">
-        <v>161605.1</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q16" s="2" t="n">
+        <v>45693</v>
+      </c>
+      <c r="R16" s="2" t="n">
+        <v>45766</v>
+      </c>
+      <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1636,16 +1846,29 @@
       <c r="P17" t="n">
         <v>95583.81</v>
       </c>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="n">
-        <v>95583.81</v>
-      </c>
-      <c r="S17" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q17" s="2" t="n">
+        <v>45705</v>
+      </c>
+      <c r="R17" s="2" t="n">
+        <v>45778</v>
+      </c>
+      <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1704,16 +1927,29 @@
       <c r="P18" t="n">
         <v>253564.24</v>
       </c>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="n">
-        <v>253564.24</v>
-      </c>
-      <c r="S18" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q18" s="2" t="n">
+        <v>46136</v>
+      </c>
+      <c r="R18" s="2" t="n">
+        <v>46196</v>
+      </c>
+      <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U18" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1772,16 +2008,29 @@
       <c r="P19" t="n">
         <v>111100.55</v>
       </c>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="n">
-        <v>111100.55</v>
-      </c>
-      <c r="S19" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q19" s="2" t="n">
+        <v>46126</v>
+      </c>
+      <c r="R19" s="2" t="n">
+        <v>46204</v>
+      </c>
+      <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U19" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1840,20 +2089,33 @@
       <c r="P20" t="n">
         <v>423679.91</v>
       </c>
-      <c r="Q20" t="inlineStr">
+      <c r="Q20" s="2" t="n">
+        <v>46023</v>
+      </c>
+      <c r="R20" s="2" t="n">
+        <v>46112</v>
+      </c>
+      <c r="S20" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R20" t="n">
-        <v>423679.91</v>
-      </c>
-      <c r="S20" t="n">
-        <v>0</v>
-      </c>
       <c r="T20" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1912,16 +2174,29 @@
       <c r="P21" t="n">
         <v>224412.65</v>
       </c>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="n">
-        <v>224412.65</v>
-      </c>
-      <c r="S21" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q21" s="2" t="n">
+        <v>46102</v>
+      </c>
+      <c r="R21" s="2" t="n">
+        <v>46179</v>
+      </c>
+      <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1980,16 +2255,29 @@
       <c r="P22" t="n">
         <v>568840.5</v>
       </c>
-      <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="n">
-        <v>568840.5</v>
-      </c>
-      <c r="S22" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q22" s="2" t="n">
+        <v>46107</v>
+      </c>
+      <c r="R22" s="2" t="n">
+        <v>46129</v>
+      </c>
+      <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U22" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2048,16 +2336,29 @@
       <c r="P23" t="n">
         <v>105951.07</v>
       </c>
-      <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="n">
-        <v>105951.07</v>
-      </c>
-      <c r="S23" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q23" s="2" t="n">
+        <v>45886</v>
+      </c>
+      <c r="R23" s="2" t="n">
+        <v>45969</v>
+      </c>
+      <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U23" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2116,16 +2417,29 @@
       <c r="P24" t="n">
         <v>280248.59</v>
       </c>
-      <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="n">
-        <v>280248.59</v>
-      </c>
-      <c r="S24" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q24" s="2" t="n">
+        <v>45832</v>
+      </c>
+      <c r="R24" s="2" t="n">
+        <v>45902</v>
+      </c>
+      <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2184,16 +2498,29 @@
       <c r="P25" t="n">
         <v>285863.23</v>
       </c>
-      <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="n">
-        <v>285863.23</v>
-      </c>
-      <c r="S25" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q25" s="2" t="n">
+        <v>45866</v>
+      </c>
+      <c r="R25" s="2" t="n">
+        <v>45943</v>
+      </c>
+      <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U25" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2252,16 +2579,29 @@
       <c r="P26" t="n">
         <v>221171.06</v>
       </c>
-      <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="n">
-        <v>221171.06</v>
-      </c>
-      <c r="S26" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q26" s="2" t="n">
+        <v>45718</v>
+      </c>
+      <c r="R26" s="2" t="n">
+        <v>45808</v>
+      </c>
+      <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U26" t="n">
+        <v>0</v>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2320,20 +2660,33 @@
       <c r="P27" t="n">
         <v>577808.88</v>
       </c>
-      <c r="Q27" t="inlineStr">
+      <c r="Q27" s="2" t="n">
+        <v>46010</v>
+      </c>
+      <c r="R27" s="2" t="n">
+        <v>46092</v>
+      </c>
+      <c r="S27" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R27" t="n">
-        <v>577808.88</v>
-      </c>
-      <c r="S27" t="n">
-        <v>0</v>
-      </c>
       <c r="T27" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U27" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2392,16 +2745,29 @@
       <c r="P28" t="n">
         <v>196777.36</v>
       </c>
-      <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="n">
-        <v>196777.36</v>
-      </c>
-      <c r="S28" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q28" s="2" t="n">
+        <v>45899</v>
+      </c>
+      <c r="R28" s="2" t="n">
+        <v>45938</v>
+      </c>
+      <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U28" t="n">
+        <v>0</v>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2460,16 +2826,29 @@
       <c r="P29" t="n">
         <v>170730.01</v>
       </c>
-      <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="n">
-        <v>170730.01</v>
-      </c>
-      <c r="S29" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q29" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="R29" s="2" t="n">
+        <v>45780</v>
+      </c>
+      <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U29" t="n">
+        <v>0</v>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2528,16 +2907,29 @@
       <c r="P30" t="n">
         <v>355660.26</v>
       </c>
-      <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="n">
-        <v>355660.26</v>
-      </c>
-      <c r="S30" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q30" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="R30" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U30" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2596,16 +2988,29 @@
       <c r="P31" t="n">
         <v>418857.39</v>
       </c>
-      <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="n">
-        <v>418857.39</v>
-      </c>
-      <c r="S31" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q31" s="2" t="n">
+        <v>45666</v>
+      </c>
+      <c r="R31" s="2" t="n">
+        <v>45765</v>
+      </c>
+      <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U31" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2664,20 +3069,33 @@
       <c r="P32" t="n">
         <v>574740.27</v>
       </c>
-      <c r="Q32" t="inlineStr">
+      <c r="Q32" s="2" t="n">
+        <v>45998</v>
+      </c>
+      <c r="R32" s="2" t="n">
+        <v>46117</v>
+      </c>
+      <c r="S32" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R32" t="n">
-        <v>574740.27</v>
-      </c>
-      <c r="S32" t="n">
-        <v>0</v>
-      </c>
       <c r="T32" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U32" t="n">
+        <v>0</v>
+      </c>
+      <c r="V32" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2736,20 +3154,33 @@
       <c r="P33" t="n">
         <v>129356.97</v>
       </c>
-      <c r="Q33" t="inlineStr">
+      <c r="Q33" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="R33" s="2" t="n">
+        <v>46093</v>
+      </c>
+      <c r="S33" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R33" t="n">
-        <v>129356.97</v>
-      </c>
-      <c r="S33" t="n">
-        <v>0</v>
-      </c>
       <c r="T33" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2808,16 +3239,29 @@
       <c r="P34" t="n">
         <v>591950.49</v>
       </c>
-      <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="n">
-        <v>591950.49</v>
-      </c>
-      <c r="S34" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q34" s="2" t="n">
+        <v>45903</v>
+      </c>
+      <c r="R34" s="2" t="n">
+        <v>45931</v>
+      </c>
+      <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U34" t="n">
+        <v>0</v>
+      </c>
+      <c r="V34" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2876,16 +3320,29 @@
       <c r="P35" t="n">
         <v>390381.81</v>
       </c>
-      <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="n">
-        <v>390381.81</v>
-      </c>
-      <c r="S35" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q35" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="R35" s="2" t="n">
+        <v>45972</v>
+      </c>
+      <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2944,16 +3401,29 @@
       <c r="P36" t="n">
         <v>128268.79</v>
       </c>
-      <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="n">
-        <v>128268.79</v>
-      </c>
-      <c r="S36" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q36" s="2" t="n">
+        <v>45863</v>
+      </c>
+      <c r="R36" s="2" t="n">
+        <v>45951</v>
+      </c>
+      <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U36" t="n">
+        <v>0</v>
+      </c>
+      <c r="V36" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3012,20 +3482,33 @@
       <c r="P37" t="n">
         <v>534024.5</v>
       </c>
-      <c r="Q37" t="inlineStr">
+      <c r="Q37" s="2" t="n">
+        <v>46066</v>
+      </c>
+      <c r="R37" s="2" t="n">
+        <v>46095</v>
+      </c>
+      <c r="S37" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R37" t="n">
-        <v>534024.5</v>
-      </c>
-      <c r="S37" t="n">
-        <v>0</v>
-      </c>
       <c r="T37" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U37" t="n">
+        <v>0</v>
+      </c>
+      <c r="V37" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3084,16 +3567,29 @@
       <c r="P38" t="n">
         <v>391196.57</v>
       </c>
-      <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="n">
-        <v>391196.57</v>
-      </c>
-      <c r="S38" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q38" s="2" t="n">
+        <v>45835</v>
+      </c>
+      <c r="R38" s="2" t="n">
+        <v>45899</v>
+      </c>
+      <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U38" t="n">
+        <v>0</v>
+      </c>
+      <c r="V38" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3152,16 +3648,29 @@
       <c r="P39" t="n">
         <v>596378.9300000001</v>
       </c>
-      <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="n">
-        <v>596378.9300000001</v>
-      </c>
-      <c r="S39" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q39" s="2" t="n">
+        <v>45887</v>
+      </c>
+      <c r="R39" s="2" t="n">
+        <v>45969</v>
+      </c>
+      <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U39" t="n">
+        <v>0</v>
+      </c>
+      <c r="V39" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3220,20 +3729,33 @@
       <c r="P40" t="n">
         <v>120089.45</v>
       </c>
-      <c r="Q40" t="inlineStr">
+      <c r="Q40" s="2" t="n">
+        <v>46023</v>
+      </c>
+      <c r="R40" s="2" t="n">
+        <v>46087</v>
+      </c>
+      <c r="S40" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R40" t="n">
-        <v>120089.45</v>
-      </c>
-      <c r="S40" t="n">
-        <v>0</v>
-      </c>
       <c r="T40" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U40" t="n">
+        <v>0</v>
+      </c>
+      <c r="V40" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3292,16 +3814,29 @@
       <c r="P41" t="n">
         <v>326276.52</v>
       </c>
-      <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="n">
-        <v>326276.52</v>
-      </c>
-      <c r="S41" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q41" s="2" t="n">
+        <v>46106</v>
+      </c>
+      <c r="R41" s="2" t="n">
+        <v>46159</v>
+      </c>
+      <c r="S41" t="inlineStr"/>
       <c r="T41" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U41" t="n">
+        <v>0</v>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3360,20 +3895,33 @@
       <c r="P42" t="n">
         <v>574267.4300000001</v>
       </c>
-      <c r="Q42" t="inlineStr">
+      <c r="Q42" s="2" t="n">
+        <v>46065</v>
+      </c>
+      <c r="R42" s="2" t="n">
+        <v>46111</v>
+      </c>
+      <c r="S42" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R42" t="n">
-        <v>574267.4300000001</v>
-      </c>
-      <c r="S42" t="n">
-        <v>0</v>
-      </c>
       <c r="T42" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U42" t="n">
+        <v>0</v>
+      </c>
+      <c r="V42" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3432,16 +3980,29 @@
       <c r="P43" t="n">
         <v>352257.46</v>
       </c>
-      <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="n">
-        <v>352257.46</v>
-      </c>
-      <c r="S43" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q43" s="2" t="n">
+        <v>45898</v>
+      </c>
+      <c r="R43" s="2" t="n">
+        <v>46015</v>
+      </c>
+      <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr">
         <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+      <c r="U43" t="n">
+        <v>0</v>
+      </c>
+      <c r="V43" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3500,16 +4061,29 @@
       <c r="P44" t="n">
         <v>267517.39</v>
       </c>
-      <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="n">
-        <v>267517.39</v>
-      </c>
-      <c r="S44" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q44" s="2" t="n">
+        <v>46096</v>
+      </c>
+      <c r="R44" s="2" t="n">
+        <v>46182</v>
+      </c>
+      <c r="S44" t="inlineStr"/>
       <c r="T44" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U44" t="n">
+        <v>0</v>
+      </c>
+      <c r="V44" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W44" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3568,20 +4142,33 @@
       <c r="P45" t="n">
         <v>354611.01</v>
       </c>
-      <c r="Q45" t="inlineStr">
+      <c r="Q45" s="2" t="n">
+        <v>46004</v>
+      </c>
+      <c r="R45" s="2" t="n">
+        <v>46082</v>
+      </c>
+      <c r="S45" t="inlineStr">
         <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="R45" t="n">
-        <v>354611.01</v>
-      </c>
-      <c r="S45" t="n">
-        <v>0</v>
-      </c>
       <c r="T45" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U45" t="n">
+        <v>0</v>
+      </c>
+      <c r="V45" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3640,16 +4227,29 @@
       <c r="P46" t="n">
         <v>498191.26</v>
       </c>
-      <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="n">
-        <v>498191.26</v>
-      </c>
-      <c r="S46" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q46" s="2" t="n">
+        <v>46091</v>
+      </c>
+      <c r="R46" s="2" t="n">
+        <v>46135</v>
+      </c>
+      <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr">
         <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+      <c r="U46" t="n">
+        <v>0</v>
+      </c>
+      <c r="V46" t="inlineStr">
+        <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3765,7 +4365,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3808,12 +4408,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Excel vs ML Disagreement Count</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>LAST_REFRESH_UTC</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2026-02-15 05:35 UTC</t>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2026-02-15 06:25 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto refresh - 16-02-2026 10:58:03.64
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -574,10 +574,10 @@
         <v>45826</v>
       </c>
       <c r="E2" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G2" t="n">
         <v>100350.37</v>
@@ -655,10 +655,10 @@
         <v>46071</v>
       </c>
       <c r="E3" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G3" t="n">
         <v>552594.63</v>
@@ -667,22 +667,22 @@
         <v>87823.07000000001</v>
       </c>
       <c r="I3" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3" t="n">
-        <v>513123.59</v>
+        <v>522991.35</v>
       </c>
       <c r="L3" t="n">
-        <v>17.12</v>
+        <v>16.79</v>
       </c>
       <c r="M3" t="n">
         <v>464771.56</v>
       </c>
       <c r="N3" t="n">
-        <v>116192.89</v>
+        <v>154923.85</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -740,10 +740,10 @@
         <v>45984</v>
       </c>
       <c r="E4" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G4" t="n">
         <v>294540.38</v>
@@ -821,10 +821,10 @@
         <v>45811</v>
       </c>
       <c r="E5" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G5" t="n">
         <v>509097.37</v>
@@ -902,10 +902,10 @@
         <v>45997</v>
       </c>
       <c r="E6" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G6" t="n">
         <v>382409.25</v>
@@ -983,10 +983,10 @@
         <v>46005</v>
       </c>
       <c r="E7" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F7" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G7" t="n">
         <v>525695.9399999999</v>
@@ -1064,10 +1064,10 @@
         <v>46102</v>
       </c>
       <c r="E8" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F8" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G8" t="n">
         <v>136840.92</v>
@@ -1076,22 +1076,22 @@
         <v>41169.63</v>
       </c>
       <c r="I8" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J8" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K8" t="n">
-        <v>55664.1</v>
+        <v>57983.44</v>
       </c>
       <c r="L8" t="n">
-        <v>73.95999999999999</v>
+        <v>71</v>
       </c>
       <c r="M8" t="n">
         <v>95671.28999999999</v>
       </c>
       <c r="N8" t="n">
-        <v>2733.47</v>
+        <v>2813.86</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1149,10 +1149,10 @@
         <v>46119</v>
       </c>
       <c r="E9" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F9" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G9" t="n">
         <v>380340.09</v>
@@ -1230,10 +1230,10 @@
         <v>46103</v>
       </c>
       <c r="E10" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G10" t="n">
         <v>448858.15</v>
@@ -1242,22 +1242,22 @@
         <v>35389.47</v>
       </c>
       <c r="I10" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J10" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K10" t="n">
-        <v>165368.79</v>
+        <v>173243.5</v>
       </c>
       <c r="L10" t="n">
-        <v>21.4</v>
+        <v>20.43</v>
       </c>
       <c r="M10" t="n">
         <v>413468.68</v>
       </c>
       <c r="N10" t="n">
-        <v>11485.24</v>
+        <v>11813.39</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1315,10 +1315,10 @@
         <v>46172</v>
       </c>
       <c r="E11" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F11" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G11" t="n">
         <v>432209.99</v>
@@ -1396,10 +1396,10 @@
         <v>46105</v>
       </c>
       <c r="E12" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F12" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G12" t="n">
         <v>559806.73</v>
@@ -1408,22 +1408,22 @@
         <v>64081.81</v>
       </c>
       <c r="I12" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J12" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K12" t="n">
-        <v>300384.1</v>
+        <v>307211.01</v>
       </c>
       <c r="L12" t="n">
-        <v>21.33</v>
+        <v>20.86</v>
       </c>
       <c r="M12" t="n">
         <v>495724.92</v>
       </c>
       <c r="N12" t="n">
-        <v>13045.39</v>
+        <v>13397.97</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1481,10 +1481,10 @@
         <v>46118</v>
       </c>
       <c r="E13" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F13" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G13" t="n">
         <v>169377.54</v>
@@ -1493,22 +1493,22 @@
         <v>38713.84</v>
       </c>
       <c r="I13" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J13" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K13" t="n">
-        <v>62732.42</v>
+        <v>64823.5</v>
       </c>
       <c r="L13" t="n">
-        <v>61.71</v>
+        <v>59.72</v>
       </c>
       <c r="M13" t="n">
         <v>130663.7</v>
       </c>
       <c r="N13" t="n">
-        <v>2562.03</v>
+        <v>2613.27</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1566,10 +1566,10 @@
         <v>45875</v>
       </c>
       <c r="E14" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F14" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F14" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G14" t="n">
         <v>334936.09</v>
@@ -1647,10 +1647,10 @@
         <v>46176</v>
       </c>
       <c r="E15" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F15" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F15" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G15" t="n">
         <v>394703.48</v>
@@ -1728,10 +1728,10 @@
         <v>45766</v>
       </c>
       <c r="E16" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F16" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F16" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G16" t="n">
         <v>161605.1</v>
@@ -1809,10 +1809,10 @@
         <v>45778</v>
       </c>
       <c r="E17" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F17" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F17" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G17" t="n">
         <v>95583.81</v>
@@ -1890,10 +1890,10 @@
         <v>46196</v>
       </c>
       <c r="E18" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F18" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G18" t="n">
         <v>253564.24</v>
@@ -1971,10 +1971,10 @@
         <v>46204</v>
       </c>
       <c r="E19" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F19" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F19" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G19" t="n">
         <v>111100.55</v>
@@ -2052,10 +2052,10 @@
         <v>46112</v>
       </c>
       <c r="E20" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F20" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F20" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G20" t="n">
         <v>423679.91</v>
@@ -2064,22 +2064,22 @@
         <v>96281.41</v>
       </c>
       <c r="I20" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J20" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K20" t="n">
-        <v>211839.95</v>
+        <v>216547.51</v>
       </c>
       <c r="L20" t="n">
-        <v>45.45</v>
+        <v>44.46</v>
       </c>
       <c r="M20" t="n">
         <v>327398.5</v>
       </c>
       <c r="N20" t="n">
-        <v>7275.52</v>
+        <v>7440.88</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -2137,10 +2137,10 @@
         <v>46179</v>
       </c>
       <c r="E21" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F21" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F21" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G21" t="n">
         <v>224412.65</v>
@@ -2218,10 +2218,10 @@
         <v>46129</v>
       </c>
       <c r="E22" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F22" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F22" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G22" t="n">
         <v>568840.5</v>
@@ -2299,10 +2299,10 @@
         <v>45969</v>
       </c>
       <c r="E23" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F23" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F23" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G23" t="n">
         <v>105951.07</v>
@@ -2380,10 +2380,10 @@
         <v>45902</v>
       </c>
       <c r="E24" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F24" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F24" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G24" t="n">
         <v>280248.59</v>
@@ -2461,10 +2461,10 @@
         <v>45943</v>
       </c>
       <c r="E25" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F25" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F25" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G25" t="n">
         <v>285863.23</v>
@@ -2542,10 +2542,10 @@
         <v>45808</v>
       </c>
       <c r="E26" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F26" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F26" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G26" t="n">
         <v>221171.06</v>
@@ -2623,10 +2623,10 @@
         <v>46092</v>
       </c>
       <c r="E27" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F27" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F27" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G27" t="n">
         <v>577808.88</v>
@@ -2635,22 +2635,22 @@
         <v>107249.68</v>
       </c>
       <c r="I27" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J27" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K27" t="n">
-        <v>403770.06</v>
+        <v>410731.61</v>
       </c>
       <c r="L27" t="n">
-        <v>26.56</v>
+        <v>26.11</v>
       </c>
       <c r="M27" t="n">
         <v>470559.2</v>
       </c>
       <c r="N27" t="n">
-        <v>18822.37</v>
+        <v>19606.63</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2708,10 +2708,10 @@
         <v>45938</v>
       </c>
       <c r="E28" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F28" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F28" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G28" t="n">
         <v>196777.36</v>
@@ -2789,10 +2789,10 @@
         <v>45780</v>
       </c>
       <c r="E29" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F29" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F29" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G29" t="n">
         <v>170730.01</v>
@@ -2870,10 +2870,10 @@
         <v>45954</v>
       </c>
       <c r="E30" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F30" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F30" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G30" t="n">
         <v>355660.26</v>
@@ -2951,10 +2951,10 @@
         <v>45765</v>
       </c>
       <c r="E31" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F31" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F31" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G31" t="n">
         <v>418857.39</v>
@@ -3032,10 +3032,10 @@
         <v>46117</v>
       </c>
       <c r="E32" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F32" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F32" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G32" t="n">
         <v>574740.27</v>
@@ -3044,22 +3044,22 @@
         <v>109593.36</v>
       </c>
       <c r="I32" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J32" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K32" t="n">
-        <v>335265.16</v>
+        <v>340054.66</v>
       </c>
       <c r="L32" t="n">
-        <v>32.69</v>
+        <v>32.23</v>
       </c>
       <c r="M32" t="n">
         <v>465146.91</v>
       </c>
       <c r="N32" t="n">
-        <v>9302.940000000001</v>
+        <v>9492.790000000001</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3117,10 +3117,10 @@
         <v>46093</v>
       </c>
       <c r="E33" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F33" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F33" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G33" t="n">
         <v>129356.97</v>
@@ -3129,22 +3129,22 @@
         <v>44817.85</v>
       </c>
       <c r="I33" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J33" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K33" t="n">
-        <v>78398.16</v>
+        <v>80358.12</v>
       </c>
       <c r="L33" t="n">
-        <v>57.17</v>
+        <v>55.77</v>
       </c>
       <c r="M33" t="n">
         <v>84539.12</v>
       </c>
       <c r="N33" t="n">
-        <v>3251.5</v>
+        <v>3381.56</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -3202,10 +3202,10 @@
         <v>45931</v>
       </c>
       <c r="E34" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F34" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F34" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G34" t="n">
         <v>591950.49</v>
@@ -3283,10 +3283,10 @@
         <v>45972</v>
       </c>
       <c r="E35" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F35" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F35" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G35" t="n">
         <v>390381.81</v>
@@ -3364,10 +3364,10 @@
         <v>45951</v>
       </c>
       <c r="E36" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F36" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F36" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G36" t="n">
         <v>128268.79</v>
@@ -3445,10 +3445,10 @@
         <v>46095</v>
       </c>
       <c r="E37" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F37" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F37" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G37" t="n">
         <v>534024.5</v>
@@ -3457,22 +3457,22 @@
         <v>1884.06</v>
       </c>
       <c r="I37" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J37" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K37" t="n">
-        <v>35601.63</v>
+        <v>53402.45</v>
       </c>
       <c r="L37" t="n">
-        <v>5.29</v>
+        <v>3.53</v>
       </c>
       <c r="M37" t="n">
         <v>532140.4399999999</v>
       </c>
       <c r="N37" t="n">
-        <v>19005.02</v>
+        <v>19708.91</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3530,10 +3530,10 @@
         <v>45899</v>
       </c>
       <c r="E38" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F38" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F38" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G38" t="n">
         <v>391196.57</v>
@@ -3611,10 +3611,10 @@
         <v>45969</v>
       </c>
       <c r="E39" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F39" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F39" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G39" t="n">
         <v>596378.9300000001</v>
@@ -3692,10 +3692,10 @@
         <v>46087</v>
       </c>
       <c r="E40" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F40" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F40" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G40" t="n">
         <v>120089.45</v>
@@ -3704,22 +3704,22 @@
         <v>40142.96</v>
       </c>
       <c r="I40" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J40" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K40" t="n">
-        <v>83138.85000000001</v>
+        <v>84986.38</v>
       </c>
       <c r="L40" t="n">
-        <v>48.28</v>
+        <v>47.23</v>
       </c>
       <c r="M40" t="n">
         <v>79946.49000000001</v>
       </c>
       <c r="N40" t="n">
-        <v>3997.32</v>
+        <v>4207.71</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3777,10 +3777,10 @@
         <v>46159</v>
       </c>
       <c r="E41" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F41" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F41" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G41" t="n">
         <v>326276.52</v>
@@ -3858,10 +3858,10 @@
         <v>46111</v>
       </c>
       <c r="E42" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F42" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F42" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G42" t="n">
         <v>574267.4300000001</v>
@@ -3870,22 +3870,22 @@
         <v>2699.06</v>
       </c>
       <c r="I42" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J42" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K42" t="n">
-        <v>36655.37</v>
+        <v>48873.82</v>
       </c>
       <c r="L42" t="n">
-        <v>7.36</v>
+        <v>5.52</v>
       </c>
       <c r="M42" t="n">
         <v>571568.37</v>
       </c>
       <c r="N42" t="n">
-        <v>12990.19</v>
+        <v>13292.29</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3943,10 +3943,10 @@
         <v>46015</v>
       </c>
       <c r="E43" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F43" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F43" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G43" t="n">
         <v>352257.46</v>
@@ -4024,10 +4024,10 @@
         <v>46182</v>
       </c>
       <c r="E44" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F44" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F44" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G44" t="n">
         <v>267517.39</v>
@@ -4105,10 +4105,10 @@
         <v>46082</v>
       </c>
       <c r="E45" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F45" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F45" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G45" t="n">
         <v>354611.01</v>
@@ -4117,22 +4117,22 @@
         <v>91143.19</v>
       </c>
       <c r="I45" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J45" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K45" t="n">
-        <v>287279.81</v>
+        <v>291768.55</v>
       </c>
       <c r="L45" t="n">
-        <v>31.73</v>
+        <v>31.24</v>
       </c>
       <c r="M45" t="n">
         <v>263467.82</v>
       </c>
       <c r="N45" t="n">
-        <v>17564.52</v>
+        <v>18819.13</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -4190,10 +4190,10 @@
         <v>46135</v>
       </c>
       <c r="E46" s="2" t="n">
+        <v>46069</v>
+      </c>
+      <c r="F46" s="2" t="n">
         <v>46068</v>
-      </c>
-      <c r="F46" s="2" t="n">
-        <v>46067</v>
       </c>
       <c r="G46" t="n">
         <v>498191.26</v>
@@ -4423,7 +4423,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2026-02-15 06:25 UTC</t>
+          <t>2026-02-16 05:28 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto refresh - 16-02-2026 11:01:35.85
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -583,7 +583,7 @@
         <v>100350.37</v>
       </c>
       <c r="H2" t="n">
-        <v>157738.34</v>
+        <v>166806.6</v>
       </c>
       <c r="I2" t="n">
         <v>104</v>
@@ -595,10 +595,10 @@
         <v>100350.37</v>
       </c>
       <c r="L2" t="n">
-        <v>157.19</v>
+        <v>166.22</v>
       </c>
       <c r="M2" t="n">
-        <v>-57387.97</v>
+        <v>-66456.23</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
@@ -664,7 +664,7 @@
         <v>552594.63</v>
       </c>
       <c r="H3" t="n">
-        <v>87823.07000000001</v>
+        <v>89972.7</v>
       </c>
       <c r="I3" t="n">
         <v>53</v>
@@ -676,13 +676,13 @@
         <v>522991.35</v>
       </c>
       <c r="L3" t="n">
-        <v>16.79</v>
+        <v>17.2</v>
       </c>
       <c r="M3" t="n">
-        <v>464771.56</v>
+        <v>462621.93</v>
       </c>
       <c r="N3" t="n">
-        <v>154923.85</v>
+        <v>154207.31</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -749,7 +749,7 @@
         <v>294540.38</v>
       </c>
       <c r="H4" t="n">
-        <v>133057.46</v>
+        <v>154346.38</v>
       </c>
       <c r="I4" t="n">
         <v>76</v>
@@ -761,10 +761,10 @@
         <v>294540.38</v>
       </c>
       <c r="L4" t="n">
-        <v>45.17</v>
+        <v>52.4</v>
       </c>
       <c r="M4" t="n">
-        <v>161482.92</v>
+        <v>140194</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -830,7 +830,7 @@
         <v>509097.37</v>
       </c>
       <c r="H5" t="n">
-        <v>28952.07</v>
+        <v>30692.27</v>
       </c>
       <c r="I5" t="n">
         <v>28</v>
@@ -842,10 +842,10 @@
         <v>509097.37</v>
       </c>
       <c r="L5" t="n">
-        <v>5.69</v>
+        <v>6.03</v>
       </c>
       <c r="M5" t="n">
-        <v>480145.3</v>
+        <v>478405.1</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -911,7 +911,7 @@
         <v>382409.25</v>
       </c>
       <c r="H6" t="n">
-        <v>88566.33</v>
+        <v>146951.89</v>
       </c>
       <c r="I6" t="n">
         <v>94</v>
@@ -923,10 +923,10 @@
         <v>382409.25</v>
       </c>
       <c r="L6" t="n">
-        <v>23.16</v>
+        <v>38.43</v>
       </c>
       <c r="M6" t="n">
-        <v>293842.92</v>
+        <v>235457.36</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
@@ -992,7 +992,7 @@
         <v>525695.9399999999</v>
       </c>
       <c r="H7" t="n">
-        <v>187552.69</v>
+        <v>121020.49</v>
       </c>
       <c r="I7" t="n">
         <v>92</v>
@@ -1004,10 +1004,10 @@
         <v>525695.9399999999</v>
       </c>
       <c r="L7" t="n">
-        <v>35.68</v>
+        <v>23.02</v>
       </c>
       <c r="M7" t="n">
-        <v>338143.25</v>
+        <v>404675.45</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
@@ -1073,7 +1073,7 @@
         <v>136840.92</v>
       </c>
       <c r="H8" t="n">
-        <v>41169.63</v>
+        <v>40927.75</v>
       </c>
       <c r="I8" t="n">
         <v>25</v>
@@ -1085,13 +1085,13 @@
         <v>57983.44</v>
       </c>
       <c r="L8" t="n">
-        <v>71</v>
+        <v>70.59</v>
       </c>
       <c r="M8" t="n">
-        <v>95671.28999999999</v>
+        <v>95913.17</v>
       </c>
       <c r="N8" t="n">
-        <v>2813.86</v>
+        <v>2820.98</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1239,7 +1239,7 @@
         <v>448858.15</v>
       </c>
       <c r="H10" t="n">
-        <v>35389.47</v>
+        <v>33037.27</v>
       </c>
       <c r="I10" t="n">
         <v>22</v>
@@ -1251,13 +1251,13 @@
         <v>173243.5</v>
       </c>
       <c r="L10" t="n">
-        <v>20.43</v>
+        <v>19.07</v>
       </c>
       <c r="M10" t="n">
-        <v>413468.68</v>
+        <v>415820.88</v>
       </c>
       <c r="N10" t="n">
-        <v>11813.39</v>
+        <v>11880.6</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>559806.73</v>
       </c>
       <c r="H12" t="n">
-        <v>64081.81</v>
+        <v>86475.62</v>
       </c>
       <c r="I12" t="n">
         <v>45</v>
@@ -1417,13 +1417,13 @@
         <v>307211.01</v>
       </c>
       <c r="L12" t="n">
-        <v>20.86</v>
+        <v>28.15</v>
       </c>
       <c r="M12" t="n">
-        <v>495724.92</v>
+        <v>473331.11</v>
       </c>
       <c r="N12" t="n">
-        <v>13397.97</v>
+        <v>12792.73</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1490,7 +1490,7 @@
         <v>169377.54</v>
       </c>
       <c r="H13" t="n">
-        <v>38713.84</v>
+        <v>63349.43</v>
       </c>
       <c r="I13" t="n">
         <v>31</v>
@@ -1502,17 +1502,17 @@
         <v>64823.5</v>
       </c>
       <c r="L13" t="n">
-        <v>59.72</v>
+        <v>97.73</v>
       </c>
       <c r="M13" t="n">
-        <v>130663.7</v>
+        <v>106028.11</v>
       </c>
       <c r="N13" t="n">
-        <v>2613.27</v>
+        <v>2120.56</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P13" t="n">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
@@ -1575,7 +1575,7 @@
         <v>334936.09</v>
       </c>
       <c r="H14" t="n">
-        <v>164342.59</v>
+        <v>81515.34</v>
       </c>
       <c r="I14" t="n">
         <v>88</v>
@@ -1587,10 +1587,10 @@
         <v>334936.09</v>
       </c>
       <c r="L14" t="n">
-        <v>49.07</v>
+        <v>24.34</v>
       </c>
       <c r="M14" t="n">
-        <v>170593.5</v>
+        <v>253420.75</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
@@ -1737,7 +1737,7 @@
         <v>161605.1</v>
       </c>
       <c r="H16" t="n">
-        <v>131961.07</v>
+        <v>65180.2</v>
       </c>
       <c r="I16" t="n">
         <v>74</v>
@@ -1749,10 +1749,10 @@
         <v>161605.1</v>
       </c>
       <c r="L16" t="n">
-        <v>81.66</v>
+        <v>40.33</v>
       </c>
       <c r="M16" t="n">
-        <v>29644.03</v>
+        <v>96424.89999999999</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
@@ -1818,7 +1818,7 @@
         <v>95583.81</v>
       </c>
       <c r="H17" t="n">
-        <v>127061.04</v>
+        <v>139657.66</v>
       </c>
       <c r="I17" t="n">
         <v>74</v>
@@ -1830,10 +1830,10 @@
         <v>95583.81</v>
       </c>
       <c r="L17" t="n">
-        <v>132.93</v>
+        <v>146.11</v>
       </c>
       <c r="M17" t="n">
-        <v>-31477.23</v>
+        <v>-44073.85</v>
       </c>
       <c r="N17" t="n">
         <v>0</v>
@@ -2061,7 +2061,7 @@
         <v>423679.91</v>
       </c>
       <c r="H20" t="n">
-        <v>96281.41</v>
+        <v>53250.78</v>
       </c>
       <c r="I20" t="n">
         <v>46</v>
@@ -2073,13 +2073,13 @@
         <v>216547.51</v>
       </c>
       <c r="L20" t="n">
-        <v>44.46</v>
+        <v>24.59</v>
       </c>
       <c r="M20" t="n">
-        <v>327398.5</v>
+        <v>370429.13</v>
       </c>
       <c r="N20" t="n">
-        <v>7440.88</v>
+        <v>8418.84</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -2308,7 +2308,7 @@
         <v>105951.07</v>
       </c>
       <c r="H23" t="n">
-        <v>80082.50999999999</v>
+        <v>150306.27</v>
       </c>
       <c r="I23" t="n">
         <v>84</v>
@@ -2320,17 +2320,17 @@
         <v>105951.07</v>
       </c>
       <c r="L23" t="n">
-        <v>75.58</v>
+        <v>141.86</v>
       </c>
       <c r="M23" t="n">
-        <v>25868.56</v>
+        <v>-44355.2</v>
       </c>
       <c r="N23" t="n">
         <v>0</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>Overpacing</t>
         </is>
       </c>
       <c r="P23" t="n">
@@ -2389,7 +2389,7 @@
         <v>280248.59</v>
       </c>
       <c r="H24" t="n">
-        <v>122270.66</v>
+        <v>118204.01</v>
       </c>
       <c r="I24" t="n">
         <v>71</v>
@@ -2401,10 +2401,10 @@
         <v>280248.59</v>
       </c>
       <c r="L24" t="n">
-        <v>43.63</v>
+        <v>42.18</v>
       </c>
       <c r="M24" t="n">
-        <v>157977.93</v>
+        <v>162044.58</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
@@ -2470,7 +2470,7 @@
         <v>285863.23</v>
       </c>
       <c r="H25" t="n">
-        <v>136777.09</v>
+        <v>156018.39</v>
       </c>
       <c r="I25" t="n">
         <v>78</v>
@@ -2482,10 +2482,10 @@
         <v>285863.23</v>
       </c>
       <c r="L25" t="n">
-        <v>47.85</v>
+        <v>54.58</v>
       </c>
       <c r="M25" t="n">
-        <v>149086.14</v>
+        <v>129844.84</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
@@ -2551,7 +2551,7 @@
         <v>221171.06</v>
       </c>
       <c r="H26" t="n">
-        <v>159211.39</v>
+        <v>94524.77</v>
       </c>
       <c r="I26" t="n">
         <v>91</v>
@@ -2563,10 +2563,10 @@
         <v>221171.06</v>
       </c>
       <c r="L26" t="n">
-        <v>71.98999999999999</v>
+        <v>42.74</v>
       </c>
       <c r="M26" t="n">
-        <v>61959.67</v>
+        <v>126646.29</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
@@ -2632,7 +2632,7 @@
         <v>577808.88</v>
       </c>
       <c r="H27" t="n">
-        <v>107249.68</v>
+        <v>85872.27</v>
       </c>
       <c r="I27" t="n">
         <v>59</v>
@@ -2644,13 +2644,13 @@
         <v>410731.61</v>
       </c>
       <c r="L27" t="n">
-        <v>26.11</v>
+        <v>20.91</v>
       </c>
       <c r="M27" t="n">
-        <v>470559.2</v>
+        <v>491936.61</v>
       </c>
       <c r="N27" t="n">
-        <v>19606.63</v>
+        <v>20497.36</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2717,7 +2717,7 @@
         <v>196777.36</v>
       </c>
       <c r="H28" t="n">
-        <v>40638.37</v>
+        <v>47231.34</v>
       </c>
       <c r="I28" t="n">
         <v>40</v>
@@ -2729,10 +2729,10 @@
         <v>196777.36</v>
       </c>
       <c r="L28" t="n">
-        <v>20.65</v>
+        <v>24</v>
       </c>
       <c r="M28" t="n">
-        <v>156138.99</v>
+        <v>149546.02</v>
       </c>
       <c r="N28" t="n">
         <v>0</v>
@@ -2798,7 +2798,7 @@
         <v>170730.01</v>
       </c>
       <c r="H29" t="n">
-        <v>159714.06</v>
+        <v>124157.16</v>
       </c>
       <c r="I29" t="n">
         <v>96</v>
@@ -2810,10 +2810,10 @@
         <v>170730.01</v>
       </c>
       <c r="L29" t="n">
-        <v>93.55</v>
+        <v>72.72</v>
       </c>
       <c r="M29" t="n">
-        <v>11015.95</v>
+        <v>46572.85</v>
       </c>
       <c r="N29" t="n">
         <v>0</v>
@@ -2879,7 +2879,7 @@
         <v>355660.26</v>
       </c>
       <c r="H30" t="n">
-        <v>82464.85000000001</v>
+        <v>83693.11</v>
       </c>
       <c r="I30" t="n">
         <v>74</v>
@@ -2891,10 +2891,10 @@
         <v>355660.26</v>
       </c>
       <c r="L30" t="n">
-        <v>23.19</v>
+        <v>23.53</v>
       </c>
       <c r="M30" t="n">
-        <v>273195.41</v>
+        <v>271967.15</v>
       </c>
       <c r="N30" t="n">
         <v>0</v>
@@ -2960,7 +2960,7 @@
         <v>418857.39</v>
       </c>
       <c r="H31" t="n">
-        <v>133740.94</v>
+        <v>180010.86</v>
       </c>
       <c r="I31" t="n">
         <v>100</v>
@@ -2972,10 +2972,10 @@
         <v>418857.39</v>
       </c>
       <c r="L31" t="n">
-        <v>31.93</v>
+        <v>42.98</v>
       </c>
       <c r="M31" t="n">
-        <v>285116.45</v>
+        <v>238846.53</v>
       </c>
       <c r="N31" t="n">
         <v>0</v>
@@ -3041,7 +3041,7 @@
         <v>574740.27</v>
       </c>
       <c r="H32" t="n">
-        <v>109593.36</v>
+        <v>80607.14999999999</v>
       </c>
       <c r="I32" t="n">
         <v>71</v>
@@ -3053,13 +3053,13 @@
         <v>340054.66</v>
       </c>
       <c r="L32" t="n">
-        <v>32.23</v>
+        <v>23.7</v>
       </c>
       <c r="M32" t="n">
-        <v>465146.91</v>
+        <v>494133.12</v>
       </c>
       <c r="N32" t="n">
-        <v>9492.790000000001</v>
+        <v>10084.35</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3126,7 +3126,7 @@
         <v>129356.97</v>
       </c>
       <c r="H33" t="n">
-        <v>44817.85</v>
+        <v>89176.62</v>
       </c>
       <c r="I33" t="n">
         <v>41</v>
@@ -3138,17 +3138,17 @@
         <v>80358.12</v>
       </c>
       <c r="L33" t="n">
-        <v>55.77</v>
+        <v>110.97</v>
       </c>
       <c r="M33" t="n">
-        <v>84539.12</v>
+        <v>40180.35</v>
       </c>
       <c r="N33" t="n">
-        <v>3381.56</v>
+        <v>1607.21</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>Overpacing</t>
         </is>
       </c>
       <c r="P33" t="n">
@@ -3162,7 +3162,7 @@
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>Overdelivered</t>
         </is>
       </c>
       <c r="T33" t="inlineStr">
@@ -3171,7 +3171,7 @@
         </is>
       </c>
       <c r="U33" t="n">
-        <v>0</v>
+        <v>40180.35000000001</v>
       </c>
       <c r="V33" t="inlineStr">
         <is>
@@ -3211,7 +3211,7 @@
         <v>591950.49</v>
       </c>
       <c r="H34" t="n">
-        <v>68647.25999999999</v>
+        <v>23560.62</v>
       </c>
       <c r="I34" t="n">
         <v>29</v>
@@ -3223,10 +3223,10 @@
         <v>591950.49</v>
       </c>
       <c r="L34" t="n">
-        <v>11.6</v>
+        <v>3.98</v>
       </c>
       <c r="M34" t="n">
-        <v>523303.23</v>
+        <v>568389.87</v>
       </c>
       <c r="N34" t="n">
         <v>0</v>
@@ -3292,7 +3292,7 @@
         <v>390381.81</v>
       </c>
       <c r="H35" t="n">
-        <v>71073.24000000001</v>
+        <v>84289.87</v>
       </c>
       <c r="I35" t="n">
         <v>64</v>
@@ -3304,10 +3304,10 @@
         <v>390381.81</v>
       </c>
       <c r="L35" t="n">
-        <v>18.21</v>
+        <v>21.59</v>
       </c>
       <c r="M35" t="n">
-        <v>319308.57</v>
+        <v>306091.94</v>
       </c>
       <c r="N35" t="n">
         <v>0</v>
@@ -3373,7 +3373,7 @@
         <v>128268.79</v>
       </c>
       <c r="H36" t="n">
-        <v>85483.77</v>
+        <v>188100.04</v>
       </c>
       <c r="I36" t="n">
         <v>89</v>
@@ -3385,17 +3385,17 @@
         <v>128268.79</v>
       </c>
       <c r="L36" t="n">
-        <v>66.64</v>
+        <v>146.65</v>
       </c>
       <c r="M36" t="n">
-        <v>42785.02</v>
+        <v>-59831.25</v>
       </c>
       <c r="N36" t="n">
         <v>0</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>Overpacing</t>
         </is>
       </c>
       <c r="P36" t="n">
@@ -3454,7 +3454,7 @@
         <v>534024.5</v>
       </c>
       <c r="H37" t="n">
-        <v>1884.06</v>
+        <v>3192.36</v>
       </c>
       <c r="I37" t="n">
         <v>3</v>
@@ -3466,13 +3466,13 @@
         <v>53402.45</v>
       </c>
       <c r="L37" t="n">
-        <v>3.53</v>
+        <v>5.98</v>
       </c>
       <c r="M37" t="n">
-        <v>532140.4399999999</v>
+        <v>530832.14</v>
       </c>
       <c r="N37" t="n">
-        <v>19708.91</v>
+        <v>19660.45</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3539,7 +3539,7 @@
         <v>391196.57</v>
       </c>
       <c r="H38" t="n">
-        <v>134655.18</v>
+        <v>71566.28999999999</v>
       </c>
       <c r="I38" t="n">
         <v>65</v>
@@ -3551,10 +3551,10 @@
         <v>391196.57</v>
       </c>
       <c r="L38" t="n">
-        <v>34.42</v>
+        <v>18.29</v>
       </c>
       <c r="M38" t="n">
-        <v>256541.39</v>
+        <v>319630.28</v>
       </c>
       <c r="N38" t="n">
         <v>0</v>
@@ -3620,7 +3620,7 @@
         <v>596378.9300000001</v>
       </c>
       <c r="H39" t="n">
-        <v>75061.8</v>
+        <v>81468.39</v>
       </c>
       <c r="I39" t="n">
         <v>83</v>
@@ -3632,10 +3632,10 @@
         <v>596378.9300000001</v>
       </c>
       <c r="L39" t="n">
-        <v>12.59</v>
+        <v>13.66</v>
       </c>
       <c r="M39" t="n">
-        <v>521317.13</v>
+        <v>514910.54</v>
       </c>
       <c r="N39" t="n">
         <v>0</v>
@@ -3701,7 +3701,7 @@
         <v>120089.45</v>
       </c>
       <c r="H40" t="n">
-        <v>40142.96</v>
+        <v>65098.05</v>
       </c>
       <c r="I40" t="n">
         <v>46</v>
@@ -3713,13 +3713,13 @@
         <v>84986.38</v>
       </c>
       <c r="L40" t="n">
-        <v>47.23</v>
+        <v>76.59999999999999</v>
       </c>
       <c r="M40" t="n">
-        <v>79946.49000000001</v>
+        <v>54991.4</v>
       </c>
       <c r="N40" t="n">
-        <v>4207.71</v>
+        <v>2894.28</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3867,7 +3867,7 @@
         <v>574267.4300000001</v>
       </c>
       <c r="H42" t="n">
-        <v>2699.06</v>
+        <v>4714.41</v>
       </c>
       <c r="I42" t="n">
         <v>4</v>
@@ -3879,13 +3879,13 @@
         <v>48873.82</v>
       </c>
       <c r="L42" t="n">
-        <v>5.52</v>
+        <v>9.65</v>
       </c>
       <c r="M42" t="n">
-        <v>571568.37</v>
+        <v>569553.02</v>
       </c>
       <c r="N42" t="n">
-        <v>13292.29</v>
+        <v>13245.42</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3952,7 +3952,7 @@
         <v>352257.46</v>
       </c>
       <c r="H43" t="n">
-        <v>251672.33</v>
+        <v>243342.65</v>
       </c>
       <c r="I43" t="n">
         <v>118</v>
@@ -3964,10 +3964,10 @@
         <v>352257.46</v>
       </c>
       <c r="L43" t="n">
-        <v>71.45</v>
+        <v>69.08</v>
       </c>
       <c r="M43" t="n">
-        <v>100585.13</v>
+        <v>108914.81</v>
       </c>
       <c r="N43" t="n">
         <v>0</v>
@@ -4114,7 +4114,7 @@
         <v>354611.01</v>
       </c>
       <c r="H45" t="n">
-        <v>91143.19</v>
+        <v>128081.01</v>
       </c>
       <c r="I45" t="n">
         <v>65</v>
@@ -4126,13 +4126,13 @@
         <v>291768.55</v>
       </c>
       <c r="L45" t="n">
-        <v>31.24</v>
+        <v>43.9</v>
       </c>
       <c r="M45" t="n">
-        <v>263467.82</v>
+        <v>226530</v>
       </c>
       <c r="N45" t="n">
-        <v>18819.13</v>
+        <v>16180.71</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -4287,61 +4287,61 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pace_Ratio</t>
+          <t>Total_Budget</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3367483364832408</v>
+        <v>0.30403800197451</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Total_Budget</t>
+          <t>Pace_Ratio</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3346764346764347</v>
+        <v>0.2978052316094644</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Spend_to_Date</t>
+          <t>Spend_Velocity</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1289845549639365</v>
+        <v>0.1651920240253574</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Spend_Velocity</t>
+          <t>Spend_to_Date</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1122651580678091</v>
+        <v>0.1346997111256371</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Flight_Days</t>
+          <t>Days_Elapsed</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.03702444939558342</v>
+        <v>0.04185972267982849</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Days_Elapsed</t>
+          <t>Flight_Days</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0321754381548196</v>
+        <v>0.0394229317615561</v>
       </c>
     </row>
     <row r="8">
@@ -4351,7 +4351,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.01812562825817613</v>
+        <v>0.01698237682364667</v>
       </c>
     </row>
   </sheetData>
@@ -4392,7 +4392,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.833</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -4402,7 +4402,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>40180.35</v>
       </c>
     </row>
     <row r="4">
@@ -4423,7 +4423,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2026-02-16 05:28 UTC</t>
+          <t>2026-02-16 05:31 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto refresh - 16-02-2026 11:39:09.39
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W46"/>
+  <dimension ref="A1:V46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,29 +517,29 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
+          <t>Flight_Start_Date_meta</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Flight_End_Date_meta</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>Total_Budget_meta</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Flight_Start_Date_meta</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Flight_End_Date_meta</t>
-        </is>
-      </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
+          <t>DSP_meta</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
           <t>ML_Prediction</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Campaign_Status</t>
-        </is>
-      </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Budget_At_Risk</t>
@@ -548,11 +548,6 @@
       <c r="V1" s="1" t="inlineStr">
         <is>
           <t>ML_Early_Warning</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Excel_vs_ML_Disagree</t>
         </is>
       </c>
     </row>
@@ -608,32 +603,27 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P2" t="n">
+      <c r="P2" s="2" t="n">
+        <v>45723</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>45826</v>
+      </c>
+      <c r="R2" t="n">
         <v>100350.37</v>
       </c>
-      <c r="Q2" s="2" t="n">
-        <v>45723</v>
-      </c>
-      <c r="R2" s="2" t="n">
-        <v>45826</v>
-      </c>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr"/>
       <c r="U2" t="n">
         <v>0</v>
       </c>
       <c r="V2" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -689,36 +679,31 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P3" t="n">
+      <c r="P3" s="2" t="n">
+        <v>46016</v>
+      </c>
+      <c r="Q3" s="2" t="n">
+        <v>46071</v>
+      </c>
+      <c r="R3" t="n">
         <v>552594.63</v>
       </c>
-      <c r="Q3" s="2" t="n">
-        <v>46016</v>
-      </c>
-      <c r="R3" s="2" t="n">
-        <v>46071</v>
-      </c>
       <c r="S3" t="inlineStr">
         <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
       <c r="U3" t="n">
         <v>0</v>
       </c>
       <c r="V3" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -774,32 +759,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P4" t="n">
+      <c r="P4" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="Q4" s="2" t="n">
+        <v>45984</v>
+      </c>
+      <c r="R4" t="n">
         <v>294540.38</v>
       </c>
-      <c r="Q4" s="2" t="n">
-        <v>45909</v>
-      </c>
-      <c r="R4" s="2" t="n">
-        <v>45984</v>
-      </c>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr"/>
       <c r="U4" t="n">
         <v>0</v>
       </c>
       <c r="V4" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -855,32 +835,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P5" t="n">
+      <c r="P5" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="Q5" s="2" t="n">
+        <v>45811</v>
+      </c>
+      <c r="R5" t="n">
         <v>509097.37</v>
       </c>
-      <c r="Q5" s="2" t="n">
-        <v>45784</v>
-      </c>
-      <c r="R5" s="2" t="n">
-        <v>45811</v>
-      </c>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr"/>
       <c r="U5" t="n">
         <v>0</v>
       </c>
       <c r="V5" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -936,32 +911,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P6" t="n">
+      <c r="P6" s="2" t="n">
+        <v>45904</v>
+      </c>
+      <c r="Q6" s="2" t="n">
+        <v>45997</v>
+      </c>
+      <c r="R6" t="n">
         <v>382409.25</v>
       </c>
-      <c r="Q6" s="2" t="n">
-        <v>45904</v>
-      </c>
-      <c r="R6" s="2" t="n">
-        <v>45997</v>
-      </c>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr"/>
       <c r="U6" t="n">
         <v>0</v>
       </c>
       <c r="V6" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1017,32 +987,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P7" t="n">
+      <c r="P7" s="2" t="n">
+        <v>45914</v>
+      </c>
+      <c r="Q7" s="2" t="n">
+        <v>46005</v>
+      </c>
+      <c r="R7" t="n">
         <v>525695.9399999999</v>
       </c>
-      <c r="Q7" s="2" t="n">
-        <v>45914</v>
-      </c>
-      <c r="R7" s="2" t="n">
-        <v>46005</v>
-      </c>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr"/>
       <c r="U7" t="n">
         <v>0</v>
       </c>
       <c r="V7" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1098,36 +1063,31 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P8" t="n">
+      <c r="P8" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="Q8" s="2" t="n">
+        <v>46102</v>
+      </c>
+      <c r="R8" t="n">
         <v>136840.92</v>
       </c>
-      <c r="Q8" s="2" t="n">
-        <v>46044</v>
-      </c>
-      <c r="R8" s="2" t="n">
-        <v>46102</v>
-      </c>
       <c r="S8" t="inlineStr">
         <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
       <c r="U8" t="n">
         <v>0</v>
       </c>
       <c r="V8" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1183,32 +1143,27 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P9" t="n">
+      <c r="P9" s="2" t="n">
+        <v>46086</v>
+      </c>
+      <c r="Q9" s="2" t="n">
+        <v>46119</v>
+      </c>
+      <c r="R9" t="n">
         <v>380340.09</v>
       </c>
-      <c r="Q9" s="2" t="n">
-        <v>46086</v>
-      </c>
-      <c r="R9" s="2" t="n">
-        <v>46119</v>
-      </c>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr"/>
       <c r="U9" t="n">
         <v>0</v>
       </c>
       <c r="V9" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1264,36 +1219,31 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P10" t="n">
+      <c r="P10" s="2" t="n">
+        <v>46047</v>
+      </c>
+      <c r="Q10" s="2" t="n">
+        <v>46103</v>
+      </c>
+      <c r="R10" t="n">
         <v>448858.15</v>
       </c>
-      <c r="Q10" s="2" t="n">
-        <v>46047</v>
-      </c>
-      <c r="R10" s="2" t="n">
-        <v>46103</v>
-      </c>
       <c r="S10" t="inlineStr">
         <is>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
       <c r="U10" t="n">
         <v>0</v>
       </c>
       <c r="V10" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1349,32 +1299,27 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P11" t="n">
+      <c r="P11" s="2" t="n">
+        <v>46089</v>
+      </c>
+      <c r="Q11" s="2" t="n">
+        <v>46172</v>
+      </c>
+      <c r="R11" t="n">
         <v>432209.99</v>
       </c>
-      <c r="Q11" s="2" t="n">
-        <v>46089</v>
-      </c>
-      <c r="R11" s="2" t="n">
-        <v>46172</v>
-      </c>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr"/>
       <c r="U11" t="n">
         <v>0</v>
       </c>
       <c r="V11" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1430,36 +1375,31 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P12" t="n">
+      <c r="P12" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="Q12" s="2" t="n">
+        <v>46105</v>
+      </c>
+      <c r="R12" t="n">
         <v>559806.73</v>
       </c>
-      <c r="Q12" s="2" t="n">
-        <v>46024</v>
-      </c>
-      <c r="R12" s="2" t="n">
-        <v>46105</v>
-      </c>
       <c r="S12" t="inlineStr">
         <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
       <c r="U12" t="n">
         <v>0</v>
       </c>
       <c r="V12" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1515,34 +1455,29 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P13" t="n">
+      <c r="P13" s="2" t="n">
+        <v>46038</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <v>46118</v>
+      </c>
+      <c r="R13" t="n">
         <v>169377.54</v>
       </c>
-      <c r="Q13" s="2" t="n">
-        <v>46038</v>
-      </c>
-      <c r="R13" s="2" t="n">
-        <v>46118</v>
-      </c>
       <c r="S13" t="inlineStr">
         <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
       <c r="U13" t="n">
         <v>0</v>
       </c>
       <c r="V13" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="W13" t="inlineStr">
         <is>
           <t>YES</t>
         </is>
@@ -1600,32 +1535,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P14" t="n">
+      <c r="P14" s="2" t="n">
+        <v>45788</v>
+      </c>
+      <c r="Q14" s="2" t="n">
+        <v>45875</v>
+      </c>
+      <c r="R14" t="n">
         <v>334936.09</v>
       </c>
-      <c r="Q14" s="2" t="n">
-        <v>45788</v>
-      </c>
-      <c r="R14" s="2" t="n">
-        <v>45875</v>
-      </c>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr"/>
       <c r="U14" t="n">
         <v>0</v>
       </c>
       <c r="V14" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1681,32 +1611,27 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P15" t="n">
+      <c r="P15" s="2" t="n">
+        <v>46120</v>
+      </c>
+      <c r="Q15" s="2" t="n">
+        <v>46176</v>
+      </c>
+      <c r="R15" t="n">
         <v>394703.48</v>
       </c>
-      <c r="Q15" s="2" t="n">
-        <v>46120</v>
-      </c>
-      <c r="R15" s="2" t="n">
-        <v>46176</v>
-      </c>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr"/>
       <c r="U15" t="n">
         <v>0</v>
       </c>
       <c r="V15" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1762,32 +1687,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P16" t="n">
+      <c r="P16" s="2" t="n">
+        <v>45693</v>
+      </c>
+      <c r="Q16" s="2" t="n">
+        <v>45766</v>
+      </c>
+      <c r="R16" t="n">
         <v>161605.1</v>
       </c>
-      <c r="Q16" s="2" t="n">
-        <v>45693</v>
-      </c>
-      <c r="R16" s="2" t="n">
-        <v>45766</v>
-      </c>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr"/>
       <c r="U16" t="n">
         <v>0</v>
       </c>
       <c r="V16" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W16" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1843,32 +1763,27 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P17" t="n">
+      <c r="P17" s="2" t="n">
+        <v>45705</v>
+      </c>
+      <c r="Q17" s="2" t="n">
+        <v>45778</v>
+      </c>
+      <c r="R17" t="n">
         <v>95583.81</v>
       </c>
-      <c r="Q17" s="2" t="n">
-        <v>45705</v>
-      </c>
-      <c r="R17" s="2" t="n">
-        <v>45778</v>
-      </c>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr"/>
       <c r="U17" t="n">
         <v>0</v>
       </c>
       <c r="V17" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W17" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -1924,32 +1839,27 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P18" t="n">
+      <c r="P18" s="2" t="n">
+        <v>46136</v>
+      </c>
+      <c r="Q18" s="2" t="n">
+        <v>46196</v>
+      </c>
+      <c r="R18" t="n">
         <v>253564.24</v>
       </c>
-      <c r="Q18" s="2" t="n">
-        <v>46136</v>
-      </c>
-      <c r="R18" s="2" t="n">
-        <v>46196</v>
-      </c>
-      <c r="S18" t="inlineStr"/>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr"/>
       <c r="U18" t="n">
         <v>0</v>
       </c>
       <c r="V18" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2005,32 +1915,27 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P19" t="n">
+      <c r="P19" s="2" t="n">
+        <v>46126</v>
+      </c>
+      <c r="Q19" s="2" t="n">
+        <v>46204</v>
+      </c>
+      <c r="R19" t="n">
         <v>111100.55</v>
       </c>
-      <c r="Q19" s="2" t="n">
-        <v>46126</v>
-      </c>
-      <c r="R19" s="2" t="n">
-        <v>46204</v>
-      </c>
-      <c r="S19" t="inlineStr"/>
-      <c r="T19" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr"/>
       <c r="U19" t="n">
         <v>0</v>
       </c>
       <c r="V19" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2086,36 +1991,31 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P20" t="n">
+      <c r="P20" s="2" t="n">
+        <v>46023</v>
+      </c>
+      <c r="Q20" s="2" t="n">
+        <v>46112</v>
+      </c>
+      <c r="R20" t="n">
         <v>423679.91</v>
       </c>
-      <c r="Q20" s="2" t="n">
-        <v>46023</v>
-      </c>
-      <c r="R20" s="2" t="n">
-        <v>46112</v>
-      </c>
       <c r="S20" t="inlineStr">
         <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="T20" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
       <c r="U20" t="n">
         <v>0</v>
       </c>
       <c r="V20" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W20" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2171,32 +2071,27 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P21" t="n">
+      <c r="P21" s="2" t="n">
+        <v>46102</v>
+      </c>
+      <c r="Q21" s="2" t="n">
+        <v>46179</v>
+      </c>
+      <c r="R21" t="n">
         <v>224412.65</v>
       </c>
-      <c r="Q21" s="2" t="n">
-        <v>46102</v>
-      </c>
-      <c r="R21" s="2" t="n">
-        <v>46179</v>
-      </c>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr"/>
       <c r="U21" t="n">
         <v>0</v>
       </c>
       <c r="V21" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W21" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2252,32 +2147,27 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P22" t="n">
+      <c r="P22" s="2" t="n">
+        <v>46107</v>
+      </c>
+      <c r="Q22" s="2" t="n">
+        <v>46129</v>
+      </c>
+      <c r="R22" t="n">
         <v>568840.5</v>
       </c>
-      <c r="Q22" s="2" t="n">
-        <v>46107</v>
-      </c>
-      <c r="R22" s="2" t="n">
-        <v>46129</v>
-      </c>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr"/>
       <c r="U22" t="n">
         <v>0</v>
       </c>
       <c r="V22" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W22" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2333,32 +2223,27 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P23" t="n">
+      <c r="P23" s="2" t="n">
+        <v>45886</v>
+      </c>
+      <c r="Q23" s="2" t="n">
+        <v>45969</v>
+      </c>
+      <c r="R23" t="n">
         <v>105951.07</v>
       </c>
-      <c r="Q23" s="2" t="n">
-        <v>45886</v>
-      </c>
-      <c r="R23" s="2" t="n">
-        <v>45969</v>
-      </c>
-      <c r="S23" t="inlineStr"/>
-      <c r="T23" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr"/>
       <c r="U23" t="n">
         <v>0</v>
       </c>
       <c r="V23" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W23" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2414,32 +2299,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P24" t="n">
+      <c r="P24" s="2" t="n">
+        <v>45832</v>
+      </c>
+      <c r="Q24" s="2" t="n">
+        <v>45902</v>
+      </c>
+      <c r="R24" t="n">
         <v>280248.59</v>
       </c>
-      <c r="Q24" s="2" t="n">
-        <v>45832</v>
-      </c>
-      <c r="R24" s="2" t="n">
-        <v>45902</v>
-      </c>
-      <c r="S24" t="inlineStr"/>
-      <c r="T24" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr"/>
       <c r="U24" t="n">
         <v>0</v>
       </c>
       <c r="V24" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2495,32 +2375,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P25" t="n">
+      <c r="P25" s="2" t="n">
+        <v>45866</v>
+      </c>
+      <c r="Q25" s="2" t="n">
+        <v>45943</v>
+      </c>
+      <c r="R25" t="n">
         <v>285863.23</v>
       </c>
-      <c r="Q25" s="2" t="n">
-        <v>45866</v>
-      </c>
-      <c r="R25" s="2" t="n">
-        <v>45943</v>
-      </c>
-      <c r="S25" t="inlineStr"/>
-      <c r="T25" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr"/>
       <c r="U25" t="n">
         <v>0</v>
       </c>
       <c r="V25" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W25" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2576,32 +2451,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P26" t="n">
+      <c r="P26" s="2" t="n">
+        <v>45718</v>
+      </c>
+      <c r="Q26" s="2" t="n">
+        <v>45808</v>
+      </c>
+      <c r="R26" t="n">
         <v>221171.06</v>
       </c>
-      <c r="Q26" s="2" t="n">
-        <v>45718</v>
-      </c>
-      <c r="R26" s="2" t="n">
-        <v>45808</v>
-      </c>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr"/>
       <c r="U26" t="n">
         <v>0</v>
       </c>
       <c r="V26" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2657,36 +2527,31 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P27" t="n">
+      <c r="P27" s="2" t="n">
+        <v>46010</v>
+      </c>
+      <c r="Q27" s="2" t="n">
+        <v>46092</v>
+      </c>
+      <c r="R27" t="n">
         <v>577808.88</v>
       </c>
-      <c r="Q27" s="2" t="n">
-        <v>46010</v>
-      </c>
-      <c r="R27" s="2" t="n">
-        <v>46092</v>
-      </c>
       <c r="S27" t="inlineStr">
         <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="T27" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
       <c r="U27" t="n">
         <v>0</v>
       </c>
       <c r="V27" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W27" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2742,32 +2607,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P28" t="n">
+      <c r="P28" s="2" t="n">
+        <v>45899</v>
+      </c>
+      <c r="Q28" s="2" t="n">
+        <v>45938</v>
+      </c>
+      <c r="R28" t="n">
         <v>196777.36</v>
       </c>
-      <c r="Q28" s="2" t="n">
-        <v>45899</v>
-      </c>
-      <c r="R28" s="2" t="n">
-        <v>45938</v>
-      </c>
-      <c r="S28" t="inlineStr"/>
-      <c r="T28" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr"/>
       <c r="U28" t="n">
         <v>0</v>
       </c>
       <c r="V28" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2823,32 +2683,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P29" t="n">
+      <c r="P29" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="Q29" s="2" t="n">
+        <v>45780</v>
+      </c>
+      <c r="R29" t="n">
         <v>170730.01</v>
       </c>
-      <c r="Q29" s="2" t="n">
-        <v>45685</v>
-      </c>
-      <c r="R29" s="2" t="n">
-        <v>45780</v>
-      </c>
-      <c r="S29" t="inlineStr"/>
-      <c r="T29" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr"/>
       <c r="U29" t="n">
         <v>0</v>
       </c>
       <c r="V29" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2904,32 +2759,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P30" t="n">
+      <c r="P30" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="Q30" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="R30" t="n">
         <v>355660.26</v>
       </c>
-      <c r="Q30" s="2" t="n">
-        <v>45881</v>
-      </c>
-      <c r="R30" s="2" t="n">
-        <v>45954</v>
-      </c>
-      <c r="S30" t="inlineStr"/>
-      <c r="T30" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr"/>
       <c r="U30" t="n">
         <v>0</v>
       </c>
       <c r="V30" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -2985,32 +2835,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P31" t="n">
+      <c r="P31" s="2" t="n">
+        <v>45666</v>
+      </c>
+      <c r="Q31" s="2" t="n">
+        <v>45765</v>
+      </c>
+      <c r="R31" t="n">
         <v>418857.39</v>
       </c>
-      <c r="Q31" s="2" t="n">
-        <v>45666</v>
-      </c>
-      <c r="R31" s="2" t="n">
-        <v>45765</v>
-      </c>
-      <c r="S31" t="inlineStr"/>
-      <c r="T31" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr"/>
       <c r="U31" t="n">
         <v>0</v>
       </c>
       <c r="V31" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3066,36 +2911,31 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P32" t="n">
+      <c r="P32" s="2" t="n">
+        <v>45998</v>
+      </c>
+      <c r="Q32" s="2" t="n">
+        <v>46117</v>
+      </c>
+      <c r="R32" t="n">
         <v>574740.27</v>
       </c>
-      <c r="Q32" s="2" t="n">
-        <v>45998</v>
-      </c>
-      <c r="R32" s="2" t="n">
-        <v>46117</v>
-      </c>
       <c r="S32" t="inlineStr">
         <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="T32" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
       <c r="U32" t="n">
         <v>0</v>
       </c>
       <c r="V32" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W32" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3151,23 +2991,23 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P33" t="n">
+      <c r="P33" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="Q33" s="2" t="n">
+        <v>46093</v>
+      </c>
+      <c r="R33" t="n">
         <v>129356.97</v>
       </c>
-      <c r="Q33" s="2" t="n">
-        <v>46028</v>
-      </c>
-      <c r="R33" s="2" t="n">
-        <v>46093</v>
-      </c>
       <c r="S33" t="inlineStr">
         <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
           <t>Overdelivered</t>
-        </is>
-      </c>
-      <c r="T33" t="inlineStr">
-        <is>
-          <t>LIVE</t>
         </is>
       </c>
       <c r="U33" t="n">
@@ -3178,11 +3018,6 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="W33" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3236,32 +3071,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P34" t="n">
+      <c r="P34" s="2" t="n">
+        <v>45903</v>
+      </c>
+      <c r="Q34" s="2" t="n">
+        <v>45931</v>
+      </c>
+      <c r="R34" t="n">
         <v>591950.49</v>
       </c>
-      <c r="Q34" s="2" t="n">
-        <v>45903</v>
-      </c>
-      <c r="R34" s="2" t="n">
-        <v>45931</v>
-      </c>
-      <c r="S34" t="inlineStr"/>
-      <c r="T34" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T34" t="inlineStr"/>
       <c r="U34" t="n">
         <v>0</v>
       </c>
       <c r="V34" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W34" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3317,32 +3147,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P35" t="n">
+      <c r="P35" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="Q35" s="2" t="n">
+        <v>45972</v>
+      </c>
+      <c r="R35" t="n">
         <v>390381.81</v>
       </c>
-      <c r="Q35" s="2" t="n">
-        <v>45909</v>
-      </c>
-      <c r="R35" s="2" t="n">
-        <v>45972</v>
-      </c>
-      <c r="S35" t="inlineStr"/>
-      <c r="T35" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T35" t="inlineStr"/>
       <c r="U35" t="n">
         <v>0</v>
       </c>
       <c r="V35" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W35" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3398,32 +3223,27 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P36" t="n">
+      <c r="P36" s="2" t="n">
+        <v>45863</v>
+      </c>
+      <c r="Q36" s="2" t="n">
+        <v>45951</v>
+      </c>
+      <c r="R36" t="n">
         <v>128268.79</v>
       </c>
-      <c r="Q36" s="2" t="n">
-        <v>45863</v>
-      </c>
-      <c r="R36" s="2" t="n">
-        <v>45951</v>
-      </c>
-      <c r="S36" t="inlineStr"/>
-      <c r="T36" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T36" t="inlineStr"/>
       <c r="U36" t="n">
         <v>0</v>
       </c>
       <c r="V36" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W36" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3479,36 +3299,31 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P37" t="n">
+      <c r="P37" s="2" t="n">
+        <v>46066</v>
+      </c>
+      <c r="Q37" s="2" t="n">
+        <v>46095</v>
+      </c>
+      <c r="R37" t="n">
         <v>534024.5</v>
       </c>
-      <c r="Q37" s="2" t="n">
-        <v>46066</v>
-      </c>
-      <c r="R37" s="2" t="n">
-        <v>46095</v>
-      </c>
       <c r="S37" t="inlineStr">
         <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T37" t="inlineStr">
+        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="T37" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
       <c r="U37" t="n">
         <v>0</v>
       </c>
       <c r="V37" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W37" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3564,32 +3379,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P38" t="n">
+      <c r="P38" s="2" t="n">
+        <v>45835</v>
+      </c>
+      <c r="Q38" s="2" t="n">
+        <v>45899</v>
+      </c>
+      <c r="R38" t="n">
         <v>391196.57</v>
       </c>
-      <c r="Q38" s="2" t="n">
-        <v>45835</v>
-      </c>
-      <c r="R38" s="2" t="n">
-        <v>45899</v>
-      </c>
-      <c r="S38" t="inlineStr"/>
-      <c r="T38" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T38" t="inlineStr"/>
       <c r="U38" t="n">
         <v>0</v>
       </c>
       <c r="V38" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W38" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3645,32 +3455,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P39" t="n">
+      <c r="P39" s="2" t="n">
+        <v>45887</v>
+      </c>
+      <c r="Q39" s="2" t="n">
+        <v>45969</v>
+      </c>
+      <c r="R39" t="n">
         <v>596378.9300000001</v>
       </c>
-      <c r="Q39" s="2" t="n">
-        <v>45887</v>
-      </c>
-      <c r="R39" s="2" t="n">
-        <v>45969</v>
-      </c>
-      <c r="S39" t="inlineStr"/>
-      <c r="T39" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T39" t="inlineStr"/>
       <c r="U39" t="n">
         <v>0</v>
       </c>
       <c r="V39" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W39" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3726,36 +3531,31 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P40" t="n">
+      <c r="P40" s="2" t="n">
+        <v>46023</v>
+      </c>
+      <c r="Q40" s="2" t="n">
+        <v>46087</v>
+      </c>
+      <c r="R40" t="n">
         <v>120089.45</v>
       </c>
-      <c r="Q40" s="2" t="n">
-        <v>46023</v>
-      </c>
-      <c r="R40" s="2" t="n">
-        <v>46087</v>
-      </c>
       <c r="S40" t="inlineStr">
         <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="T40" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
       <c r="U40" t="n">
         <v>0</v>
       </c>
       <c r="V40" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W40" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3811,32 +3611,27 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P41" t="n">
+      <c r="P41" s="2" t="n">
+        <v>46106</v>
+      </c>
+      <c r="Q41" s="2" t="n">
+        <v>46159</v>
+      </c>
+      <c r="R41" t="n">
         <v>326276.52</v>
       </c>
-      <c r="Q41" s="2" t="n">
-        <v>46106</v>
-      </c>
-      <c r="R41" s="2" t="n">
-        <v>46159</v>
-      </c>
-      <c r="S41" t="inlineStr"/>
-      <c r="T41" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T41" t="inlineStr"/>
       <c r="U41" t="n">
         <v>0</v>
       </c>
       <c r="V41" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W41" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3892,36 +3687,31 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P42" t="n">
+      <c r="P42" s="2" t="n">
+        <v>46065</v>
+      </c>
+      <c r="Q42" s="2" t="n">
+        <v>46111</v>
+      </c>
+      <c r="R42" t="n">
         <v>574267.4300000001</v>
       </c>
-      <c r="Q42" s="2" t="n">
-        <v>46065</v>
-      </c>
-      <c r="R42" s="2" t="n">
-        <v>46111</v>
-      </c>
       <c r="S42" t="inlineStr">
         <is>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="T42" t="inlineStr">
+        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="T42" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
       <c r="U42" t="n">
         <v>0</v>
       </c>
       <c r="V42" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W42" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -3977,32 +3767,27 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P43" t="n">
+      <c r="P43" s="2" t="n">
+        <v>45898</v>
+      </c>
+      <c r="Q43" s="2" t="n">
+        <v>46015</v>
+      </c>
+      <c r="R43" t="n">
         <v>352257.46</v>
       </c>
-      <c r="Q43" s="2" t="n">
-        <v>45898</v>
-      </c>
-      <c r="R43" s="2" t="n">
-        <v>46015</v>
-      </c>
-      <c r="S43" t="inlineStr"/>
-      <c r="T43" t="inlineStr">
-        <is>
-          <t>ENDED</t>
-        </is>
-      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T43" t="inlineStr"/>
       <c r="U43" t="n">
         <v>0</v>
       </c>
       <c r="V43" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W43" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -4058,32 +3843,27 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P44" t="n">
+      <c r="P44" s="2" t="n">
+        <v>46096</v>
+      </c>
+      <c r="Q44" s="2" t="n">
+        <v>46182</v>
+      </c>
+      <c r="R44" t="n">
         <v>267517.39</v>
       </c>
-      <c r="Q44" s="2" t="n">
-        <v>46096</v>
-      </c>
-      <c r="R44" s="2" t="n">
-        <v>46182</v>
-      </c>
-      <c r="S44" t="inlineStr"/>
-      <c r="T44" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T44" t="inlineStr"/>
       <c r="U44" t="n">
         <v>0</v>
       </c>
       <c r="V44" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W44" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -4139,36 +3919,31 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P45" t="n">
+      <c r="P45" s="2" t="n">
+        <v>46004</v>
+      </c>
+      <c r="Q45" s="2" t="n">
+        <v>46082</v>
+      </c>
+      <c r="R45" t="n">
         <v>354611.01</v>
       </c>
-      <c r="Q45" s="2" t="n">
-        <v>46004</v>
-      </c>
-      <c r="R45" s="2" t="n">
-        <v>46082</v>
-      </c>
       <c r="S45" t="inlineStr">
         <is>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="T45" t="inlineStr">
+        <is>
           <t>Underdelivered</t>
         </is>
       </c>
-      <c r="T45" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
       <c r="U45" t="n">
         <v>0</v>
       </c>
       <c r="V45" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W45" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -4224,32 +3999,27 @@
           <t>No Data</t>
         </is>
       </c>
-      <c r="P46" t="n">
+      <c r="P46" s="2" t="n">
+        <v>46091</v>
+      </c>
+      <c r="Q46" s="2" t="n">
+        <v>46135</v>
+      </c>
+      <c r="R46" t="n">
         <v>498191.26</v>
       </c>
-      <c r="Q46" s="2" t="n">
-        <v>46091</v>
-      </c>
-      <c r="R46" s="2" t="n">
-        <v>46135</v>
-      </c>
-      <c r="S46" t="inlineStr"/>
-      <c r="T46" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T46" t="inlineStr"/>
       <c r="U46" t="n">
         <v>0</v>
       </c>
       <c r="V46" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W46" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
     </row>
@@ -4365,7 +4135,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4408,22 +4178,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Excel vs ML Disagreement Count</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
           <t>LAST_REFRESH_UTC</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2026-02-16 05:31 UTC</t>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2026-02-16 06:09 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto refresh - 16-02-2026 12:23:22.69
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V46"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,10 +563,10 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45723</v>
+        <v>46025</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45826</v>
+        <v>46049</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>46069</v>
@@ -578,10 +578,10 @@
         <v>100350.37</v>
       </c>
       <c r="H2" t="n">
-        <v>166806.6</v>
+        <v>84854.23</v>
       </c>
       <c r="I2" t="n">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -590,24 +590,24 @@
         <v>100350.37</v>
       </c>
       <c r="L2" t="n">
-        <v>166.22</v>
+        <v>84.56</v>
       </c>
       <c r="M2" t="n">
-        <v>-66456.23</v>
+        <v>15496.14</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P2" s="2" t="n">
-        <v>45723</v>
+        <v>46025</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>45826</v>
+        <v>46049</v>
       </c>
       <c r="R2" t="n">
         <v>100350.37</v>
@@ -639,10 +639,10 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>46071</v>
+        <v>46057</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>46069</v>
@@ -654,36 +654,36 @@
         <v>552594.63</v>
       </c>
       <c r="H3" t="n">
-        <v>89972.7</v>
+        <v>664449.42</v>
       </c>
       <c r="I3" t="n">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="J3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>522991.35</v>
+        <v>552594.63</v>
       </c>
       <c r="L3" t="n">
-        <v>17.2</v>
+        <v>120.24</v>
       </c>
       <c r="M3" t="n">
-        <v>462621.93</v>
+        <v>-111854.79</v>
       </c>
       <c r="N3" t="n">
-        <v>154207.31</v>
+        <v>0</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>Overpacing</t>
         </is>
       </c>
       <c r="P3" s="2" t="n">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="Q3" s="2" t="n">
-        <v>46071</v>
+        <v>46057</v>
       </c>
       <c r="R3" t="n">
         <v>552594.63</v>
@@ -693,11 +693,7 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
-      </c>
+      <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
         <v>0</v>
       </c>
@@ -719,10 +715,10 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45909</v>
+        <v>46030</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45984</v>
+        <v>46063</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>46069</v>
@@ -734,10 +730,10 @@
         <v>294540.38</v>
       </c>
       <c r="H4" t="n">
-        <v>154346.38</v>
+        <v>287441.18</v>
       </c>
       <c r="I4" t="n">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -746,24 +742,24 @@
         <v>294540.38</v>
       </c>
       <c r="L4" t="n">
-        <v>52.4</v>
+        <v>97.59</v>
       </c>
       <c r="M4" t="n">
-        <v>140194</v>
+        <v>7099.2</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P4" s="2" t="n">
-        <v>45909</v>
+        <v>46030</v>
       </c>
       <c r="Q4" s="2" t="n">
-        <v>45984</v>
+        <v>46063</v>
       </c>
       <c r="R4" t="n">
         <v>294540.38</v>
@@ -795,10 +791,10 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45784</v>
+        <v>46055</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45811</v>
+        <v>46081</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>46069</v>
@@ -810,25 +806,25 @@
         <v>509097.37</v>
       </c>
       <c r="H5" t="n">
-        <v>30692.27</v>
+        <v>201726.35</v>
       </c>
       <c r="I5" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K5" t="n">
-        <v>509097.37</v>
+        <v>263976.41</v>
       </c>
       <c r="L5" t="n">
-        <v>6.03</v>
+        <v>76.42</v>
       </c>
       <c r="M5" t="n">
-        <v>478405.1</v>
+        <v>307371.02</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>23643.92</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -836,10 +832,10 @@
         </is>
       </c>
       <c r="P5" s="2" t="n">
-        <v>45784</v>
+        <v>46055</v>
       </c>
       <c r="Q5" s="2" t="n">
-        <v>45811</v>
+        <v>46081</v>
       </c>
       <c r="R5" t="n">
         <v>509097.37</v>
@@ -849,7 +845,11 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr"/>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Underdelivered</t>
+        </is>
+      </c>
       <c r="U5" t="n">
         <v>0</v>
       </c>
@@ -871,10 +871,10 @@
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45904</v>
+        <v>46010</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>45997</v>
+        <v>46052</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>46069</v>
@@ -886,10 +886,10 @@
         <v>382409.25</v>
       </c>
       <c r="H6" t="n">
-        <v>146951.89</v>
+        <v>283257.35</v>
       </c>
       <c r="I6" t="n">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -898,10 +898,10 @@
         <v>382409.25</v>
       </c>
       <c r="L6" t="n">
-        <v>38.43</v>
+        <v>74.06999999999999</v>
       </c>
       <c r="M6" t="n">
-        <v>235457.36</v>
+        <v>99151.89999999999</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
@@ -912,10 +912,10 @@
         </is>
       </c>
       <c r="P6" s="2" t="n">
-        <v>45904</v>
+        <v>46010</v>
       </c>
       <c r="Q6" s="2" t="n">
-        <v>45997</v>
+        <v>46052</v>
       </c>
       <c r="R6" t="n">
         <v>382409.25</v>
@@ -947,10 +947,10 @@
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45914</v>
+        <v>46030</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>46005</v>
+        <v>46050</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>46069</v>
@@ -962,10 +962,10 @@
         <v>525695.9399999999</v>
       </c>
       <c r="H7" t="n">
-        <v>121020.49</v>
+        <v>518561.35</v>
       </c>
       <c r="I7" t="n">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -974,24 +974,24 @@
         <v>525695.9399999999</v>
       </c>
       <c r="L7" t="n">
-        <v>23.02</v>
+        <v>98.64</v>
       </c>
       <c r="M7" t="n">
-        <v>404675.45</v>
+        <v>7134.59</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P7" s="2" t="n">
-        <v>45914</v>
+        <v>46030</v>
       </c>
       <c r="Q7" s="2" t="n">
-        <v>46005</v>
+        <v>46050</v>
       </c>
       <c r="R7" t="n">
         <v>525695.9399999999</v>
@@ -1023,10 +1023,10 @@
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>46044</v>
+        <v>46019</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>46102</v>
+        <v>46048</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>46069</v>
@@ -1038,25 +1038,25 @@
         <v>136840.92</v>
       </c>
       <c r="H8" t="n">
-        <v>40927.75</v>
+        <v>118651.79</v>
       </c>
       <c r="I8" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J8" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>57983.44</v>
+        <v>136840.92</v>
       </c>
       <c r="L8" t="n">
-        <v>70.59</v>
+        <v>86.70999999999999</v>
       </c>
       <c r="M8" t="n">
-        <v>95913.17</v>
+        <v>18189.13</v>
       </c>
       <c r="N8" t="n">
-        <v>2820.98</v>
+        <v>0</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1064,10 +1064,10 @@
         </is>
       </c>
       <c r="P8" s="2" t="n">
-        <v>46044</v>
+        <v>46019</v>
       </c>
       <c r="Q8" s="2" t="n">
-        <v>46102</v>
+        <v>46048</v>
       </c>
       <c r="R8" t="n">
         <v>136840.92</v>
@@ -1077,11 +1077,7 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
-      </c>
+      <c r="T8" t="inlineStr"/>
       <c r="U8" t="n">
         <v>0</v>
       </c>
@@ -1094,19 +1090,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CAMP_008</t>
+          <t>CAMP_009</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TTD</t>
+          <t>Amazon DSP</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>46086</v>
+        <v>46014</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>46119</v>
+        <v>46058</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>46069</v>
@@ -1115,46 +1111,46 @@
         <v>46068</v>
       </c>
       <c r="G9" t="n">
-        <v>380340.09</v>
+        <v>448858.15</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>389686.77</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J9" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>448858.15</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>86.81999999999999</v>
       </c>
       <c r="M9" t="n">
-        <v>380340.09</v>
+        <v>59171.38</v>
       </c>
       <c r="N9" t="n">
-        <v>11186.47</v>
+        <v>0</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P9" s="2" t="n">
-        <v>46086</v>
+        <v>46014</v>
       </c>
       <c r="Q9" s="2" t="n">
-        <v>46119</v>
+        <v>46058</v>
       </c>
       <c r="R9" t="n">
-        <v>380340.09</v>
+        <v>448858.15</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>TTD</t>
+          <t>Amazon DSP</t>
         </is>
       </c>
       <c r="T9" t="inlineStr"/>
@@ -1170,19 +1166,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CAMP_009</t>
+          <t>CAMP_011</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Amazon DSP</t>
+          <t>Yahoo</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>46047</v>
+        <v>46030</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>46103</v>
+        <v>46064</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>46069</v>
@@ -1191,28 +1187,28 @@
         <v>46068</v>
       </c>
       <c r="G10" t="n">
-        <v>448858.15</v>
+        <v>559806.73</v>
       </c>
       <c r="H10" t="n">
-        <v>33037.27</v>
+        <v>478951.63</v>
       </c>
       <c r="I10" t="n">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="J10" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>173243.5</v>
+        <v>559806.73</v>
       </c>
       <c r="L10" t="n">
-        <v>19.07</v>
+        <v>85.56</v>
       </c>
       <c r="M10" t="n">
-        <v>415820.88</v>
+        <v>80855.10000000001</v>
       </c>
       <c r="N10" t="n">
-        <v>11880.6</v>
+        <v>0</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1220,24 +1216,20 @@
         </is>
       </c>
       <c r="P10" s="2" t="n">
-        <v>46047</v>
+        <v>46030</v>
       </c>
       <c r="Q10" s="2" t="n">
-        <v>46103</v>
+        <v>46064</v>
       </c>
       <c r="R10" t="n">
-        <v>448858.15</v>
+        <v>559806.73</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
-      </c>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr"/>
       <c r="U10" t="n">
         <v>0</v>
       </c>
@@ -1250,19 +1242,19 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CAMP_010</t>
+          <t>CAMP_012</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>46089</v>
+        <v>46015</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>46172</v>
+        <v>46059</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>46069</v>
@@ -1271,46 +1263,46 @@
         <v>46068</v>
       </c>
       <c r="G11" t="n">
-        <v>432209.99</v>
+        <v>169377.54</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>164408.91</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J11" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>169377.54</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>97.06999999999999</v>
       </c>
       <c r="M11" t="n">
-        <v>432209.99</v>
+        <v>4968.63</v>
       </c>
       <c r="N11" t="n">
-        <v>5145.36</v>
+        <v>0</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P11" s="2" t="n">
-        <v>46089</v>
+        <v>46015</v>
       </c>
       <c r="Q11" s="2" t="n">
-        <v>46172</v>
+        <v>46059</v>
       </c>
       <c r="R11" t="n">
-        <v>432209.99</v>
+        <v>169377.54</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="T11" t="inlineStr"/>
@@ -1326,19 +1318,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CAMP_011</t>
+          <t>CAMP_013</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>Amazon DSP</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>46024</v>
+        <v>46020</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>46105</v>
+        <v>46056</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>46069</v>
@@ -1347,28 +1339,28 @@
         <v>46068</v>
       </c>
       <c r="G12" t="n">
-        <v>559806.73</v>
+        <v>334936.09</v>
       </c>
       <c r="H12" t="n">
-        <v>86475.62</v>
+        <v>247498.8</v>
       </c>
       <c r="I12" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="J12" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>307211.01</v>
+        <v>334936.09</v>
       </c>
       <c r="L12" t="n">
-        <v>28.15</v>
+        <v>73.89</v>
       </c>
       <c r="M12" t="n">
-        <v>473331.11</v>
+        <v>87437.28999999999</v>
       </c>
       <c r="N12" t="n">
-        <v>12792.73</v>
+        <v>0</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1376,24 +1368,20 @@
         </is>
       </c>
       <c r="P12" s="2" t="n">
-        <v>46024</v>
+        <v>46020</v>
       </c>
       <c r="Q12" s="2" t="n">
-        <v>46105</v>
+        <v>46056</v>
       </c>
       <c r="R12" t="n">
-        <v>559806.73</v>
+        <v>334936.09</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
-      </c>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr"/>
       <c r="U12" t="n">
         <v>0</v>
       </c>
@@ -1406,19 +1394,19 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CAMP_012</t>
+          <t>CAMP_015</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TTD</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>46038</v>
+        <v>46064</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>46118</v>
+        <v>46090</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>46069</v>
@@ -1427,78 +1415,78 @@
         <v>46068</v>
       </c>
       <c r="G13" t="n">
-        <v>169377.54</v>
+        <v>161605.1</v>
       </c>
       <c r="H13" t="n">
-        <v>63349.43</v>
+        <v>34326.92</v>
       </c>
       <c r="I13" t="n">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="J13" t="n">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="K13" t="n">
-        <v>64823.5</v>
+        <v>29926.87</v>
       </c>
       <c r="L13" t="n">
-        <v>97.73</v>
+        <v>114.7</v>
       </c>
       <c r="M13" t="n">
-        <v>106028.11</v>
+        <v>127278.18</v>
       </c>
       <c r="N13" t="n">
-        <v>2120.56</v>
+        <v>5785.37</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
+          <t>Overpacing</t>
+        </is>
+      </c>
+      <c r="P13" s="2" t="n">
+        <v>46064</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <v>46090</v>
+      </c>
+      <c r="R13" t="n">
+        <v>161605.1</v>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
           <t>On Track</t>
         </is>
       </c>
-      <c r="P13" s="2" t="n">
-        <v>46038</v>
-      </c>
-      <c r="Q13" s="2" t="n">
-        <v>46118</v>
-      </c>
-      <c r="R13" t="n">
-        <v>169377.54</v>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
-      </c>
       <c r="U13" t="n">
         <v>0</v>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CAMP_013</t>
+          <t>CAMP_016</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Amazon DSP</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45788</v>
+        <v>46018</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>45875</v>
+        <v>46061</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>46069</v>
@@ -1507,46 +1495,46 @@
         <v>46068</v>
       </c>
       <c r="G14" t="n">
-        <v>334936.09</v>
+        <v>95583.81</v>
       </c>
       <c r="H14" t="n">
-        <v>81515.34</v>
+        <v>92301.7</v>
       </c>
       <c r="I14" t="n">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>334936.09</v>
+        <v>95583.81</v>
       </c>
       <c r="L14" t="n">
-        <v>24.34</v>
+        <v>96.56999999999999</v>
       </c>
       <c r="M14" t="n">
-        <v>253420.75</v>
+        <v>3282.11</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P14" s="2" t="n">
-        <v>45788</v>
+        <v>46018</v>
       </c>
       <c r="Q14" s="2" t="n">
-        <v>45875</v>
+        <v>46061</v>
       </c>
       <c r="R14" t="n">
-        <v>334936.09</v>
+        <v>95583.81</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>Amazon DSP</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="T14" t="inlineStr"/>
@@ -1562,19 +1550,19 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CAMP_014</t>
+          <t>CAMP_019</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TTD</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>46120</v>
+        <v>46056</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>46176</v>
+        <v>46098</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>46069</v>
@@ -1583,49 +1571,53 @@
         <v>46068</v>
       </c>
       <c r="G15" t="n">
-        <v>394703.48</v>
+        <v>423679.91</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>168144.14</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J15" t="n">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>128089.28</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>131.27</v>
       </c>
       <c r="M15" t="n">
-        <v>394703.48</v>
+        <v>255535.77</v>
       </c>
       <c r="N15" t="n">
-        <v>6924.62</v>
+        <v>8517.860000000001</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>Overpacing</t>
         </is>
       </c>
       <c r="P15" s="2" t="n">
-        <v>46120</v>
+        <v>46056</v>
       </c>
       <c r="Q15" s="2" t="n">
-        <v>46176</v>
+        <v>46098</v>
       </c>
       <c r="R15" t="n">
-        <v>394703.48</v>
+        <v>423679.91</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>TTD</t>
-        </is>
-      </c>
-      <c r="T15" t="inlineStr"/>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
       <c r="U15" t="n">
         <v>0</v>
       </c>
@@ -1638,19 +1630,19 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CAMP_015</t>
+          <t>CAMP_022</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45693</v>
+        <v>46058</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>45766</v>
+        <v>46076</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>46069</v>
@@ -1659,28 +1651,28 @@
         <v>46068</v>
       </c>
       <c r="G16" t="n">
-        <v>161605.1</v>
+        <v>105951.07</v>
       </c>
       <c r="H16" t="n">
-        <v>65180.2</v>
+        <v>47147.09</v>
       </c>
       <c r="I16" t="n">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K16" t="n">
-        <v>161605.1</v>
+        <v>61340.09</v>
       </c>
       <c r="L16" t="n">
-        <v>40.33</v>
+        <v>76.86</v>
       </c>
       <c r="M16" t="n">
-        <v>96424.89999999999</v>
+        <v>58803.98</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>7350.5</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1688,20 +1680,24 @@
         </is>
       </c>
       <c r="P16" s="2" t="n">
-        <v>45693</v>
+        <v>46058</v>
       </c>
       <c r="Q16" s="2" t="n">
-        <v>45766</v>
+        <v>46076</v>
       </c>
       <c r="R16" t="n">
-        <v>161605.1</v>
+        <v>105951.07</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>DV360</t>
-        </is>
-      </c>
-      <c r="T16" t="inlineStr"/>
+          <t>TTD</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>Underdelivered</t>
+        </is>
+      </c>
       <c r="U16" t="n">
         <v>0</v>
       </c>
@@ -1714,7 +1710,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CAMP_016</t>
+          <t>CAMP_023</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1723,10 +1719,10 @@
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45705</v>
+        <v>46023</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>45778</v>
+        <v>46050</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>46069</v>
@@ -1735,42 +1731,42 @@
         <v>46068</v>
       </c>
       <c r="G17" t="n">
-        <v>95583.81</v>
+        <v>280248.59</v>
       </c>
       <c r="H17" t="n">
-        <v>139657.66</v>
+        <v>238064.17</v>
       </c>
       <c r="I17" t="n">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>95583.81</v>
+        <v>280248.59</v>
       </c>
       <c r="L17" t="n">
-        <v>146.11</v>
+        <v>84.95</v>
       </c>
       <c r="M17" t="n">
-        <v>-44073.85</v>
+        <v>42184.42</v>
       </c>
       <c r="N17" t="n">
         <v>0</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P17" s="2" t="n">
-        <v>45705</v>
+        <v>46023</v>
       </c>
       <c r="Q17" s="2" t="n">
-        <v>45778</v>
+        <v>46050</v>
       </c>
       <c r="R17" t="n">
-        <v>95583.81</v>
+        <v>280248.59</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
@@ -1790,19 +1786,19 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CAMP_017</t>
+          <t>CAMP_024</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>Yahoo</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>46136</v>
+        <v>46064</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>46196</v>
+        <v>46079</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>46069</v>
@@ -1811,49 +1807,53 @@
         <v>46068</v>
       </c>
       <c r="G18" t="n">
-        <v>253564.24</v>
+        <v>285863.23</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>71983.91</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J18" t="n">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>89332.25999999999</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>80.58</v>
       </c>
       <c r="M18" t="n">
-        <v>253564.24</v>
+        <v>213879.32</v>
       </c>
       <c r="N18" t="n">
-        <v>4156.79</v>
+        <v>19443.57</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P18" s="2" t="n">
-        <v>46136</v>
+        <v>46064</v>
       </c>
       <c r="Q18" s="2" t="n">
-        <v>46196</v>
+        <v>46079</v>
       </c>
       <c r="R18" t="n">
-        <v>253564.24</v>
+        <v>285863.23</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>DV360</t>
-        </is>
-      </c>
-      <c r="T18" t="inlineStr"/>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>Underdelivered</t>
+        </is>
+      </c>
       <c r="U18" t="n">
         <v>0</v>
       </c>
@@ -1866,7 +1866,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CAMP_018</t>
+          <t>CAMP_025</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1875,10 +1875,10 @@
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>46126</v>
+        <v>46027</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>46204</v>
+        <v>46059</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>46069</v>
@@ -1887,42 +1887,42 @@
         <v>46068</v>
       </c>
       <c r="G19" t="n">
-        <v>111100.55</v>
+        <v>221171.06</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>214329.85</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="J19" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>221171.06</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>96.91</v>
       </c>
       <c r="M19" t="n">
-        <v>111100.55</v>
+        <v>6841.21</v>
       </c>
       <c r="N19" t="n">
-        <v>1406.34</v>
+        <v>0</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P19" s="2" t="n">
-        <v>46126</v>
+        <v>46027</v>
       </c>
       <c r="Q19" s="2" t="n">
-        <v>46204</v>
+        <v>46059</v>
       </c>
       <c r="R19" t="n">
-        <v>111100.55</v>
+        <v>221171.06</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
@@ -1942,19 +1942,19 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CAMP_019</t>
+          <t>CAMP_026</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>Yahoo</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>46023</v>
+        <v>46020</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>46112</v>
+        <v>46054</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>46069</v>
@@ -1963,53 +1963,49 @@
         <v>46068</v>
       </c>
       <c r="G20" t="n">
-        <v>423679.91</v>
+        <v>577808.88</v>
       </c>
       <c r="H20" t="n">
-        <v>53250.78</v>
+        <v>563296.1</v>
       </c>
       <c r="I20" t="n">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="J20" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>216547.51</v>
+        <v>577808.88</v>
       </c>
       <c r="L20" t="n">
-        <v>24.59</v>
+        <v>97.48999999999999</v>
       </c>
       <c r="M20" t="n">
-        <v>370429.13</v>
+        <v>14512.78</v>
       </c>
       <c r="N20" t="n">
-        <v>8418.84</v>
+        <v>0</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P20" s="2" t="n">
-        <v>46023</v>
+        <v>46020</v>
       </c>
       <c r="Q20" s="2" t="n">
-        <v>46112</v>
+        <v>46054</v>
       </c>
       <c r="R20" t="n">
-        <v>423679.91</v>
+        <v>577808.88</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>DV360</t>
-        </is>
-      </c>
-      <c r="T20" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
-      </c>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr"/>
       <c r="U20" t="n">
         <v>0</v>
       </c>
@@ -2022,19 +2018,19 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CAMP_020</t>
+          <t>CAMP_027</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>Amazon DSP</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>46102</v>
+        <v>46056</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>46179</v>
+        <v>46074</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>46069</v>
@@ -2043,49 +2039,53 @@
         <v>46068</v>
       </c>
       <c r="G21" t="n">
-        <v>224412.65</v>
+        <v>196777.36</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>131920.99</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J21" t="n">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>134637.14</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>97.98</v>
       </c>
       <c r="M21" t="n">
-        <v>224412.65</v>
+        <v>64856.37</v>
       </c>
       <c r="N21" t="n">
-        <v>2877.09</v>
+        <v>10809.39</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P21" s="2" t="n">
-        <v>46102</v>
+        <v>46056</v>
       </c>
       <c r="Q21" s="2" t="n">
-        <v>46179</v>
+        <v>46074</v>
       </c>
       <c r="R21" t="n">
-        <v>224412.65</v>
+        <v>196777.36</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>DV360</t>
-        </is>
-      </c>
-      <c r="T21" t="inlineStr"/>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
       <c r="U21" t="n">
         <v>0</v>
       </c>
@@ -2098,19 +2098,19 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CAMP_021</t>
+          <t>CAMP_028</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>Amazon DSP</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>46107</v>
+        <v>46027</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>46129</v>
+        <v>46063</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>46069</v>
@@ -2119,46 +2119,46 @@
         <v>46068</v>
       </c>
       <c r="G22" t="n">
-        <v>568840.5</v>
+        <v>170730.01</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>206115.8</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="J22" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>170730.01</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>120.73</v>
       </c>
       <c r="M22" t="n">
-        <v>568840.5</v>
+        <v>-35385.79</v>
       </c>
       <c r="N22" t="n">
-        <v>24732.2</v>
+        <v>0</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>Overpacing</t>
         </is>
       </c>
       <c r="P22" s="2" t="n">
-        <v>46107</v>
+        <v>46027</v>
       </c>
       <c r="Q22" s="2" t="n">
-        <v>46129</v>
+        <v>46063</v>
       </c>
       <c r="R22" t="n">
-        <v>568840.5</v>
+        <v>170730.01</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>Amazon DSP</t>
         </is>
       </c>
       <c r="T22" t="inlineStr"/>
@@ -2174,7 +2174,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CAMP_022</t>
+          <t>CAMP_029</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2183,10 +2183,10 @@
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45886</v>
+        <v>46061</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>45969</v>
+        <v>46098</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>46069</v>
@@ -2195,28 +2195,28 @@
         <v>46068</v>
       </c>
       <c r="G23" t="n">
-        <v>105951.07</v>
+        <v>355660.26</v>
       </c>
       <c r="H23" t="n">
-        <v>150306.27</v>
+        <v>96491.92</v>
       </c>
       <c r="I23" t="n">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K23" t="n">
-        <v>105951.07</v>
+        <v>74875.84</v>
       </c>
       <c r="L23" t="n">
-        <v>141.86</v>
+        <v>128.87</v>
       </c>
       <c r="M23" t="n">
-        <v>-44355.2</v>
+        <v>259168.34</v>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>8638.940000000001</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2224,20 +2224,24 @@
         </is>
       </c>
       <c r="P23" s="2" t="n">
-        <v>45886</v>
+        <v>46061</v>
       </c>
       <c r="Q23" s="2" t="n">
-        <v>45969</v>
+        <v>46098</v>
       </c>
       <c r="R23" t="n">
-        <v>105951.07</v>
+        <v>355660.26</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
           <t>TTD</t>
         </is>
       </c>
-      <c r="T23" t="inlineStr"/>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
       <c r="U23" t="n">
         <v>0</v>
       </c>
@@ -2250,7 +2254,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CAMP_023</t>
+          <t>CAMP_030</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2259,10 +2263,10 @@
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45832</v>
+        <v>46018</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>45902</v>
+        <v>46055</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>46069</v>
@@ -2271,42 +2275,42 @@
         <v>46068</v>
       </c>
       <c r="G24" t="n">
-        <v>280248.59</v>
+        <v>418857.39</v>
       </c>
       <c r="H24" t="n">
-        <v>118204.01</v>
+        <v>405534.37</v>
       </c>
       <c r="I24" t="n">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="J24" t="n">
         <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>280248.59</v>
+        <v>418857.39</v>
       </c>
       <c r="L24" t="n">
-        <v>42.18</v>
+        <v>96.81999999999999</v>
       </c>
       <c r="M24" t="n">
-        <v>162044.58</v>
+        <v>13323.02</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P24" s="2" t="n">
-        <v>45832</v>
+        <v>46018</v>
       </c>
       <c r="Q24" s="2" t="n">
-        <v>45902</v>
+        <v>46055</v>
       </c>
       <c r="R24" t="n">
-        <v>280248.59</v>
+        <v>418857.39</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2326,19 +2330,19 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CAMP_024</t>
+          <t>CAMP_031</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>45866</v>
+        <v>46018</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>45943</v>
+        <v>46057</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>46069</v>
@@ -2347,46 +2351,46 @@
         <v>46068</v>
       </c>
       <c r="G25" t="n">
-        <v>285863.23</v>
+        <v>574740.27</v>
       </c>
       <c r="H25" t="n">
-        <v>156018.39</v>
+        <v>555850.78</v>
       </c>
       <c r="I25" t="n">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>285863.23</v>
+        <v>574740.27</v>
       </c>
       <c r="L25" t="n">
-        <v>54.58</v>
+        <v>96.70999999999999</v>
       </c>
       <c r="M25" t="n">
-        <v>129844.84</v>
+        <v>18889.49</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P25" s="2" t="n">
-        <v>45866</v>
+        <v>46018</v>
       </c>
       <c r="Q25" s="2" t="n">
-        <v>45943</v>
+        <v>46057</v>
       </c>
       <c r="R25" t="n">
-        <v>285863.23</v>
+        <v>574740.27</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
@@ -2402,19 +2406,19 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CAMP_025</t>
+          <t>CAMP_032</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>TTD</t>
+          <t>Yahoo</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45718</v>
+        <v>46016</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>45808</v>
+        <v>46054</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>46069</v>
@@ -2423,25 +2427,25 @@
         <v>46068</v>
       </c>
       <c r="G26" t="n">
-        <v>221171.06</v>
+        <v>129356.97</v>
       </c>
       <c r="H26" t="n">
-        <v>94524.77</v>
+        <v>110654.88</v>
       </c>
       <c r="I26" t="n">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="J26" t="n">
         <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>221171.06</v>
+        <v>129356.97</v>
       </c>
       <c r="L26" t="n">
-        <v>42.74</v>
+        <v>85.54000000000001</v>
       </c>
       <c r="M26" t="n">
-        <v>126646.29</v>
+        <v>18702.09</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
@@ -2452,17 +2456,17 @@
         </is>
       </c>
       <c r="P26" s="2" t="n">
-        <v>45718</v>
+        <v>46016</v>
       </c>
       <c r="Q26" s="2" t="n">
-        <v>45808</v>
+        <v>46054</v>
       </c>
       <c r="R26" t="n">
-        <v>221171.06</v>
+        <v>129356.97</v>
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>TTD</t>
+          <t>Yahoo</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
@@ -2478,7 +2482,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CAMP_026</t>
+          <t>CAMP_033</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2487,10 +2491,10 @@
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>46010</v>
+        <v>46064</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>46092</v>
+        <v>46083</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>46069</v>
@@ -2499,28 +2503,28 @@
         <v>46068</v>
       </c>
       <c r="G27" t="n">
-        <v>577808.88</v>
+        <v>591950.49</v>
       </c>
       <c r="H27" t="n">
-        <v>85872.27</v>
+        <v>113778.18</v>
       </c>
       <c r="I27" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="J27" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K27" t="n">
-        <v>410731.61</v>
+        <v>147987.62</v>
       </c>
       <c r="L27" t="n">
-        <v>20.91</v>
+        <v>76.88</v>
       </c>
       <c r="M27" t="n">
-        <v>491936.61</v>
+        <v>478172.31</v>
       </c>
       <c r="N27" t="n">
-        <v>20497.36</v>
+        <v>31878.15</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2528,13 +2532,13 @@
         </is>
       </c>
       <c r="P27" s="2" t="n">
-        <v>46010</v>
+        <v>46064</v>
       </c>
       <c r="Q27" s="2" t="n">
-        <v>46092</v>
+        <v>46083</v>
       </c>
       <c r="R27" t="n">
-        <v>577808.88</v>
+        <v>591950.49</v>
       </c>
       <c r="S27" t="inlineStr">
         <is>
@@ -2558,19 +2562,19 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CAMP_027</t>
+          <t>CAMP_034</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Amazon DSP</t>
+          <t>Yahoo</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45899</v>
+        <v>46061</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>45938</v>
+        <v>46084</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>46069</v>
@@ -2579,28 +2583,28 @@
         <v>46068</v>
       </c>
       <c r="G28" t="n">
-        <v>196777.36</v>
+        <v>390381.81</v>
       </c>
       <c r="H28" t="n">
-        <v>47231.34</v>
+        <v>101311.1</v>
       </c>
       <c r="I28" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="J28" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K28" t="n">
-        <v>196777.36</v>
+        <v>130127.27</v>
       </c>
       <c r="L28" t="n">
-        <v>24</v>
+        <v>77.86</v>
       </c>
       <c r="M28" t="n">
-        <v>149546.02</v>
+        <v>289070.71</v>
       </c>
       <c r="N28" t="n">
-        <v>0</v>
+        <v>18066.92</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2608,20 +2612,24 @@
         </is>
       </c>
       <c r="P28" s="2" t="n">
-        <v>45899</v>
+        <v>46061</v>
       </c>
       <c r="Q28" s="2" t="n">
-        <v>45938</v>
+        <v>46084</v>
       </c>
       <c r="R28" t="n">
-        <v>196777.36</v>
+        <v>390381.81</v>
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
-      <c r="T28" t="inlineStr"/>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>Underdelivered</t>
+        </is>
+      </c>
       <c r="U28" t="n">
         <v>0</v>
       </c>
@@ -2634,19 +2642,19 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CAMP_028</t>
+          <t>CAMP_035</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Amazon DSP</t>
+          <t>DV360</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45685</v>
+        <v>46054</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>45780</v>
+        <v>46080</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>46069</v>
@@ -2655,49 +2663,53 @@
         <v>46068</v>
       </c>
       <c r="G29" t="n">
-        <v>170730.01</v>
+        <v>128268.79</v>
       </c>
       <c r="H29" t="n">
-        <v>124157.16</v>
+        <v>69540.46000000001</v>
       </c>
       <c r="I29" t="n">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K29" t="n">
-        <v>170730.01</v>
+        <v>71260.44</v>
       </c>
       <c r="L29" t="n">
-        <v>72.72</v>
+        <v>97.59</v>
       </c>
       <c r="M29" t="n">
-        <v>46572.85</v>
+        <v>58728.33</v>
       </c>
       <c r="N29" t="n">
-        <v>0</v>
+        <v>4894.03</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P29" s="2" t="n">
-        <v>45685</v>
+        <v>46054</v>
       </c>
       <c r="Q29" s="2" t="n">
-        <v>45780</v>
+        <v>46080</v>
       </c>
       <c r="R29" t="n">
-        <v>170730.01</v>
+        <v>128268.79</v>
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
-      <c r="T29" t="inlineStr"/>
+          <t>DV360</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
       <c r="U29" t="n">
         <v>0</v>
       </c>
@@ -2710,7 +2722,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CAMP_029</t>
+          <t>CAMP_036</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2719,10 +2731,10 @@
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>45881</v>
+        <v>46056</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>45954</v>
+        <v>46097</v>
       </c>
       <c r="E30" s="2" t="n">
         <v>46069</v>
@@ -2731,49 +2743,53 @@
         <v>46068</v>
       </c>
       <c r="G30" t="n">
-        <v>355660.26</v>
+        <v>534024.5</v>
       </c>
       <c r="H30" t="n">
-        <v>83693.11</v>
+        <v>160793.8</v>
       </c>
       <c r="I30" t="n">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="K30" t="n">
-        <v>355660.26</v>
+        <v>165293.3</v>
       </c>
       <c r="L30" t="n">
-        <v>23.53</v>
+        <v>97.28</v>
       </c>
       <c r="M30" t="n">
-        <v>271967.15</v>
+        <v>373230.7</v>
       </c>
       <c r="N30" t="n">
-        <v>0</v>
+        <v>12870.02</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P30" s="2" t="n">
-        <v>45881</v>
+        <v>46056</v>
       </c>
       <c r="Q30" s="2" t="n">
-        <v>45954</v>
+        <v>46097</v>
       </c>
       <c r="R30" t="n">
-        <v>355660.26</v>
+        <v>534024.5</v>
       </c>
       <c r="S30" t="inlineStr">
         <is>
           <t>TTD</t>
         </is>
       </c>
-      <c r="T30" t="inlineStr"/>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
       <c r="U30" t="n">
         <v>0</v>
       </c>
@@ -2786,19 +2802,19 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CAMP_030</t>
+          <t>CAMP_037</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>TTD</t>
+          <t>Yahoo</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>45666</v>
+        <v>46024</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>45765</v>
+        <v>46064</v>
       </c>
       <c r="E31" s="2" t="n">
         <v>46069</v>
@@ -2807,46 +2823,46 @@
         <v>46068</v>
       </c>
       <c r="G31" t="n">
-        <v>418857.39</v>
+        <v>391196.57</v>
       </c>
       <c r="H31" t="n">
-        <v>180010.86</v>
+        <v>379184.45</v>
       </c>
       <c r="I31" t="n">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="J31" t="n">
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>418857.39</v>
+        <v>391196.57</v>
       </c>
       <c r="L31" t="n">
-        <v>42.98</v>
+        <v>96.93000000000001</v>
       </c>
       <c r="M31" t="n">
-        <v>238846.53</v>
+        <v>12012.12</v>
       </c>
       <c r="N31" t="n">
         <v>0</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P31" s="2" t="n">
-        <v>45666</v>
+        <v>46024</v>
       </c>
       <c r="Q31" s="2" t="n">
-        <v>45765</v>
+        <v>46064</v>
       </c>
       <c r="R31" t="n">
-        <v>418857.39</v>
+        <v>391196.57</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>TTD</t>
+          <t>Yahoo</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
@@ -2862,19 +2878,19 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CAMP_031</t>
+          <t>CAMP_038</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>Yahoo</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>45998</v>
+        <v>46050</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>46117</v>
+        <v>46087</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>46069</v>
@@ -2883,51 +2899,51 @@
         <v>46068</v>
       </c>
       <c r="G32" t="n">
-        <v>574740.27</v>
+        <v>596378.9300000001</v>
       </c>
       <c r="H32" t="n">
-        <v>80607.14999999999</v>
+        <v>357739.38</v>
       </c>
       <c r="I32" t="n">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="J32" t="n">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="K32" t="n">
-        <v>340054.66</v>
+        <v>298189.47</v>
       </c>
       <c r="L32" t="n">
-        <v>23.7</v>
+        <v>119.97</v>
       </c>
       <c r="M32" t="n">
-        <v>494133.12</v>
+        <v>238639.55</v>
       </c>
       <c r="N32" t="n">
-        <v>10084.35</v>
+        <v>12559.98</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>Overpacing</t>
         </is>
       </c>
       <c r="P32" s="2" t="n">
-        <v>45998</v>
+        <v>46050</v>
       </c>
       <c r="Q32" s="2" t="n">
-        <v>46117</v>
+        <v>46087</v>
       </c>
       <c r="R32" t="n">
-        <v>574740.27</v>
+        <v>596378.9300000001</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>Yahoo</t>
         </is>
       </c>
       <c r="T32" t="inlineStr">
         <is>
-          <t>Underdelivered</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="U32" t="n">
@@ -2942,7 +2958,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CAMP_032</t>
+          <t>CAMP_039</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2951,10 +2967,10 @@
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>46093</v>
+        <v>46054</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>46069</v>
@@ -2963,55 +2979,51 @@
         <v>46068</v>
       </c>
       <c r="G33" t="n">
-        <v>129356.97</v>
+        <v>120089.45</v>
       </c>
       <c r="H33" t="n">
-        <v>89176.62</v>
+        <v>116246.03</v>
       </c>
       <c r="I33" t="n">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="J33" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="K33" t="n">
-        <v>80358.12</v>
+        <v>120089.45</v>
       </c>
       <c r="L33" t="n">
-        <v>110.97</v>
+        <v>96.8</v>
       </c>
       <c r="M33" t="n">
-        <v>40180.35</v>
+        <v>3843.42</v>
       </c>
       <c r="N33" t="n">
-        <v>1607.21</v>
+        <v>0</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P33" s="2" t="n">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="Q33" s="2" t="n">
-        <v>46093</v>
+        <v>46054</v>
       </c>
       <c r="R33" t="n">
-        <v>129356.97</v>
+        <v>120089.45</v>
       </c>
       <c r="S33" t="inlineStr">
         <is>
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="T33" t="inlineStr">
-        <is>
-          <t>Overdelivered</t>
-        </is>
-      </c>
+      <c r="T33" t="inlineStr"/>
       <c r="U33" t="n">
-        <v>40180.35000000001</v>
+        <v>0</v>
       </c>
       <c r="V33" t="inlineStr">
         <is>
@@ -3022,19 +3034,19 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CAMP_033</t>
+          <t>CAMP_041</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>Amazon DSP</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>45903</v>
+        <v>46054</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>45931</v>
+        <v>46095</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>46069</v>
@@ -3043,28 +3055,28 @@
         <v>46068</v>
       </c>
       <c r="G34" t="n">
-        <v>591950.49</v>
+        <v>574267.4300000001</v>
       </c>
       <c r="H34" t="n">
-        <v>23560.62</v>
+        <v>146242.53</v>
       </c>
       <c r="I34" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="K34" t="n">
-        <v>591950.49</v>
+        <v>205095.51</v>
       </c>
       <c r="L34" t="n">
-        <v>3.98</v>
+        <v>71.3</v>
       </c>
       <c r="M34" t="n">
-        <v>568389.87</v>
+        <v>428024.9</v>
       </c>
       <c r="N34" t="n">
-        <v>0</v>
+        <v>15852.77</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3072,20 +3084,24 @@
         </is>
       </c>
       <c r="P34" s="2" t="n">
-        <v>45903</v>
+        <v>46054</v>
       </c>
       <c r="Q34" s="2" t="n">
-        <v>45931</v>
+        <v>46095</v>
       </c>
       <c r="R34" t="n">
-        <v>591950.49</v>
+        <v>574267.4300000001</v>
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
-      <c r="T34" t="inlineStr"/>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>Underdelivered</t>
+        </is>
+      </c>
       <c r="U34" t="n">
         <v>0</v>
       </c>
@@ -3098,19 +3114,19 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CAMP_034</t>
+          <t>CAMP_042</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>45909</v>
+        <v>46023</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>45972</v>
+        <v>46063</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>46069</v>
@@ -3119,46 +3135,46 @@
         <v>46068</v>
       </c>
       <c r="G35" t="n">
-        <v>390381.81</v>
+        <v>352257.46</v>
       </c>
       <c r="H35" t="n">
-        <v>84289.87</v>
+        <v>340306.3</v>
       </c>
       <c r="I35" t="n">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="J35" t="n">
         <v>0</v>
       </c>
       <c r="K35" t="n">
-        <v>390381.81</v>
+        <v>352257.46</v>
       </c>
       <c r="L35" t="n">
-        <v>21.59</v>
+        <v>96.61</v>
       </c>
       <c r="M35" t="n">
-        <v>306091.94</v>
+        <v>11951.16</v>
       </c>
       <c r="N35" t="n">
         <v>0</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Underpacing</t>
+          <t>On Track</t>
         </is>
       </c>
       <c r="P35" s="2" t="n">
-        <v>45909</v>
+        <v>46023</v>
       </c>
       <c r="Q35" s="2" t="n">
-        <v>45972</v>
+        <v>46063</v>
       </c>
       <c r="R35" t="n">
-        <v>390381.81</v>
+        <v>352257.46</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Yahoo</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
@@ -3174,19 +3190,19 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CAMP_035</t>
+          <t>CAMP_044</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>DV360</t>
+          <t>Amazon DSP</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45863</v>
+        <v>46050</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>45951</v>
+        <v>46090</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>46069</v>
@@ -3195,829 +3211,57 @@
         <v>46068</v>
       </c>
       <c r="G36" t="n">
-        <v>128268.79</v>
+        <v>354611.01</v>
       </c>
       <c r="H36" t="n">
-        <v>188100.04</v>
+        <v>116037.92</v>
       </c>
       <c r="I36" t="n">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K36" t="n">
-        <v>128268.79</v>
+        <v>164331.93</v>
       </c>
       <c r="L36" t="n">
-        <v>146.65</v>
+        <v>70.61</v>
       </c>
       <c r="M36" t="n">
-        <v>-59831.25</v>
+        <v>238573.09</v>
       </c>
       <c r="N36" t="n">
-        <v>0</v>
+        <v>10844.23</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Overpacing</t>
+          <t>Underpacing</t>
         </is>
       </c>
       <c r="P36" s="2" t="n">
-        <v>45863</v>
+        <v>46050</v>
       </c>
       <c r="Q36" s="2" t="n">
-        <v>45951</v>
+        <v>46090</v>
       </c>
       <c r="R36" t="n">
-        <v>128268.79</v>
+        <v>354611.01</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>DV360</t>
-        </is>
-      </c>
-      <c r="T36" t="inlineStr"/>
+          <t>Amazon DSP</t>
+        </is>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>Underdelivered</t>
+        </is>
+      </c>
       <c r="U36" t="n">
         <v>0</v>
       </c>
       <c r="V36" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>CAMP_036</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
-      <c r="C37" s="2" t="n">
-        <v>46066</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <v>46095</v>
-      </c>
-      <c r="E37" s="2" t="n">
-        <v>46069</v>
-      </c>
-      <c r="F37" s="2" t="n">
-        <v>46068</v>
-      </c>
-      <c r="G37" t="n">
-        <v>534024.5</v>
-      </c>
-      <c r="H37" t="n">
-        <v>3192.36</v>
-      </c>
-      <c r="I37" t="n">
-        <v>3</v>
-      </c>
-      <c r="J37" t="n">
-        <v>27</v>
-      </c>
-      <c r="K37" t="n">
-        <v>53402.45</v>
-      </c>
-      <c r="L37" t="n">
-        <v>5.98</v>
-      </c>
-      <c r="M37" t="n">
-        <v>530832.14</v>
-      </c>
-      <c r="N37" t="n">
-        <v>19660.45</v>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P37" s="2" t="n">
-        <v>46066</v>
-      </c>
-      <c r="Q37" s="2" t="n">
-        <v>46095</v>
-      </c>
-      <c r="R37" t="n">
-        <v>534024.5</v>
-      </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
-      <c r="T37" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
-      </c>
-      <c r="U37" t="n">
-        <v>0</v>
-      </c>
-      <c r="V37" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>CAMP_037</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
-      <c r="C38" s="2" t="n">
-        <v>45835</v>
-      </c>
-      <c r="D38" s="2" t="n">
-        <v>45899</v>
-      </c>
-      <c r="E38" s="2" t="n">
-        <v>46069</v>
-      </c>
-      <c r="F38" s="2" t="n">
-        <v>46068</v>
-      </c>
-      <c r="G38" t="n">
-        <v>391196.57</v>
-      </c>
-      <c r="H38" t="n">
-        <v>71566.28999999999</v>
-      </c>
-      <c r="I38" t="n">
-        <v>65</v>
-      </c>
-      <c r="J38" t="n">
-        <v>0</v>
-      </c>
-      <c r="K38" t="n">
-        <v>391196.57</v>
-      </c>
-      <c r="L38" t="n">
-        <v>18.29</v>
-      </c>
-      <c r="M38" t="n">
-        <v>319630.28</v>
-      </c>
-      <c r="N38" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P38" s="2" t="n">
-        <v>45835</v>
-      </c>
-      <c r="Q38" s="2" t="n">
-        <v>45899</v>
-      </c>
-      <c r="R38" t="n">
-        <v>391196.57</v>
-      </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
-      <c r="T38" t="inlineStr"/>
-      <c r="U38" t="n">
-        <v>0</v>
-      </c>
-      <c r="V38" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>CAMP_038</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
-      <c r="C39" s="2" t="n">
-        <v>45887</v>
-      </c>
-      <c r="D39" s="2" t="n">
-        <v>45969</v>
-      </c>
-      <c r="E39" s="2" t="n">
-        <v>46069</v>
-      </c>
-      <c r="F39" s="2" t="n">
-        <v>46068</v>
-      </c>
-      <c r="G39" t="n">
-        <v>596378.9300000001</v>
-      </c>
-      <c r="H39" t="n">
-        <v>81468.39</v>
-      </c>
-      <c r="I39" t="n">
-        <v>83</v>
-      </c>
-      <c r="J39" t="n">
-        <v>0</v>
-      </c>
-      <c r="K39" t="n">
-        <v>596378.9300000001</v>
-      </c>
-      <c r="L39" t="n">
-        <v>13.66</v>
-      </c>
-      <c r="M39" t="n">
-        <v>514910.54</v>
-      </c>
-      <c r="N39" t="n">
-        <v>0</v>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P39" s="2" t="n">
-        <v>45887</v>
-      </c>
-      <c r="Q39" s="2" t="n">
-        <v>45969</v>
-      </c>
-      <c r="R39" t="n">
-        <v>596378.9300000001</v>
-      </c>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
-      <c r="T39" t="inlineStr"/>
-      <c r="U39" t="n">
-        <v>0</v>
-      </c>
-      <c r="V39" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>CAMP_039</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
-      <c r="C40" s="2" t="n">
-        <v>46023</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <v>46087</v>
-      </c>
-      <c r="E40" s="2" t="n">
-        <v>46069</v>
-      </c>
-      <c r="F40" s="2" t="n">
-        <v>46068</v>
-      </c>
-      <c r="G40" t="n">
-        <v>120089.45</v>
-      </c>
-      <c r="H40" t="n">
-        <v>65098.05</v>
-      </c>
-      <c r="I40" t="n">
-        <v>46</v>
-      </c>
-      <c r="J40" t="n">
-        <v>19</v>
-      </c>
-      <c r="K40" t="n">
-        <v>84986.38</v>
-      </c>
-      <c r="L40" t="n">
-        <v>76.59999999999999</v>
-      </c>
-      <c r="M40" t="n">
-        <v>54991.4</v>
-      </c>
-      <c r="N40" t="n">
-        <v>2894.28</v>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P40" s="2" t="n">
-        <v>46023</v>
-      </c>
-      <c r="Q40" s="2" t="n">
-        <v>46087</v>
-      </c>
-      <c r="R40" t="n">
-        <v>120089.45</v>
-      </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
-      <c r="T40" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
-      </c>
-      <c r="U40" t="n">
-        <v>0</v>
-      </c>
-      <c r="V40" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>CAMP_040</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>DV360</t>
-        </is>
-      </c>
-      <c r="C41" s="2" t="n">
-        <v>46106</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>46159</v>
-      </c>
-      <c r="E41" s="2" t="n">
-        <v>46069</v>
-      </c>
-      <c r="F41" s="2" t="n">
-        <v>46068</v>
-      </c>
-      <c r="G41" t="n">
-        <v>326276.52</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" t="n">
-        <v>54</v>
-      </c>
-      <c r="K41" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" t="n">
-        <v>326276.52</v>
-      </c>
-      <c r="N41" t="n">
-        <v>6042.16</v>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="P41" s="2" t="n">
-        <v>46106</v>
-      </c>
-      <c r="Q41" s="2" t="n">
-        <v>46159</v>
-      </c>
-      <c r="R41" t="n">
-        <v>326276.52</v>
-      </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>DV360</t>
-        </is>
-      </c>
-      <c r="T41" t="inlineStr"/>
-      <c r="U41" t="n">
-        <v>0</v>
-      </c>
-      <c r="V41" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>CAMP_041</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
-      <c r="C42" s="2" t="n">
-        <v>46065</v>
-      </c>
-      <c r="D42" s="2" t="n">
-        <v>46111</v>
-      </c>
-      <c r="E42" s="2" t="n">
-        <v>46069</v>
-      </c>
-      <c r="F42" s="2" t="n">
-        <v>46068</v>
-      </c>
-      <c r="G42" t="n">
-        <v>574267.4300000001</v>
-      </c>
-      <c r="H42" t="n">
-        <v>4714.41</v>
-      </c>
-      <c r="I42" t="n">
-        <v>4</v>
-      </c>
-      <c r="J42" t="n">
-        <v>43</v>
-      </c>
-      <c r="K42" t="n">
-        <v>48873.82</v>
-      </c>
-      <c r="L42" t="n">
-        <v>9.65</v>
-      </c>
-      <c r="M42" t="n">
-        <v>569553.02</v>
-      </c>
-      <c r="N42" t="n">
-        <v>13245.42</v>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P42" s="2" t="n">
-        <v>46065</v>
-      </c>
-      <c r="Q42" s="2" t="n">
-        <v>46111</v>
-      </c>
-      <c r="R42" t="n">
-        <v>574267.4300000001</v>
-      </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
-      <c r="T42" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
-      </c>
-      <c r="U42" t="n">
-        <v>0</v>
-      </c>
-      <c r="V42" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>CAMP_042</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
-      <c r="C43" s="2" t="n">
-        <v>45898</v>
-      </c>
-      <c r="D43" s="2" t="n">
-        <v>46015</v>
-      </c>
-      <c r="E43" s="2" t="n">
-        <v>46069</v>
-      </c>
-      <c r="F43" s="2" t="n">
-        <v>46068</v>
-      </c>
-      <c r="G43" t="n">
-        <v>352257.46</v>
-      </c>
-      <c r="H43" t="n">
-        <v>243342.65</v>
-      </c>
-      <c r="I43" t="n">
-        <v>118</v>
-      </c>
-      <c r="J43" t="n">
-        <v>0</v>
-      </c>
-      <c r="K43" t="n">
-        <v>352257.46</v>
-      </c>
-      <c r="L43" t="n">
-        <v>69.08</v>
-      </c>
-      <c r="M43" t="n">
-        <v>108914.81</v>
-      </c>
-      <c r="N43" t="n">
-        <v>0</v>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P43" s="2" t="n">
-        <v>45898</v>
-      </c>
-      <c r="Q43" s="2" t="n">
-        <v>46015</v>
-      </c>
-      <c r="R43" t="n">
-        <v>352257.46</v>
-      </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
-      <c r="T43" t="inlineStr"/>
-      <c r="U43" t="n">
-        <v>0</v>
-      </c>
-      <c r="V43" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>CAMP_043</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>DV360</t>
-        </is>
-      </c>
-      <c r="C44" s="2" t="n">
-        <v>46096</v>
-      </c>
-      <c r="D44" s="2" t="n">
-        <v>46182</v>
-      </c>
-      <c r="E44" s="2" t="n">
-        <v>46069</v>
-      </c>
-      <c r="F44" s="2" t="n">
-        <v>46068</v>
-      </c>
-      <c r="G44" t="n">
-        <v>267517.39</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" t="n">
-        <v>87</v>
-      </c>
-      <c r="K44" t="n">
-        <v>0</v>
-      </c>
-      <c r="L44" t="n">
-        <v>0</v>
-      </c>
-      <c r="M44" t="n">
-        <v>267517.39</v>
-      </c>
-      <c r="N44" t="n">
-        <v>3074.91</v>
-      </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="P44" s="2" t="n">
-        <v>46096</v>
-      </c>
-      <c r="Q44" s="2" t="n">
-        <v>46182</v>
-      </c>
-      <c r="R44" t="n">
-        <v>267517.39</v>
-      </c>
-      <c r="S44" t="inlineStr">
-        <is>
-          <t>DV360</t>
-        </is>
-      </c>
-      <c r="T44" t="inlineStr"/>
-      <c r="U44" t="n">
-        <v>0</v>
-      </c>
-      <c r="V44" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>CAMP_044</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
-      <c r="C45" s="2" t="n">
-        <v>46004</v>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>46082</v>
-      </c>
-      <c r="E45" s="2" t="n">
-        <v>46069</v>
-      </c>
-      <c r="F45" s="2" t="n">
-        <v>46068</v>
-      </c>
-      <c r="G45" t="n">
-        <v>354611.01</v>
-      </c>
-      <c r="H45" t="n">
-        <v>128081.01</v>
-      </c>
-      <c r="I45" t="n">
-        <v>65</v>
-      </c>
-      <c r="J45" t="n">
-        <v>14</v>
-      </c>
-      <c r="K45" t="n">
-        <v>291768.55</v>
-      </c>
-      <c r="L45" t="n">
-        <v>43.9</v>
-      </c>
-      <c r="M45" t="n">
-        <v>226530</v>
-      </c>
-      <c r="N45" t="n">
-        <v>16180.71</v>
-      </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>Underpacing</t>
-        </is>
-      </c>
-      <c r="P45" s="2" t="n">
-        <v>46004</v>
-      </c>
-      <c r="Q45" s="2" t="n">
-        <v>46082</v>
-      </c>
-      <c r="R45" t="n">
-        <v>354611.01</v>
-      </c>
-      <c r="S45" t="inlineStr">
-        <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
-      <c r="T45" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
-      </c>
-      <c r="U45" t="n">
-        <v>0</v>
-      </c>
-      <c r="V45" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>CAMP_045</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
-      <c r="C46" s="2" t="n">
-        <v>46091</v>
-      </c>
-      <c r="D46" s="2" t="n">
-        <v>46135</v>
-      </c>
-      <c r="E46" s="2" t="n">
-        <v>46069</v>
-      </c>
-      <c r="F46" s="2" t="n">
-        <v>46068</v>
-      </c>
-      <c r="G46" t="n">
-        <v>498191.26</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" t="n">
-        <v>0</v>
-      </c>
-      <c r="J46" t="n">
-        <v>45</v>
-      </c>
-      <c r="K46" t="n">
-        <v>0</v>
-      </c>
-      <c r="L46" t="n">
-        <v>0</v>
-      </c>
-      <c r="M46" t="n">
-        <v>498191.26</v>
-      </c>
-      <c r="N46" t="n">
-        <v>11070.92</v>
-      </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="P46" s="2" t="n">
-        <v>46091</v>
-      </c>
-      <c r="Q46" s="2" t="n">
-        <v>46135</v>
-      </c>
-      <c r="R46" t="n">
-        <v>498191.26</v>
-      </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
-      <c r="T46" t="inlineStr"/>
-      <c r="U46" t="n">
-        <v>0</v>
-      </c>
-      <c r="V46" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -4057,21 +3301,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Total_Budget</t>
+          <t>Pace_Ratio</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.30403800197451</v>
+        <v>0.4100336047361106</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Pace_Ratio</t>
+          <t>Spend_to_Date</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2978052316094644</v>
+        <v>0.138517092081769</v>
       </c>
     </row>
     <row r="4">
@@ -4081,27 +3325,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1651920240253574</v>
+        <v>0.1359775077325613</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Spend_to_Date</t>
+          <t>DSP_enc</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1346997111256371</v>
+        <v>0.09527462607891371</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Days_Elapsed</t>
+          <t>Total_Budget</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.04185972267982849</v>
+        <v>0.09011695109864845</v>
       </c>
     </row>
     <row r="7">
@@ -4111,17 +3355,17 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0394229317615561</v>
+        <v>0.07122699442576116</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DSP_enc</t>
+          <t>Days_Elapsed</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.01698237682364667</v>
+        <v>0.05885322384623567</v>
       </c>
     </row>
   </sheetData>
@@ -4162,7 +3406,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.833</v>
       </c>
     </row>
     <row r="3">
@@ -4172,7 +3416,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>40180.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -4183,7 +3427,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2026-02-16 06:09 UTC</t>
+          <t>2026-02-16 06:53 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto refresh - 16-02-2026 13:02:31.38
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V36"/>
+  <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,17 +537,27 @@
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>ML_Prediction</t>
+          <t>Predicted_Final_Deviation_%</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Budget_At_Risk</t>
+          <t>Risk_Score</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>ML_Early_Warning</t>
+          <t>Predicted_Impact_Amount</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Risk_Level</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Early_Warning</t>
         </is>
       </c>
     </row>
@@ -618,10 +628,14 @@
         </is>
       </c>
       <c r="T2" t="inlineStr"/>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="inlineStr">
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -694,10 +708,14 @@
         </is>
       </c>
       <c r="T3" t="inlineStr"/>
-      <c r="U3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" t="inlineStr">
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -770,10 +788,14 @@
         </is>
       </c>
       <c r="T4" t="inlineStr"/>
-      <c r="U4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" t="inlineStr">
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -845,15 +867,21 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
+      <c r="T5" t="n">
+        <v>-18.71</v>
       </c>
       <c r="U5" t="n">
-        <v>0</v>
-      </c>
-      <c r="V5" t="inlineStr">
+        <v>93.55</v>
+      </c>
+      <c r="V5" t="n">
+        <v>-95252.11792700001</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>CRITICAL – Immediate Action</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -926,10 +954,14 @@
         </is>
       </c>
       <c r="T6" t="inlineStr"/>
-      <c r="U6" t="n">
-        <v>0</v>
-      </c>
-      <c r="V6" t="inlineStr">
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1002,10 +1034,14 @@
         </is>
       </c>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="n">
-        <v>0</v>
-      </c>
-      <c r="V7" t="inlineStr">
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1078,10 +1114,14 @@
         </is>
       </c>
       <c r="T8" t="inlineStr"/>
-      <c r="U8" t="n">
-        <v>0</v>
-      </c>
-      <c r="V8" t="inlineStr">
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1154,10 +1194,14 @@
         </is>
       </c>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="n">
-        <v>0</v>
-      </c>
-      <c r="V9" t="inlineStr">
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1230,10 +1274,14 @@
         </is>
       </c>
       <c r="T10" t="inlineStr"/>
-      <c r="U10" t="n">
-        <v>0</v>
-      </c>
-      <c r="V10" t="inlineStr">
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1306,10 +1354,14 @@
         </is>
       </c>
       <c r="T11" t="inlineStr"/>
-      <c r="U11" t="n">
-        <v>0</v>
-      </c>
-      <c r="V11" t="inlineStr">
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1382,10 +1434,14 @@
         </is>
       </c>
       <c r="T12" t="inlineStr"/>
-      <c r="U12" t="n">
-        <v>0</v>
-      </c>
-      <c r="V12" t="inlineStr">
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1457,15 +1513,21 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
+      <c r="T13" t="n">
+        <v>-1.51</v>
       </c>
       <c r="U13" t="n">
-        <v>0</v>
-      </c>
-      <c r="V13" t="inlineStr">
+        <v>7.55</v>
+      </c>
+      <c r="V13" t="n">
+        <v>-2440.23701</v>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1538,10 +1600,14 @@
         </is>
       </c>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="n">
-        <v>0</v>
-      </c>
-      <c r="V14" t="inlineStr">
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1613,15 +1679,21 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
+      <c r="T15" t="n">
+        <v>9.02</v>
       </c>
       <c r="U15" t="n">
-        <v>0</v>
-      </c>
-      <c r="V15" t="inlineStr">
+        <v>45.09999999999999</v>
+      </c>
+      <c r="V15" t="n">
+        <v>38215.927882</v>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>MODERATE – Monitor Closely</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1693,15 +1765,21 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
+      <c r="T16" t="n">
+        <v>-22.13</v>
       </c>
       <c r="U16" t="n">
-        <v>0</v>
-      </c>
-      <c r="V16" t="inlineStr">
+        <v>100</v>
+      </c>
+      <c r="V16" t="n">
+        <v>-23446.971791</v>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>CRITICAL – Immediate Action</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1774,10 +1852,14 @@
         </is>
       </c>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="n">
-        <v>0</v>
-      </c>
-      <c r="V17" t="inlineStr">
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1849,15 +1931,21 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
+      <c r="T18" t="n">
+        <v>-18.92</v>
       </c>
       <c r="U18" t="n">
-        <v>0</v>
-      </c>
-      <c r="V18" t="inlineStr">
+        <v>94.60000000000001</v>
+      </c>
+      <c r="V18" t="n">
+        <v>-54085.323116</v>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>CRITICAL – Immediate Action</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1930,10 +2018,14 @@
         </is>
       </c>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="n">
-        <v>0</v>
-      </c>
-      <c r="V19" t="inlineStr">
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2006,10 +2098,14 @@
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="n">
-        <v>0</v>
-      </c>
-      <c r="V20" t="inlineStr">
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2081,15 +2177,21 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
+      <c r="T21" t="n">
+        <v>-0.19</v>
       </c>
       <c r="U21" t="n">
-        <v>0</v>
-      </c>
-      <c r="V21" t="inlineStr">
+        <v>0.95</v>
+      </c>
+      <c r="V21" t="n">
+        <v>-373.876984</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2162,10 +2264,14 @@
         </is>
       </c>
       <c r="T22" t="inlineStr"/>
-      <c r="U22" t="n">
-        <v>0</v>
-      </c>
-      <c r="V22" t="inlineStr">
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X22" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2237,15 +2343,21 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="T23" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
+      <c r="T23" t="n">
+        <v>9.6</v>
       </c>
       <c r="U23" t="n">
-        <v>0</v>
-      </c>
-      <c r="V23" t="inlineStr">
+        <v>48</v>
+      </c>
+      <c r="V23" t="n">
+        <v>34143.38496</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>MODERATE – Monitor Closely</t>
+        </is>
+      </c>
+      <c r="X23" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2318,10 +2430,14 @@
         </is>
       </c>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="n">
-        <v>0</v>
-      </c>
-      <c r="V24" t="inlineStr">
+      <c r="U24" t="inlineStr"/>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X24" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2394,10 +2510,14 @@
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
-      <c r="U25" t="n">
-        <v>0</v>
-      </c>
-      <c r="V25" t="inlineStr">
+      <c r="U25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X25" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2470,10 +2590,14 @@
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
-      <c r="U26" t="n">
-        <v>0</v>
-      </c>
-      <c r="V26" t="inlineStr">
+      <c r="U26" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X26" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2545,15 +2669,21 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="T27" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
+      <c r="T27" t="n">
+        <v>-18.44</v>
       </c>
       <c r="U27" t="n">
-        <v>0</v>
-      </c>
-      <c r="V27" t="inlineStr">
+        <v>92.2</v>
+      </c>
+      <c r="V27" t="n">
+        <v>-109155.670356</v>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>CRITICAL – Immediate Action</t>
+        </is>
+      </c>
+      <c r="X27" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2625,15 +2755,21 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="T28" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
+      <c r="T28" t="n">
+        <v>-18.95</v>
       </c>
       <c r="U28" t="n">
-        <v>0</v>
-      </c>
-      <c r="V28" t="inlineStr">
+        <v>94.75</v>
+      </c>
+      <c r="V28" t="n">
+        <v>-73977.35299499999</v>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>CRITICAL – Immediate Action</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2705,15 +2841,21 @@
           <t>DV360</t>
         </is>
       </c>
-      <c r="T29" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
+      <c r="T29" t="n">
+        <v>-1.6</v>
       </c>
       <c r="U29" t="n">
-        <v>0</v>
-      </c>
-      <c r="V29" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="V29" t="n">
+        <v>-2052.30064</v>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X29" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2785,15 +2927,21 @@
           <t>TTD</t>
         </is>
       </c>
-      <c r="T30" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
+      <c r="T30" t="n">
+        <v>-2.91</v>
       </c>
       <c r="U30" t="n">
-        <v>0</v>
-      </c>
-      <c r="V30" t="inlineStr">
+        <v>14.55</v>
+      </c>
+      <c r="V30" t="n">
+        <v>-15540.11295</v>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X30" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2866,10 +3014,14 @@
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
-      <c r="U31" t="n">
-        <v>0</v>
-      </c>
-      <c r="V31" t="inlineStr">
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X31" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -2941,15 +3093,21 @@
           <t>Yahoo</t>
         </is>
       </c>
-      <c r="T32" t="inlineStr">
-        <is>
-          <t>On Track</t>
-        </is>
+      <c r="T32" t="n">
+        <v>9.08</v>
       </c>
       <c r="U32" t="n">
-        <v>0</v>
-      </c>
-      <c r="V32" t="inlineStr">
+        <v>45.4</v>
+      </c>
+      <c r="V32" t="n">
+        <v>54151.20684400001</v>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>MODERATE – Monitor Closely</t>
+        </is>
+      </c>
+      <c r="X32" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -3022,10 +3180,14 @@
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="n">
-        <v>0</v>
-      </c>
-      <c r="V33" t="inlineStr">
+      <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X33" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -3097,15 +3259,21 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="T34" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
+      <c r="T34" t="n">
+        <v>-16.29</v>
       </c>
       <c r="U34" t="n">
-        <v>0</v>
-      </c>
-      <c r="V34" t="inlineStr">
+        <v>81.45</v>
+      </c>
+      <c r="V34" t="n">
+        <v>-93548.164347</v>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>CRITICAL – Immediate Action</t>
+        </is>
+      </c>
+      <c r="X34" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -3178,10 +3346,14 @@
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="n">
-        <v>0</v>
-      </c>
-      <c r="V35" t="inlineStr">
+      <c r="U35" t="inlineStr"/>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>LOW – Stable</t>
+        </is>
+      </c>
+      <c r="X35" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -3253,15 +3425,21 @@
           <t>Amazon DSP</t>
         </is>
       </c>
-      <c r="T36" t="inlineStr">
-        <is>
-          <t>Underdelivered</t>
-        </is>
+      <c r="T36" t="n">
+        <v>-20.61</v>
       </c>
       <c r="U36" t="n">
-        <v>0</v>
-      </c>
-      <c r="V36" t="inlineStr">
+        <v>100</v>
+      </c>
+      <c r="V36" t="n">
+        <v>-73085.329161</v>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>CRITICAL – Immediate Action</t>
+        </is>
+      </c>
+      <c r="X36" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -3305,17 +3483,17 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4100336047361106</v>
+        <v>0.8767043416575715</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Spend_to_Date</t>
+          <t>DSP_enc</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.138517092081769</v>
+        <v>0.03902579892808492</v>
       </c>
     </row>
     <row r="4">
@@ -3325,17 +3503,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1359775077325613</v>
+        <v>0.03885957600547516</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DSP_enc</t>
+          <t>Spend_to_Date</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.09527462607891371</v>
+        <v>0.02013960227352946</v>
       </c>
     </row>
     <row r="6">
@@ -3345,7 +3523,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.09011695109864845</v>
+        <v>0.0131773290904567</v>
       </c>
     </row>
     <row r="7">
@@ -3355,7 +3533,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.07122699442576116</v>
+        <v>0.006460673297380543</v>
       </c>
     </row>
     <row r="8">
@@ -3365,7 +3543,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.05885322384623567</v>
+        <v>0.005632678747501668</v>
       </c>
     </row>
   </sheetData>
@@ -3402,21 +3580,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ML Validation Accuracy</t>
+          <t>ML Validation MAE</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.833</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Total Budget At Risk</t>
+          <t>Total Predicted Impact</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>-416446.94</v>
       </c>
     </row>
     <row r="4">
@@ -3427,7 +3605,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2026-02-16 06:54 UTC</t>
+          <t>2026-02-16 07:32 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto refresh - 16-02-2026 13:33:53.19
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X36"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,11 +555,6 @@
           <t>Risk_Level</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Early_Warning</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -635,11 +630,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -715,11 +705,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -795,11 +780,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -868,22 +848,17 @@
         </is>
       </c>
       <c r="T5" t="n">
-        <v>-18.71</v>
+        <v>-18.51</v>
       </c>
       <c r="U5" t="n">
-        <v>93.55</v>
+        <v>92.55000000000001</v>
       </c>
       <c r="V5" t="n">
-        <v>-95252.11792700001</v>
+        <v>-94233.92318700001</v>
       </c>
       <c r="W5" t="inlineStr">
         <is>
           <t>CRITICAL – Immediate Action</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>NO</t>
         </is>
       </c>
     </row>
@@ -961,11 +936,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1041,11 +1011,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1121,11 +1086,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1201,11 +1161,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1281,11 +1236,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1361,11 +1311,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1441,11 +1386,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X12" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1514,22 +1454,17 @@
         </is>
       </c>
       <c r="T13" t="n">
-        <v>-1.51</v>
+        <v>-10.37</v>
       </c>
       <c r="U13" t="n">
-        <v>7.55</v>
+        <v>51.84999999999999</v>
       </c>
       <c r="V13" t="n">
-        <v>-2440.23701</v>
+        <v>-16758.44887</v>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>LOW – Stable</t>
-        </is>
-      </c>
-      <c r="X13" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>MODERATE – Monitor Closely</t>
         </is>
       </c>
     </row>
@@ -1607,11 +1542,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1680,22 +1610,17 @@
         </is>
       </c>
       <c r="T15" t="n">
-        <v>9.02</v>
+        <v>-9.32</v>
       </c>
       <c r="U15" t="n">
-        <v>45.09999999999999</v>
+        <v>46.6</v>
       </c>
       <c r="V15" t="n">
-        <v>38215.927882</v>
+        <v>-39486.967612</v>
       </c>
       <c r="W15" t="inlineStr">
         <is>
           <t>MODERATE – Monitor Closely</t>
-        </is>
-      </c>
-      <c r="X15" t="inlineStr">
-        <is>
-          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1766,22 +1691,17 @@
         </is>
       </c>
       <c r="T16" t="n">
-        <v>-22.13</v>
+        <v>-18.78</v>
       </c>
       <c r="U16" t="n">
-        <v>100</v>
+        <v>93.90000000000001</v>
       </c>
       <c r="V16" t="n">
-        <v>-23446.971791</v>
+        <v>-19897.610946</v>
       </c>
       <c r="W16" t="inlineStr">
         <is>
           <t>CRITICAL – Immediate Action</t>
-        </is>
-      </c>
-      <c r="X16" t="inlineStr">
-        <is>
-          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1859,11 +1779,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X17" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1932,22 +1847,17 @@
         </is>
       </c>
       <c r="T18" t="n">
-        <v>-18.92</v>
+        <v>-10.8</v>
       </c>
       <c r="U18" t="n">
-        <v>94.60000000000001</v>
+        <v>54</v>
       </c>
       <c r="V18" t="n">
-        <v>-54085.323116</v>
+        <v>-30873.22884</v>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>CRITICAL – Immediate Action</t>
-        </is>
-      </c>
-      <c r="X18" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>MODERATE – Monitor Closely</t>
         </is>
       </c>
     </row>
@@ -2025,11 +1935,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X19" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2105,11 +2010,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X20" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2178,22 +2078,17 @@
         </is>
       </c>
       <c r="T21" t="n">
-        <v>-0.19</v>
+        <v>4.31</v>
       </c>
       <c r="U21" t="n">
-        <v>0.95</v>
+        <v>21.55</v>
       </c>
       <c r="V21" t="n">
-        <v>-373.876984</v>
+        <v>8481.104216</v>
       </c>
       <c r="W21" t="inlineStr">
         <is>
           <t>LOW – Stable</t>
-        </is>
-      </c>
-      <c r="X21" t="inlineStr">
-        <is>
-          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2271,11 +2166,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X22" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2344,22 +2234,17 @@
         </is>
       </c>
       <c r="T23" t="n">
-        <v>9.6</v>
+        <v>-10.51</v>
       </c>
       <c r="U23" t="n">
-        <v>48</v>
+        <v>52.55</v>
       </c>
       <c r="V23" t="n">
-        <v>34143.38496</v>
+        <v>-37379.893326</v>
       </c>
       <c r="W23" t="inlineStr">
         <is>
           <t>MODERATE – Monitor Closely</t>
-        </is>
-      </c>
-      <c r="X23" t="inlineStr">
-        <is>
-          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2437,11 +2322,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X24" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2517,11 +2397,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X25" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2597,11 +2472,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X26" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2670,22 +2540,17 @@
         </is>
       </c>
       <c r="T27" t="n">
-        <v>-18.44</v>
+        <v>-10.57</v>
       </c>
       <c r="U27" t="n">
-        <v>92.2</v>
+        <v>52.84999999999999</v>
       </c>
       <c r="V27" t="n">
-        <v>-109155.670356</v>
+        <v>-62569.166793</v>
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>CRITICAL – Immediate Action</t>
-        </is>
-      </c>
-      <c r="X27" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>MODERATE – Monitor Closely</t>
         </is>
       </c>
     </row>
@@ -2756,22 +2621,17 @@
         </is>
       </c>
       <c r="T28" t="n">
-        <v>-18.95</v>
+        <v>-17.56</v>
       </c>
       <c r="U28" t="n">
-        <v>94.75</v>
+        <v>87.79999999999998</v>
       </c>
       <c r="V28" t="n">
-        <v>-73977.35299499999</v>
+        <v>-68551.04583599999</v>
       </c>
       <c r="W28" t="inlineStr">
         <is>
           <t>CRITICAL – Immediate Action</t>
-        </is>
-      </c>
-      <c r="X28" t="inlineStr">
-        <is>
-          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2842,22 +2702,17 @@
         </is>
       </c>
       <c r="T29" t="n">
-        <v>-1.6</v>
+        <v>-2.03</v>
       </c>
       <c r="U29" t="n">
-        <v>8</v>
+        <v>10.15</v>
       </c>
       <c r="V29" t="n">
-        <v>-2052.30064</v>
+        <v>-2603.856437</v>
       </c>
       <c r="W29" t="inlineStr">
         <is>
           <t>LOW – Stable</t>
-        </is>
-      </c>
-      <c r="X29" t="inlineStr">
-        <is>
-          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2928,22 +2783,17 @@
         </is>
       </c>
       <c r="T30" t="n">
-        <v>-2.91</v>
+        <v>-10.39</v>
       </c>
       <c r="U30" t="n">
-        <v>14.55</v>
+        <v>51.95000000000001</v>
       </c>
       <c r="V30" t="n">
-        <v>-15540.11295</v>
+        <v>-55485.14555</v>
       </c>
       <c r="W30" t="inlineStr">
         <is>
-          <t>LOW – Stable</t>
-        </is>
-      </c>
-      <c r="X30" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>MODERATE – Monitor Closely</t>
         </is>
       </c>
     </row>
@@ -3021,11 +2871,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X31" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3094,22 +2939,17 @@
         </is>
       </c>
       <c r="T32" t="n">
-        <v>9.08</v>
+        <v>3.1</v>
       </c>
       <c r="U32" t="n">
-        <v>45.4</v>
+        <v>15.5</v>
       </c>
       <c r="V32" t="n">
-        <v>54151.20684400001</v>
+        <v>18487.74683</v>
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>MODERATE – Monitor Closely</t>
-        </is>
-      </c>
-      <c r="X32" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>LOW – Stable</t>
         </is>
       </c>
     </row>
@@ -3187,11 +3027,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X33" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3260,22 +3095,17 @@
         </is>
       </c>
       <c r="T34" t="n">
-        <v>-16.29</v>
+        <v>-17.92</v>
       </c>
       <c r="U34" t="n">
-        <v>81.45</v>
+        <v>89.60000000000001</v>
       </c>
       <c r="V34" t="n">
-        <v>-93548.164347</v>
+        <v>-102908.723456</v>
       </c>
       <c r="W34" t="inlineStr">
         <is>
           <t>CRITICAL – Immediate Action</t>
-        </is>
-      </c>
-      <c r="X34" t="inlineStr">
-        <is>
-          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3353,11 +3183,6 @@
           <t>LOW – Stable</t>
         </is>
       </c>
-      <c r="X35" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3426,22 +3251,17 @@
         </is>
       </c>
       <c r="T36" t="n">
-        <v>-20.61</v>
+        <v>-21.28</v>
       </c>
       <c r="U36" t="n">
         <v>100</v>
       </c>
       <c r="V36" t="n">
-        <v>-73085.329161</v>
+        <v>-75461.222928</v>
       </c>
       <c r="W36" t="inlineStr">
         <is>
           <t>CRITICAL – Immediate Action</t>
-        </is>
-      </c>
-      <c r="X36" t="inlineStr">
-        <is>
-          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3456,7 +3276,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3479,71 +3299,111 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pace_Ratio</t>
+          <t>Budget_Pct</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8767043416575715</v>
+        <v>0.4243173945580014</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DSP_enc</t>
+          <t>Gap_Pct</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.03902579892808492</v>
+        <v>0.4213112563496177</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Spend_Velocity</t>
+          <t>Acceleration</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.03885957600547516</v>
+        <v>0.06059531511456343</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Spend_to_Date</t>
+          <t>Spend_Velocity</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.02013960227352946</v>
+        <v>0.02982975275704113</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Total_Budget</t>
+          <t>DSP_enc</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0131773290904567</v>
+        <v>0.0185569584511927</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Flight_Days</t>
+          <t>Total_Budget</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.006460673297380543</v>
+        <v>0.0134733367276791</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Time_Pct</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.01223233831247451</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Spend_to_Date</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.01064231977620999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Days_Remaining</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.003280289219582662</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Flight_Days</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.00323182397208861</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>Days_Elapsed</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>0.005632678747501668</v>
+      <c r="B12" t="n">
+        <v>0.002529214761548717</v>
       </c>
     </row>
   </sheetData>
@@ -3584,7 +3444,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.045</v>
+        <v>0.0463</v>
       </c>
     </row>
     <row r="3">
@@ -3594,7 +3454,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-416446.94</v>
+        <v>-579240.38</v>
       </c>
     </row>
     <row r="4">
@@ -3605,7 +3465,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2026-02-16 07:38 UTC</t>
+          <t>2026-02-16 08:03 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto refresh - 16-02-2026 15:26:23.45
</commit_message>
<xml_diff>
--- a/PaceSmart_ML_vs_Excel_Output.xlsx
+++ b/PaceSmart_ML_vs_Excel_Output.xlsx
@@ -517,22 +517,22 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
+          <t>DSP_meta</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Total_Budget_meta</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>Flight_Start_Date_meta</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Flight_End_Date_meta</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Total_Budget_meta</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>DSP_meta</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
@@ -608,20 +608,10 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P2" s="2" t="n">
-        <v>46025</v>
-      </c>
-      <c r="Q2" s="2" t="n">
-        <v>46049</v>
-      </c>
-      <c r="R2" t="n">
-        <v>100350.37</v>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
@@ -683,20 +673,10 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P3" s="2" t="n">
-        <v>46021</v>
-      </c>
-      <c r="Q3" s="2" t="n">
-        <v>46057</v>
-      </c>
-      <c r="R3" t="n">
-        <v>552594.63</v>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>DV360</t>
-        </is>
-      </c>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
@@ -758,20 +738,10 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P4" s="2" t="n">
-        <v>46030</v>
-      </c>
-      <c r="Q4" s="2" t="n">
-        <v>46063</v>
-      </c>
-      <c r="R4" t="n">
-        <v>294540.38</v>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
@@ -833,32 +803,16 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P5" s="2" t="n">
-        <v>46055</v>
-      </c>
-      <c r="Q5" s="2" t="n">
-        <v>46081</v>
-      </c>
-      <c r="R5" t="n">
-        <v>509097.37</v>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
-      <c r="T5" t="n">
-        <v>-18.51</v>
-      </c>
-      <c r="U5" t="n">
-        <v>92.55000000000001</v>
-      </c>
-      <c r="V5" t="n">
-        <v>-94233.92318700001</v>
-      </c>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr">
         <is>
-          <t>CRITICAL – Immediate Action</t>
+          <t>LOW – Stable</t>
         </is>
       </c>
     </row>
@@ -914,20 +868,10 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P6" s="2" t="n">
-        <v>46010</v>
-      </c>
-      <c r="Q6" s="2" t="n">
-        <v>46052</v>
-      </c>
-      <c r="R6" t="n">
-        <v>382409.25</v>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>DV360</t>
-        </is>
-      </c>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
@@ -989,20 +933,10 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P7" s="2" t="n">
-        <v>46030</v>
-      </c>
-      <c r="Q7" s="2" t="n">
-        <v>46050</v>
-      </c>
-      <c r="R7" t="n">
-        <v>525695.9399999999</v>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>DV360</t>
-        </is>
-      </c>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
@@ -1064,20 +998,10 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P8" s="2" t="n">
-        <v>46019</v>
-      </c>
-      <c r="Q8" s="2" t="n">
-        <v>46048</v>
-      </c>
-      <c r="R8" t="n">
-        <v>136840.92</v>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
@@ -1139,20 +1063,10 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P9" s="2" t="n">
-        <v>46014</v>
-      </c>
-      <c r="Q9" s="2" t="n">
-        <v>46058</v>
-      </c>
-      <c r="R9" t="n">
-        <v>448858.15</v>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
@@ -1214,20 +1128,10 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P10" s="2" t="n">
-        <v>46030</v>
-      </c>
-      <c r="Q10" s="2" t="n">
-        <v>46064</v>
-      </c>
-      <c r="R10" t="n">
-        <v>559806.73</v>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
@@ -1289,20 +1193,10 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P11" s="2" t="n">
-        <v>46015</v>
-      </c>
-      <c r="Q11" s="2" t="n">
-        <v>46059</v>
-      </c>
-      <c r="R11" t="n">
-        <v>169377.54</v>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
@@ -1364,20 +1258,10 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P12" s="2" t="n">
-        <v>46020</v>
-      </c>
-      <c r="Q12" s="2" t="n">
-        <v>46056</v>
-      </c>
-      <c r="R12" t="n">
-        <v>334936.09</v>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
@@ -1439,32 +1323,16 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P13" s="2" t="n">
-        <v>46064</v>
-      </c>
-      <c r="Q13" s="2" t="n">
-        <v>46090</v>
-      </c>
-      <c r="R13" t="n">
-        <v>161605.1</v>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>DV360</t>
-        </is>
-      </c>
-      <c r="T13" t="n">
-        <v>-10.37</v>
-      </c>
-      <c r="U13" t="n">
-        <v>51.84999999999999</v>
-      </c>
-      <c r="V13" t="n">
-        <v>-16758.44887</v>
-      </c>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
       <c r="W13" t="inlineStr">
         <is>
-          <t>MODERATE – Monitor Closely</t>
+          <t>LOW – Stable</t>
         </is>
       </c>
     </row>
@@ -1520,20 +1388,10 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P14" s="2" t="n">
-        <v>46018</v>
-      </c>
-      <c r="Q14" s="2" t="n">
-        <v>46061</v>
-      </c>
-      <c r="R14" t="n">
-        <v>95583.81</v>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
@@ -1595,32 +1453,16 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P15" s="2" t="n">
-        <v>46056</v>
-      </c>
-      <c r="Q15" s="2" t="n">
-        <v>46098</v>
-      </c>
-      <c r="R15" t="n">
-        <v>423679.91</v>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>DV360</t>
-        </is>
-      </c>
-      <c r="T15" t="n">
-        <v>-9.32</v>
-      </c>
-      <c r="U15" t="n">
-        <v>46.6</v>
-      </c>
-      <c r="V15" t="n">
-        <v>-39486.967612</v>
-      </c>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
       <c r="W15" t="inlineStr">
         <is>
-          <t>MODERATE – Monitor Closely</t>
+          <t>LOW – Stable</t>
         </is>
       </c>
     </row>
@@ -1676,32 +1518,16 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P16" s="2" t="n">
-        <v>46058</v>
-      </c>
-      <c r="Q16" s="2" t="n">
-        <v>46076</v>
-      </c>
-      <c r="R16" t="n">
-        <v>105951.07</v>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
-      <c r="T16" t="n">
-        <v>-18.78</v>
-      </c>
-      <c r="U16" t="n">
-        <v>93.90000000000001</v>
-      </c>
-      <c r="V16" t="n">
-        <v>-19897.610946</v>
-      </c>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
       <c r="W16" t="inlineStr">
         <is>
-          <t>CRITICAL – Immediate Action</t>
+          <t>LOW – Stable</t>
         </is>
       </c>
     </row>
@@ -1757,20 +1583,10 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P17" s="2" t="n">
-        <v>46023</v>
-      </c>
-      <c r="Q17" s="2" t="n">
-        <v>46050</v>
-      </c>
-      <c r="R17" t="n">
-        <v>280248.59</v>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr"/>
@@ -1832,32 +1648,16 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P18" s="2" t="n">
-        <v>46064</v>
-      </c>
-      <c r="Q18" s="2" t="n">
-        <v>46079</v>
-      </c>
-      <c r="R18" t="n">
-        <v>285863.23</v>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
-      <c r="T18" t="n">
-        <v>-10.8</v>
-      </c>
-      <c r="U18" t="n">
-        <v>54</v>
-      </c>
-      <c r="V18" t="n">
-        <v>-30873.22884</v>
-      </c>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
       <c r="W18" t="inlineStr">
         <is>
-          <t>MODERATE – Monitor Closely</t>
+          <t>LOW – Stable</t>
         </is>
       </c>
     </row>
@@ -1913,20 +1713,10 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P19" s="2" t="n">
-        <v>46027</v>
-      </c>
-      <c r="Q19" s="2" t="n">
-        <v>46059</v>
-      </c>
-      <c r="R19" t="n">
-        <v>221171.06</v>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
@@ -1988,20 +1778,10 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P20" s="2" t="n">
-        <v>46020</v>
-      </c>
-      <c r="Q20" s="2" t="n">
-        <v>46054</v>
-      </c>
-      <c r="R20" t="n">
-        <v>577808.88</v>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr"/>
@@ -2063,29 +1843,13 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P21" s="2" t="n">
-        <v>46056</v>
-      </c>
-      <c r="Q21" s="2" t="n">
-        <v>46074</v>
-      </c>
-      <c r="R21" t="n">
-        <v>196777.36</v>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
-      <c r="T21" t="n">
-        <v>4.31</v>
-      </c>
-      <c r="U21" t="n">
-        <v>21.55</v>
-      </c>
-      <c r="V21" t="n">
-        <v>8481.104216</v>
-      </c>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
       <c r="W21" t="inlineStr">
         <is>
           <t>LOW – Stable</t>
@@ -2144,20 +1908,10 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P22" s="2" t="n">
-        <v>46027</v>
-      </c>
-      <c r="Q22" s="2" t="n">
-        <v>46063</v>
-      </c>
-      <c r="R22" t="n">
-        <v>170730.01</v>
-      </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
@@ -2219,32 +1973,16 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P23" s="2" t="n">
-        <v>46061</v>
-      </c>
-      <c r="Q23" s="2" t="n">
-        <v>46098</v>
-      </c>
-      <c r="R23" t="n">
-        <v>355660.26</v>
-      </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
-      <c r="T23" t="n">
-        <v>-10.51</v>
-      </c>
-      <c r="U23" t="n">
-        <v>52.55</v>
-      </c>
-      <c r="V23" t="n">
-        <v>-37379.893326</v>
-      </c>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr">
         <is>
-          <t>MODERATE – Monitor Closely</t>
+          <t>LOW – Stable</t>
         </is>
       </c>
     </row>
@@ -2300,20 +2038,10 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P24" s="2" t="n">
-        <v>46018</v>
-      </c>
-      <c r="Q24" s="2" t="n">
-        <v>46055</v>
-      </c>
-      <c r="R24" t="n">
-        <v>418857.39</v>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr"/>
       <c r="V24" t="inlineStr"/>
@@ -2375,20 +2103,10 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P25" s="2" t="n">
-        <v>46018</v>
-      </c>
-      <c r="Q25" s="2" t="n">
-        <v>46057</v>
-      </c>
-      <c r="R25" t="n">
-        <v>574740.27</v>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>DV360</t>
-        </is>
-      </c>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr"/>
@@ -2450,20 +2168,10 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P26" s="2" t="n">
-        <v>46016</v>
-      </c>
-      <c r="Q26" s="2" t="n">
-        <v>46054</v>
-      </c>
-      <c r="R26" t="n">
-        <v>129356.97</v>
-      </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr"/>
@@ -2525,32 +2233,16 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P27" s="2" t="n">
-        <v>46064</v>
-      </c>
-      <c r="Q27" s="2" t="n">
-        <v>46083</v>
-      </c>
-      <c r="R27" t="n">
-        <v>591950.49</v>
-      </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
-      <c r="T27" t="n">
-        <v>-10.57</v>
-      </c>
-      <c r="U27" t="n">
-        <v>52.84999999999999</v>
-      </c>
-      <c r="V27" t="n">
-        <v>-62569.166793</v>
-      </c>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" t="inlineStr"/>
+      <c r="V27" t="inlineStr"/>
       <c r="W27" t="inlineStr">
         <is>
-          <t>MODERATE – Monitor Closely</t>
+          <t>LOW – Stable</t>
         </is>
       </c>
     </row>
@@ -2606,32 +2298,16 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P28" s="2" t="n">
-        <v>46061</v>
-      </c>
-      <c r="Q28" s="2" t="n">
-        <v>46084</v>
-      </c>
-      <c r="R28" t="n">
-        <v>390381.81</v>
-      </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
-      <c r="T28" t="n">
-        <v>-17.56</v>
-      </c>
-      <c r="U28" t="n">
-        <v>87.79999999999998</v>
-      </c>
-      <c r="V28" t="n">
-        <v>-68551.04583599999</v>
-      </c>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
       <c r="W28" t="inlineStr">
         <is>
-          <t>CRITICAL – Immediate Action</t>
+          <t>LOW – Stable</t>
         </is>
       </c>
     </row>
@@ -2687,29 +2363,13 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P29" s="2" t="n">
-        <v>46054</v>
-      </c>
-      <c r="Q29" s="2" t="n">
-        <v>46080</v>
-      </c>
-      <c r="R29" t="n">
-        <v>128268.79</v>
-      </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>DV360</t>
-        </is>
-      </c>
-      <c r="T29" t="n">
-        <v>-2.03</v>
-      </c>
-      <c r="U29" t="n">
-        <v>10.15</v>
-      </c>
-      <c r="V29" t="n">
-        <v>-2603.856437</v>
-      </c>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
       <c r="W29" t="inlineStr">
         <is>
           <t>LOW – Stable</t>
@@ -2768,32 +2428,16 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P30" s="2" t="n">
-        <v>46056</v>
-      </c>
-      <c r="Q30" s="2" t="n">
-        <v>46097</v>
-      </c>
-      <c r="R30" t="n">
-        <v>534024.5</v>
-      </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
-      <c r="T30" t="n">
-        <v>-10.39</v>
-      </c>
-      <c r="U30" t="n">
-        <v>51.95000000000001</v>
-      </c>
-      <c r="V30" t="n">
-        <v>-55485.14555</v>
-      </c>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
       <c r="W30" t="inlineStr">
         <is>
-          <t>MODERATE – Monitor Closely</t>
+          <t>LOW – Stable</t>
         </is>
       </c>
     </row>
@@ -2849,20 +2493,10 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P31" s="2" t="n">
-        <v>46024</v>
-      </c>
-      <c r="Q31" s="2" t="n">
-        <v>46064</v>
-      </c>
-      <c r="R31" t="n">
-        <v>391196.57</v>
-      </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
       <c r="V31" t="inlineStr"/>
@@ -2924,29 +2558,13 @@
           <t>Overpacing</t>
         </is>
       </c>
-      <c r="P32" s="2" t="n">
-        <v>46050</v>
-      </c>
-      <c r="Q32" s="2" t="n">
-        <v>46087</v>
-      </c>
-      <c r="R32" t="n">
-        <v>596378.9300000001</v>
-      </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
-      <c r="T32" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="U32" t="n">
-        <v>15.5</v>
-      </c>
-      <c r="V32" t="n">
-        <v>18487.74683</v>
-      </c>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr"/>
+      <c r="T32" t="inlineStr"/>
+      <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr"/>
       <c r="W32" t="inlineStr">
         <is>
           <t>LOW – Stable</t>
@@ -3005,20 +2623,10 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P33" s="2" t="n">
-        <v>46029</v>
-      </c>
-      <c r="Q33" s="2" t="n">
-        <v>46054</v>
-      </c>
-      <c r="R33" t="n">
-        <v>120089.45</v>
-      </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>Yahoo</t>
-        </is>
-      </c>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
       <c r="V33" t="inlineStr"/>
@@ -3080,32 +2688,16 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P34" s="2" t="n">
-        <v>46054</v>
-      </c>
-      <c r="Q34" s="2" t="n">
-        <v>46095</v>
-      </c>
-      <c r="R34" t="n">
-        <v>574267.4300000001</v>
-      </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
-      <c r="T34" t="n">
-        <v>-17.92</v>
-      </c>
-      <c r="U34" t="n">
-        <v>89.60000000000001</v>
-      </c>
-      <c r="V34" t="n">
-        <v>-102908.723456</v>
-      </c>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr"/>
+      <c r="T34" t="inlineStr"/>
+      <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
       <c r="W34" t="inlineStr">
         <is>
-          <t>CRITICAL – Immediate Action</t>
+          <t>LOW – Stable</t>
         </is>
       </c>
     </row>
@@ -3161,20 +2753,10 @@
           <t>On Track</t>
         </is>
       </c>
-      <c r="P35" s="2" t="n">
-        <v>46023</v>
-      </c>
-      <c r="Q35" s="2" t="n">
-        <v>46063</v>
-      </c>
-      <c r="R35" t="n">
-        <v>352257.46</v>
-      </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr"/>
       <c r="V35" t="inlineStr"/>
@@ -3236,32 +2818,16 @@
           <t>Underpacing</t>
         </is>
       </c>
-      <c r="P36" s="2" t="n">
-        <v>46050</v>
-      </c>
-      <c r="Q36" s="2" t="n">
-        <v>46090</v>
-      </c>
-      <c r="R36" t="n">
-        <v>354611.01</v>
-      </c>
-      <c r="S36" t="inlineStr">
-        <is>
-          <t>Amazon DSP</t>
-        </is>
-      </c>
-      <c r="T36" t="n">
-        <v>-21.28</v>
-      </c>
-      <c r="U36" t="n">
-        <v>100</v>
-      </c>
-      <c r="V36" t="n">
-        <v>-75461.222928</v>
-      </c>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr"/>
+      <c r="T36" t="inlineStr"/>
+      <c r="U36" t="inlineStr"/>
+      <c r="V36" t="inlineStr"/>
       <c r="W36" t="inlineStr">
         <is>
-          <t>CRITICAL – Immediate Action</t>
+          <t>LOW – Stable</t>
         </is>
       </c>
     </row>
@@ -3299,111 +2865,111 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Budget_Pct</t>
+          <t>Days_Remaining</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4243173945580014</v>
+        <v>0.2787783402760992</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Gap_Pct</t>
+          <t>Flight_Days</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4213112563496177</v>
+        <v>0.263697424323086</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Acceleration</t>
+          <t>Days_Elapsed</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.06059531511456343</v>
+        <v>0.1903035724284907</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Spend_Velocity</t>
+          <t>Total_Budget</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.02982975275704113</v>
+        <v>0.1701008344279234</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DSP_enc</t>
+          <t>Gap_Pct</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0185569584511927</v>
+        <v>0.05106095104037819</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Total_Budget</t>
+          <t>Time_Pct</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0134733367276791</v>
+        <v>0.03578353437387945</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Time_Pct</t>
+          <t>DSP_enc</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.01223233831247451</v>
+        <v>0.01027534313014306</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Spend_to_Date</t>
+          <t>Spend_Velocity</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.01064231977620999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Days_Remaining</t>
+          <t>Spend_to_Date</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.003280289219582662</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Flight_Days</t>
+          <t>Acceleration</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.00323182397208861</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Days_Elapsed</t>
+          <t>Budget_Pct</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.002529214761548717</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3444,7 +3010,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0463</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -3454,7 +3020,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-579240.38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -3465,7 +3031,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2026-02-16 08:03 UTC</t>
+          <t>2026-02-16 09:56 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>